<commit_message>
Common: Added cell-types to mods
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD7D390-720A-E54A-9D04-1D765EFB8B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75241726-5D4F-A345-AE8A-1F43825D9E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -3305,7 +3305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -3484,8 +3484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243831E-E3E3-1C43-AE4D-34D8FEF2F724}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3574,7 +3574,7 @@
         <v>775</v>
       </c>
       <c r="F4" s="11">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Common: Some new interesting stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F10253-0BCE-C347-A3FB-6BA04340C1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F893317B-4232-1448-853B-0F4F692F51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="947">
   <si>
     <t>cs</t>
   </si>
@@ -2909,6 +2909,21 @@
   </si>
   <si>
     <t>Richmond</t>
+  </si>
+  <si>
+    <t>draws</t>
+  </si>
+  <si>
+    <t>DL, MTL</t>
+  </si>
+  <si>
+    <t>market.filter.type.label</t>
+  </si>
+  <si>
+    <t>Typ článku</t>
+  </si>
+  <si>
+    <t>market.filter.cell.off.label</t>
   </si>
 </sst>
 </file>
@@ -3627,7 +3642,7 @@
   <dimension ref="A1:A98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4126,6 +4141,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A98">
+    <sortCondition ref="A18:A98"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="A59" r:id="rId1" display="https://www.eliquidshop.cz/my-vape/" xr:uid="{6FAF1889-3DC2-2045-966A-88495D335037}"/>
   </hyperlinks>
@@ -4308,8 +4326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4335,10 +4353,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>241</v>
+        <v>573</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>242</v>
+        <v>574</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4346,10 +4364,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>269</v>
+        <v>575</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>270</v>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4357,10 +4375,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4368,10 +4386,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4379,10 +4397,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -4390,10 +4408,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4401,10 +4419,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>303</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4412,10 +4430,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4423,10 +4441,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4434,10 +4452,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>252</v>
+        <v>545</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>255</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4445,10 +4463,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>259</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4456,10 +4474,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>314</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>266</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -4467,10 +4485,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>312</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>134</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4478,10 +4496,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -4489,21 +4507,21 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>465</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4511,10 +4529,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>307</v>
+        <v>389</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>352</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4522,21 +4540,21 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>311</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4544,10 +4562,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4555,10 +4573,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4566,10 +4584,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>467</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4577,10 +4595,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -4599,10 +4617,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4610,10 +4628,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>248</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4632,10 +4650,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>329</v>
+        <v>467</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4654,10 +4672,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>332</v>
+        <v>557</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>320</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4665,10 +4683,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>333</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>334</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -4676,10 +4694,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>335</v>
+        <v>254</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -4687,10 +4705,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>389</v>
+        <v>256</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -4698,10 +4716,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>545</v>
+        <v>252</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>546</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -4709,10 +4727,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>557</v>
+        <v>258</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -4742,10 +4760,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>573</v>
+        <v>648</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>574</v>
+        <v>649</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -4753,10 +4771,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>575</v>
+        <v>265</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>576</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -4764,13 +4782,16 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>648</v>
+        <v>133</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>649</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
+    <sortCondition ref="B26:B41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4824,7 +4845,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4900,15 +4921,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4916,10 +4937,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4927,10 +4948,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4949,21 +4970,21 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4971,21 +4992,21 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="225" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4993,21 +5014,21 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5021,15 +5042,15 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>360</v>
+        <v>529</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>367</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -5037,32 +5058,32 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>355</v>
+        <v>532</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="225" x14ac:dyDescent="0.2">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="180" x14ac:dyDescent="0.2">
@@ -5081,10 +5102,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>529</v>
+        <v>350</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>530</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -5092,13 +5113,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>532</v>
+        <v>353</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>531</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="B21:B24"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5108,8 +5132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5957,7 +5981,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
-    <sortCondition ref="B71:B76"/>
+    <sortCondition ref="B51:B76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5969,7 +5993,7 @@
   <dimension ref="A1:C96"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6512,21 +6536,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>324</v>
+        <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>361</v>
+        <v>34</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>362</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -6534,21 +6558,21 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>280</v>
+        <v>324</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>282</v>
+        <v>361</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>283</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -6556,10 +6580,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -6567,10 +6591,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>32</v>
+        <v>282</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>33</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -6578,10 +6602,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>34</v>
+        <v>287</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>33</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -7037,7 +7061,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
-    <sortCondition ref="B87:B96"/>
+    <sortCondition ref="B85:B96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7931,7 +7955,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8056,10 +8080,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>338</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -8067,32 +8091,32 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -8100,10 +8124,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -8111,10 +8135,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -8122,10 +8146,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -8133,10 +8157,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -8144,10 +8168,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -8155,10 +8179,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -8166,10 +8190,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -8177,10 +8201,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -8188,10 +8212,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -8199,10 +8223,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -8210,10 +8234,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -8221,10 +8245,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -8232,10 +8256,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -8243,10 +8267,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -8254,10 +8278,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -8265,10 +8289,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -8276,10 +8300,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -8287,10 +8311,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -8298,10 +8322,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -8309,10 +8333,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -8320,10 +8344,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -8331,10 +8355,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -8342,10 +8366,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -8353,10 +8377,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -8364,10 +8388,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -8375,10 +8399,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -8386,10 +8410,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -8397,10 +8421,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -8408,10 +8432,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -8419,10 +8443,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -8430,10 +8454,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -8441,10 +8465,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -8452,10 +8476,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -8463,10 +8487,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -8474,10 +8498,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -8485,10 +8509,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -8496,10 +8520,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>156</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -8507,10 +8531,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -8518,10 +8542,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -8529,10 +8553,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -8540,10 +8564,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -8551,10 +8575,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -8562,10 +8586,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -8573,10 +8597,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -8584,23 +8608,26 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>338</v>
+        <v>148</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>339</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C59">
+    <sortCondition ref="B6:B59"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8626,21 +8653,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>375</v>
+        <v>498</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>376</v>
+        <v>496</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>377</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -8648,10 +8675,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>378</v>
+        <v>494</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -8659,10 +8686,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>379</v>
+        <v>499</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -8670,10 +8697,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>380</v>
+        <v>485</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>341</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -8681,10 +8708,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>381</v>
+        <v>480</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>235</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -8692,21 +8719,21 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>238</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -8714,10 +8741,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>237</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -8725,10 +8752,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>235</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -8736,10 +8763,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>386</v>
+        <v>423</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>236</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -8747,10 +8774,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>387</v>
+        <v>421</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>238</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -8758,10 +8785,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>388</v>
+        <v>419</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>237</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -8769,10 +8796,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>273</v>
+        <v>426</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -8780,10 +8807,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>392</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -8791,21 +8818,21 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>447</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -8813,21 +8840,21 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>396</v>
+        <v>512</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>419</v>
+        <v>510</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>420</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -8835,10 +8862,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>421</v>
+        <v>508</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>422</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -8846,10 +8873,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>423</v>
+        <v>513</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>424</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -8857,10 +8884,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>425</v>
+        <v>487</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>426</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -8868,32 +8895,32 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>427</v>
+        <v>484</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>429</v>
+        <v>505</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>430</v>
+        <v>503</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>431</v>
+        <v>504</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -8901,10 +8928,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>432</v>
+        <v>501</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>433</v>
+        <v>502</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -8912,21 +8939,21 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>434</v>
+        <v>506</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>436</v>
+        <v>486</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>445</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -8934,10 +8961,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>437</v>
+        <v>482</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>431</v>
+        <v>483</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -8945,32 +8972,32 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -8978,10 +9005,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -8989,10 +9016,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>448</v>
+        <v>388</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>449</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -9000,10 +9027,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>458</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -9011,32 +9038,32 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -9044,10 +9071,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -9055,10 +9082,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>461</v>
+        <v>387</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>459</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -9066,10 +9093,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>462</v>
+        <v>383</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>460</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -9077,10 +9104,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>463</v>
+        <v>652</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>464</v>
+        <v>653</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -9088,10 +9115,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>468</v>
+        <v>656</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>469</v>
+        <v>655</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -9099,10 +9126,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>470</v>
+        <v>650</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>471</v>
+        <v>651</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -9110,10 +9137,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>472</v>
+        <v>654</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>473</v>
+        <v>655</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -9121,10 +9148,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>474</v>
+        <v>378</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>475</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -9132,10 +9159,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>476</v>
+        <v>376</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>477</v>
+        <v>377</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -9143,10 +9170,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>478</v>
+        <v>380</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>479</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -9154,10 +9181,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>480</v>
+        <v>375</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>481</v>
+        <v>341</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -9165,10 +9192,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>482</v>
+        <v>379</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>483</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -9176,21 +9203,21 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>484</v>
+        <v>437</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>485</v>
+        <v>436</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>481</v>
+        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -9198,10 +9225,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>486</v>
+        <v>434</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>483</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -9209,10 +9236,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>487</v>
+        <v>438</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>240</v>
+        <v>439</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -9220,21 +9247,21 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>494</v>
+        <v>386</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>496</v>
+        <v>382</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -9242,21 +9269,21 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>499</v>
+        <v>454</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>500</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -9264,21 +9291,21 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>501</v>
+        <v>452</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -9286,10 +9313,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>505</v>
+        <v>476</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>431</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -9297,10 +9324,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -9308,21 +9335,21 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>508</v>
+        <v>451</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>510</v>
+        <v>450</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>511</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9330,10 +9357,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>512</v>
+        <v>461</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>431</v>
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -9341,10 +9368,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>514</v>
+        <v>471</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -9352,10 +9379,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>650</v>
+        <v>462</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>651</v>
+        <v>460</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -9363,10 +9390,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>652</v>
+        <v>468</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>653</v>
+        <v>469</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -9374,10 +9401,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>654</v>
+        <v>472</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>655</v>
+        <v>473</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -9385,13 +9412,38 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>656</v>
+        <v>463</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>655</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C71">
+    <sortCondition ref="B45:B71"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10177,7 +10229,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10201,7 +10253,7 @@
         <v>772</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>797</v>
+        <v>942</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>835</v>
@@ -10607,7 +10659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D757F10-66C2-2941-A49E-7F0FD3F6574C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -10785,10 +10837,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F5805-0158-F34C-9256-85EB751C6431}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10797,7 +10849,7 @@
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>670</v>
       </c>
@@ -10805,149 +10857,176 @@
         <v>659</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>743</v>
       </c>
       <c r="B2" t="s">
         <v>809</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>943</v>
+      </c>
+      <c r="D2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>745</v>
       </c>
       <c r="B3" t="s">
         <v>810</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>689</v>
       </c>
       <c r="B4" t="s">
         <v>811</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>943</v>
+      </c>
+      <c r="D4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>759</v>
       </c>
       <c r="B5" t="s">
         <v>812</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>840</v>
+      </c>
+      <c r="D5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>685</v>
       </c>
       <c r="B6" t="s">
         <v>685</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>840</v>
+      </c>
+      <c r="D6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>689</v>
       </c>
       <c r="B7" t="s">
         <v>813</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>686</v>
       </c>
       <c r="B8" t="s">
         <v>686</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>943</v>
+      </c>
+      <c r="D8">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>749</v>
       </c>
       <c r="B9" t="s">
         <v>814</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>707</v>
       </c>
       <c r="B10" t="s">
         <v>815</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>757</v>
       </c>
       <c r="B11" t="s">
         <v>816</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>721</v>
       </c>
       <c r="B12" t="s">
         <v>817</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>943</v>
+      </c>
+      <c r="D12">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>721</v>
       </c>
       <c r="B13" t="s">
         <v>818</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>943</v>
+      </c>
+      <c r="D13">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>705</v>
       </c>
       <c r="B14" t="s">
         <v>819</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Improved liquid listing
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F893317B-4232-1448-853B-0F4F692F51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ACEEE3-5B5A-1442-942D-5C89A73BD53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="957">
   <si>
     <t>cs</t>
   </si>
@@ -2924,6 +2924,36 @@
   </si>
   <si>
     <t>market.filter.cell.off.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.age.tooltip</t>
+  </si>
+  <si>
+    <t>Stáří liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.steeping.tooltip</t>
+  </si>
+  <si>
+    <t>lab.liquid.nicotine.tooltip</t>
+  </si>
+  <si>
+    <t>Množství nikotinu obsaženého v liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.steep.done</t>
+  </si>
+  <si>
+    <t>Zrání dokončeno</t>
+  </si>
+  <si>
+    <t>lab.liquid.steep.done.tooltip</t>
+  </si>
+  <si>
+    <t>Liquid je uzrálý (datum míchání {{data.mixed}})</t>
+  </si>
+  <si>
+    <t>Doba zrání liquidu (datum míchání {{data.mixed}})</t>
   </si>
 </sst>
 </file>
@@ -5130,10 +5160,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5423,10 +5453,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>559</v>
+        <v>947</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>560</v>
+        <v>948</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -5434,10 +5464,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -5445,10 +5475,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -5456,10 +5486,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>240</v>
+        <v>570</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -5467,10 +5497,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>585</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -5478,10 +5508,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>571</v>
+        <v>584</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -5489,10 +5519,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>614</v>
+        <v>571</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>615</v>
+        <v>572</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -5500,10 +5530,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>636</v>
+        <v>614</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>637</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -5511,10 +5541,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -5522,10 +5552,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>542</v>
+        <v>616</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>543</v>
+        <v>617</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -5533,10 +5563,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>642</v>
+        <v>542</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>643</v>
+        <v>543</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -5544,10 +5574,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>596</v>
+        <v>642</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>611</v>
+        <v>643</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -5555,10 +5585,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>567</v>
+        <v>611</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -5566,10 +5596,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>594</v>
+        <v>641</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -5577,10 +5607,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>535</v>
+        <v>594</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>544</v>
+        <v>595</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -5588,21 +5618,21 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>558</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5610,10 +5640,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5621,10 +5651,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>601</v>
+        <v>633</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>602</v>
+        <v>638</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5632,10 +5662,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5643,10 +5673,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5654,10 +5684,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5665,10 +5695,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5676,21 +5706,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>624</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -5698,32 +5728,32 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -5731,10 +5761,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>233</v>
+        <v>547</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>234</v>
+        <v>548</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -5742,10 +5772,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>540</v>
+        <v>233</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>541</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -5753,10 +5783,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>639</v>
+        <v>540</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>640</v>
+        <v>541</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -5764,10 +5794,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>537</v>
+        <v>639</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>186</v>
+        <v>640</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -5775,32 +5805,32 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>621</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -5808,10 +5838,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>592</v>
+        <v>950</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>593</v>
+        <v>951</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -5819,10 +5849,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -5830,10 +5860,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -5841,10 +5871,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>627</v>
+        <v>591</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>628</v>
+        <v>609</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -5852,10 +5882,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>586</v>
+        <v>625</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>587</v>
+        <v>626</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -5863,10 +5893,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -5874,10 +5904,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>634</v>
+        <v>586</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>635</v>
+        <v>587</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -5885,10 +5915,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -5896,10 +5926,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>588</v>
+        <v>634</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>589</v>
+        <v>635</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -5907,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>646</v>
+        <v>612</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>647</v>
+        <v>613</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -5918,10 +5948,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>538</v>
+        <v>588</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>539</v>
+        <v>589</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -5929,10 +5959,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>533</v>
+        <v>646</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>341</v>
+        <v>647</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -5940,10 +5970,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>521</v>
+        <v>952</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>236</v>
+        <v>953</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -5951,10 +5981,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>519</v>
+        <v>954</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>236</v>
+        <v>955</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -5962,10 +5992,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>493</v>
+        <v>949</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>492</v>
+        <v>956</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -5973,15 +6003,70 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
-    <sortCondition ref="B51:B76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C81">
+    <sortCondition ref="B79:B81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8626,8 +8711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9104,10 +9189,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>652</v>
+        <v>946</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -9115,10 +9200,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -9126,10 +9211,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -9137,10 +9222,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -9148,10 +9233,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>378</v>
+        <v>654</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>655</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -9159,10 +9244,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>376</v>
+        <v>944</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>377</v>
+        <v>945</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -9170,10 +9255,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>341</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -9181,10 +9266,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -9192,10 +9277,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -9203,21 +9288,21 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>445</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -9225,21 +9310,21 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -9247,10 +9332,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>386</v>
+        <v>434</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>236</v>
+        <v>435</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -9258,10 +9343,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>236</v>
+        <v>439</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -9269,21 +9354,21 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>455</v>
+        <v>386</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>454</v>
+        <v>382</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>453</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -9291,21 +9376,21 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -9313,10 +9398,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -9324,10 +9409,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -9335,10 +9420,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>458</v>
+        <v>477</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -9346,10 +9431,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>450</v>
+        <v>478</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9357,10 +9442,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -9368,10 +9453,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -9379,10 +9464,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -9390,10 +9475,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -9401,10 +9486,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -9412,10 +9497,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -9423,10 +9508,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>944</v>
+        <v>472</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>945</v>
+        <v>473</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -9434,15 +9519,15 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>946</v>
+        <v>463</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>655</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C71">
-    <sortCondition ref="B45:B71"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
+    <sortCondition ref="B55:B73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Added universal quick filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ACEEE3-5B5A-1442-942D-5C89A73BD53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE36753-F209-4D4A-995F-916598E82FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="959">
   <si>
     <t>cs</t>
   </si>
@@ -2954,6 +2954,12 @@
   </si>
   <si>
     <t>Doba zrání liquidu (datum míchání {{data.mixed}})</t>
+  </si>
+  <si>
+    <t>lab.liquid.filter.pgvg.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.filter.pgvg.reset</t>
   </si>
 </sst>
 </file>
@@ -5160,10 +5166,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5635,26 +5641,26 @@
         <v>558</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>631</v>
+        <v>957</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>633</v>
+        <v>958</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>638</v>
+        <v>655</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5662,10 +5668,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>601</v>
+        <v>631</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>602</v>
+        <v>632</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5673,10 +5679,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>603</v>
+        <v>633</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>604</v>
+        <v>638</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5684,10 +5690,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5695,10 +5701,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5706,10 +5712,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5717,43 +5723,43 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>623</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -5761,21 +5767,21 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>233</v>
+        <v>549</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>234</v>
+        <v>610</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -5783,10 +5789,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -5794,10 +5800,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>639</v>
+        <v>233</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>640</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -5805,10 +5811,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>186</v>
+        <v>541</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -5816,21 +5822,21 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>618</v>
+        <v>639</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>620</v>
+        <v>537</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>621</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -5838,21 +5844,21 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>950</v>
+        <v>618</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>590</v>
+        <v>620</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>608</v>
+        <v>621</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -5860,10 +5866,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>592</v>
+        <v>950</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>593</v>
+        <v>951</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -5871,10 +5877,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -5882,10 +5888,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -5893,10 +5899,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>627</v>
+        <v>591</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>628</v>
+        <v>609</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -5904,10 +5910,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>586</v>
+        <v>625</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>587</v>
+        <v>626</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -5915,10 +5921,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -5926,10 +5932,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>634</v>
+        <v>586</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>635</v>
+        <v>587</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -5937,10 +5943,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -5948,10 +5954,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>588</v>
+        <v>634</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>589</v>
+        <v>635</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -5959,10 +5965,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>646</v>
+        <v>612</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>647</v>
+        <v>613</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -5970,10 +5976,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>952</v>
+        <v>588</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>953</v>
+        <v>589</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -5981,10 +5987,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>954</v>
+        <v>646</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>955</v>
+        <v>647</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -5992,10 +5998,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -6003,10 +6009,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>538</v>
+        <v>954</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>539</v>
+        <v>955</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -6014,10 +6020,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>533</v>
+        <v>949</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>341</v>
+        <v>956</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -6025,10 +6031,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>521</v>
+        <v>538</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -6036,10 +6042,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -6047,10 +6053,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>493</v>
+        <v>521</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>492</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -6058,15 +6064,37 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C81">
-    <sortCondition ref="B79:B81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">
+    <sortCondition ref="B75:B83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Improved another quick filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE36753-F209-4D4A-995F-916598E82FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FBDEE9-5183-134E-8602-2DFB6FB34363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="961">
   <si>
     <t>cs</t>
   </si>
@@ -2960,6 +2960,12 @@
   </si>
   <si>
     <t>lab.liquid.filter.pgvg.reset</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.filter.pgvg.label</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.filter.pgvg.reset</t>
   </si>
 </sst>
 </file>
@@ -5168,7 +5174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
@@ -8737,9 +8743,9 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
@@ -9250,7 +9256,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>650</v>
+        <v>959</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>651</v>
@@ -9261,7 +9267,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>654</v>
+        <v>960</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>655</v>
@@ -9272,10 +9278,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>944</v>
+        <v>650</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>945</v>
+        <v>651</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -9283,10 +9289,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>378</v>
+        <v>654</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>4</v>
+        <v>655</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -9294,10 +9300,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>376</v>
+        <v>944</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>377</v>
+        <v>945</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -9305,10 +9311,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>341</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -9316,10 +9322,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -9327,10 +9333,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -9338,21 +9344,21 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>445</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -9360,21 +9366,21 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -9382,10 +9388,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>386</v>
+        <v>434</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>236</v>
+        <v>435</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -9393,10 +9399,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>236</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -9404,21 +9410,21 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>455</v>
+        <v>386</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>454</v>
+        <v>382</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>453</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -9426,21 +9432,21 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -9448,10 +9454,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -9459,10 +9465,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9470,10 +9476,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>458</v>
+        <v>477</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -9481,10 +9487,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>450</v>
+        <v>478</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -9492,10 +9498,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -9503,10 +9509,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -9514,10 +9520,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -9525,10 +9531,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -9536,10 +9542,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -9547,15 +9553,37 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>464</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
-    <sortCondition ref="B55:B73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
+    <sortCondition ref="B64:B75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: So inline filter works nice, but there is still a bug with mutliple groups
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FBDEE9-5183-134E-8602-2DFB6FB34363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B970E1E1-8AB8-4347-B682-7E4F5E5C0DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="963">
   <si>
     <t>cs</t>
   </si>
@@ -2966,6 +2966,12 @@
   </si>
   <si>
     <t>market.filter.pgvg.filter.pgvg.reset</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.filter.nicotine.label</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.filter.nicotine.reset</t>
   </si>
 </sst>
 </file>
@@ -8743,10 +8749,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9256,10 +9262,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -9267,7 +9273,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>655</v>
@@ -9278,7 +9284,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>650</v>
+        <v>959</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>651</v>
@@ -9289,7 +9295,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>654</v>
+        <v>960</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>655</v>
@@ -9300,10 +9306,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>944</v>
+        <v>650</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>945</v>
+        <v>651</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -9311,10 +9317,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>378</v>
+        <v>654</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>4</v>
+        <v>655</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -9322,10 +9328,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>376</v>
+        <v>944</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>377</v>
+        <v>945</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -9333,10 +9339,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>341</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -9344,10 +9350,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -9355,10 +9361,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -9366,21 +9372,21 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>445</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -9388,21 +9394,21 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -9410,10 +9416,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>386</v>
+        <v>434</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>236</v>
+        <v>435</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -9421,10 +9427,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>236</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -9432,21 +9438,21 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>455</v>
+        <v>386</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>454</v>
+        <v>382</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>453</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -9454,21 +9460,21 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9476,10 +9482,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -9487,10 +9493,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -9498,10 +9504,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>458</v>
+        <v>477</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -9509,10 +9515,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>450</v>
+        <v>478</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -9520,10 +9526,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -9531,10 +9537,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -9542,10 +9548,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -9553,10 +9559,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -9564,10 +9570,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -9575,15 +9581,37 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>464</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
-    <sortCondition ref="B64:B75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C77">
+    <sortCondition ref="B73:B77"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Cells are using new quick filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B970E1E1-8AB8-4347-B682-7E4F5E5C0DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B8B35C-7C00-6141-9592-347A1A71A500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="965">
   <si>
     <t>cs</t>
   </si>
@@ -2972,6 +2972,12 @@
   </si>
   <si>
     <t>market.filter.pgvg.filter.nicotine.reset</t>
+  </si>
+  <si>
+    <t>market.filter.cell.filter.type.label</t>
+  </si>
+  <si>
+    <t>market.filter.cell.filter.type.reset</t>
   </si>
 </sst>
 </file>
@@ -8749,10 +8755,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9229,10 +9235,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>946</v>
+        <v>963</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>655</v>
+        <v>945</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -9240,10 +9246,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>652</v>
+        <v>964</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -9251,7 +9257,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>656</v>
+        <v>946</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>655</v>
@@ -9262,7 +9268,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>961</v>
+        <v>652</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>653</v>
@@ -9273,7 +9279,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>962</v>
+        <v>656</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>655</v>
@@ -9284,10 +9290,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -9295,7 +9301,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>655</v>
@@ -9306,7 +9312,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>650</v>
+        <v>959</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>651</v>
@@ -9317,7 +9323,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>654</v>
+        <v>960</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>655</v>
@@ -9328,10 +9334,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>944</v>
+        <v>650</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>945</v>
+        <v>651</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -9339,10 +9345,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>378</v>
+        <v>654</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>4</v>
+        <v>655</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -9350,10 +9356,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>376</v>
+        <v>944</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>377</v>
+        <v>945</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -9361,10 +9367,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>341</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -9372,10 +9378,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -9383,10 +9389,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -9394,21 +9400,21 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>437</v>
+        <v>375</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>445</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -9416,21 +9422,21 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -9438,10 +9444,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>386</v>
+        <v>434</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>236</v>
+        <v>435</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -9449,10 +9455,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>236</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -9460,21 +9466,21 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>455</v>
+        <v>386</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>454</v>
+        <v>382</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>453</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9482,21 +9488,21 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>475</v>
+        <v>453</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -9504,10 +9510,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -9515,10 +9521,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -9526,10 +9532,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>458</v>
+        <v>477</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -9537,10 +9543,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>450</v>
+        <v>478</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -9548,10 +9554,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -9559,10 +9565,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -9570,10 +9576,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -9581,10 +9587,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -9592,10 +9598,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -9603,15 +9609,37 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>464</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C77">
-    <sortCondition ref="B73:B77"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C79">
+    <sortCondition ref="B73:B79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Improved empty lists
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98334BEA-8514-4667-BF34-719757731861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A646C4-1B74-4462-9F0C-EEAA514A38CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1470" windowWidth="23610" windowHeight="18390" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="1590" windowWidth="23610" windowHeight="18390" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="1006">
   <si>
     <t>cs</t>
   </si>
@@ -3002,6 +3002,105 @@
   </si>
   <si>
     <t>Je nám líto, ale na vytvoření nového liquidu již nemáte dostatek puffíků.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné atomizéry.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Ve vašem inventáři zatím nejsou žádné atomizéry, přejděte prosím do obchodu a pořiďte si nějaký.</t>
+  </si>
+  <si>
+    <t>lab.market.atomizer.label</t>
+  </si>
+  <si>
+    <t>lab.mod.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné mody.</t>
+  </si>
+  <si>
+    <t>Ve vašem inventáři zatím nejsou žádné mody, přejděte prosím do obchodu a pořiďte si nějaký.</t>
+  </si>
+  <si>
+    <t>lab.mod.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.market.mod.label</t>
+  </si>
+  <si>
+    <t>lab.cell.list.empty.title</t>
+  </si>
+  <si>
+    <t>Ve vašem inventáři zatím nejsou žádné články, přejděte prosím do obchodu a pořiďte si nějaký.</t>
+  </si>
+  <si>
+    <t>lab.cell.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné články.</t>
+  </si>
+  <si>
+    <t>lab.market.cell.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné vaty.</t>
+  </si>
+  <si>
+    <t>lab.cotton.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Ve vašem inventáři zatím nejsou žádné vaty, přejděte prosím do obchodu a pořiďte si nějakou.</t>
+  </si>
+  <si>
+    <t>lab.market.cotton.label</t>
+  </si>
+  <si>
+    <t>lab.market.aroma.label</t>
+  </si>
+  <si>
+    <t>lab.market.base.label</t>
+  </si>
+  <si>
+    <t>lab.base.list.filter.empty.title</t>
+  </si>
+  <si>
+    <t>lab.base.list.filter.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Vybranému filtru neodpovídají žádné báze.</t>
+  </si>
+  <si>
+    <t>lab.booster.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné boostery.</t>
+  </si>
+  <si>
+    <t>Ve vašem inventáři zatím nejsou žádné boostery, přejděte prosím do obchodu a pořiďte si nějaký.</t>
+  </si>
+  <si>
+    <t>lab.booster.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.market.booster.label</t>
+  </si>
+  <si>
+    <t>lab.booster.list.filter.empty.title</t>
+  </si>
+  <si>
+    <t>lab.booster.list.filter.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Vybranému filtru neodpovídají žádné boostery.</t>
   </si>
 </sst>
 </file>
@@ -5208,10 +5307,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6176,6 +6275,237 @@
       </c>
       <c r="C87" s="1" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>1005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added aroma taste
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A646C4-1B74-4462-9F0C-EEAA514A38CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74C7C87-CF4A-4955-8DB6-8F66B5325B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1590" windowWidth="23610" windowHeight="18390" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="1800" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="1039">
   <si>
     <t>cs</t>
   </si>
@@ -3101,6 +3101,105 @@
   </si>
   <si>
     <t>Vybranému filtru neodpovídají žádné boostery.</t>
+  </si>
+  <si>
+    <t>fruit</t>
+  </si>
+  <si>
+    <t>taste</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>tobacco</t>
+  </si>
+  <si>
+    <t>dessert</t>
+  </si>
+  <si>
+    <t>lemonade</t>
+  </si>
+  <si>
+    <t>milkshake</t>
+  </si>
+  <si>
+    <t>cookie</t>
+  </si>
+  <si>
+    <t>fruit, cake</t>
+  </si>
+  <si>
+    <t>vanilla</t>
+  </si>
+  <si>
+    <t>caramel</t>
+  </si>
+  <si>
+    <t>tobacco, caramel</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>menthol</t>
+  </si>
+  <si>
+    <t>fruit, ice</t>
+  </si>
+  <si>
+    <t>menthol, fruit</t>
+  </si>
+  <si>
+    <t>methol, fruit</t>
+  </si>
+  <si>
+    <t>tastes</t>
+  </si>
+  <si>
+    <t>common.taste.ice</t>
+  </si>
+  <si>
+    <t>Ledové</t>
+  </si>
+  <si>
+    <t>common.taste.fruit</t>
+  </si>
+  <si>
+    <t>Ovocné</t>
+  </si>
+  <si>
+    <t>common.taste.tobacco</t>
+  </si>
+  <si>
+    <t>common.taste.cake</t>
+  </si>
+  <si>
+    <t>Buchtovka</t>
+  </si>
+  <si>
+    <t>Tabákovka</t>
+  </si>
+  <si>
+    <t>common.taste.menthol</t>
+  </si>
+  <si>
+    <t>Mentolové</t>
+  </si>
+  <si>
+    <t>common.taste.milkshake</t>
+  </si>
+  <si>
+    <t>Milkshake</t>
+  </si>
+  <si>
+    <t>common.taste.caramel</t>
+  </si>
+  <si>
+    <t>Karamel</t>
+  </si>
+  <si>
+    <t>vanilla, tobacco</t>
   </si>
 </sst>
 </file>
@@ -4501,10 +4600,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4963,6 +5062,83 @@
       </c>
       <c r="C41" s="1" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -5309,7 +5485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
@@ -7599,19 +7775,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>670</v>
       </c>
@@ -7636,8 +7813,11 @@
       <c r="H1" s="5" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>675</v>
       </c>
@@ -7662,8 +7842,11 @@
       <c r="H2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>675</v>
       </c>
@@ -7688,8 +7871,11 @@
       <c r="H3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>679</v>
       </c>
@@ -7715,7 +7901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>690</v>
       </c>
@@ -7741,7 +7927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>692</v>
       </c>
@@ -7766,8 +7952,11 @@
       <c r="H6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>692</v>
       </c>
@@ -7792,8 +7981,11 @@
       <c r="H7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>692</v>
       </c>
@@ -7818,8 +8010,11 @@
       <c r="H8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>696</v>
       </c>
@@ -7844,8 +8039,11 @@
       <c r="H9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>696</v>
       </c>
@@ -7871,7 +8069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>696</v>
       </c>
@@ -7896,8 +8094,11 @@
       <c r="H11">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>696</v>
       </c>
@@ -7922,8 +8123,11 @@
       <c r="H12">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>696</v>
       </c>
@@ -7949,7 +8153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>696</v>
       </c>
@@ -7974,8 +8178,11 @@
       <c r="H14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>702</v>
       </c>
@@ -8000,8 +8207,11 @@
       <c r="H15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>704</v>
       </c>
@@ -8026,8 +8236,11 @@
       <c r="H16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>704</v>
       </c>
@@ -8052,8 +8265,11 @@
       <c r="H17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>709</v>
       </c>
@@ -8078,8 +8294,11 @@
       <c r="H18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>714</v>
       </c>
@@ -8104,8 +8323,11 @@
       <c r="H19">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>714</v>
       </c>
@@ -8131,7 +8353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>714</v>
       </c>
@@ -8157,7 +8379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>716</v>
       </c>
@@ -8182,8 +8404,11 @@
       <c r="H22">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>717</v>
       </c>
@@ -8208,8 +8433,11 @@
       <c r="H23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>717</v>
       </c>
@@ -8234,8 +8462,11 @@
       <c r="H24">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>722</v>
       </c>
@@ -8260,8 +8491,11 @@
       <c r="H25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>722</v>
       </c>
@@ -8287,7 +8521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>726</v>
       </c>
@@ -8312,8 +8546,11 @@
       <c r="H27">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>726</v>
       </c>
@@ -8338,8 +8575,11 @@
       <c r="H28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>726</v>
       </c>
@@ -8364,8 +8604,11 @@
       <c r="H29">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>730</v>
       </c>
@@ -8390,8 +8633,11 @@
       <c r="H30">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>733</v>
       </c>
@@ -8416,8 +8662,11 @@
       <c r="H31">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>750</v>
       </c>
@@ -8442,8 +8691,11 @@
       <c r="H32">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>751</v>
       </c>
@@ -8467,6 +8719,9 @@
       </c>
       <c r="H33">
         <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1009</v>
       </c>
     </row>
   </sheetData>
@@ -11632,10 +11887,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11897,6 +12152,127 @@
         <v>2</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: A little improvement
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46D297A-3520-9147-9EE8-AB7B9A16B899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078B51E7-0B57-6944-A167-F336ED68CE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="500" windowWidth="23620" windowHeight="16280" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="1053">
   <si>
     <t>cs</t>
   </si>
@@ -3236,6 +3236,12 @@
   </si>
   <si>
     <t>Vybrat</t>
+  </si>
+  <si>
+    <t>lab.aroma.select.title.tooltip</t>
+  </si>
+  <si>
+    <t>common.selection.cancel.label</t>
   </si>
 </sst>
 </file>
@@ -4636,10 +4642,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5116,10 +5122,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1050</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -5127,10 +5133,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>265</v>
+        <v>1049</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>266</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -5138,10 +5144,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -5149,10 +5155,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1029</v>
+        <v>133</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1030</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -5160,10 +5166,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -5171,10 +5177,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1027</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -5182,10 +5188,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -5193,10 +5199,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1033</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -5204,10 +5210,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -5215,10 +5221,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -5226,15 +5232,26 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>1040</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C53">
-    <sortCondition ref="B45:B53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C54">
+    <sortCondition ref="B42:B54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5574,10 +5591,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5669,32 +5686,32 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>975</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -5702,10 +5719,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -5713,10 +5730,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>525</v>
+        <v>973</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>240</v>
+        <v>974</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -5724,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>240</v>
@@ -5735,10 +5752,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>578</v>
+        <v>518</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>579</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -5746,10 +5763,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -5757,10 +5774,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>996</v>
+        <v>577</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>997</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5768,10 +5785,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>968</v>
+        <v>997</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5779,10 +5796,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>580</v>
+        <v>995</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>582</v>
+        <v>968</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -5790,10 +5807,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>526</v>
+        <v>580</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>483</v>
+        <v>582</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -5801,7 +5818,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>483</v>
@@ -5812,10 +5829,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1001</v>
+        <v>517</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1000</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -5823,10 +5840,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -5834,10 +5851,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -5845,10 +5862,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>968</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -5856,10 +5873,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>1003</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>131</v>
+        <v>968</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -5867,10 +5884,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>522</v>
+        <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>237</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -5878,7 +5895,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>237</v>
@@ -5889,10 +5906,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>985</v>
+        <v>528</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>984</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -5900,10 +5917,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -5911,10 +5928,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>523</v>
+        <v>983</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>238</v>
+        <v>986</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -5922,7 +5939,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>238</v>
@@ -5933,10 +5950,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>990</v>
+        <v>527</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>991</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -5944,10 +5961,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -5955,10 +5972,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>132</v>
+        <v>988</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>989</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -5966,10 +5983,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>231</v>
+        <v>132</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>489</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -5977,10 +5994,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -5988,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>488</v>
+        <v>129</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>126</v>
@@ -5999,10 +6016,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>491</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -6010,10 +6027,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>947</v>
+        <v>490</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>948</v>
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -6021,10 +6038,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>559</v>
+        <v>947</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>560</v>
+        <v>948</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -6032,10 +6049,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -6043,10 +6060,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -6054,10 +6071,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>240</v>
+        <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -6065,10 +6082,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>585</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -6076,10 +6093,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>571</v>
+        <v>584</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -6087,10 +6104,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>614</v>
+        <v>571</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>615</v>
+        <v>572</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -6098,10 +6115,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>636</v>
+        <v>614</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>637</v>
+        <v>615</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -6109,10 +6126,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -6120,10 +6137,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>542</v>
+        <v>616</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>543</v>
+        <v>617</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -6131,10 +6148,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>642</v>
+        <v>542</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>643</v>
+        <v>543</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -6142,10 +6159,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>971</v>
+        <v>642</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>972</v>
+        <v>643</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -6153,10 +6170,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -6164,10 +6181,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>596</v>
+        <v>969</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>611</v>
+        <v>970</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -6175,10 +6192,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>567</v>
+        <v>611</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -6186,10 +6203,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>594</v>
+        <v>641</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -6197,10 +6214,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>535</v>
+        <v>594</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>544</v>
+        <v>595</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -6208,10 +6225,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -6219,10 +6236,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>957</v>
+        <v>536</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>651</v>
+        <v>558</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -6230,21 +6247,21 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>655</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6252,10 +6269,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6263,10 +6280,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>601</v>
+        <v>633</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>602</v>
+        <v>638</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6274,10 +6291,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6285,10 +6302,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6296,10 +6313,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6307,10 +6324,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6318,21 +6335,21 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>624</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -6340,32 +6357,32 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="1" t="s">
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -6373,10 +6390,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>966</v>
+        <v>547</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>967</v>
+        <v>548</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -6384,10 +6401,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -6395,10 +6412,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>233</v>
+        <v>965</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>234</v>
+        <v>968</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -6406,10 +6423,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>540</v>
+        <v>233</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>541</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -6417,10 +6434,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>639</v>
+        <v>540</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>640</v>
+        <v>541</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -6428,10 +6445,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>537</v>
+        <v>639</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>186</v>
+        <v>640</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -6439,32 +6456,32 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>621</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -6472,10 +6489,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>590</v>
+        <v>950</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>608</v>
+        <v>951</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -6483,10 +6500,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>593</v>
+        <v>608</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -6494,10 +6511,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>609</v>
+        <v>593</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -6505,10 +6522,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -6516,10 +6533,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -6527,10 +6544,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>586</v>
+        <v>627</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>587</v>
+        <v>628</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -6538,10 +6555,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>629</v>
+        <v>586</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>630</v>
+        <v>587</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -6549,10 +6566,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -6560,10 +6577,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>612</v>
+        <v>634</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>613</v>
+        <v>635</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -6571,10 +6588,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -6582,10 +6599,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>646</v>
+        <v>588</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>647</v>
+        <v>589</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -6593,10 +6610,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>952</v>
+        <v>646</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>953</v>
+        <v>647</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -6604,10 +6621,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -6615,10 +6632,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -6626,10 +6643,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>538</v>
+        <v>949</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>539</v>
+        <v>956</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -6637,10 +6654,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>993</v>
+        <v>538</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>481</v>
+        <v>539</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -6648,10 +6665,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>977</v>
+        <v>993</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>235</v>
+        <v>481</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -6659,10 +6676,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>994</v>
+        <v>977</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -6670,10 +6687,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>483</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -6681,32 +6698,32 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B101" s="1" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -6714,10 +6731,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>982</v>
+        <v>533</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -6725,7 +6742,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>521</v>
+        <v>982</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>236</v>
@@ -6736,7 +6753,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>236</v>
@@ -6747,10 +6764,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>981</v>
+        <v>519</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>980</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -6758,10 +6775,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -6769,10 +6786,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>493</v>
+        <v>978</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>492</v>
+        <v>979</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -6780,15 +6797,26 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C109">
-    <sortCondition ref="B100:B109"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C110">
+    <sortCondition ref="B102:B110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Liquid mix works quite well... I hope
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D872D84E-EF32-4C2B-A7F7-24F16E2B155C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D55A1B-14F2-428D-AFE8-57CEAC237E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1710" windowWidth="23610" windowHeight="18390" firstSheet="16" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1710" windowWidth="23610" windowHeight="18390" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1059">
   <si>
     <t>cs</t>
   </si>
@@ -3248,6 +3248,18 @@
   </si>
   <si>
     <t>Vygenerovat SDK</t>
+  </si>
+  <si>
+    <t>lab.liquid.quick-info.title</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>lab.liquid.quick-info.subtitle</t>
+  </si>
+  <si>
+    <t>Zde se zobrazí informace o složení liquidu.</t>
   </si>
 </sst>
 </file>
@@ -5597,10 +5609,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6616,10 +6628,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>646</v>
+        <v>1057</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>647</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6627,10 +6639,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>952</v>
+        <v>1055</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>953</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,10 +6650,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>954</v>
+        <v>646</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>955</v>
+        <v>647</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6649,10 +6661,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6660,10 +6672,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>538</v>
+        <v>954</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>539</v>
+        <v>955</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6671,10 +6683,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>993</v>
+        <v>949</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>481</v>
+        <v>956</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6682,10 +6694,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>977</v>
+        <v>538</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>235</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6693,10 +6705,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>240</v>
+        <v>481</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6704,10 +6716,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>1002</v>
+        <v>977</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>483</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6715,21 +6727,21 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>992</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>238</v>
+        <v>1002</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6737,21 +6749,21 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>533</v>
+        <v>987</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>341</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>982</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>236</v>
+        <v>992</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -6759,10 +6771,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -6770,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>519</v>
+        <v>982</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>236</v>
@@ -6781,10 +6793,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>981</v>
+        <v>521</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>980</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -6792,10 +6804,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>978</v>
+        <v>519</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>979</v>
+        <v>236</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -6803,10 +6815,10 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>493</v>
+        <v>981</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>492</v>
+        <v>980</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -6814,15 +6826,37 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C110">
-    <sortCondition ref="B102:B110"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C112">
+    <sortCondition ref="B109:B112"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6833,7 +6867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Improved inventory stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B32873-BE23-4B0F-831D-9D65A5912699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73236051-82BF-473E-8662-3397AB1377EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1710" windowWidth="23610" windowHeight="18390" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1065">
   <si>
     <t>cs</t>
   </si>
@@ -3272,6 +3272,12 @@
   </si>
   <si>
     <t>Výběr boosteru</t>
+  </si>
+  <si>
+    <t>common.inventory.code.tooltip</t>
+  </si>
+  <si>
+    <t>Kód v inventáři pro rozlišení produktů stejného typu.</t>
   </si>
 </sst>
 </file>
@@ -4672,10 +4678,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4800,10 +4806,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>545</v>
+        <v>1063</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>546</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4811,10 +4817,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>310</v>
+        <v>545</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>311</v>
+        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4822,10 +4828,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4833,10 +4839,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4844,10 +4850,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4855,10 +4861,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>248</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4866,10 +4872,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>322</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4877,10 +4883,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>389</v>
+        <v>321</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4888,32 +4894,32 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>465</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4921,10 +4927,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4932,10 +4938,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4943,76 +4949,76 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5020,32 +5026,32 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>1044</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5053,10 +5059,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5064,10 +5070,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>1041</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5075,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5086,10 +5092,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5097,10 +5103,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5108,10 +5114,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,10 +5125,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>563</v>
+        <v>258</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>564</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,10 +5136,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5141,10 +5147,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>648</v>
+        <v>565</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>649</v>
+        <v>566</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5152,10 +5158,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1052</v>
+        <v>648</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>242</v>
+        <v>649</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5163,10 +5169,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1059</v>
+        <v>1052</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1060</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5174,10 +5180,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5185,10 +5191,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1049</v>
+        <v>1061</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1050</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,10 +5202,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>265</v>
+        <v>1049</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>266</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5207,10 +5213,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5218,10 +5224,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1029</v>
+        <v>133</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1030</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5229,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,10 +5246,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1027</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5251,10 +5257,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5262,10 +5268,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1033</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5273,10 +5279,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5284,10 +5290,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5295,15 +5301,26 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>1040</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C56">
-    <sortCondition ref="B55:B56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C57">
+    <sortCondition ref="B53:B57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Renamed liquid create to quick mix as the original idea
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73236051-82BF-473E-8662-3397AB1377EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43A0910-0162-4EBD-881E-D0B4DD8A88AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1710" windowWidth="23610" windowHeight="18390" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1067">
   <si>
     <t>cs</t>
   </si>
@@ -3278,6 +3278,12 @@
   </si>
   <si>
     <t>Kód v inventáři pro rozlišení produktů stejného typu.</t>
+  </si>
+  <si>
+    <t>common.selection.InventoryAromas.title</t>
+  </si>
+  <si>
+    <t>Výběr příchutě</t>
   </si>
 </sst>
 </file>
@@ -4678,10 +4684,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5180,10 +5186,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1060</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5191,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5202,10 +5208,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1049</v>
+        <v>1061</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1050</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5213,10 +5219,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>265</v>
+        <v>1049</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>266</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5224,10 +5230,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5235,10 +5241,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1029</v>
+        <v>133</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1030</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5246,10 +5252,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5257,10 +5263,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1026</v>
+        <v>1036</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1027</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5268,10 +5274,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5279,10 +5285,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1033</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5290,10 +5296,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5301,10 +5307,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5312,15 +5318,26 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>1040</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C57">
-    <sortCondition ref="B53:B57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
+    <sortCondition ref="B46:B58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: A bit more boilerplate
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F316E2-633C-4F15-851F-C316912FF392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81DFCC-C60A-4CAA-8953-FBDFB5BC3886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1710" windowWidth="23610" windowHeight="18390" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15960" yWindow="1845" windowWidth="23610" windowHeight="18390" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="1074">
   <si>
     <t>cs</t>
   </si>
@@ -3296,6 +3296,15 @@
   </si>
   <si>
     <t>Tato funkce umožní namíchání liquidu zadáním požadované příchutě, poměru VG/PG a síly nikotinu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.clever-info.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.clever-info.subtitle</t>
+  </si>
+  <si>
+    <t>Zde se zobrazí nabídky chytrého mixu</t>
   </si>
 </sst>
 </file>
@@ -5689,10 +5698,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6246,10 +6255,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>542</v>
+        <v>1072</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>543</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6257,10 +6266,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>641</v>
+        <v>1071</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>642</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6268,10 +6277,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1069</v>
+        <v>542</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1070</v>
+        <v>543</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6279,10 +6288,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1066</v>
+        <v>641</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1067</v>
+        <v>642</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6290,10 +6299,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6301,10 +6310,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>970</v>
+        <v>1066</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>971</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6312,21 +6321,21 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>968</v>
+        <v>1068</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>595</v>
+        <v>970</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>610</v>
+        <v>971</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6334,21 +6343,21 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>640</v>
+        <v>968</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>567</v>
+        <v>610</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6356,10 +6365,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>535</v>
+        <v>640</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>544</v>
+        <v>567</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6367,10 +6376,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>536</v>
+        <v>594</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6378,10 +6387,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>956</v>
+        <v>535</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>650</v>
+        <v>544</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6389,32 +6398,32 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>957</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>654</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6422,10 +6431,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>601</v>
+        <v>631</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6433,10 +6442,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>602</v>
+        <v>632</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>603</v>
+        <v>637</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6444,10 +6453,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6455,10 +6464,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6466,21 +6475,21 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>623</v>
+        <v>597</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6488,21 +6497,21 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>534</v>
+        <v>604</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>234</v>
+        <v>623</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6510,10 +6519,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>549</v>
+        <v>621</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>609</v>
+        <v>622</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6521,21 +6530,21 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>965</v>
+        <v>549</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>966</v>
+        <v>609</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6543,10 +6552,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>964</v>
+        <v>547</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>967</v>
+        <v>548</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6554,10 +6563,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>233</v>
+        <v>965</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>234</v>
+        <v>966</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6565,10 +6574,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>540</v>
+        <v>964</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>541</v>
+        <v>967</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6576,10 +6585,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>638</v>
+        <v>233</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>639</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6587,10 +6596,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>186</v>
+        <v>541</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,21 +6607,21 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>617</v>
+        <v>638</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>619</v>
+        <v>537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>620</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6620,21 +6629,21 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>949</v>
+        <v>617</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>590</v>
+        <v>619</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>607</v>
+        <v>620</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6642,10 +6651,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>592</v>
+        <v>949</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>593</v>
+        <v>950</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6653,10 +6662,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6664,10 +6673,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>624</v>
+        <v>592</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6675,10 +6684,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>626</v>
+        <v>591</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6686,10 +6695,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>586</v>
+        <v>624</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>587</v>
+        <v>625</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6697,10 +6706,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6708,10 +6717,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>633</v>
+        <v>586</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6719,10 +6728,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>611</v>
+        <v>628</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6730,10 +6739,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>588</v>
+        <v>633</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>589</v>
+        <v>634</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6741,10 +6750,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1056</v>
+        <v>611</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1057</v>
+        <v>612</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6752,10 +6761,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1054</v>
+        <v>588</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1055</v>
+        <v>589</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6763,10 +6772,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>645</v>
+        <v>1056</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>646</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6774,10 +6783,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>951</v>
+        <v>1054</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>952</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6785,10 +6794,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>953</v>
+        <v>645</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>954</v>
+        <v>646</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6796,10 +6805,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6807,10 +6816,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>538</v>
+        <v>953</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>539</v>
+        <v>954</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6818,10 +6827,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>992</v>
+        <v>948</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>481</v>
+        <v>955</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6829,10 +6838,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>976</v>
+        <v>538</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>235</v>
+        <v>539</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6840,10 +6849,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>240</v>
+        <v>481</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -6851,10 +6860,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1001</v>
+        <v>976</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>483</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -6862,21 +6871,21 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>986</v>
+        <v>993</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>991</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>238</v>
+        <v>1001</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -6884,21 +6893,21 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>533</v>
+        <v>986</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>341</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>981</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>236</v>
+        <v>991</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -6906,10 +6915,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -6917,7 +6926,7 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>519</v>
+        <v>981</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>236</v>
@@ -6928,10 +6937,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>980</v>
+        <v>521</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>979</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -6939,10 +6948,10 @@
         <v>0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>977</v>
+        <v>519</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>978</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -6950,10 +6959,10 @@
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>493</v>
+        <v>980</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>492</v>
+        <v>979</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -6961,15 +6970,37 @@
         <v>0</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C115">
-    <sortCondition ref="B110:B115"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C117">
+    <sortCondition ref="B110:B117"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Preparing liquid toolbar with archiving
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81DFCC-C60A-4CAA-8953-FBDFB5BC3886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8A3D62-9F22-471D-8AF6-678DA8E4BFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="1845" windowWidth="23610" windowHeight="18390" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14910" yWindow="2460" windowWidth="33795" windowHeight="18390" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="1083">
   <si>
     <t>cs</t>
   </si>
@@ -3305,6 +3305,33 @@
   </si>
   <si>
     <t>Zde se zobrazí nabídky chytrého mixu</t>
+  </si>
+  <si>
+    <t>Odstranit</t>
+  </si>
+  <si>
+    <t>lab.liquid.delete.modal.button</t>
+  </si>
+  <si>
+    <t>lab.liquid.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit liquidy</t>
+  </si>
+  <si>
+    <t>lab.liquid.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybrané liquidy?</t>
+  </si>
+  <si>
+    <t>common.modal.cancel.button</t>
+  </si>
+  <si>
+    <t>lab.liquid.delete.failure</t>
+  </si>
+  <si>
+    <t>Liquidy se nepodařilo odstranit.</t>
   </si>
 </sst>
 </file>
@@ -4705,10 +4732,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5070,26 +5097,26 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>1043</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5097,10 +5124,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5108,10 +5135,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>1040</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,10 +5146,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,10 +5157,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5141,10 +5168,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5152,10 +5179,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5163,10 +5190,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>563</v>
+        <v>258</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>564</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5174,10 +5201,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5185,10 +5212,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>647</v>
+        <v>565</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>648</v>
+        <v>566</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,10 +5223,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1051</v>
+        <v>647</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>242</v>
+        <v>648</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5207,10 +5234,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1064</v>
+        <v>1051</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1065</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5218,10 +5245,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1059</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5229,10 +5256,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,10 +5267,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1048</v>
+        <v>1060</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1049</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5251,10 +5278,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>265</v>
+        <v>1048</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>266</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5262,10 +5289,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5273,10 +5300,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1028</v>
+        <v>133</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1029</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5284,10 +5311,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1035</v>
+        <v>1028</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5295,10 +5322,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1026</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5306,10 +5333,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5317,10 +5344,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1031</v>
+        <v>1023</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5328,10 +5355,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5339,10 +5366,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1027</v>
+        <v>1033</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5350,15 +5377,26 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>1038</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>1039</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
-    <sortCondition ref="B46:B58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C59">
+    <sortCondition ref="B58:B59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5698,10 +5736,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6409,10 +6447,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>956</v>
+        <v>1081</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>650</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6420,54 +6458,54 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>957</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>654</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6475,10 +6513,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>598</v>
+        <v>630</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>599</v>
+        <v>631</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6486,10 +6524,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>596</v>
+        <v>632</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>597</v>
+        <v>637</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6497,21 +6535,21 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6519,21 +6557,21 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>534</v>
+        <v>596</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>234</v>
+        <v>597</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6541,32 +6579,32 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>549</v>
+        <v>605</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>547</v>
+        <v>604</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>965</v>
+        <v>621</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>966</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6574,21 +6612,21 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>964</v>
+        <v>534</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>233</v>
+        <v>549</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>234</v>
+        <v>609</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6596,10 +6634,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6607,10 +6645,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>638</v>
+        <v>965</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>639</v>
+        <v>966</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6618,10 +6656,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>537</v>
+        <v>964</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>186</v>
+        <v>967</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6629,21 +6667,21 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>617</v>
+        <v>233</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>619</v>
+        <v>540</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>620</v>
+        <v>541</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6651,10 +6689,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>949</v>
+        <v>638</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>950</v>
+        <v>639</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6662,10 +6700,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>590</v>
+        <v>537</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>607</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6673,21 +6711,21 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>592</v>
+        <v>617</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>591</v>
+        <v>619</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>608</v>
+        <v>620</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6695,10 +6733,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>624</v>
+        <v>949</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>625</v>
+        <v>950</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6706,10 +6744,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>626</v>
+        <v>590</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -6717,10 +6755,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>587</v>
+        <v>593</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -6728,10 +6766,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>628</v>
+        <v>591</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>629</v>
+        <v>608</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6739,10 +6777,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6750,10 +6788,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>611</v>
+        <v>626</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>612</v>
+        <v>627</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6761,10 +6799,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,10 +6810,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1056</v>
+        <v>628</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1057</v>
+        <v>629</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6783,10 +6821,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1054</v>
+        <v>633</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1055</v>
+        <v>634</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6794,10 +6832,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>646</v>
+        <v>612</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6805,10 +6843,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>951</v>
+        <v>588</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>952</v>
+        <v>589</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6816,10 +6854,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>953</v>
+        <v>1056</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>954</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6827,10 +6865,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>948</v>
+        <v>1054</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>955</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6838,10 +6876,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>538</v>
+        <v>645</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>539</v>
+        <v>646</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6849,10 +6887,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>992</v>
+        <v>951</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>481</v>
+        <v>952</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -6860,10 +6898,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>976</v>
+        <v>953</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>235</v>
+        <v>954</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -6871,10 +6909,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>993</v>
+        <v>948</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>240</v>
+        <v>955</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -6882,10 +6920,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1001</v>
+        <v>538</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>483</v>
+        <v>539</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -6893,21 +6931,21 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>237</v>
+        <v>481</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>991</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>238</v>
+        <v>976</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -6915,10 +6953,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>533</v>
+        <v>993</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>341</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -6926,10 +6964,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>981</v>
+        <v>1001</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>236</v>
+        <v>483</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -6937,21 +6975,21 @@
         <v>0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>521</v>
+        <v>986</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>236</v>
+        <v>991</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -6959,10 +6997,10 @@
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>980</v>
+        <v>533</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>979</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -6970,10 +7008,10 @@
         <v>0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>978</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -6981,10 +7019,10 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>493</v>
+        <v>521</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>492</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -6992,15 +7030,59 @@
         <v>0</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C117">
-    <sortCondition ref="B110:B117"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C121">
+    <sortCondition ref="B116:B121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Fixed some ugly UI stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C798A19C-5586-4D47-8C79-72D2EDF41549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC4117-1266-F340-A4E2-080D5663B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1086">
   <si>
     <t>cs</t>
   </si>
@@ -3338,6 +3338,9 @@
   </si>
   <si>
     <t>Úspěch</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.button</t>
   </si>
 </sst>
 </file>
@@ -4740,7 +4743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -5742,10 +5745,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7106,6 +7109,17 @@
       </c>
       <c r="C123" s="1" t="s">
         <v>1082</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved liquid mix
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC4117-1266-F340-A4E2-080D5663B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFCCAD4-2F06-A747-A346-6CF8AC1FCF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="1090">
   <si>
     <t>cs</t>
   </si>
@@ -3341,6 +3341,18 @@
   </si>
   <si>
     <t>lab.liquid.create.button</t>
+  </si>
+  <si>
+    <t>lab.liquid.quick-mix.preview.tab</t>
+  </si>
+  <si>
+    <t>Náhled</t>
+  </si>
+  <si>
+    <t>lab.liquid.quick-mix.details.tab</t>
+  </si>
+  <si>
+    <t>Detaily</t>
   </si>
 </sst>
 </file>
@@ -5745,7 +5757,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
       <selection activeCell="B114" sqref="B114"/>
@@ -6346,10 +6358,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1065</v>
+        <v>1085</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1066</v>
+        <v>554</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -6357,10 +6369,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -6368,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>1063</v>
@@ -6379,10 +6391,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>966</v>
+        <v>1064</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>967</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -6390,10 +6402,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -6401,10 +6413,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>591</v>
+        <v>964</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>606</v>
+        <v>965</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -6412,10 +6424,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>636</v>
+        <v>591</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>563</v>
+        <v>606</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -6423,7 +6435,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>590</v>
+        <v>636</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>563</v>
@@ -6434,10 +6446,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>531</v>
+        <v>590</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>540</v>
+        <v>563</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -6445,10 +6457,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -6456,10 +6468,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1077</v>
+        <v>532</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1078</v>
+        <v>554</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -6467,10 +6479,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1071</v>
+        <v>1077</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -6478,10 +6490,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -6489,10 +6501,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -6500,10 +6512,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1079</v>
+        <v>1072</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1080</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -6511,10 +6523,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>952</v>
+        <v>1079</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>646</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -6522,21 +6534,21 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>953</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>650</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6544,10 +6556,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6555,10 +6567,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>596</v>
+        <v>628</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>597</v>
+        <v>633</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6566,10 +6578,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6577,10 +6589,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6588,10 +6600,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6599,10 +6611,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -6610,21 +6622,21 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>619</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -6632,21 +6644,21 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -6654,21 +6666,21 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>543</v>
+        <v>1081</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>961</v>
+        <v>545</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>962</v>
+        <v>605</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -6676,10 +6688,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>960</v>
+        <v>543</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>963</v>
+        <v>544</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -6687,10 +6699,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>233</v>
+        <v>961</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>234</v>
+        <v>962</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -6698,10 +6710,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>536</v>
+        <v>960</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>537</v>
+        <v>963</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -6709,10 +6721,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>634</v>
+        <v>233</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>635</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -6720,10 +6732,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>186</v>
+        <v>537</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -6731,21 +6743,21 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>613</v>
+        <v>634</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>615</v>
+        <v>533</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>616</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -6753,21 +6765,21 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>945</v>
+        <v>613</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>586</v>
+        <v>615</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>603</v>
+        <v>616</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -6775,10 +6787,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>588</v>
+        <v>945</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>589</v>
+        <v>946</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -6786,10 +6798,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -6797,10 +6809,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>620</v>
+        <v>588</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>621</v>
+        <v>589</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -6808,10 +6820,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>622</v>
+        <v>587</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>623</v>
+        <v>604</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -6819,10 +6831,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>582</v>
+        <v>620</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>583</v>
+        <v>621</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -6830,10 +6842,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -6841,10 +6853,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>629</v>
+        <v>582</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>630</v>
+        <v>583</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -6852,10 +6864,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>607</v>
+        <v>624</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>608</v>
+        <v>625</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -6863,10 +6875,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>584</v>
+        <v>629</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>585</v>
+        <v>630</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -6874,10 +6886,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1052</v>
+        <v>607</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1053</v>
+        <v>608</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -6885,10 +6897,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1050</v>
+        <v>584</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1051</v>
+        <v>585</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -6896,10 +6908,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>641</v>
+        <v>1052</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>642</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -6907,10 +6919,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>947</v>
+        <v>1050</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>948</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -6918,10 +6930,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>949</v>
+        <v>1088</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>950</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -6929,10 +6941,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>944</v>
+        <v>1086</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>951</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -6940,10 +6952,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>534</v>
+        <v>641</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>535</v>
+        <v>642</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -6951,10 +6963,10 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>988</v>
+        <v>947</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>477</v>
+        <v>948</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -6962,10 +6974,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>972</v>
+        <v>949</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>235</v>
+        <v>950</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -6973,10 +6985,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>989</v>
+        <v>944</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>240</v>
+        <v>951</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -6984,10 +6996,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>997</v>
+        <v>534</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>479</v>
+        <v>535</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -6995,21 +7007,21 @@
         <v>0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>237</v>
+        <v>477</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>987</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>238</v>
+        <v>972</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -7017,10 +7029,10 @@
         <v>0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>529</v>
+        <v>989</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>341</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -7028,10 +7040,10 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>977</v>
+        <v>997</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>236</v>
+        <v>479</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -7039,21 +7051,21 @@
         <v>0</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>517</v>
+        <v>982</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>236</v>
+        <v>987</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -7061,10 +7073,10 @@
         <v>0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>976</v>
+        <v>529</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>975</v>
+        <v>341</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -7072,10 +7084,10 @@
         <v>0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>974</v>
+        <v>236</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -7083,10 +7095,10 @@
         <v>0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>489</v>
+        <v>517</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>488</v>
+        <v>236</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -7094,10 +7106,10 @@
         <v>0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>232</v>
+        <v>515</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -7105,10 +7117,10 @@
         <v>0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1081</v>
+        <v>976</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1082</v>
+        <v>975</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -7116,15 +7128,37 @@
         <v>0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1085</v>
+        <v>973</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>554</v>
+        <v>974</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
-    <sortCondition ref="B116:B122"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C126">
+    <sortCondition ref="B124:B126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9190,8 +9224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FAEBF3-753C-4AE9-A2FF-818B5E33C44A}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Common: It's time for some job refactoring
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFCCAD4-2F06-A747-A346-6CF8AC1FCF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9870073-347B-5B4F-BF8E-FC41A7F6F9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="1092">
   <si>
     <t>cs</t>
   </si>
@@ -3353,6 +3353,12 @@
   </si>
   <si>
     <t>Detaily</t>
+  </si>
+  <si>
+    <t>common.job.name.job.mixture</t>
+  </si>
+  <si>
+    <t>Aktualizace mixů</t>
   </si>
 </sst>
 </file>
@@ -4753,10 +4759,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4980,10 +4986,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>335</v>
+        <v>1090</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>268</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4991,10 +4997,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>306</v>
+        <v>335</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>162</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -5002,10 +5008,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>334</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -5013,10 +5019,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -5024,10 +5030,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -5035,10 +5041,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>267</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -5046,10 +5052,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -5057,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>320</v>
@@ -5068,10 +5074,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1083</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -5079,10 +5085,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>327</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -5090,10 +5096,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1084</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -5101,10 +5107,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>331</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -5112,10 +5118,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>553</v>
+        <v>330</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -5123,32 +5129,32 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>1039</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>1038</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -5156,10 +5162,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -5167,10 +5173,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>1036</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -5178,10 +5184,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -5189,10 +5195,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -5200,10 +5206,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -5211,10 +5217,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -5222,10 +5228,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>559</v>
+        <v>258</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>560</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -5233,10 +5239,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -5244,10 +5250,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>643</v>
+        <v>561</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>644</v>
+        <v>562</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -5255,10 +5261,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1047</v>
+        <v>643</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>242</v>
+        <v>644</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -5266,10 +5272,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1060</v>
+        <v>1047</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1061</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -5277,10 +5283,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1055</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -5288,10 +5294,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -5299,10 +5305,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1044</v>
+        <v>1056</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1045</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -5310,10 +5316,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>265</v>
+        <v>1044</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>266</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -5321,10 +5327,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -5332,10 +5338,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1024</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1025</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -5343,10 +5349,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1032</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -5354,10 +5360,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1021</v>
+        <v>1031</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1022</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -5365,10 +5371,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -5376,10 +5382,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1027</v>
+        <v>1019</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1028</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -5387,10 +5393,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -5398,10 +5404,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1023</v>
+        <v>1029</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -5409,15 +5415,26 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>1035</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C59">
-    <sortCondition ref="B58:B59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="B46:B60"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5759,8 +5776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Common: Another little job improvement stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF6BA08-2371-4F74-978D-B29024126854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F2CCA2-FFF4-4BFA-8045-51D2D893A2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="1065" windowWidth="33795" windowHeight="18390" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="1100">
   <si>
     <t>cs</t>
   </si>
@@ -3377,6 +3377,12 @@
   </si>
   <si>
     <t>Čas startu úlohy {{data.date}}</t>
+  </si>
+  <si>
+    <t>root.job.performance.tooltip</t>
+  </si>
+  <si>
+    <t>Výkon úlohy - počet položek za sekundu</t>
   </si>
 </sst>
 </file>
@@ -7224,10 +7230,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7935,10 +7941,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -7946,10 +7952,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>302</v>
+        <v>1096</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>59</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -7957,10 +7963,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>125</v>
+        <v>302</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -7968,10 +7974,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>340</v>
+        <v>125</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>341</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -7979,10 +7985,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>113</v>
+        <v>340</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>114</v>
+        <v>341</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -7990,10 +7996,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -8001,10 +8007,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1048</v>
+        <v>127</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1049</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -8012,10 +8018,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>24</v>
+        <v>1048</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>25</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -8023,10 +8029,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -8034,10 +8040,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>410</v>
+        <v>117</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>411</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -8045,10 +8051,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>639</v>
+        <v>410</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>640</v>
+        <v>411</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -8056,10 +8062,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>412</v>
+        <v>639</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>413</v>
+        <v>640</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8067,10 +8073,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8078,10 +8084,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8089,10 +8095,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8100,10 +8106,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8111,32 +8117,32 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8144,10 +8150,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -8155,7 +8161,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>179</v>
@@ -8166,10 +8172,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -8177,10 +8183,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -8188,10 +8194,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -8199,10 +8205,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -8210,10 +8216,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -8221,10 +8227,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -8232,10 +8238,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>399</v>
+        <v>183</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -8243,10 +8249,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>400</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -8254,10 +8260,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -8265,10 +8271,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>115</v>
+        <v>396</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>116</v>
+        <v>397</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -8276,10 +8282,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>402</v>
+        <v>115</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>403</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -8287,10 +8293,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>230</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -8298,10 +8304,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>337</v>
+        <v>401</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -8309,15 +8315,26 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>405</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C98">
-    <sortCondition ref="B93:B98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C99">
+    <sortCondition ref="B96:B99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Preparing mixture UI
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DEDA5F-A0D8-4DE8-9A6D-C4E2F2CA11EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9563939D-1FD8-4AD4-A7CA-525E5F2558A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1065" windowWidth="33795" windowHeight="18390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14490" yWindow="2190" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="1111">
   <si>
     <t>cs</t>
   </si>
@@ -3395,6 +3395,27 @@
   </si>
   <si>
     <t>DL+</t>
+  </si>
+  <si>
+    <t>lab.build.index.title</t>
+  </si>
+  <si>
+    <t>Seznam buildů</t>
+  </si>
+  <si>
+    <t>lab.vape.index.title</t>
+  </si>
+  <si>
+    <t>Seznam vapů</t>
+  </si>
+  <si>
+    <t>lab.mixture.menu</t>
+  </si>
+  <si>
+    <t>Mixy</t>
+  </si>
+  <si>
+    <t>lab.mixture.index.title</t>
   </si>
 </sst>
 </file>
@@ -5838,10 +5859,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6131,10 +6152,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>130</v>
+        <v>1104</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>131</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6142,10 +6163,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>518</v>
+        <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>237</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6153,7 +6174,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>237</v>
@@ -6164,10 +6185,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>979</v>
+        <v>524</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>978</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6175,10 +6196,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6186,10 +6207,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>519</v>
+        <v>977</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>238</v>
+        <v>980</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6197,7 +6218,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>238</v>
@@ -6208,10 +6229,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>984</v>
+        <v>523</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>985</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6219,10 +6240,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6230,32 +6251,32 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>485</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6263,7 +6284,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>484</v>
+        <v>129</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>126</v>
@@ -6274,10 +6295,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>487</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6285,10 +6306,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>941</v>
+        <v>486</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>942</v>
+        <v>487</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6296,10 +6317,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>555</v>
+        <v>941</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>556</v>
+        <v>942</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6307,10 +6328,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6318,10 +6339,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6329,10 +6350,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>240</v>
+        <v>566</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6340,10 +6361,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>580</v>
+        <v>564</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>581</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6351,10 +6372,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>567</v>
+        <v>580</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>568</v>
+        <v>581</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6362,10 +6383,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>609</v>
+        <v>567</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>610</v>
+        <v>568</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6373,10 +6394,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>631</v>
+        <v>609</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>632</v>
+        <v>610</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6384,10 +6405,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6395,10 +6416,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1067</v>
+        <v>611</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1068</v>
+        <v>612</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6406,10 +6427,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1050</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6417,10 +6438,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>538</v>
+        <v>1066</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>539</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6428,10 +6449,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>637</v>
+        <v>538</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>638</v>
+        <v>539</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6439,10 +6460,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1084</v>
+        <v>637</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>554</v>
+        <v>638</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6450,10 +6471,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1064</v>
+        <v>1084</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1065</v>
+        <v>554</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6461,10 +6482,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6472,7 +6493,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>1062</v>
@@ -6483,10 +6504,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>965</v>
+        <v>1063</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>966</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6494,32 +6515,32 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>606</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6527,7 +6548,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>590</v>
+        <v>636</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>563</v>
@@ -6538,10 +6559,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>531</v>
+        <v>590</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>540</v>
+        <v>563</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6549,10 +6570,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6560,10 +6581,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1076</v>
+        <v>532</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1077</v>
+        <v>554</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6571,10 +6592,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1070</v>
+        <v>1076</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1069</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6582,10 +6603,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6593,10 +6614,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6604,10 +6625,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1078</v>
+        <v>1071</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1079</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6615,10 +6636,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>951</v>
+        <v>1078</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>646</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6626,21 +6647,21 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>650</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6648,10 +6669,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6659,10 +6680,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>596</v>
+        <v>628</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>597</v>
+        <v>633</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6670,10 +6691,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6681,10 +6702,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6692,10 +6713,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -6703,43 +6724,43 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="80" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>618</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6747,32 +6768,32 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>1080</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>1081</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="1" t="s">
+    <row r="84" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>605</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -6780,10 +6801,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>960</v>
+        <v>543</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>961</v>
+        <v>544</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -6791,10 +6812,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6802,10 +6823,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>233</v>
+        <v>959</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>234</v>
+        <v>962</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6813,10 +6834,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>536</v>
+        <v>233</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>537</v>
+        <v>234</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -6824,10 +6845,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>634</v>
+        <v>536</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>635</v>
+        <v>537</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6835,10 +6856,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>533</v>
+        <v>634</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>186</v>
+        <v>635</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6846,32 +6867,32 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="1" t="s">
+    <row r="93" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>944</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -6879,10 +6900,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>586</v>
+        <v>944</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>603</v>
+        <v>945</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -6890,10 +6911,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>589</v>
+        <v>603</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -6901,10 +6922,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -6912,10 +6933,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>621</v>
+        <v>604</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -6923,10 +6944,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -6934,10 +6955,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>582</v>
+        <v>622</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>583</v>
+        <v>623</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -6945,10 +6966,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>624</v>
+        <v>582</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>625</v>
+        <v>583</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -6956,10 +6977,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -6967,10 +6988,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>607</v>
+        <v>629</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>608</v>
+        <v>630</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -6978,10 +6999,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>584</v>
+        <v>607</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>585</v>
+        <v>608</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -6989,10 +7010,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1051</v>
+        <v>584</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1052</v>
+        <v>585</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -7000,10 +7021,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -7011,10 +7032,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1087</v>
+        <v>1049</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1088</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -7022,10 +7043,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -7033,10 +7054,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>641</v>
+        <v>1085</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>642</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -7044,10 +7065,10 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>946</v>
+        <v>641</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>947</v>
+        <v>642</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -7055,10 +7076,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -7066,10 +7087,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -7077,10 +7098,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>534</v>
+        <v>943</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>535</v>
+        <v>950</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -7088,10 +7109,10 @@
         <v>0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>987</v>
+        <v>534</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>477</v>
+        <v>535</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -7099,10 +7120,10 @@
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>971</v>
+        <v>987</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>235</v>
+        <v>477</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -7110,10 +7131,10 @@
         <v>0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>988</v>
+        <v>971</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -7121,10 +7142,10 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>996</v>
+        <v>988</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>479</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -7132,32 +7153,32 @@
         <v>0</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" s="1" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -7165,10 +7186,10 @@
         <v>0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>976</v>
+        <v>529</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -7176,7 +7197,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>517</v>
+        <v>976</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>236</v>
@@ -7187,10 +7208,10 @@
         <v>0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>515</v>
+        <v>1110</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>236</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -7198,10 +7219,10 @@
         <v>0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>975</v>
+        <v>1108</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>974</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -7209,10 +7230,10 @@
         <v>0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>972</v>
+        <v>517</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>973</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -7220,10 +7241,10 @@
         <v>0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>488</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -7231,15 +7252,59 @@
         <v>0</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C126">
-    <sortCondition ref="B124:B126"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C130">
+    <sortCondition ref="B110:B130"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11415,7 +11480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E80EDE8-D86E-1440-915D-7FDF56424186}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Mixture is quite useful now
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19C7263-24B8-49D6-98E1-44463A2FE4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD54F03A-DBD7-4F6F-8B9B-2AF7BCFA3141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1134">
   <si>
     <t>cs</t>
   </si>
@@ -3464,6 +3464,27 @@
   </si>
   <si>
     <t>Výrobce aromatu</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat mix</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.ratio.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.nicotine.label</t>
+  </si>
+  <si>
+    <t>Obsah nikotinu</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.aromaId.label</t>
   </si>
 </sst>
 </file>
@@ -4870,10 +4891,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4965,10 +4986,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1113</v>
+        <v>1123</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>608</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4976,10 +4997,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1112</v>
+        <v>1125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1111</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4987,10 +5008,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1115</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4998,10 +5019,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1122</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5009,10 +5030,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>608</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5020,10 +5041,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1116</v>
+        <v>1121</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1117</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5031,10 +5052,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1120</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5042,10 +5063,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>249</v>
+        <v>1116</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>250</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5053,10 +5074,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>303</v>
+        <v>1119</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>304</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5064,10 +5085,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5075,10 +5096,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>263</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5086,10 +5107,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1057</v>
+        <v>1133</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1058</v>
+        <v>556</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5097,10 +5118,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>541</v>
+        <v>1131</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>542</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5108,10 +5129,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>310</v>
+        <v>1129</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>311</v>
+        <v>608</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,10 +5140,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>314</v>
+        <v>1127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>315</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,10 +5151,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>312</v>
+        <v>1130</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>313</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5141,10 +5162,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>318</v>
+        <v>251</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>317</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5152,10 +5173,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>323</v>
+        <v>264</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5163,10 +5184,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>321</v>
+        <v>1057</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>322</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5174,10 +5195,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>388</v>
+        <v>541</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>10</v>
+        <v>542</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5185,10 +5206,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1089</v>
+        <v>310</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1090</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,10 +5217,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5207,10 +5228,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5218,10 +5239,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5229,10 +5250,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,10 +5261,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5251,10 +5272,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>305</v>
+        <v>388</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>267</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5262,10 +5283,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>319</v>
+        <v>1089</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>320</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5273,10 +5294,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5284,10 +5305,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1082</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5295,10 +5316,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5306,10 +5327,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1083</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5317,10 +5338,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5328,10 +5349,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>553</v>
+        <v>305</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5339,21 +5360,21 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1075</v>
+        <v>319</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1036</v>
+        <v>332</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1038</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5361,10 +5382,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1037</v>
+        <v>307</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1039</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5372,10 +5393,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1035</v>
+        <v>326</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1040</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5383,10 +5404,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>69</v>
+        <v>316</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5394,10 +5415,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>253</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5405,10 +5426,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>256</v>
+        <v>553</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>257</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5416,21 +5437,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>252</v>
+        <v>1075</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>258</v>
+        <v>1036</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>259</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5438,10 +5459,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>559</v>
+        <v>1037</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>560</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5449,10 +5470,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>561</v>
+        <v>1035</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>562</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5460,10 +5481,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>643</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>644</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5471,10 +5492,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1046</v>
+        <v>254</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5482,10 +5503,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1059</v>
+        <v>256</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1060</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5493,10 +5514,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1053</v>
+        <v>252</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1054</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5504,10 +5525,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1055</v>
+        <v>258</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1056</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5515,10 +5536,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1043</v>
+        <v>559</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1044</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5526,10 +5547,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>265</v>
+        <v>561</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>266</v>
+        <v>562</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5537,10 +5558,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
+        <v>643</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>134</v>
+        <v>644</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5548,10 +5569,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1023</v>
+        <v>1046</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1024</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5559,10 +5580,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1030</v>
+        <v>1059</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1031</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5570,10 +5591,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1020</v>
+        <v>1053</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1021</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5581,10 +5602,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1018</v>
+        <v>1055</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1019</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5592,10 +5613,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1026</v>
+        <v>1043</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1027</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5603,10 +5624,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1028</v>
+        <v>265</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1029</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5614,10 +5635,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1022</v>
+        <v>133</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1025</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5625,10 +5646,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1033</v>
+        <v>1023</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1034</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5636,10 +5657,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1093</v>
+        <v>1030</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1094</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5647,10 +5668,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1123</v>
+        <v>1020</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1124</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5658,15 +5679,70 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1125</v>
+        <v>1018</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1126</v>
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C69">
-    <sortCondition ref="B67:B69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
+    <sortCondition ref="B71:B76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Improved mix stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD54F03A-DBD7-4F6F-8B9B-2AF7BCFA3141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9171A09F-349D-41B1-B3B3-18E893187C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1135">
   <si>
     <t>cs</t>
   </si>
@@ -3485,6 +3485,9 @@
   </si>
   <si>
     <t>common.filter.Mixtures.filter.aromaId.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.boosterId.label</t>
   </si>
 </sst>
 </file>
@@ -4891,10 +4894,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5738,6 +5741,17 @@
       </c>
       <c r="C76" s="1" t="s">
         <v>1094</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved mix stuff II
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9171A09F-349D-41B1-B3B3-18E893187C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E6BE18-37FD-45D8-AA0F-67DEBCBB0C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="1136">
   <si>
     <t>cs</t>
   </si>
@@ -3488,6 +3488,9 @@
   </si>
   <si>
     <t>common.filter.Mixtures.filter.boosterId.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.baseId.label</t>
   </si>
 </sst>
 </file>
@@ -4894,10 +4897,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5121,10 +5124,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1131</v>
+        <v>1135</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1132</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5132,10 +5135,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1129</v>
+        <v>1134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>608</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5143,10 +5146,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1127</v>
+        <v>1131</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1128</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5154,10 +5157,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1126</v>
+        <v>608</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5165,10 +5168,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>251</v>
+        <v>1127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>248</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5176,10 +5179,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>264</v>
+        <v>1130</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>263</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5187,10 +5190,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1057</v>
+        <v>251</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1058</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5198,10 +5201,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>541</v>
+        <v>264</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>542</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5209,10 +5212,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>310</v>
+        <v>1057</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>311</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5220,10 +5223,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>314</v>
+        <v>541</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>315</v>
+        <v>542</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5231,10 +5234,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5242,10 +5245,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5253,10 +5256,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>248</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5264,10 +5267,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5275,10 +5278,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>388</v>
+        <v>323</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5286,10 +5289,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1089</v>
+        <v>321</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1090</v>
+        <v>322</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5297,10 +5300,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>335</v>
+        <v>388</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>268</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5308,10 +5311,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>306</v>
+        <v>1089</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>162</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5319,10 +5322,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>334</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5330,10 +5333,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>309</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5341,10 +5344,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5352,10 +5355,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5363,10 +5366,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5374,10 +5377,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5385,10 +5388,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1082</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5396,10 +5399,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5407,10 +5410,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5418,10 +5421,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5429,10 +5432,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>553</v>
+        <v>316</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5440,21 +5443,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1075</v>
+        <v>330</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1036</v>
+        <v>553</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1038</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5462,21 +5465,21 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1037</v>
+        <v>1075</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5484,10 +5487,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>69</v>
+        <v>1037</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>70</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5495,10 +5498,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>254</v>
+        <v>1035</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>253</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5506,10 +5509,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>256</v>
+        <v>69</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>257</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5517,10 +5520,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5528,10 +5531,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5539,10 +5542,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>559</v>
+        <v>252</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>560</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5550,10 +5553,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>561</v>
+        <v>258</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>562</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5561,10 +5564,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>643</v>
+        <v>559</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>644</v>
+        <v>560</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5572,10 +5575,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1046</v>
+        <v>561</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>242</v>
+        <v>562</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5583,10 +5586,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1059</v>
+        <v>643</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1060</v>
+        <v>644</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5594,10 +5597,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1053</v>
+        <v>1046</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1054</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5605,10 +5608,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5616,10 +5619,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1043</v>
+        <v>1053</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1044</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5627,10 +5630,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>265</v>
+        <v>1055</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>266</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5638,10 +5641,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>133</v>
+        <v>1043</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>134</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5649,10 +5652,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1023</v>
+        <v>265</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1024</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5660,10 +5663,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1030</v>
+        <v>133</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1031</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5671,10 +5674,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5682,10 +5685,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1018</v>
+        <v>1030</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1019</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5693,10 +5696,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5704,10 +5707,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1028</v>
+        <v>1018</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1029</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -5715,10 +5718,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -5726,10 +5729,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1033</v>
+        <v>1028</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1034</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -5737,10 +5740,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1093</v>
+        <v>1022</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1094</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5748,15 +5751,26 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1134</v>
+        <v>1033</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1056</v>
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
-    <sortCondition ref="B71:B76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
+    <sortCondition ref="B78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: A lot of intereting stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E6BE18-37FD-45D8-AA0F-67DEBCBB0C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06214CE8-2BB8-4AFC-8F95-2250B9184288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="1153">
   <si>
     <t>cs</t>
   </si>
@@ -3491,6 +3491,57 @@
   </si>
   <si>
     <t>common.filter.Mixtures.filter.baseId.label</t>
+  </si>
+  <si>
+    <t>common.job.name.migrate</t>
+  </si>
+  <si>
+    <t>Migrace</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.button</t>
+  </si>
+  <si>
+    <t>Namíchat</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.title</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.content</t>
+  </si>
+  <si>
+    <t>Přejete si namíchat liquid z vybraného mixu? Datum zrání započne jeho vytvořením.</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.aroma</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.pgvg</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.content</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.base</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.booster</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.ok.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.success</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquid.create.failure</t>
+  </si>
+  <si>
+    <t>Liquid se nepodařilo namíchat.</t>
+  </si>
+  <si>
+    <t>Liquid úspěšně namíchán.</t>
   </si>
 </sst>
 </file>
@@ -4897,10 +4948,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5322,10 +5373,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>335</v>
+        <v>1136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>268</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5333,10 +5384,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>306</v>
+        <v>335</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>162</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5344,10 +5395,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>334</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5355,10 +5406,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5366,10 +5417,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5377,10 +5428,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>267</v>
+        <v>329</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5388,10 +5439,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5399,7 +5450,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>320</v>
@@ -5410,10 +5461,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1082</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,10 +5472,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>327</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5432,10 +5483,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1083</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5443,10 +5494,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>331</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5454,10 +5505,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>553</v>
+        <v>330</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5465,32 +5516,32 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>1038</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5498,10 +5549,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5509,10 +5560,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>69</v>
+        <v>1035</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>70</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5520,10 +5571,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5531,10 +5582,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5542,10 +5593,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5553,10 +5604,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5564,10 +5615,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>559</v>
+        <v>258</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>560</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5575,10 +5626,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5586,10 +5637,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>643</v>
+        <v>561</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>644</v>
+        <v>562</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5597,10 +5648,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1046</v>
+        <v>643</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>242</v>
+        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5608,10 +5659,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1059</v>
+        <v>1046</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1060</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5619,10 +5670,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1053</v>
+        <v>1059</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1054</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5630,10 +5681,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5641,10 +5692,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1043</v>
+        <v>1055</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1044</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5652,10 +5703,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>265</v>
+        <v>1043</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>266</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5663,10 +5714,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5674,10 +5725,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1023</v>
+        <v>133</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1024</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5685,10 +5736,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5696,10 +5747,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1020</v>
+        <v>1030</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1021</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5707,10 +5758,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -5718,10 +5769,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1026</v>
+        <v>1018</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1027</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -5729,10 +5780,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -5740,10 +5791,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5751,10 +5802,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1033</v>
+        <v>1022</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1034</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5762,15 +5813,26 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>1093</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>1094</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
-    <sortCondition ref="B78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C79">
+    <sortCondition ref="B70:B79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6110,10 +6172,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7470,10 +7532,10 @@
         <v>0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1108</v>
+        <v>1138</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1109</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -7481,10 +7543,10 @@
         <v>0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>517</v>
+        <v>1108</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>236</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -7492,7 +7554,7 @@
         <v>0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>236</v>
@@ -7503,10 +7565,10 @@
         <v>0</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>975</v>
+        <v>515</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>974</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -7514,10 +7576,10 @@
         <v>0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -7525,10 +7587,10 @@
         <v>0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>489</v>
+        <v>972</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>488</v>
+        <v>973</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -7536,10 +7598,10 @@
         <v>0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1106</v>
+        <v>489</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1107</v>
+        <v>488</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -7547,15 +7609,136 @@
         <v>0</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>239</v>
       </c>
     </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C130">
-    <sortCondition ref="B110:B130"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C131">
+    <sortCondition ref="B126:B131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Added another filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE90E6B-2668-4356-847C-30866595AA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7243CD31-75C2-47F9-81FE-63CFC4253099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1161">
   <si>
     <t>cs</t>
   </si>
@@ -3557,6 +3557,15 @@
   </si>
   <si>
     <t>common.filter.Liquids.filter.baseId.label</t>
+  </si>
+  <si>
+    <t>common.filter.Aromas.filter.tasteIds.label</t>
+  </si>
+  <si>
+    <t>Filtr příchutí</t>
+  </si>
+  <si>
+    <t>common.filter.Mixtures.filter.tasteIds.label</t>
   </si>
 </sst>
 </file>
@@ -4964,10 +4973,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5888,6 +5897,28 @@
       </c>
       <c r="C83" s="1" t="s">
         <v>1094</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -12924,7 +12955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F5805-0158-F34C-9256-85EB751C6431}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Atomizer filter is quite clever now
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DCB537-2147-4C74-9083-4B53BB4E8F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587F51A6-F306-4A86-8405-8B0EA8129F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1174">
   <si>
     <t>cs</t>
   </si>
@@ -3583,10 +3583,28 @@
     <t>Výrobce atomizéru</t>
   </si>
   <si>
-    <t>common.filter.Atomizers.filter.drawIds.label</t>
-  </si>
-  <si>
-    <t>Typ potahu</t>
+    <t>common.filter.Atomizers.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.Atomizers.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Atomizér musí splnit všechny vybrané typy potahů.</t>
+  </si>
+  <si>
+    <t>Typ potahu (veškeré)</t>
+  </si>
+  <si>
+    <t>common.filter.Atomizers.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>Typ potahu (některé)</t>
+  </si>
+  <si>
+    <t>common.filter.Atomizers.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Atomizér může splnit některý z vybraného typu potahu.</t>
   </si>
 </sst>
 </file>
@@ -4994,10 +5012,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,7 +5990,40 @@
         <v>1166</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>1167</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved aroma filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587F51A6-F306-4A86-8405-8B0EA8129F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B3B36-359C-4BF7-8BB4-F34B40B1D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="1181">
   <si>
     <t>cs</t>
   </si>
@@ -3559,9 +3559,6 @@
     <t>common.filter.Liquids.filter.baseId.label</t>
   </si>
   <si>
-    <t>common.filter.Aromas.filter.tasteIds.label</t>
-  </si>
-  <si>
     <t>Filtr příchutí</t>
   </si>
   <si>
@@ -3605,13 +3602,37 @@
   </si>
   <si>
     <t>Atomizér může splnit některý z vybraného typu potahu.</t>
+  </si>
+  <si>
+    <t>common.filter.Aromas.filter.andTasteIds.label</t>
+  </si>
+  <si>
+    <t>Filtr příchutí (veškeré)</t>
+  </si>
+  <si>
+    <t>common.filter.Aromas.filter.orTasteIds.label</t>
+  </si>
+  <si>
+    <t>Filtr příchutí (některé)</t>
+  </si>
+  <si>
+    <t>common.filter.Aromas.filter.andTasteIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Aroma musí odpovídat všem vybraným příchutím.</t>
+  </si>
+  <si>
+    <t>common.filter.Aromas.filter.orTasteIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Aroma musí obsahovat některou z vybraných příchutí.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3650,6 +3671,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3694,7 +3722,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -3718,6 +3746,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="import" xfId="2" xr:uid="{DD1BC027-BC6C-4B34-B536-A533FDE94B7A}"/>
@@ -5012,10 +5043,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5102,15 +5133,15 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>1123</v>
+      <c r="B8" s="19" t="s">
+        <v>1173</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1124</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5118,10 +5149,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1125</v>
+        <v>1177</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1126</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5129,10 +5160,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1113</v>
+        <v>1175</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>608</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5140,10 +5171,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1112</v>
+        <v>1179</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1111</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5151,10 +5182,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1114</v>
+        <v>1123</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1115</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5162,10 +5193,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1122</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5173,10 +5204,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1118</v>
+        <v>1165</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>608</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5184,10 +5215,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1116</v>
+        <v>1166</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1117</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5195,10 +5226,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1119</v>
+        <v>1169</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1120</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5206,10 +5237,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>249</v>
+        <v>1171</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>250</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5217,10 +5248,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>303</v>
+        <v>1161</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>304</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5228,10 +5259,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1155</v>
+        <v>1163</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1042</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5239,10 +5270,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1157</v>
+        <v>1113</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1054</v>
+        <v>608</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5250,10 +5281,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1156</v>
+        <v>1112</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1056</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5261,10 +5292,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1153</v>
+        <v>1114</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1154</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5272,10 +5303,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1133</v>
+        <v>1121</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>556</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5283,10 +5314,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1135</v>
+        <v>1118</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1054</v>
+        <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5294,10 +5325,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1134</v>
+        <v>1116</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1056</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5305,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1131</v>
+        <v>1119</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1132</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5316,10 +5347,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1129</v>
+        <v>249</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>608</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5327,10 +5358,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1127</v>
+        <v>303</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1128</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5338,10 +5369,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1130</v>
+        <v>1155</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1126</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5349,10 +5380,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>251</v>
+        <v>1157</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>248</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5360,10 +5391,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>264</v>
+        <v>1156</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>263</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5371,10 +5402,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1057</v>
+        <v>1153</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1058</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5382,10 +5413,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>541</v>
+        <v>1133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>542</v>
+        <v>556</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5393,10 +5424,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>310</v>
+        <v>1135</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>311</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5404,10 +5435,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>314</v>
+        <v>1134</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>315</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5415,10 +5446,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>312</v>
+        <v>1131</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>313</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5426,10 +5457,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>318</v>
+        <v>1129</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>317</v>
+        <v>608</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5437,10 +5468,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>323</v>
+        <v>1159</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>248</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5448,10 +5479,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>321</v>
+        <v>1127</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>322</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5459,10 +5490,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>388</v>
+        <v>1130</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>10</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5470,10 +5501,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1089</v>
+        <v>251</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1090</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5481,10 +5512,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1136</v>
+        <v>264</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1137</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5492,10 +5523,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>335</v>
+        <v>1057</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>268</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5503,10 +5534,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>306</v>
+        <v>541</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>162</v>
+        <v>542</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5514,10 +5545,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5525,10 +5556,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,10 +5567,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5547,10 +5578,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5558,10 +5589,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>320</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5569,10 +5600,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5580,10 +5611,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>307</v>
+        <v>388</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1082</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5591,10 +5622,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>326</v>
+        <v>1089</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>327</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5602,10 +5633,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>316</v>
+        <v>1136</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1083</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5613,10 +5644,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>331</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5624,10 +5655,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>553</v>
+        <v>306</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5635,21 +5666,21 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1075</v>
+        <v>333</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1036</v>
+        <v>308</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1038</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5657,10 +5688,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1037</v>
+        <v>328</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1039</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5668,10 +5699,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1035</v>
+        <v>305</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1040</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5679,10 +5710,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>319</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>70</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5690,10 +5721,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>254</v>
+        <v>332</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>253</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5701,10 +5732,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>257</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5712,10 +5743,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>252</v>
+        <v>326</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>255</v>
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5723,10 +5754,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>258</v>
+        <v>316</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>259</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5734,10 +5765,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>559</v>
+        <v>330</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>560</v>
+        <v>331</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5745,10 +5776,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>562</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5756,21 +5787,21 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>643</v>
+        <v>1075</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1046</v>
+        <v>1036</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>242</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5778,10 +5809,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1059</v>
+        <v>1037</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1060</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5789,10 +5820,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1053</v>
+        <v>1035</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1054</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5800,10 +5831,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1055</v>
+        <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1056</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5811,10 +5842,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1043</v>
+        <v>254</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1044</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5822,10 +5853,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -5833,10 +5864,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>134</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -5844,10 +5875,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1023</v>
+        <v>258</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1024</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -5855,10 +5886,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1030</v>
+        <v>559</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1031</v>
+        <v>560</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5866,10 +5897,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1020</v>
+        <v>561</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1021</v>
+        <v>562</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5877,10 +5908,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1018</v>
+        <v>643</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1019</v>
+        <v>644</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -5888,10 +5919,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1026</v>
+        <v>1046</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1027</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -5899,10 +5930,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1028</v>
+        <v>1059</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1029</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -5910,10 +5941,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1022</v>
+        <v>1053</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1025</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -5921,10 +5952,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1033</v>
+        <v>1055</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1034</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -5932,10 +5963,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1093</v>
+        <v>1043</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1094</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -5943,10 +5974,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1158</v>
+        <v>265</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1159</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -5954,10 +5985,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1160</v>
+        <v>133</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -5965,10 +5996,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1162</v>
+        <v>1023</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1163</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5976,10 +6007,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1164</v>
+        <v>1030</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1165</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -5987,10 +6018,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1166</v>
+        <v>1020</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1169</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -5998,10 +6029,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1167</v>
+        <v>1018</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1168</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -6009,10 +6040,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1170</v>
+        <v>1026</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1171</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -6020,15 +6051,48 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>1172</v>
+        <v>1028</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1173</v>
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">
-    <sortCondition ref="B82:B83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C94">
+    <sortCondition ref="B81:B94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7849,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>1132</v>

</xml_diff>

<commit_message>
Common: Added mod search
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B3B36-359C-4BF7-8BB4-F34B40B1D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB025A-0211-4B7C-BB29-8F36A0FCE4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1193">
   <si>
     <t>cs</t>
   </si>
@@ -3626,6 +3626,42 @@
   </si>
   <si>
     <t>Aroma musí obsahovat některou z vybraných příchutí.</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledávání modů</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce modu</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.andCellIds.label</t>
+  </si>
+  <si>
+    <t>Typ článku (veškeré)</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.orCellIds.label</t>
+  </si>
+  <si>
+    <t>Typ článku (některé)</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.andCellIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Mod musí podporovat všechny vybrané typy článků.</t>
+  </si>
+  <si>
+    <t>common.filter.Mods.filter.orCellIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Mod musí podporovat některý z vybraného typu článku.</t>
   </si>
 </sst>
 </file>
@@ -5043,10 +5079,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6088,6 +6124,72 @@
       </c>
       <c r="C94" s="1" t="s">
         <v>1094</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added cotton search
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB025A-0211-4B7C-BB29-8F36A0FCE4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35600043-DBFE-4C67-B456-1D3EB045BC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="1205">
   <si>
     <t>cs</t>
   </si>
@@ -3662,6 +3662,42 @@
   </si>
   <si>
     <t>Mod musí podporovat některý z vybraného typu článku.</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat vatu</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce vaty</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>Vhodný typ potahu (veškeré)</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>Vhodný typ potahu (některý)</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vata musí být vhodná pro veškeré vybrané typy potahů.</t>
+  </si>
+  <si>
+    <t>common.filter.Cottons.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vata musí být vhodná pro některý z vybraného typu potahu.</t>
   </si>
 </sst>
 </file>
@@ -5079,10 +5115,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6190,6 +6226,72 @@
       </c>
       <c r="C100" s="1" t="s">
         <v>1192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>1204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added cell search
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35600043-DBFE-4C67-B456-1D3EB045BC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AA97A2-70AC-4A6E-8B0E-9766A2CE40E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6210" yWindow="1860" windowWidth="33795" windowHeight="18495" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="1205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="1215">
   <si>
     <t>cs</t>
   </si>
@@ -3698,6 +3698,36 @@
   </si>
   <si>
     <t>Vata musí být vhodná pro některý z vybraného typu potahu.</t>
+  </si>
+  <si>
+    <t>common.cell.ohm.tooltip</t>
+  </si>
+  <si>
+    <t>Minimální bezpečný odpor pro článek; započítán je nižší vybíjecí proud článku, než je uvedený.</t>
+  </si>
+  <si>
+    <t>common.filter.Cells.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat článek</t>
+  </si>
+  <si>
+    <t>common.filter.Cells.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce článku</t>
+  </si>
+  <si>
+    <t>common.filter.Cells.filter.orTypeIds.label</t>
+  </si>
+  <si>
+    <t>Typ článku (některý)</t>
+  </si>
+  <si>
+    <t>common.filter.Cells.filter.orTypeIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Článek musí být některý z vybraného typu.</t>
   </si>
 </sst>
 </file>
@@ -5115,10 +5145,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6292,6 +6322,61 @@
       </c>
       <c r="C106" s="1" t="s">
         <v>1204</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>1214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed menus II
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D71DCB-3D15-6B4E-9F8A-229FE6EB2A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217B016-F312-CF49-930D-6A84B584C8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="6" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1219">
   <si>
     <t>cs</t>
   </si>
@@ -3737,6 +3737,9 @@
   </si>
   <si>
     <t>lab.mixture.preview.aromaContent</t>
+  </si>
+  <si>
+    <t>market.liquid.menu</t>
   </si>
 </sst>
 </file>
@@ -6732,8 +6735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11188,10 +11191,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12068,6 +12071,17 @@
       </c>
       <c r="C79" s="1" t="s">
         <v>463</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing coil stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217B016-F312-CF49-930D-6A84B584C8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DF9D87-13A6-EF43-B655-2D1F653D69FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1218">
   <si>
     <t>cs</t>
   </si>
@@ -2428,36 +2428,9 @@
     <t>sort</t>
   </si>
   <si>
-    <t>glass</t>
-  </si>
-  <si>
     <t>material</t>
   </si>
   <si>
-    <t>delrin</t>
-  </si>
-  <si>
-    <t>wood</t>
-  </si>
-  <si>
-    <t>metal</t>
-  </si>
-  <si>
-    <t>carbon</t>
-  </si>
-  <si>
-    <t>acryl</t>
-  </si>
-  <si>
-    <t>plastic</t>
-  </si>
-  <si>
-    <t>resin</t>
-  </si>
-  <si>
-    <t>silicon</t>
-  </si>
-  <si>
     <t>rmtl</t>
   </si>
   <si>
@@ -3740,6 +3713,30 @@
   </si>
   <si>
     <t>market.liquid.menu</t>
+  </si>
+  <si>
+    <t>SS316</t>
+  </si>
+  <si>
+    <t>SS316L</t>
+  </si>
+  <si>
+    <t>Kanthal</t>
+  </si>
+  <si>
+    <t>Ni80</t>
+  </si>
+  <si>
+    <t>Ni90</t>
+  </si>
+  <si>
+    <t>NiFe30</t>
+  </si>
+  <si>
+    <t>NiFe48</t>
+  </si>
+  <si>
+    <t>common.vendor.generic</t>
   </si>
 </sst>
 </file>
@@ -4263,58 +4260,58 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="B14" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="B15" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="B16" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>857</v>
+        <v>848</v>
       </c>
       <c r="B17" t="s">
-        <v>858</v>
+        <v>849</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>866</v>
+        <v>857</v>
       </c>
       <c r="B18" t="s">
-        <v>867</v>
+        <v>858</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="B19" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="B20" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -4466,10 +4463,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
-  <dimension ref="A1:A99"/>
+  <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4624,7 +4621,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>1101</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -4970,6 +4967,11 @@
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>762</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1217</v>
       </c>
     </row>
   </sheetData>
@@ -5230,10 +5232,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1091</v>
+        <v>1082</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1092</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -5252,10 +5254,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -5263,10 +5265,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1177</v>
+        <v>1168</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -5274,10 +5276,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -5285,10 +5287,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1179</v>
+        <v>1170</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1180</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -5296,10 +5298,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1123</v>
+        <v>1114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1124</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -5307,10 +5309,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1125</v>
+        <v>1116</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1126</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -5318,10 +5320,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1165</v>
+        <v>1156</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1168</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -5329,10 +5331,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -5340,10 +5342,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1170</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5351,10 +5353,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1171</v>
+        <v>1162</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5362,10 +5364,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1161</v>
+        <v>1152</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1162</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -5373,10 +5375,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -5384,7 +5386,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1113</v>
+        <v>1104</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>608</v>
@@ -5395,10 +5397,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1112</v>
+        <v>1103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1111</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -5406,10 +5408,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1114</v>
+        <v>1105</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1115</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -5417,10 +5419,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1122</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -5428,7 +5430,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1118</v>
+        <v>1109</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>608</v>
@@ -5439,10 +5441,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1116</v>
+        <v>1107</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1117</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -5450,10 +5452,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1119</v>
+        <v>1110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1120</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -5483,10 +5485,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1155</v>
+        <v>1146</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -5494,10 +5496,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1054</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -5505,10 +5507,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1156</v>
+        <v>1147</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1056</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -5516,10 +5518,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1154</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -5527,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1133</v>
+        <v>1124</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>556</v>
@@ -5538,10 +5540,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1135</v>
+        <v>1126</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1054</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -5549,10 +5551,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1134</v>
+        <v>1125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1056</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -5560,10 +5562,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1131</v>
+        <v>1122</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1132</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -5571,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1129</v>
+        <v>1120</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>608</v>
@@ -5582,10 +5584,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1159</v>
+        <v>1150</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1158</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -5593,10 +5595,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1127</v>
+        <v>1118</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1128</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -5604,10 +5606,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1130</v>
+        <v>1121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1126</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -5637,10 +5639,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1057</v>
+        <v>1048</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1058</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -5736,10 +5738,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1089</v>
+        <v>1080</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1090</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -5747,10 +5749,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1136</v>
+        <v>1127</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1137</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -5849,7 +5851,7 @@
         <v>307</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1082</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -5871,7 +5873,7 @@
         <v>316</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1083</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -5901,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1075</v>
+        <v>1066</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>242</v>
@@ -5912,10 +5914,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1036</v>
+        <v>1027</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1038</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -5923,10 +5925,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1037</v>
+        <v>1028</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1039</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -5934,10 +5936,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1035</v>
+        <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1040</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -6033,7 +6035,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1046</v>
+        <v>1037</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>242</v>
@@ -6044,10 +6046,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1059</v>
+        <v>1050</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1060</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -6055,10 +6057,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1053</v>
+        <v>1044</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1054</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -6066,10 +6068,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1055</v>
+        <v>1046</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1056</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -6077,10 +6079,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1043</v>
+        <v>1034</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1044</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -6110,10 +6112,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -6121,10 +6123,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1031</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -6132,10 +6134,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1020</v>
+        <v>1011</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1021</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -6143,10 +6145,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1018</v>
+        <v>1009</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -6154,10 +6156,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1027</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -6165,10 +6167,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>1028</v>
+        <v>1019</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1029</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -6176,10 +6178,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1025</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -6187,10 +6189,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1033</v>
+        <v>1024</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1034</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -6198,10 +6200,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1093</v>
+        <v>1084</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1094</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -6209,10 +6211,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1181</v>
+        <v>1172</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1182</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -6220,10 +6222,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1183</v>
+        <v>1174</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1184</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -6231,10 +6233,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1185</v>
+        <v>1176</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1186</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -6242,10 +6244,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1188</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -6253,10 +6255,10 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1190</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -6264,10 +6266,10 @@
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>1191</v>
+        <v>1182</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -6275,10 +6277,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1194</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -6286,10 +6288,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1196</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -6297,10 +6299,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1197</v>
+        <v>1188</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1198</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -6308,10 +6310,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1199</v>
+        <v>1190</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1200</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -6319,10 +6321,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1201</v>
+        <v>1192</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1202</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -6330,10 +6332,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1203</v>
+        <v>1194</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1204</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -6341,10 +6343,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1205</v>
+        <v>1196</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1206</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -6352,10 +6354,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1207</v>
+        <v>1198</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1208</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -6363,10 +6365,10 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>1209</v>
+        <v>1200</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1210</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -6374,10 +6376,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1211</v>
+        <v>1202</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1212</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -6385,10 +6387,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>1213</v>
+        <v>1204</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1214</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -6817,10 +6819,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1041</v>
+        <v>1032</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6828,10 +6830,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1045</v>
+        <v>1036</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -6861,10 +6863,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>969</v>
+        <v>960</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>970</v>
+        <v>961</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -6872,10 +6874,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>967</v>
+        <v>958</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -6927,10 +6929,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>990</v>
+        <v>981</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>991</v>
+        <v>982</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6938,10 +6940,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -6982,10 +6984,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>995</v>
+        <v>986</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -6993,10 +6995,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>992</v>
+        <v>983</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -7004,10 +7006,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -7015,10 +7017,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -7026,10 +7028,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1104</v>
+        <v>1095</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1105</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -7070,10 +7072,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -7081,10 +7083,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>977</v>
+        <v>968</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -7114,10 +7116,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>984</v>
+        <v>975</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>985</v>
+        <v>976</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -7125,10 +7127,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -7191,10 +7193,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>941</v>
+        <v>932</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -7301,10 +7303,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1067</v>
+        <v>1058</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1068</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -7312,10 +7314,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1066</v>
+        <v>1057</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -7345,7 +7347,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1084</v>
+        <v>1075</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>554</v>
@@ -7356,10 +7358,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1064</v>
+        <v>1055</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1065</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -7367,10 +7369,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1061</v>
+        <v>1052</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1062</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -7378,10 +7380,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1063</v>
+        <v>1054</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1062</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -7389,10 +7391,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>965</v>
+        <v>956</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>966</v>
+        <v>957</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -7400,10 +7402,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -7466,10 +7468,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1076</v>
+        <v>1067</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1077</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -7477,10 +7479,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1070</v>
+        <v>1061</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1069</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -7488,10 +7490,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1073</v>
+        <v>1064</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1074</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -7499,10 +7501,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1071</v>
+        <v>1062</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1072</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -7510,10 +7512,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1078</v>
+        <v>1069</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1079</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -7521,7 +7523,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>951</v>
+        <v>942</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>646</v>
@@ -7532,7 +7534,7 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>952</v>
+        <v>943</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>650</v>
@@ -7653,10 +7655,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1080</v>
+        <v>1071</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1081</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -7686,10 +7688,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -7697,10 +7699,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -7774,10 +7776,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>945</v>
+        <v>936</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -7895,10 +7897,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1051</v>
+        <v>1042</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1052</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -7906,10 +7908,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1049</v>
+        <v>1040</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -7917,10 +7919,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1087</v>
+        <v>1078</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1088</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -7928,10 +7930,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1085</v>
+        <v>1076</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1086</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -7950,10 +7952,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>946</v>
+        <v>937</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>947</v>
+        <v>938</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -7961,10 +7963,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -7972,10 +7974,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>943</v>
+        <v>934</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -7994,7 +7996,7 @@
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>477</v>
@@ -8005,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>971</v>
+        <v>962</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>235</v>
@@ -8016,7 +8018,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>988</v>
+        <v>979</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>240</v>
@@ -8027,7 +8029,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>996</v>
+        <v>987</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>479</v>
@@ -8038,7 +8040,7 @@
         <v>0</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>981</v>
+        <v>972</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>237</v>
@@ -8049,7 +8051,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>986</v>
+        <v>977</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>238</v>
@@ -8071,7 +8073,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>236</v>
@@ -8082,10 +8084,10 @@
         <v>0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1110</v>
+        <v>1101</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1109</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -8093,10 +8095,10 @@
         <v>0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1138</v>
+        <v>1129</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -8104,10 +8106,10 @@
         <v>0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1141</v>
+        <v>1132</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1142</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -8115,10 +8117,10 @@
         <v>0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1151</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -8126,10 +8128,10 @@
         <v>0</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -8137,10 +8139,10 @@
         <v>0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1149</v>
+        <v>1140</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1152</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -8148,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1140</v>
+        <v>1131</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>554</v>
@@ -8159,10 +8161,10 @@
         <v>0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1108</v>
+        <v>1099</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1109</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -8170,7 +8172,7 @@
         <v>0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>556</v>
@@ -8181,7 +8183,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>240</v>
@@ -8192,7 +8194,7 @@
         <v>0</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1147</v>
+        <v>1138</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>610</v>
@@ -8203,7 +8205,7 @@
         <v>0</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1145</v>
+        <v>1136</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>583</v>
@@ -8214,10 +8216,10 @@
         <v>0</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1160</v>
+        <v>1151</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1132</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -8225,7 +8227,7 @@
         <v>0</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1144</v>
+        <v>1135</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>608</v>
@@ -8258,10 +8260,10 @@
         <v>0</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -8269,10 +8271,10 @@
         <v>0</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>972</v>
+        <v>963</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>973</v>
+        <v>964</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -8291,10 +8293,10 @@
         <v>0</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1106</v>
+        <v>1097</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1107</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -8313,10 +8315,10 @@
         <v>0</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1215</v>
+        <v>1206</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -8324,7 +8326,7 @@
         <v>0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>1216</v>
+        <v>1207</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>537</v>
@@ -8335,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1217</v>
+        <v>1208</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>583</v>
@@ -9063,10 +9065,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1097</v>
+        <v>1088</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1098</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -9074,10 +9076,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1095</v>
+        <v>1086</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1096</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -9140,10 +9142,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1047</v>
+        <v>1038</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1048</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -9486,25 +9488,25 @@
         <v>654</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>868</v>
+        <v>859</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>869</v>
+        <v>860</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>768</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -9512,7 +9514,7 @@
         <v>670</v>
       </c>
       <c r="B2" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="C2">
         <v>24</v>
@@ -9533,7 +9535,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>1006</v>
+        <v>997</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -9541,7 +9543,7 @@
         <v>670</v>
       </c>
       <c r="B3" t="s">
-        <v>905</v>
+        <v>896</v>
       </c>
       <c r="C3">
         <v>24</v>
@@ -9562,7 +9564,7 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -9570,7 +9572,7 @@
         <v>670</v>
       </c>
       <c r="B4" t="s">
-        <v>1099</v>
+        <v>1090</v>
       </c>
       <c r="C4">
         <v>24</v>
@@ -9591,7 +9593,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -9599,7 +9601,7 @@
         <v>674</v>
       </c>
       <c r="B5" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -9625,7 +9627,7 @@
         <v>685</v>
       </c>
       <c r="B6" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -9651,7 +9653,7 @@
         <v>687</v>
       </c>
       <c r="B7" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -9672,7 +9674,7 @@
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -9680,7 +9682,7 @@
         <v>687</v>
       </c>
       <c r="B8" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -9701,7 +9703,7 @@
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -9709,7 +9711,7 @@
         <v>687</v>
       </c>
       <c r="B9" t="s">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -9730,7 +9732,7 @@
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -9738,7 +9740,7 @@
         <v>691</v>
       </c>
       <c r="B10" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -9759,7 +9761,7 @@
         <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -9767,7 +9769,7 @@
         <v>691</v>
       </c>
       <c r="B11" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -9793,7 +9795,7 @@
         <v>691</v>
       </c>
       <c r="B12" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -9814,7 +9816,7 @@
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -9822,7 +9824,7 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -9843,7 +9845,7 @@
         <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -9851,7 +9853,7 @@
         <v>691</v>
       </c>
       <c r="B14" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -9872,7 +9874,7 @@
         <v>14</v>
       </c>
       <c r="I14" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -9880,7 +9882,7 @@
         <v>691</v>
       </c>
       <c r="B15" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -9901,15 +9903,15 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>1101</v>
+        <v>1092</v>
       </c>
       <c r="B16" t="s">
-        <v>1102</v>
+        <v>1093</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -9930,7 +9932,7 @@
         <v>30</v>
       </c>
       <c r="I16" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -9938,7 +9940,7 @@
         <v>697</v>
       </c>
       <c r="B17" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -9959,7 +9961,7 @@
         <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -9967,7 +9969,7 @@
         <v>699</v>
       </c>
       <c r="B18" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -9988,7 +9990,7 @@
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>1011</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -9996,7 +9998,7 @@
         <v>699</v>
       </c>
       <c r="B19" t="s">
-        <v>919</v>
+        <v>910</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -10017,7 +10019,7 @@
         <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>1032</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -10025,7 +10027,7 @@
         <v>704</v>
       </c>
       <c r="B20" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -10046,7 +10048,7 @@
         <v>14</v>
       </c>
       <c r="I20" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -10054,7 +10056,7 @@
         <v>709</v>
       </c>
       <c r="B21" t="s">
-        <v>921</v>
+        <v>912</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -10075,7 +10077,7 @@
         <v>14</v>
       </c>
       <c r="I21" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -10083,7 +10085,7 @@
         <v>709</v>
       </c>
       <c r="B22" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="C22">
         <v>20</v>
@@ -10109,7 +10111,7 @@
         <v>709</v>
       </c>
       <c r="B23" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="C23">
         <v>12</v>
@@ -10135,7 +10137,7 @@
         <v>711</v>
       </c>
       <c r="B24" t="s">
-        <v>924</v>
+        <v>915</v>
       </c>
       <c r="C24">
         <v>18</v>
@@ -10156,7 +10158,7 @@
         <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -10164,7 +10166,7 @@
         <v>712</v>
       </c>
       <c r="B25" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -10185,7 +10187,7 @@
         <v>14</v>
       </c>
       <c r="I25" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -10193,7 +10195,7 @@
         <v>712</v>
       </c>
       <c r="B26" t="s">
-        <v>926</v>
+        <v>917</v>
       </c>
       <c r="C26">
         <v>15</v>
@@ -10214,7 +10216,7 @@
         <v>14</v>
       </c>
       <c r="I26" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -10222,7 +10224,7 @@
         <v>717</v>
       </c>
       <c r="B27" t="s">
-        <v>927</v>
+        <v>918</v>
       </c>
       <c r="C27">
         <v>30</v>
@@ -10243,7 +10245,7 @@
         <v>14</v>
       </c>
       <c r="I27" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -10251,7 +10253,7 @@
         <v>717</v>
       </c>
       <c r="B28" t="s">
-        <v>928</v>
+        <v>919</v>
       </c>
       <c r="C28">
         <v>30</v>
@@ -10277,7 +10279,7 @@
         <v>721</v>
       </c>
       <c r="B29" t="s">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="C29">
         <v>20</v>
@@ -10298,7 +10300,7 @@
         <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -10306,7 +10308,7 @@
         <v>721</v>
       </c>
       <c r="B30" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -10327,7 +10329,7 @@
         <v>14</v>
       </c>
       <c r="I30" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -10335,7 +10337,7 @@
         <v>721</v>
       </c>
       <c r="B31" t="s">
-        <v>931</v>
+        <v>922</v>
       </c>
       <c r="C31">
         <v>20</v>
@@ -10356,7 +10358,7 @@
         <v>14</v>
       </c>
       <c r="I31" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -10364,7 +10366,7 @@
         <v>725</v>
       </c>
       <c r="B32" t="s">
-        <v>932</v>
+        <v>923</v>
       </c>
       <c r="C32">
         <v>20</v>
@@ -10385,7 +10387,7 @@
         <v>14</v>
       </c>
       <c r="I32" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -10393,7 +10395,7 @@
         <v>728</v>
       </c>
       <c r="B33" t="s">
-        <v>933</v>
+        <v>924</v>
       </c>
       <c r="C33">
         <v>20</v>
@@ -10414,7 +10416,7 @@
         <v>14</v>
       </c>
       <c r="I33" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -10422,7 +10424,7 @@
         <v>743</v>
       </c>
       <c r="B34" t="s">
-        <v>1100</v>
+        <v>1091</v>
       </c>
       <c r="C34">
         <v>30</v>
@@ -10443,7 +10445,7 @@
         <v>14</v>
       </c>
       <c r="I34" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -10451,7 +10453,7 @@
         <v>745</v>
       </c>
       <c r="B35" t="s">
-        <v>934</v>
+        <v>925</v>
       </c>
       <c r="C35">
         <v>20</v>
@@ -10472,7 +10474,7 @@
         <v>14</v>
       </c>
       <c r="I35" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -10480,7 +10482,7 @@
         <v>746</v>
       </c>
       <c r="B36" t="s">
-        <v>935</v>
+        <v>926</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -10501,7 +10503,7 @@
         <v>14</v>
       </c>
       <c r="I36" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
     </row>
   </sheetData>
@@ -11193,7 +11195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -11671,10 +11673,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>957</v>
+        <v>948</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -11682,7 +11684,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>958</v>
+        <v>949</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>650</v>
@@ -11693,7 +11695,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>940</v>
+        <v>931</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>650</v>
@@ -11726,7 +11728,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>648</v>
@@ -11737,7 +11739,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>956</v>
+        <v>947</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>650</v>
@@ -11748,7 +11750,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>953</v>
+        <v>944</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>646</v>
@@ -11759,7 +11761,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>954</v>
+        <v>945</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>650</v>
@@ -11792,10 +11794,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>938</v>
+        <v>929</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -12078,7 +12080,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1218</v>
+        <v>1209</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>234</v>
@@ -12115,16 +12117,16 @@
         <v>654</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>868</v>
+        <v>859</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>869</v>
+        <v>860</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>881</v>
+        <v>872</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>768</v>
@@ -12135,7 +12137,7 @@
         <v>708</v>
       </c>
       <c r="B2" t="s">
-        <v>883</v>
+        <v>874</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -12158,7 +12160,7 @@
         <v>708</v>
       </c>
       <c r="B3" t="s">
-        <v>884</v>
+        <v>875</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -12181,7 +12183,7 @@
         <v>708</v>
       </c>
       <c r="B4" t="s">
-        <v>885</v>
+        <v>876</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -12204,7 +12206,7 @@
         <v>708</v>
       </c>
       <c r="B5" t="s">
-        <v>886</v>
+        <v>877</v>
       </c>
       <c r="C5">
         <v>50</v>
@@ -12227,7 +12229,7 @@
         <v>708</v>
       </c>
       <c r="B6" t="s">
-        <v>887</v>
+        <v>878</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -12250,7 +12252,7 @@
         <v>708</v>
       </c>
       <c r="B7" t="s">
-        <v>888</v>
+        <v>879</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -12273,7 +12275,7 @@
         <v>708</v>
       </c>
       <c r="B8" t="s">
-        <v>889</v>
+        <v>880</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -12296,7 +12298,7 @@
         <v>708</v>
       </c>
       <c r="B9" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -12319,7 +12321,7 @@
         <v>708</v>
       </c>
       <c r="B10" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -12342,7 +12344,7 @@
         <v>708</v>
       </c>
       <c r="B11" t="s">
-        <v>892</v>
+        <v>883</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -12365,7 +12367,7 @@
         <v>708</v>
       </c>
       <c r="B12" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -12388,7 +12390,7 @@
         <v>708</v>
       </c>
       <c r="B13" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -12411,7 +12413,7 @@
         <v>708</v>
       </c>
       <c r="B14" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -12434,7 +12436,7 @@
         <v>708</v>
       </c>
       <c r="B15" t="s">
-        <v>896</v>
+        <v>887</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -12457,7 +12459,7 @@
         <v>708</v>
       </c>
       <c r="B16" t="s">
-        <v>897</v>
+        <v>888</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -12480,7 +12482,7 @@
         <v>708</v>
       </c>
       <c r="B17" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -12503,7 +12505,7 @@
         <v>708</v>
       </c>
       <c r="B18" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
       <c r="C18">
         <v>70</v>
@@ -12548,10 +12550,10 @@
         <v>654</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>868</v>
+        <v>859</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>869</v>
+        <v>860</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>768</v>
@@ -12562,7 +12564,7 @@
         <v>708</v>
       </c>
       <c r="B2" t="s">
-        <v>870</v>
+        <v>861</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -12579,7 +12581,7 @@
         <v>708</v>
       </c>
       <c r="B3" t="s">
-        <v>871</v>
+        <v>862</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -12596,7 +12598,7 @@
         <v>708</v>
       </c>
       <c r="B4" t="s">
-        <v>872</v>
+        <v>863</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -12613,7 +12615,7 @@
         <v>708</v>
       </c>
       <c r="B5" t="s">
-        <v>873</v>
+        <v>864</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -12630,7 +12632,7 @@
         <v>708</v>
       </c>
       <c r="B6" t="s">
-        <v>874</v>
+        <v>865</v>
       </c>
       <c r="C6">
         <v>70</v>
@@ -12647,7 +12649,7 @@
         <v>708</v>
       </c>
       <c r="B7" t="s">
-        <v>875</v>
+        <v>866</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -12664,7 +12666,7 @@
         <v>723</v>
       </c>
       <c r="B8" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="C8">
         <v>70</v>
@@ -12681,7 +12683,7 @@
         <v>723</v>
       </c>
       <c r="B9" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -12698,7 +12700,7 @@
         <v>723</v>
       </c>
       <c r="B10" t="s">
-        <v>1103</v>
+        <v>1094</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -12715,7 +12717,7 @@
         <v>725</v>
       </c>
       <c r="B11" t="s">
-        <v>876</v>
+        <v>867</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -12732,7 +12734,7 @@
         <v>725</v>
       </c>
       <c r="B12" t="s">
-        <v>877</v>
+        <v>868</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -12749,7 +12751,7 @@
         <v>725</v>
       </c>
       <c r="B13" t="s">
-        <v>878</v>
+        <v>869</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -12791,12 +12793,12 @@
         <v>768</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -12807,7 +12809,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>861</v>
+        <v>852</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -12818,7 +12820,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>862</v>
+        <v>853</v>
       </c>
       <c r="B4">
         <v>250</v>
@@ -12829,7 +12831,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>863</v>
+        <v>854</v>
       </c>
       <c r="B5">
         <v>500</v>
@@ -12840,7 +12842,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>864</v>
+        <v>855</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -12851,7 +12853,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>865</v>
+        <v>856</v>
       </c>
       <c r="B7">
         <v>10000</v>
@@ -12888,16 +12890,16 @@
         <v>654</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>767</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>768</v>
@@ -12908,19 +12910,19 @@
         <v>668</v>
       </c>
       <c r="B2" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="C2" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D2" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="E2" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="F2" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G2">
         <v>50</v>
@@ -12931,19 +12933,19 @@
         <v>732</v>
       </c>
       <c r="B3" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="C3" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D3" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="E3" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="F3" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G3">
         <v>150</v>
@@ -12954,19 +12956,19 @@
         <v>758</v>
       </c>
       <c r="B4" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
       <c r="C4" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D4" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E4" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="F4" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G4">
         <v>250</v>
@@ -12977,19 +12979,19 @@
         <v>679</v>
       </c>
       <c r="B5" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="C5" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D5" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E5" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="F5" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G5">
         <v>25</v>
@@ -13000,19 +13002,19 @@
         <v>739</v>
       </c>
       <c r="B6" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="C6" t="s">
+        <v>823</v>
+      </c>
+      <c r="D6" t="s">
+        <v>789</v>
+      </c>
+      <c r="E6" t="s">
         <v>832</v>
       </c>
-      <c r="D6" t="s">
-        <v>798</v>
-      </c>
-      <c r="E6" t="s">
-        <v>841</v>
-      </c>
       <c r="F6" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G6">
         <v>75</v>
@@ -13023,19 +13025,19 @@
         <v>755</v>
       </c>
       <c r="B7" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
       <c r="C7" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D7" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="E7" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="F7" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G7">
         <v>275</v>
@@ -13046,19 +13048,19 @@
         <v>673</v>
       </c>
       <c r="B8" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="C8" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D8" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="E8" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="F8" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G8">
         <v>10</v>
@@ -13069,19 +13071,19 @@
         <v>707</v>
       </c>
       <c r="B9" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="C9" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D9" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="E9" t="s">
-        <v>845</v>
+        <v>836</v>
       </c>
       <c r="F9" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G9">
         <v>300</v>
@@ -13092,19 +13094,19 @@
         <v>755</v>
       </c>
       <c r="B10" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="C10" t="s">
+        <v>829</v>
+      </c>
+      <c r="D10" t="s">
+        <v>792</v>
+      </c>
+      <c r="E10" t="s">
         <v>838</v>
       </c>
-      <c r="D10" t="s">
-        <v>801</v>
-      </c>
-      <c r="E10" t="s">
-        <v>847</v>
-      </c>
       <c r="F10" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G10">
         <v>275</v>
@@ -13115,19 +13117,19 @@
         <v>755</v>
       </c>
       <c r="B11" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
       <c r="C11" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="D11" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="E11" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="F11" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G11">
         <v>275</v>
@@ -13138,19 +13140,19 @@
         <v>760</v>
       </c>
       <c r="B12" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="C12" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="D12" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E12" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="F12" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -13158,19 +13160,19 @@
         <v>730</v>
       </c>
       <c r="B13" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
       <c r="C13" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D13" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E13" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="F13" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -13178,19 +13180,19 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="C14" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D14" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E14" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="F14" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G14">
         <v>75</v>
@@ -13201,19 +13203,19 @@
         <v>707</v>
       </c>
       <c r="B15" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="C15" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D15" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="E15" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="F15" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G15">
         <v>275</v>
@@ -13224,19 +13226,19 @@
         <v>753</v>
       </c>
       <c r="B16" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
       <c r="C16" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="D16" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="E16" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="F16" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G16">
         <v>75</v>
@@ -13247,19 +13249,19 @@
         <v>755</v>
       </c>
       <c r="B17" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="C17" t="s">
+        <v>823</v>
+      </c>
+      <c r="D17" t="s">
+        <v>789</v>
+      </c>
+      <c r="E17" t="s">
         <v>832</v>
       </c>
-      <c r="D17" t="s">
-        <v>798</v>
-      </c>
-      <c r="E17" t="s">
-        <v>841</v>
-      </c>
       <c r="F17" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G17">
         <v>275</v>
@@ -13270,19 +13272,19 @@
         <v>700</v>
       </c>
       <c r="B18" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="C18" t="s">
+        <v>823</v>
+      </c>
+      <c r="D18" t="s">
+        <v>789</v>
+      </c>
+      <c r="E18" t="s">
         <v>832</v>
       </c>
-      <c r="D18" t="s">
-        <v>798</v>
-      </c>
-      <c r="E18" t="s">
-        <v>841</v>
-      </c>
       <c r="F18" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
     </row>
   </sheetData>
@@ -13319,7 +13321,7 @@
         <v>654</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>765</v>
@@ -13336,7 +13338,7 @@
         <v>719</v>
       </c>
       <c r="B2" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="C2" s="12">
         <v>100</v>
@@ -13345,7 +13347,7 @@
         <v>3.7</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="F2" s="12">
         <v>275</v>
@@ -13356,7 +13358,7 @@
         <v>748</v>
       </c>
       <c r="B3" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="C3" s="12">
         <v>25</v>
@@ -13376,7 +13378,7 @@
         <v>676</v>
       </c>
       <c r="B4" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="C4" s="12">
         <v>70</v>
@@ -13396,7 +13398,7 @@
         <v>673</v>
       </c>
       <c r="B5" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="C5" s="12">
         <v>50</v>
@@ -13405,7 +13407,7 @@
         <v>3.7</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="F5" s="12">
         <v>150</v>
@@ -13416,7 +13418,7 @@
         <v>689</v>
       </c>
       <c r="B6" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="C6" s="12">
         <v>80</v>
@@ -13436,7 +13438,7 @@
         <v>751</v>
       </c>
       <c r="B7" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="C7" s="12">
         <v>95</v>
@@ -13445,7 +13447,7 @@
         <v>3.7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="F7" s="12">
         <v>150</v>
@@ -13456,7 +13458,7 @@
         <v>677</v>
       </c>
       <c r="B8" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
       <c r="C8" s="12">
         <v>60</v>
@@ -13465,7 +13467,7 @@
         <v>3.7</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="F8" s="12">
         <v>125</v>
@@ -13498,7 +13500,7 @@
         <v>654</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>768</v>
@@ -13509,10 +13511,10 @@
         <v>738</v>
       </c>
       <c r="B2" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="C2" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -13523,10 +13525,10 @@
         <v>740</v>
       </c>
       <c r="B3" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="C3" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -13537,10 +13539,10 @@
         <v>684</v>
       </c>
       <c r="B4" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="C4" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -13551,10 +13553,10 @@
         <v>754</v>
       </c>
       <c r="B5" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="C5" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -13568,7 +13570,7 @@
         <v>680</v>
       </c>
       <c r="C6" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -13579,7 +13581,7 @@
         <v>684</v>
       </c>
       <c r="B7" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -13593,7 +13595,7 @@
         <v>681</v>
       </c>
       <c r="C8" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -13604,10 +13606,10 @@
         <v>744</v>
       </c>
       <c r="B9" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="C9" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
       <c r="D9">
         <v>75</v>
@@ -13618,7 +13620,7 @@
         <v>702</v>
       </c>
       <c r="B10" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -13629,7 +13631,7 @@
         <v>752</v>
       </c>
       <c r="B11" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -13640,10 +13642,10 @@
         <v>716</v>
       </c>
       <c r="B12" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="C12" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -13654,10 +13656,10 @@
         <v>716</v>
       </c>
       <c r="B13" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="C13" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D13">
         <v>75</v>
@@ -13668,7 +13670,7 @@
         <v>700</v>
       </c>
       <c r="B14" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="D14">
         <v>50</v>
@@ -13681,10 +13683,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13706,329 +13708,329 @@
     </row>
     <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B3" t="s">
         <v>783</v>
       </c>
-      <c r="B3" t="s">
-        <v>782</v>
-      </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B4" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B5" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B6" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>787</v>
+      <c r="A7" s="7">
+        <v>18350</v>
       </c>
       <c r="B7" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>18650</v>
+      </c>
+      <c r="B8" t="s">
+        <v>788</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>20700</v>
+      </c>
+      <c r="B9" t="s">
+        <v>788</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>21700</v>
+      </c>
+      <c r="B10" t="s">
+        <v>788</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>26650</v>
+      </c>
+      <c r="B11" t="s">
+        <v>788</v>
+      </c>
+      <c r="C11">
         <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="B8" t="s">
-        <v>782</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>789</v>
-      </c>
-      <c r="B9" t="s">
-        <v>782</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>790</v>
-      </c>
-      <c r="B10" t="s">
-        <v>782</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B11" t="s">
-        <v>792</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="B12" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B13" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B14" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>796</v>
+        <v>991</v>
       </c>
       <c r="B15" t="s">
-        <v>792</v>
+        <v>992</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>18350</v>
+      <c r="A16" s="7" t="s">
+        <v>993</v>
       </c>
       <c r="B16" t="s">
-        <v>797</v>
+        <v>992</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>18650</v>
+      <c r="A17" s="7" t="s">
+        <v>994</v>
       </c>
       <c r="B17" t="s">
-        <v>797</v>
+        <v>992</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>20700</v>
+      <c r="A18" s="7" t="s">
+        <v>995</v>
       </c>
       <c r="B18" t="s">
-        <v>797</v>
+        <v>992</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>21700</v>
+      <c r="A19" s="7" t="s">
+        <v>996</v>
       </c>
       <c r="B19" t="s">
-        <v>797</v>
+        <v>992</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>26650</v>
+      <c r="A20" s="7" t="s">
+        <v>997</v>
       </c>
       <c r="B20" t="s">
-        <v>797</v>
+        <v>992</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>798</v>
+        <v>998</v>
       </c>
       <c r="B21" t="s">
-        <v>799</v>
+        <v>992</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="B22" t="s">
-        <v>799</v>
+        <v>992</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>801</v>
+        <v>1001</v>
       </c>
       <c r="B23" t="s">
-        <v>799</v>
+        <v>992</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="B24" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="B25" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="C25">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>1003</v>
+        <v>1210</v>
       </c>
       <c r="B26" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>1004</v>
+        <v>1211</v>
       </c>
       <c r="B27" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>1005</v>
+        <v>1212</v>
       </c>
       <c r="B28" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>1006</v>
+        <v>1213</v>
       </c>
       <c r="B29" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>1007</v>
+        <v>1214</v>
       </c>
       <c r="B30" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C30">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>1009</v>
+        <v>1215</v>
       </c>
       <c r="B31" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -14036,35 +14038,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>1010</v>
+        <v>1216</v>
       </c>
       <c r="B32" t="s">
-        <v>1001</v>
+        <v>781</v>
       </c>
       <c r="C32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>1013</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial fiber import works
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DF9D87-13A6-EF43-B655-2D1F653D69FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF103AE-6A8E-C447-B975-7289EF5782A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
     <sheet name="aromas" sheetId="23" r:id="rId2"/>
     <sheet name="boosters" sheetId="22" r:id="rId3"/>
     <sheet name="bases" sheetId="21" r:id="rId4"/>
-    <sheet name="vouchers" sheetId="20" r:id="rId5"/>
-    <sheet name="atomizers" sheetId="19" r:id="rId6"/>
-    <sheet name="mods" sheetId="18" r:id="rId7"/>
-    <sheet name="cottons" sheetId="17" r:id="rId8"/>
-    <sheet name="tags" sheetId="16" r:id="rId9"/>
-    <sheet name="cells" sheetId="15" r:id="rId10"/>
-    <sheet name="vendors" sheetId="14" r:id="rId11"/>
-    <sheet name="prices" sheetId="13" r:id="rId12"/>
-    <sheet name="tariffs" sheetId="12" r:id="rId13"/>
-    <sheet name="translations" sheetId="3" r:id="rId14"/>
-    <sheet name="Translations - Common" sheetId="4" r:id="rId15"/>
-    <sheet name="Translations - Errors" sheetId="6" r:id="rId16"/>
-    <sheet name="Translations - Public" sheetId="8" r:id="rId17"/>
-    <sheet name="Translations - Lab" sheetId="7" r:id="rId18"/>
-    <sheet name="Translations - Root" sheetId="9" r:id="rId19"/>
-    <sheet name="Translations - Shared" sheetId="10" r:id="rId20"/>
-    <sheet name="Translations - Market" sheetId="11" r:id="rId21"/>
+    <sheet name="fibers" sheetId="24" r:id="rId5"/>
+    <sheet name="vouchers" sheetId="20" r:id="rId6"/>
+    <sheet name="atomizers" sheetId="19" r:id="rId7"/>
+    <sheet name="mods" sheetId="18" r:id="rId8"/>
+    <sheet name="cottons" sheetId="17" r:id="rId9"/>
+    <sheet name="tags" sheetId="16" r:id="rId10"/>
+    <sheet name="cells" sheetId="15" r:id="rId11"/>
+    <sheet name="vendors" sheetId="14" r:id="rId12"/>
+    <sheet name="prices" sheetId="13" r:id="rId13"/>
+    <sheet name="tariffs" sheetId="12" r:id="rId14"/>
+    <sheet name="translations" sheetId="3" r:id="rId15"/>
+    <sheet name="Translations - Common" sheetId="4" r:id="rId16"/>
+    <sheet name="Translations - Errors" sheetId="6" r:id="rId17"/>
+    <sheet name="Translations - Public" sheetId="8" r:id="rId18"/>
+    <sheet name="Translations - Lab" sheetId="7" r:id="rId19"/>
+    <sheet name="Translations - Root" sheetId="9" r:id="rId20"/>
+    <sheet name="Translations - Shared" sheetId="10" r:id="rId21"/>
+    <sheet name="Translations - Market" sheetId="11" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="1223">
   <si>
     <t>cs</t>
   </si>
@@ -3737,6 +3738,21 @@
   </si>
   <si>
     <t>common.vendor.generic</t>
+  </si>
+  <si>
+    <t>ga</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>fibers</t>
+  </si>
+  <si>
+    <t>fiber</t>
   </si>
 </sst>
 </file>
@@ -4142,10 +4158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4314,12 +4330,391 @@
         <v>892</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B2" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B3" t="s">
+        <v>783</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="B4" t="s">
+        <v>783</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B5" t="s">
+        <v>783</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="B6" t="s">
+        <v>783</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>18350</v>
+      </c>
+      <c r="B7" t="s">
+        <v>788</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>18650</v>
+      </c>
+      <c r="B8" t="s">
+        <v>788</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>20700</v>
+      </c>
+      <c r="B9" t="s">
+        <v>788</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>21700</v>
+      </c>
+      <c r="B10" t="s">
+        <v>788</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>26650</v>
+      </c>
+      <c r="B11" t="s">
+        <v>788</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="B12" t="s">
+        <v>790</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="B13" t="s">
+        <v>790</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B14" t="s">
+        <v>790</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="B15" t="s">
+        <v>992</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="B16" t="s">
+        <v>992</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="B17" t="s">
+        <v>992</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="B18" t="s">
+        <v>992</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="B19" t="s">
+        <v>992</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="B20" t="s">
+        <v>992</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="B21" t="s">
+        <v>992</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>992</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B23" t="s">
+        <v>992</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B24" t="s">
+        <v>992</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B25" t="s">
+        <v>992</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B26" t="s">
+        <v>781</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>781</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>781</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B29" t="s">
+        <v>781</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B30" t="s">
+        <v>781</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B31" t="s">
+        <v>781</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B32" t="s">
+        <v>781</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243831E-E3E3-1C43-AE4D-34D8FEF2F724}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -4461,11 +4856,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
@@ -4985,7 +5380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1AB5C-3BBA-9E49-B566-51FB3B75CDAA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -5058,7 +5453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1822C792-D890-E542-B44B-A4E33F805828}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5106,7 +5501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C36761-E560-4615-98DB-D2A406A4AE09}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5157,7 +5552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <dimension ref="A1:C111"/>
   <sheetViews>
@@ -6402,7 +6797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF25BB5F-E340-4075-9636-DA5C9C989624}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -6444,7 +6839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC49E62-0AEE-40E6-B00F-514263105890}">
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C24"/>
@@ -6733,7 +7128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C145"/>
   <sheetViews>
@@ -8346,1119 +8741,6 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C142">
     <sortCondition ref="B139:B142"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C99"/>
-  <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="69.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>1038</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C99">
-    <sortCondition ref="B96:B99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10520,6 +9802,1119 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
+  <dimension ref="A1:C99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="62.5" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C99">
+    <sortCondition ref="B96:B99"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FAEBF3-753C-4AE9-A2FF-818B5E33C44A}">
   <dimension ref="A1:C59"/>
   <sheetViews>
@@ -11191,7 +11586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
   <dimension ref="A1:C80"/>
   <sheetViews>
@@ -12772,6 +13167,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF980A1E-67C8-2046-AD3D-9A8AA002E628}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -12867,7 +13300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -13298,7 +13731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D757F10-66C2-2941-A49E-7F0FD3F6574C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -13478,7 +13911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F5805-0158-F34C-9256-85EB751C6431}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -13679,375 +14112,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
-  <dimension ref="A1:C32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>656</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>779</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>782</v>
-      </c>
-      <c r="B2" t="s">
-        <v>783</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>784</v>
-      </c>
-      <c r="B3" t="s">
-        <v>783</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>785</v>
-      </c>
-      <c r="B4" t="s">
-        <v>783</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>786</v>
-      </c>
-      <c r="B5" t="s">
-        <v>783</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>787</v>
-      </c>
-      <c r="B6" t="s">
-        <v>783</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>18350</v>
-      </c>
-      <c r="B7" t="s">
-        <v>788</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>18650</v>
-      </c>
-      <c r="B8" t="s">
-        <v>788</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>20700</v>
-      </c>
-      <c r="B9" t="s">
-        <v>788</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>21700</v>
-      </c>
-      <c r="B10" t="s">
-        <v>788</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>26650</v>
-      </c>
-      <c r="B11" t="s">
-        <v>788</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>789</v>
-      </c>
-      <c r="B12" t="s">
-        <v>790</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B13" t="s">
-        <v>790</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>792</v>
-      </c>
-      <c r="B14" t="s">
-        <v>790</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>991</v>
-      </c>
-      <c r="B15" t="s">
-        <v>992</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>993</v>
-      </c>
-      <c r="B16" t="s">
-        <v>992</v>
-      </c>
-      <c r="C16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>994</v>
-      </c>
-      <c r="B17" t="s">
-        <v>992</v>
-      </c>
-      <c r="C17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>995</v>
-      </c>
-      <c r="B18" t="s">
-        <v>992</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>996</v>
-      </c>
-      <c r="B19" t="s">
-        <v>992</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>997</v>
-      </c>
-      <c r="B20" t="s">
-        <v>992</v>
-      </c>
-      <c r="C20">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>998</v>
-      </c>
-      <c r="B21" t="s">
-        <v>992</v>
-      </c>
-      <c r="C21">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B22" t="s">
-        <v>992</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B23" t="s">
-        <v>992</v>
-      </c>
-      <c r="C23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B24" t="s">
-        <v>992</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B25" t="s">
-        <v>992</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B26" t="s">
-        <v>781</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>1211</v>
-      </c>
-      <c r="B27" t="s">
-        <v>781</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>1212</v>
-      </c>
-      <c r="B28" t="s">
-        <v>781</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>1213</v>
-      </c>
-      <c r="B29" t="s">
-        <v>781</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B30" t="s">
-        <v>781</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B31" t="s">
-        <v>781</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B32" t="s">
-        <v>781</v>
-      </c>
-      <c r="C32">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Simplified Fiber; ohms cannot be simply harvested
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF103AE-6A8E-C447-B975-7289EF5782A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2E3D3D-DE5B-AC45-9F1B-C6108B9B08F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="1243">
   <si>
     <t>cs</t>
   </si>
@@ -3746,20 +3746,80 @@
     <t>mm</t>
   </si>
   <si>
-    <t>ohm</t>
-  </si>
-  <si>
     <t>fibers</t>
   </si>
   <si>
     <t>fiber</t>
+  </si>
+  <si>
+    <t>0.405</t>
+  </si>
+  <si>
+    <t>0.361</t>
+  </si>
+  <si>
+    <t>0.321</t>
+  </si>
+  <si>
+    <t>0.286</t>
+  </si>
+  <si>
+    <t>0.255</t>
+  </si>
+  <si>
+    <t>0.227</t>
+  </si>
+  <si>
+    <t>0.202</t>
+  </si>
+  <si>
+    <t>0.180</t>
+  </si>
+  <si>
+    <t>0.160</t>
+  </si>
+  <si>
+    <t>0.143</t>
+  </si>
+  <si>
+    <t>0.127</t>
+  </si>
+  <si>
+    <t>0.113</t>
+  </si>
+  <si>
+    <t>0.101</t>
+  </si>
+  <si>
+    <t>0.0897</t>
+  </si>
+  <si>
+    <t>0.0799</t>
+  </si>
+  <si>
+    <t>0.812</t>
+  </si>
+  <si>
+    <t>0.723</t>
+  </si>
+  <si>
+    <t>0.644</t>
+  </si>
+  <si>
+    <t>0.573</t>
+  </si>
+  <si>
+    <t>0.511</t>
+  </si>
+  <si>
+    <t>0.455</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3805,6 +3865,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4332,10 +4398,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B21" t="s">
         <v>1221</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1222</v>
       </c>
     </row>
   </sheetData>
@@ -4347,8 +4413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13168,20 +13234,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1218</v>
       </c>
@@ -13189,17 +13254,1673 @@
         <v>1219</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1220</v>
+        <v>781</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>39</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>40</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>20</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>21</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>22</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>24</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>26</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>27</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>28</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>29</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>30</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>31</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>32</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>33</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>34</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>35</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>36</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>37</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>39</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>40</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>20</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>21</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>22</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>23</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>24</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>25</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>26</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>27</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>28</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>29</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>30</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>31</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>32</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>33</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>34</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>35</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>36</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>37</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>38</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>39</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>40</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>20</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>21</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>22</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>23</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>24</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>25</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>26</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>27</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>28</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>29</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>30</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>31</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>32</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>33</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>34</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>35</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>36</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>37</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>38</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>39</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>40</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>20</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>21</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>22</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>23</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>24</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>25</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>26</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>27</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>28</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>29</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>30</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>31</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>32</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>33</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>34</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>35</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>36</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>37</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>38</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>39</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>40</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>20</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>21</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>22</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>23</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>24</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>25</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>26</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>27</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>28</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>29</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>30</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>31</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>32</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>33</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>34</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>35</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>36</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>37</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>38</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>39</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>40</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Common: Added some boilerplate for wires
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E113CD16-DC13-448B-84C5-D369448541C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA8E4C3-A7E0-413A-8480-6DE0CBFBD8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15495" yWindow="2865" windowWidth="33795" windowHeight="18495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="1256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="1265">
   <si>
     <t>cs</t>
   </si>
@@ -3723,9 +3723,6 @@
     <t>SS316L</t>
   </si>
   <si>
-    <t>Kanthal</t>
-  </si>
-  <si>
     <t>Ni80</t>
   </si>
   <si>
@@ -3853,6 +3850,36 @@
   </si>
   <si>
     <t>[{count: 2, fiber: Ni80 32GA},{count: 1, fiber: Ni80 38GA}]</t>
+  </si>
+  <si>
+    <t>Stifs Coils</t>
+  </si>
+  <si>
+    <t>Kanthal A1</t>
+  </si>
+  <si>
+    <t>[{count: 1, fiber: Kanthal A1 26GA}]</t>
+  </si>
+  <si>
+    <t>[{count: 1, fiber: Kanthal A1 32GA}]</t>
+  </si>
+  <si>
+    <t>[{count: 1, fiber: Kanthal A1 30GA}]</t>
+  </si>
+  <si>
+    <t>[{count: 1, fiber: Kanthal A1 24GA}]</t>
+  </si>
+  <si>
+    <t>Flat Clapton Kanthal A1 26ga*18ga+32ga</t>
+  </si>
+  <si>
+    <t>[{count: 1, fiber: Kanthal A1 26GA},{count: 1, fiber: Kanthal A1 18GA},{count: 1, fiber: Kanthal A1 32GA}]</t>
+  </si>
+  <si>
+    <t>1.024</t>
+  </si>
+  <si>
+    <t>0.912</t>
   </si>
 </sst>
 </file>
@@ -4438,18 +4465,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B21" t="s">
         <v>1220</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1221</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B22" t="s">
         <v>1243</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1244</v>
       </c>
     </row>
   </sheetData>
@@ -4665,7 +4692,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4973,7 +5000,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
       <c r="B28" t="s">
         <v>781</v>
@@ -4984,7 +5011,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B29" t="s">
         <v>781</v>
@@ -4995,7 +5022,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B30" t="s">
         <v>781</v>
@@ -5006,7 +5033,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B31" t="s">
         <v>781</v>
@@ -5017,7 +5044,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B32" t="s">
         <v>781</v>
@@ -5175,10 +5202,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5283,415 +5310,420 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>684</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
         <v>1092</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>738</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>1217</v>
+        <v>761</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>762</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A99">
-    <sortCondition ref="A95:A99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A101">
+    <sortCondition ref="A95:A101"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A60" r:id="rId1" display="https://www.eliquidshop.cz/my-vape/" xr:uid="{6FAF1889-3DC2-2045-966A-88495D335037}"/>
+    <hyperlink ref="A61" r:id="rId1" display="https://www.eliquidshop.cz/my-vape/" xr:uid="{6FAF1889-3DC2-2045-966A-88495D335037}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7447,10 +7479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F7C88A-203F-48DC-ACBE-CE6221C44C48}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7458,13 +7490,14 @@
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="72.28515625" customWidth="1"/>
+    <col min="4" max="4" width="126.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>665</v>
       </c>
@@ -7475,157 +7508,284 @@
         <v>927</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1245</v>
-      </c>
-      <c r="F1" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1246</v>
-      </c>
+        <v>747</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>784</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1254</v>
+        <v>1257</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2">
+        <v>15</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>784</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1247</v>
+        <v>1258</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3">
+        <v>15</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>784</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1248</v>
+        <v>1259</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4">
+        <v>15</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>784</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1249</v>
+        <v>1260</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5">
+        <v>15</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>751</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1245</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>1250</v>
+        <v>784</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>823</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>1250</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1252</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7">
+        <v>15</v>
+      </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>1250</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>823</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>751</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>1261</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>784</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>1255</v>
+        <v>1262</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9">
+        <v>15</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
+    <sortCondition ref="A5:A14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11941,10 +12101,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11955,10 +12115,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1218</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1219</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>781</v>
@@ -11969,10 +12129,10 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1237</v>
+        <v>1263</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1211</v>
@@ -11981,10 +12141,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1238</v>
+        <v>1264</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1211</v>
@@ -11993,10 +12153,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1211</v>
@@ -12005,10 +12165,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1211</v>
@@ -12017,10 +12177,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1211</v>
@@ -12029,10 +12189,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1211</v>
@@ -12041,10 +12201,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1222</v>
+        <v>1240</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1211</v>
@@ -12053,10 +12213,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1223</v>
+        <v>1241</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1211</v>
@@ -12065,10 +12225,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1211</v>
@@ -12077,10 +12237,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1211</v>
@@ -12089,10 +12249,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1211</v>
@@ -12101,10 +12261,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1211</v>
@@ -12113,10 +12273,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1211</v>
@@ -12125,10 +12285,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1211</v>
@@ -12137,10 +12297,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1211</v>
@@ -12149,10 +12309,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1211</v>
@@ -12161,10 +12321,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1211</v>
@@ -12173,10 +12333,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1211</v>
@@ -12185,10 +12345,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1211</v>
@@ -12197,10 +12357,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1211</v>
@@ -12209,10 +12369,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1211</v>
@@ -12221,482 +12381,488 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1239</v>
+        <v>1263</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1240</v>
+        <v>1264</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1242</v>
+        <v>1237</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1222</v>
+        <v>1238</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1223</v>
+        <v>1239</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1224</v>
+        <v>1240</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1225</v>
+        <v>1241</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1226</v>
+        <v>1221</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1227</v>
+        <v>1222</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1228</v>
+        <v>1223</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1232</v>
+        <v>1227</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1233</v>
+        <v>1228</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1234</v>
+        <v>1229</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1235</v>
+        <v>1230</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1237</v>
+        <v>1232</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1210</v>
-      </c>
+        <v>1212</v>
+      </c>
+      <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1238</v>
+        <v>1233</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1210</v>
-      </c>
+        <v>1212</v>
+      </c>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1239</v>
+        <v>1234</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1210</v>
-      </c>
+        <v>1212</v>
+      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1240</v>
+        <v>1235</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1210</v>
-      </c>
+        <v>1212</v>
+      </c>
+      <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1241</v>
+        <v>1263</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1242</v>
+        <v>1264</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1222</v>
+        <v>1236</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1223</v>
+        <v>1237</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1224</v>
+        <v>1238</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1225</v>
+        <v>1239</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1226</v>
+        <v>1240</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1227</v>
+        <v>1241</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1228</v>
+        <v>1221</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1230</v>
+        <v>1223</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1231</v>
+        <v>1224</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1232</v>
+        <v>1225</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1233</v>
+        <v>1226</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1234</v>
+        <v>1227</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1235</v>
+        <v>1228</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1236</v>
+        <v>1229</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>1210</v>
@@ -12704,926 +12870,1080 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1237</v>
+        <v>1230</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1238</v>
+        <v>1231</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1239</v>
+        <v>1232</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1240</v>
+        <v>1233</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1241</v>
+        <v>1234</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1242</v>
+        <v>1235</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1222</v>
+        <v>1263</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1223</v>
+        <v>1264</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1224</v>
+        <v>1236</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1225</v>
+        <v>1237</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1226</v>
+        <v>1238</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1227</v>
+        <v>1239</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1228</v>
+        <v>1240</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1229</v>
+        <v>1241</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1230</v>
+        <v>1221</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1233</v>
+        <v>1224</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1234</v>
+        <v>1225</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1235</v>
+        <v>1226</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1236</v>
+        <v>1227</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1237</v>
+        <v>1228</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1238</v>
+        <v>1229</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1239</v>
+        <v>1230</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1240</v>
+        <v>1231</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1241</v>
+        <v>1232</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>1242</v>
+        <v>1233</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1222</v>
+        <v>1234</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1223</v>
+        <v>1235</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1224</v>
+        <v>1263</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1225</v>
+        <v>1264</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1226</v>
+        <v>1236</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1227</v>
+        <v>1237</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1228</v>
+        <v>1238</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1229</v>
+        <v>1239</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>1231</v>
+        <v>1241</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1232</v>
+        <v>1221</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1233</v>
+        <v>1222</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1234</v>
+        <v>1223</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1235</v>
+        <v>1224</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1236</v>
+        <v>1225</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1237</v>
+        <v>1226</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1238</v>
+        <v>1227</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>1239</v>
+        <v>1228</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1240</v>
+        <v>1229</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>1241</v>
+        <v>1230</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1242</v>
+        <v>1231</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1222</v>
+        <v>1232</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>1223</v>
+        <v>1233</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>1224</v>
+        <v>1234</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1225</v>
+        <v>1235</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>1226</v>
+        <v>1263</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1227</v>
+        <v>1264</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>1228</v>
+        <v>1236</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1229</v>
+        <v>1237</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1230</v>
+        <v>1238</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1231</v>
+        <v>1239</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1232</v>
+        <v>1240</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1233</v>
+        <v>1241</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1234</v>
+        <v>1221</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1235</v>
+        <v>1222</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1236</v>
+        <v>1223</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1212</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1237</v>
+        <v>1224</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1238</v>
+        <v>1225</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1239</v>
+        <v>1226</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1240</v>
+        <v>1227</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1241</v>
+        <v>1228</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1242</v>
+        <v>1229</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1222</v>
+        <v>1230</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1223</v>
+        <v>1231</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1224</v>
+        <v>1232</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1225</v>
+        <v>1233</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1226</v>
+        <v>1234</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1227</v>
+        <v>1235</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1214</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1228</v>
+        <v>1263</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1229</v>
+        <v>1264</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1231</v>
+        <v>1237</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>1232</v>
+        <v>1238</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1233</v>
+        <v>1239</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>1234</v>
+        <v>1240</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1235</v>
+        <v>1241</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
+        <v>26</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>27</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>28</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>29</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>30</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>31</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>32</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>33</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>34</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>35</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>36</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>37</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>38</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>39</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
         <v>40</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>1214</v>
+      <c r="B162" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>1213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added initial wire section to market
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA8E4C3-A7E0-413A-8480-6DE0CBFBD8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A725B9D-B0AA-4B71-A087-27AA26E6E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1289">
   <si>
     <t>cs</t>
   </si>
@@ -3880,6 +3880,79 @@
   </si>
   <si>
     <t>0.912</t>
+  </si>
+  <si>
+    <t>market.build.menu</t>
+  </si>
+  <si>
+    <t>market.wire.menu</t>
+  </si>
+  <si>
+    <t>Odporové dráty</t>
+  </si>
+  <si>
+    <t>market.wire.index.title</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat drát</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce drátu</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>Vhodný pro (veškeré)</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>Vhodný pro (některé)</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Drát musí být vhodný pro veškeré vybrané druhy potahů.</t>
+  </si>
+  <si>
+    <t>Drát musí být vhodný pro některý vybraný druh potahu.</t>
+  </si>
+  <si>
+    <t>common.filter.Wires.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>market.wire.buy.confirm.title</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete zakoupit vybraný drát?</t>
+  </si>
+  <si>
+    <t>market.wire.buy.confirm.content</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete zakoupit vybraný drát?&lt;br/&gt;
+Bude vás stát &lt;strong&gt;{{cost}} puffíků&lt;/strong&gt;.</t>
+  </si>
+  <si>
+    <t>market.wire.buy.confirm.button</t>
+  </si>
+  <si>
+    <t>Pořídít</t>
+  </si>
+  <si>
+    <t>market.wire.buy.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste si pořídili drát [{{data.wire.vendor.name}} {{data.wire.name}}].</t>
   </si>
 </sst>
 </file>
@@ -5903,10 +5976,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7135,6 +7208,72 @@
       </c>
       <c r="C111" s="1" t="s">
         <v>1205</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>1279</v>
       </c>
     </row>
   </sheetData>
@@ -7481,7 +7620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F7C88A-203F-48DC-ACBE-CE6221C44C48}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -11197,10 +11336,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11545,32 +11684,32 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -11578,10 +11717,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -11589,10 +11728,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>387</v>
+        <v>431</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>237</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -11600,7 +11739,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>237</v>
@@ -11611,32 +11750,32 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    <row r="39" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -11644,10 +11783,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -11655,10 +11794,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>386</v>
+        <v>447</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>238</v>
+        <v>448</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -11666,7 +11805,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>238</v>
@@ -11677,10 +11816,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>948</v>
+        <v>382</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>930</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -11688,10 +11827,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>650</v>
+        <v>930</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -11699,7 +11838,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>931</v>
+        <v>949</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>650</v>
@@ -11710,10 +11849,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>647</v>
+        <v>931</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -11721,10 +11860,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -11732,10 +11871,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>946</v>
+        <v>651</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -11743,10 +11882,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -11754,10 +11893,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -11765,10 +11904,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -11776,10 +11915,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>645</v>
+        <v>945</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -11787,10 +11926,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -11798,10 +11937,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>929</v>
+        <v>649</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>930</v>
+        <v>650</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -11809,10 +11948,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>377</v>
+        <v>929</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>4</v>
+        <v>930</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -11820,10 +11959,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>376</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -11831,10 +11970,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>341</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -11842,7 +11981,7 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>341</v>
@@ -11853,10 +11992,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -11864,21 +12003,21 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>436</v>
+        <v>378</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>435</v>
+        <v>1209</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>444</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -11886,21 +12025,21 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -11908,10 +12047,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>385</v>
+        <v>433</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>236</v>
+        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -11919,10 +12058,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>381</v>
+        <v>437</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>236</v>
+        <v>438</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -11930,21 +12069,21 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>454</v>
+        <v>385</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>453</v>
+        <v>381</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>452</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -11952,21 +12091,21 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -11974,10 +12113,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -11985,10 +12124,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -11996,10 +12135,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -12007,10 +12146,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>449</v>
+        <v>474</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -12018,10 +12157,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -12029,10 +12168,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -12040,21 +12179,21 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>461</v>
+        <v>1285</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>464</v>
+        <v>1283</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>465</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -12062,10 +12201,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>468</v>
+        <v>1281</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>469</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -12073,10 +12212,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>462</v>
+        <v>1287</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>463</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -12084,15 +12223,92 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1209</v>
+        <v>1268</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>234</v>
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C79">
-    <sortCondition ref="B73:B79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C87">
+    <sortCondition ref="B82:B87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: A bit improved market menu
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A725B9D-B0AA-4B71-A087-27AA26E6E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29FD9D6-C9B4-43B2-8CD8-A7F4167DE773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="1293">
   <si>
     <t>cs</t>
   </si>
@@ -3953,6 +3953,18 @@
   </si>
   <si>
     <t>Úspěšně jste si pořídili drát [{{data.wire.vendor.name}} {{data.wire.name}}].</t>
+  </si>
+  <si>
+    <t>market.other.menu</t>
+  </si>
+  <si>
+    <t>Ostatní</t>
+  </si>
+  <si>
+    <t>market.hardware.menu</t>
+  </si>
+  <si>
+    <t>Hardware</t>
   </si>
 </sst>
 </file>
@@ -11336,10 +11348,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11959,10 +11971,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>377</v>
+        <v>1291</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>4</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -11970,10 +11982,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>376</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -11981,10 +11993,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>341</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -11992,7 +12004,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>341</v>
@@ -12003,10 +12015,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -12014,10 +12026,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1209</v>
+        <v>378</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>234</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -12025,32 +12037,32 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -12058,10 +12070,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -12069,10 +12081,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>385</v>
+        <v>437</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>236</v>
+        <v>438</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -12080,7 +12092,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>236</v>
@@ -12091,21 +12103,21 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>453</v>
+        <v>1289</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>452</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -12113,21 +12125,21 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -12135,10 +12147,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -12146,10 +12158,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -12157,10 +12169,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -12168,10 +12180,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>449</v>
+        <v>474</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -12179,21 +12191,21 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1285</v>
+        <v>450</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1283</v>
+        <v>449</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1284</v>
+        <v>457</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -12201,21 +12213,21 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1281</v>
+        <v>1285</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -12223,10 +12235,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1268</v>
+        <v>1281</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1267</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -12234,10 +12246,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1266</v>
+        <v>1287</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1267</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -12245,10 +12257,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>460</v>
+        <v>1268</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>458</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -12256,10 +12268,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>466</v>
+        <v>1266</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>467</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -12267,10 +12279,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -12278,10 +12290,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -12289,10 +12301,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -12300,15 +12312,37 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>463</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C87">
-    <sortCondition ref="B82:B87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C89">
+    <sortCondition ref="B82:B89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Added empty mixture page
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45B759C-25AC-8742-8161-CC0BDC7E3207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805E4D3B-D80F-E243-946F-805E4B9D5EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2612" uniqueCount="1297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2618" uniqueCount="1299">
   <si>
     <t>cs</t>
   </si>
@@ -3977,6 +3977,12 @@
   </si>
   <si>
     <t>Mixy se zobrazí po zakoupení aromatu a báze - ty se využívají k nabízení dostupných liquidů, které je možné namíchat.</t>
+  </si>
+  <si>
+    <t>market.mixture.menu</t>
+  </si>
+  <si>
+    <t>market.mixture.index.title</t>
   </si>
 </sst>
 </file>
@@ -7958,7 +7964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
@@ -11382,10 +11388,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12082,21 +12088,21 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>436</v>
+        <v>1298</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>435</v>
+        <v>1297</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>444</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -12104,21 +12110,21 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -12126,10 +12132,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>385</v>
+        <v>433</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>236</v>
+        <v>434</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -12137,10 +12143,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>381</v>
+        <v>437</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>236</v>
+        <v>438</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -12148,10 +12154,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1289</v>
+        <v>385</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1290</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -12159,21 +12165,21 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>453</v>
+        <v>1289</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>452</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -12181,21 +12187,21 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -12203,10 +12209,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -12214,10 +12220,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -12225,10 +12231,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -12236,10 +12242,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>449</v>
+        <v>474</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -12247,21 +12253,21 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1285</v>
+        <v>450</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1283</v>
+        <v>449</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1284</v>
+        <v>457</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -12269,21 +12275,21 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1281</v>
+        <v>1285</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -12291,10 +12297,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1268</v>
+        <v>1281</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1267</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -12302,10 +12308,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1266</v>
+        <v>1287</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1267</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -12313,10 +12319,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>460</v>
+        <v>1268</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>458</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -12324,10 +12330,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>466</v>
+        <v>1266</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>467</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -12335,10 +12341,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -12346,10 +12352,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -12357,10 +12363,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -12368,15 +12374,37 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>463</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C89">
-    <sortCondition ref="B82:B89"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C91">
+    <sortCondition ref="B81:B91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Some improvement, trying to fix connection pool timeouts
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FDFC40-49CF-4293-8FCA-B5DA414A555C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05FD0D-4DA2-4651-81B9-5469D292B85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" firstSheet="14" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="360" windowWidth="43095" windowHeight="18495" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="1307">
   <si>
     <t>cs</t>
   </si>
@@ -4002,12 +4002,18 @@
   <si>
     <t>Aktualizace mixů aromatu</t>
   </si>
+  <si>
+    <t>root.job.finished.tooltip</t>
+  </si>
+  <si>
+    <t>Čas dokončení úlohy {{data.date}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4046,13 +4052,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="8"/>
@@ -4103,7 +4102,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4127,9 +4126,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="import" xfId="2" xr:uid="{DD1BC027-BC6C-4B34-B536-A533FDE94B7A}"/>
@@ -6026,8 +6022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6125,11 +6121,11 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="1" t="s">
         <v>1163</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -9654,10 +9650,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10288,10 +10284,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>107</v>
+        <v>1305</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>59</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -10299,10 +10295,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>195</v>
+        <v>107</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -10310,10 +10306,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>194</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -10321,10 +10317,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -10332,10 +10328,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>59</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -10343,10 +10339,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>198</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -10354,10 +10350,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>292</v>
+        <v>197</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -10365,10 +10361,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1087</v>
+        <v>292</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1088</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -10376,10 +10372,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -10387,10 +10383,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>302</v>
+        <v>1085</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>59</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -10398,10 +10394,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>125</v>
+        <v>302</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -10409,10 +10405,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>340</v>
+        <v>125</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>341</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -10420,10 +10416,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>113</v>
+        <v>340</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>114</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -10431,10 +10427,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -10442,10 +10438,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1038</v>
+        <v>127</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1039</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -10453,10 +10449,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>24</v>
+        <v>1038</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>25</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -10464,10 +10460,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -10475,10 +10471,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>410</v>
+        <v>117</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>411</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -10486,10 +10482,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>639</v>
+        <v>410</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>640</v>
+        <v>411</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10497,10 +10493,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>412</v>
+        <v>639</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>413</v>
+        <v>640</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10508,10 +10504,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10519,10 +10515,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10530,10 +10526,10 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10541,10 +10537,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10552,32 +10548,32 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="1" t="s">
+    <row r="83" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -10585,10 +10581,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -10596,7 +10592,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>179</v>
@@ -10607,10 +10603,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -10618,10 +10614,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -10629,10 +10625,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -10640,10 +10636,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -10651,10 +10647,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -10662,10 +10658,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -10673,10 +10669,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>399</v>
+        <v>183</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -10684,10 +10680,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>400</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -10695,10 +10691,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -10706,10 +10702,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>115</v>
+        <v>396</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>116</v>
+        <v>397</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -10717,10 +10713,10 @@
         <v>0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>402</v>
+        <v>115</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>403</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -10728,10 +10724,10 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>230</v>
+        <v>403</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -10739,10 +10735,10 @@
         <v>0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>337</v>
+        <v>401</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -10750,15 +10746,26 @@
         <v>0</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>405</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C99">
-    <sortCondition ref="B96:B99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C100">
+    <sortCondition ref="B100"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14310,7 +14317,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Common: Mixture filter is quite good noew
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FC4B6A-2299-4943-9EF4-AE0A2AA5B7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A51E40B-442B-42D7-A5E0-64E1AFC41E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="1650" windowWidth="43095" windowHeight="18495" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="1428">
   <si>
     <t>cs</t>
   </si>
@@ -4367,6 +4367,27 @@
   </si>
   <si>
     <t>Drát musí odpovídat některým z vybraných druhů drátků; vrátí veškeré typy drátů, jak jednoduchých, tak případných komplikovaných.</t>
+  </si>
+  <si>
+    <t>market.mixture.filter.ratio.tab</t>
+  </si>
+  <si>
+    <t>market.mixture.filter.draw.tab</t>
+  </si>
+  <si>
+    <t>Typ potahu</t>
+  </si>
+  <si>
+    <t>common.filter.and.tab</t>
+  </si>
+  <si>
+    <t>Veškeré</t>
+  </si>
+  <si>
+    <t>common.filter.or.tab</t>
+  </si>
+  <si>
+    <t>Některé</t>
   </si>
 </sst>
 </file>
@@ -6580,10 +6601,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C585"/>
+  <dimension ref="A1:C589"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A558" workbookViewId="0">
-      <selection activeCell="C579" sqref="C579"/>
+      <selection activeCell="B584" sqref="B584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13026,6 +13047,50 @@
       </c>
       <c r="C585" s="1" t="s">
         <v>1420</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A586" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A587" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A588" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A589" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>1427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Refactoring mixture stuff, moving towards mixture inventory
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A51E40B-442B-42D7-A5E0-64E1AFC41E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649E68C-98BA-42D0-B16D-D6647FA41998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="1650" windowWidth="43095" windowHeight="18495" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="1428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="1437">
   <si>
     <t>cs</t>
   </si>
@@ -4388,6 +4388,33 @@
   </si>
   <si>
     <t>Některé</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.nicotineToRound.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.andTasteIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.orTasteIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.andTasteIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>common.filter.Mixture.filter.orTasteIds.label.tooltip</t>
   </si>
 </sst>
 </file>
@@ -6601,10 +6628,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C589"/>
+  <dimension ref="A1:C598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A558" workbookViewId="0">
-      <selection activeCell="B584" sqref="B584"/>
+    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
+      <selection activeCell="B593" sqref="B593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13091,6 +13118,105 @@
       </c>
       <c r="C589" s="1" t="s">
         <v>1427</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A590" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A591" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A592" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A593" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A594" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A595" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A596" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A597" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A598" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>1129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added more deletion support
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBA190-8C9E-434B-BE32-FF9319F38035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6EE558-9893-48E5-AA7B-B5B19F5D2E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="570" yWindow="1305" windowWidth="43095" windowHeight="18495" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="1450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="1460">
   <si>
     <t>cs</t>
   </si>
@@ -4454,6 +4454,36 @@
   </si>
   <si>
     <t>&lt;p&gt;&lt;strong&gt;Opravdu&lt;/strong&gt; si přejete odstranit vybrané liquidy?&lt;/p&gt;&lt;p&gt;Tato akce je silně destruktivní a může odstranit velké množství dat (statistiky, vapování, komentáře a další). Buďte prosím tedy &lt;strong&gt;extrémně opatrní&lt;/strong&gt; a raději si ten červený čudlík třikrát rozmyslete!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.booster.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané boostery byly úspěšně odstraněny.</t>
+  </si>
+  <si>
+    <t>lab.booster.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané boostery?</t>
+  </si>
+  <si>
+    <t>lab.booster.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Opravdu si přejete odstranit vybrané boostery? Tato akce je silně &lt;strong&gt;destruktivní&lt;/strong&gt; a není cesty zpět. Třikrát si proto rozmyslete, zda budete pokračovat.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.base.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané báze?</t>
+  </si>
+  <si>
+    <t>lab.base.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Opravdu si přejete odstranit vybrané báze? Tato akce je silně &lt;strong&gt;destruktivní&lt;/strong&gt; a není cesty zpět. Třikrát si proto rozmyslete, zda budete pokračovat.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -6667,10 +6697,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C605"/>
+  <dimension ref="A1:C610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C210" sqref="C210"/>
+    <sheetView tabSelected="1" topLeftCell="A586" workbookViewId="0">
+      <selection activeCell="B606" sqref="B606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13333,6 +13363,61 @@
       </c>
       <c r="C605" s="1" t="s">
         <v>1448</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A606" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A607" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B607" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A608" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A609" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A610" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Translated some missing tastes
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3360923A-C9D5-4E40-91BF-C9E9EB9EF795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77A13F7-6A42-46A9-9220-00583974139D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1305" windowWidth="22920" windowHeight="18495" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="1305" windowWidth="22920" windowHeight="18495" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="1501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="1531">
   <si>
     <t>cs</t>
   </si>
@@ -4607,6 +4607,96 @@
   </si>
   <si>
     <t>lemon, cookie</t>
+  </si>
+  <si>
+    <t>common.taste.apple</t>
+  </si>
+  <si>
+    <t>Jablko</t>
+  </si>
+  <si>
+    <t>common.taste.pear</t>
+  </si>
+  <si>
+    <t>Hruška</t>
+  </si>
+  <si>
+    <t>common.taste.apricot</t>
+  </si>
+  <si>
+    <t>Meruňka</t>
+  </si>
+  <si>
+    <t>common.taste.cinnamon</t>
+  </si>
+  <si>
+    <t>Skořice</t>
+  </si>
+  <si>
+    <t>common.taste.mint</t>
+  </si>
+  <si>
+    <t>Máta</t>
+  </si>
+  <si>
+    <t>common.taste.grape</t>
+  </si>
+  <si>
+    <t>Hrozen</t>
+  </si>
+  <si>
+    <t>common.taste.hazelnut</t>
+  </si>
+  <si>
+    <t>Oříšky</t>
+  </si>
+  <si>
+    <t>common.taste.cherry</t>
+  </si>
+  <si>
+    <t>Třešeň</t>
+  </si>
+  <si>
+    <t>common.taste.bourbon</t>
+  </si>
+  <si>
+    <t>Bourbon</t>
+  </si>
+  <si>
+    <t>common.taste.orange</t>
+  </si>
+  <si>
+    <t>Pomeranč</t>
+  </si>
+  <si>
+    <t>common.taste.cookie</t>
+  </si>
+  <si>
+    <t>Sušenka</t>
+  </si>
+  <si>
+    <t>common.taste.lemon</t>
+  </si>
+  <si>
+    <t>Citron</t>
+  </si>
+  <si>
+    <t>common.taste.peanut</t>
+  </si>
+  <si>
+    <t>Arašídy</t>
+  </si>
+  <si>
+    <t>common.taste.pistachio</t>
+  </si>
+  <si>
+    <t>Pistácie</t>
+  </si>
+  <si>
+    <t>common.taste.plum</t>
+  </si>
+  <si>
+    <t>Švestka</t>
   </si>
 </sst>
 </file>
@@ -6974,10 +7064,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C610"/>
+  <dimension ref="A1:C625"/>
   <sheetViews>
-    <sheetView topLeftCell="A586" workbookViewId="0">
-      <selection activeCell="B606" sqref="B606"/>
+    <sheetView tabSelected="1" topLeftCell="A595" workbookViewId="0">
+      <selection activeCell="B620" sqref="B620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13695,6 +13785,171 @@
       </c>
       <c r="C610" s="1" t="s">
         <v>1459</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A611" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A612" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A613" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A614" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B614" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A615" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A616" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A617" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A618" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B618" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A619" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A620" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A621" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A622" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A623" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A624" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>1530</v>
       </c>
     </row>
   </sheetData>
@@ -15929,7 +16184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Improved agenda config
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F188AD54-6E42-4A01-BED4-2E0FB9C8CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0678C3-44C7-4C7A-9123-0CB8FD31021A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1305" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3204" uniqueCount="1633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3207" uniqueCount="1635">
   <si>
     <t>cs</t>
   </si>
@@ -5003,6 +5003,12 @@
   </si>
   <si>
     <t>BoosterInventory.list.total</t>
+  </si>
+  <si>
+    <t>common.job.name.job.mixture-update</t>
+  </si>
+  <si>
+    <t>Výpočet mixu</t>
   </si>
 </sst>
 </file>
@@ -7366,10 +7372,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C647"/>
+  <dimension ref="A1:C648"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A610" workbookViewId="0">
-      <selection activeCell="B637" sqref="B637"/>
+      <selection activeCell="B635" sqref="B635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14494,6 +14500,17 @@
       </c>
       <c r="C647" s="1" t="s">
         <v>1604</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A648" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C648" s="1" t="s">
+        <v>1634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved empty list of mixtures
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F723929-11B8-3E4D-991A-ABB28BD33402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAFD2A9-D5C8-8D4D-9E61-8EAF654162ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="28540" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3276" uniqueCount="1679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1682">
   <si>
     <t>cs</t>
   </si>
@@ -5141,6 +5141,15 @@
   </si>
   <si>
     <t>Komentáře k aromatu {{data.aroma.name}} - {{data.aroma.vendor.name}}</t>
+  </si>
+  <si>
+    <t>Vybrali jste kombinaci vyhledávání, pro kterou neexistuje výsledek. Zkontrolujte prosím parametry hledání.</t>
+  </si>
+  <si>
+    <t>lab.mixture.filter.empty.title</t>
+  </si>
+  <si>
+    <t>lab.mixture.filter.empty.subtitle</t>
   </si>
 </sst>
 </file>
@@ -7504,10 +7513,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C671"/>
+  <dimension ref="A1:C673"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A639" workbookViewId="0">
-      <selection activeCell="C671" sqref="C671"/>
+    <sheetView tabSelected="1" topLeftCell="A647" workbookViewId="0">
+      <selection activeCell="B666" sqref="B666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14896,6 +14905,28 @@
       </c>
       <c r="C671" s="1" t="s">
         <v>1678</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A672" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B672" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C672" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A673" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B673" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C673" s="1" t="s">
+        <v>1679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed mixture material purchases
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAFD2A9-D5C8-8D4D-9E61-8EAF654162ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC234571-AC34-B740-ADF0-3D575621BFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="28540" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3285" uniqueCount="1684">
   <si>
     <t>cs</t>
   </si>
@@ -5150,6 +5150,12 @@
   </si>
   <si>
     <t>lab.mixture.filter.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.base.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste odstranili vybrané báze.</t>
   </si>
 </sst>
 </file>
@@ -7513,10 +7519,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C673"/>
+  <dimension ref="A1:C674"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A647" workbookViewId="0">
-      <selection activeCell="B666" sqref="B666"/>
+    <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
+      <selection activeCell="B671" sqref="B671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14927,6 +14933,17 @@
       </c>
       <c r="C673" s="1" t="s">
         <v>1679</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A674" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B674" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C674" s="1" t="s">
+        <v>1683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added mixture update response for user
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC234571-AC34-B740-ADF0-3D575621BFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD92EAAC-9705-A344-B6FE-85BAF6E48BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="28540" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3285" uniqueCount="1684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3291" uniqueCount="1688">
   <si>
     <t>cs</t>
   </si>
@@ -5157,6 +5157,18 @@
   <si>
     <t>Úspěšně jste odstranili vybrané báze.</t>
   </si>
+  <si>
+    <t>lab.mixture.job.NEW.alert.message</t>
+  </si>
+  <si>
+    <t>Je naplánována aktualizace vašeho seznamu mixů. Než se spustí, neuvidíte nová data (typycky po zakoupení nového aromatu, báze nebo boosteru).</t>
+  </si>
+  <si>
+    <t>lab.mixture.job.RUNNING.alert.message</t>
+  </si>
+  <si>
+    <t>Právě probíhá aktualizace vašeho seznamu mixů. Vyčkejte prosím. {{job.progress}}%</t>
+  </si>
 </sst>
 </file>
 
@@ -5165,7 +5177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5207,6 +5219,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5254,7 +5273,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5281,6 +5300,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7519,10 +7541,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C674"/>
+  <dimension ref="A1:C676"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
-      <selection activeCell="B671" sqref="B671"/>
+      <selection activeCell="C676" sqref="C676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14944,6 +14966,28 @@
       </c>
       <c r="C674" s="1" t="s">
         <v>1683</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A675" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B675" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C675" s="1" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A676" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B676" s="21" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C676" s="20" t="s">
+        <v>1687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added mixture update button
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD92EAAC-9705-A344-B6FE-85BAF6E48BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD8356E-776C-7A4B-93EE-67F4A9D53EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="28540" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3291" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1689">
   <si>
     <t>cs</t>
   </si>
@@ -5158,16 +5158,19 @@
     <t>Úspěšně jste odstranili vybrané báze.</t>
   </si>
   <si>
-    <t>lab.mixture.job.NEW.alert.message</t>
-  </si>
-  <si>
-    <t>Je naplánována aktualizace vašeho seznamu mixů. Než se spustí, neuvidíte nová data (typycky po zakoupení nového aromatu, báze nebo boosteru).</t>
-  </si>
-  <si>
-    <t>lab.mixture.job.RUNNING.alert.message</t>
-  </si>
-  <si>
-    <t>Právě probíhá aktualizace vašeho seznamu mixů. Vyčkejte prosím. {{job.progress}}%</t>
+    <t>lab.mixture.user.job.schedule.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.user.job.schedule.NEW.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.user.job.schedule.RUNNING.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.user.job.schedule.success</t>
+  </si>
+  <si>
+    <t>Aktualizace mixů vyžádána. Úloha běží na pozadí, můžete pokračovat v práci.</t>
   </si>
 </sst>
 </file>
@@ -5177,7 +5180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5219,13 +5222,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5273,7 +5269,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5300,9 +5296,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7541,10 +7534,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C676"/>
+  <dimension ref="A1:C678"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
-      <selection activeCell="C676" sqref="C676"/>
+    <sheetView tabSelected="1" topLeftCell="A652" workbookViewId="0">
+      <selection activeCell="B671" sqref="B671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14976,18 +14969,40 @@
         <v>1684</v>
       </c>
       <c r="C675" s="1" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A676" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B676" s="1" t="s">
         <v>1685</v>
       </c>
-    </row>
-    <row r="676" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A676" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B676" s="21" t="s">
+      <c r="C676" s="1" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A677" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B677" s="1" t="s">
         <v>1686</v>
       </c>
-      <c r="C676" s="20" t="s">
+      <c r="C677" s="1" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A678" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B678" s="1" t="s">
         <v>1687</v>
+      </c>
+      <c r="C678" s="1" t="s">
+        <v>1688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite a cool idea how to improve mixture filtering stuff!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12A8E03-BAF9-4E21-AD4A-4CE442281FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE7604-676D-4A26-86FA-D66619769C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3320" uniqueCount="1701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1704">
   <si>
     <t>cs</t>
   </si>
@@ -5207,6 +5207,15 @@
   </si>
   <si>
     <t>MAX VG</t>
+  </si>
+  <si>
+    <t>market.aroma.mixture.filter.title</t>
+  </si>
+  <si>
+    <t>market.aroma.mixture.filter.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud jste zvědaví, vyhledejte si požadovaný mix.</t>
   </si>
 </sst>
 </file>
@@ -7570,10 +7579,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C686"/>
+  <dimension ref="A1:C688"/>
   <sheetViews>
-    <sheetView topLeftCell="A652" workbookViewId="0">
-      <selection activeCell="B678" sqref="B678"/>
+    <sheetView tabSelected="1" topLeftCell="A664" workbookViewId="0">
+      <selection activeCell="B683" sqref="B683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15127,6 +15136,28 @@
       </c>
       <c r="C686" s="1" t="s">
         <v>1696</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A687" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B687" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A688" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B688" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C688" s="1" t="s">
+        <v>1703</v>
       </c>
     </row>
   </sheetData>
@@ -17361,7 +17392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Improved mixture filtering stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE7604-676D-4A26-86FA-D66619769C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013E2F65-50B4-4894-9218-8694E1B62C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1706">
   <si>
     <t>cs</t>
   </si>
@@ -5216,6 +5216,12 @@
   </si>
   <si>
     <t>Pokud jste zvědaví, vyhledejte si požadovaný mix.</t>
+  </si>
+  <si>
+    <t>Aktualizace vašich mixů</t>
+  </si>
+  <si>
+    <t>Probíhá aktualizace vašich mixů</t>
   </si>
 </sst>
 </file>
@@ -7582,7 +7588,7 @@
   <dimension ref="A1:C688"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A664" workbookViewId="0">
-      <selection activeCell="B683" sqref="B683"/>
+      <selection activeCell="C677" sqref="C677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15014,7 +15020,7 @@
         <v>1683</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1656</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
@@ -15036,7 +15042,7 @@
         <v>1685</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>1655</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Common: Fixed booster/base in market
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD9E84-DD13-4429-88D3-48512CDC3721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E607A74-5252-4035-A0F0-8CADF5CE49A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="1725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3364" uniqueCount="1729">
   <si>
     <t>cs</t>
   </si>
@@ -5279,6 +5279,27 @@
   </si>
   <si>
     <t>Liči</t>
+  </si>
+  <si>
+    <t>market.aroma.index.subtitle</t>
+  </si>
+  <si>
+    <t>Zde můžete prozkoumat dostupná aromata, prohlédnout si dostupné mixy těchto aromat a případně si je zařadit do svého inventáře.</t>
+  </si>
+  <si>
+    <t>market.aroma.index.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Aromata jsou obecně již hotové liquidy (ty nemají k nabídce žádné mixy), příchutě (tzn. zpravidla malé lahvičky) a Shake and Vape.
+&lt;/p&gt;
+&lt;p&gt;
+	Smyslem této sekce je nabídnout přehled všech možných aromat a kombinací možností jejich namíchání, tudíž je snadné si vyhledat patřičný
+	poměr VG/PG, síly nikotinu a další.
+&lt;/p&gt;
+&lt;p&gt;
+	Zakoupením aromatu jej získáte jako formu "licence", nejedná se přímo o "naskladnění", takže jej budete moci využívat neomezeně, dokud aroma neodstraníte ze svého inventáře.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -7686,10 +7707,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C693"/>
+  <dimension ref="A1:C695"/>
   <sheetViews>
-    <sheetView topLeftCell="A664" workbookViewId="0">
-      <selection activeCell="C693" sqref="C693"/>
+    <sheetView tabSelected="1" topLeftCell="A673" workbookViewId="0">
+      <selection activeCell="B693" sqref="B693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15290,36 +15311,58 @@
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A691" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B691" s="20" t="s">
+      <c r="A691" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B691" s="1" t="s">
         <v>1714</v>
       </c>
-      <c r="C691" s="20" t="s">
+      <c r="C691" s="1" t="s">
         <v>1715</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A692" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B692" s="20" t="s">
+      <c r="A692" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B692" s="1" t="s">
         <v>1721</v>
       </c>
-      <c r="C692" s="20" t="s">
+      <c r="C692" s="1" t="s">
         <v>1722</v>
       </c>
     </row>
     <row r="693" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A693" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B693" s="20" t="s">
+      <c r="A693" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B693" s="1" t="s">
         <v>1723</v>
       </c>
-      <c r="C693" s="20" t="s">
+      <c r="C693" s="1" t="s">
         <v>1724</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A694" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B694" s="1" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C694" s="1" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="695" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A695" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B695" s="1" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C695" s="1" t="s">
+        <v>1728</v>
       </c>
     </row>
   </sheetData>
@@ -17554,8 +17597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Another fixes V
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956147A7-7B9F-400B-83B1-86AE665C39C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAF886F-F54E-46CB-918C-877002616BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="1731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="1732">
   <si>
     <t>cs</t>
   </si>
@@ -5306,6 +5306,9 @@
   </si>
   <si>
     <t>common.filter.MixtureInventory.filter.title</t>
+  </si>
+  <si>
+    <t>MixtureInventory.list.total</t>
   </si>
 </sst>
 </file>
@@ -7713,10 +7716,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C697"/>
+  <dimension ref="A1:C698"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
+      <selection activeCell="B638" sqref="B638"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14771,7 +14774,7 @@
         <v>0</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>1609</v>
+        <v>1731</v>
       </c>
       <c r="C641" s="1" t="s">
         <v>1590</v>
@@ -14782,10 +14785,10 @@
         <v>0</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>1600</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.25">
@@ -14793,10 +14796,10 @@
         <v>0</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.25">
@@ -14804,10 +14807,10 @@
         <v>0</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.25">
@@ -14815,10 +14818,10 @@
         <v>0</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>1596</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.25">
@@ -14826,10 +14829,10 @@
         <v>0</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>1584</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="647" spans="1:3" x14ac:dyDescent="0.25">
@@ -14837,10 +14840,10 @@
         <v>0</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.25">
@@ -14848,10 +14851,10 @@
         <v>0</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
@@ -14859,10 +14862,10 @@
         <v>0</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>1618</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.25">
@@ -14870,10 +14873,10 @@
         <v>0</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>1622</v>
+        <v>1617</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>1625</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
@@ -14881,10 +14884,10 @@
         <v>0</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>1619</v>
+        <v>1622</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>1086</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -14892,10 +14895,10 @@
         <v>0</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>1630</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.25">
@@ -14903,10 +14906,10 @@
         <v>0</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.25">
@@ -14914,10 +14917,10 @@
         <v>0</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>1624</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.25">
@@ -14925,10 +14928,10 @@
         <v>0</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.25">
@@ -14936,10 +14939,10 @@
         <v>0</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.25">
@@ -14947,10 +14950,10 @@
         <v>0</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.25">
@@ -14958,32 +14961,32 @@
         <v>0</v>
       </c>
       <c r="B658" s="1" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C658" s="1" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A659" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B659" s="1" t="s">
         <v>1634</v>
       </c>
-      <c r="C658" s="1" t="s">
+      <c r="C659" s="1" t="s">
         <v>1641</v>
       </c>
     </row>
-    <row r="659" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A659" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B659" s="1" t="s">
+    <row r="660" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A660" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B660" s="1" t="s">
         <v>1635</v>
       </c>
-      <c r="C659" s="1" t="s">
+      <c r="C660" s="1" t="s">
         <v>1636</v>
-      </c>
-    </row>
-    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A660" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B660" s="1" t="s">
-        <v>1637</v>
-      </c>
-      <c r="C660" s="1" t="s">
-        <v>1638</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.25">
@@ -14991,10 +14994,10 @@
         <v>0</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.25">
@@ -15002,10 +15005,10 @@
         <v>0</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.25">
@@ -15013,10 +15016,10 @@
         <v>0</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.25">
@@ -15024,10 +15027,10 @@
         <v>0</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1656</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -15035,10 +15038,10 @@
         <v>0</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1648</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
@@ -15046,10 +15049,10 @@
         <v>0</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -15057,10 +15060,10 @@
         <v>0</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>601</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.25">
@@ -15068,10 +15071,10 @@
         <v>0</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1653</v>
+        <v>601</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
@@ -15079,10 +15082,10 @@
         <v>0</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
@@ -15090,10 +15093,10 @@
         <v>0</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.25">
@@ -15101,10 +15104,10 @@
         <v>0</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.25">
@@ -15112,10 +15115,10 @@
         <v>0</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.25">
@@ -15123,10 +15126,10 @@
         <v>0</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>941</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -15134,10 +15137,10 @@
         <v>0</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>1663</v>
+        <v>941</v>
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.25">
@@ -15145,10 +15148,10 @@
         <v>0</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
@@ -15156,10 +15159,10 @@
         <v>0</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>1689</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
@@ -15167,10 +15170,10 @@
         <v>0</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>1643</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
@@ -15178,10 +15181,10 @@
         <v>0</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>1690</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="679" spans="1:3" x14ac:dyDescent="0.25">
@@ -15189,10 +15192,10 @@
         <v>0</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>1672</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.25">
@@ -15200,10 +15203,10 @@
         <v>0</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1641</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.25">
@@ -15211,10 +15214,10 @@
         <v>0</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>1675</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
@@ -15222,10 +15225,10 @@
         <v>0</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.25">
@@ -15233,10 +15236,10 @@
         <v>0</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
@@ -15244,10 +15247,10 @@
         <v>0</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="685" spans="1:3" x14ac:dyDescent="0.25">
@@ -15255,10 +15258,10 @@
         <v>0</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1640</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
@@ -15266,10 +15269,10 @@
         <v>0</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="C686" s="1" t="s">
-        <v>1676</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="687" spans="1:3" x14ac:dyDescent="0.25">
@@ -15277,10 +15280,10 @@
         <v>0</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1681</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
@@ -15288,10 +15291,10 @@
         <v>0</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1095</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
@@ -15299,10 +15302,10 @@
         <v>0</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>1688</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="690" spans="1:3" x14ac:dyDescent="0.25">
@@ -15310,10 +15313,10 @@
         <v>0</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>1694</v>
+        <v>1687</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>1695</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -15321,10 +15324,10 @@
         <v>0</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>941</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
@@ -15332,10 +15335,10 @@
         <v>0</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="C692" s="1" t="s">
-        <v>1701</v>
+        <v>941</v>
       </c>
     </row>
     <row r="693" spans="1:3" x14ac:dyDescent="0.25">
@@ -15343,10 +15346,10 @@
         <v>0</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>1707</v>
+        <v>1700</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>1708</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="694" spans="1:3" x14ac:dyDescent="0.25">
@@ -15354,10 +15357,10 @@
         <v>0</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
@@ -15365,31 +15368,42 @@
         <v>0</v>
       </c>
       <c r="B695" s="1" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C695" s="1" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="696" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A696" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B696" s="1" t="s">
         <v>1711</v>
       </c>
-      <c r="C695" s="1" t="s">
+      <c r="C696" s="1" t="s">
         <v>1712</v>
       </c>
     </row>
-    <row r="696" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A696" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B696" s="1" t="s">
+    <row r="697" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A697" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B697" s="1" t="s">
         <v>1713</v>
       </c>
-      <c r="C696" s="1" t="s">
+      <c r="C697" s="1" t="s">
         <v>1714</v>
       </c>
     </row>
-    <row r="697" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A697" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B697" s="1" t="s">
+    <row r="698" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A698" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B698" s="1" t="s">
         <v>1728</v>
       </c>
-      <c r="C697" s="1" t="s">
+      <c r="C698" s="1" t="s">
         <v>1729</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Added an ability to create aromas, yaaay!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6348E-4AB1-4B64-BE2B-50D6FF8201EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45FBCB2-DE3F-4344-91AE-B040B46C4CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3427" uniqueCount="1761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1764">
   <si>
     <t>cs</t>
   </si>
@@ -5396,6 +5396,15 @@
   </si>
   <si>
     <t>Poměr VG/PG v aromatu je důležité nastavit správně, poněvadž z této hodnoty se odvíjí výpočty poměrů výsledných liquidů. Spousta liquidů má 100PG, nicméně dbejte prosím zvýšené pozornosti, zda tomu není jinak. V případě hotových liquidů je tato hodnota jasná.</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.success</t>
+  </si>
+  <si>
+    <t>Aroma {{name}}-{{vendor.name}} bylo úspěšně vytvořeno.</t>
+  </si>
+  <si>
+    <t>component.loading</t>
   </si>
 </sst>
 </file>
@@ -7803,10 +7812,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C716"/>
+  <dimension ref="A1:C718"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A699" workbookViewId="0">
-      <selection activeCell="B711" sqref="B711"/>
+      <selection activeCell="B716" sqref="B716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15690,6 +15699,28 @@
       </c>
       <c r="C716" s="1" t="s">
         <v>1760</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A717" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B717" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C717" s="1" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A718" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B718" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C718" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Created initial inventory stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4547BF5-9456-4995-832B-561125B8DF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E11473-A458-471B-8008-AA4C2D2334B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3484" uniqueCount="1783">
   <si>
     <t>cs</t>
   </si>
@@ -5405,6 +5405,63 @@
   </si>
   <si>
     <t>component.loading</t>
+  </si>
+  <si>
+    <t>inventory.index.title</t>
+  </si>
+  <si>
+    <t>inventory.home.title</t>
+  </si>
+  <si>
+    <t>inventory.home.subtitle</t>
+  </si>
+  <si>
+    <t>V této sekci naleznete veškeré předměty, které jste si pořídili na tržišti.</t>
+  </si>
+  <si>
+    <t>inventory.home.menu</t>
+  </si>
+  <si>
+    <t>inventory.atomizer.menu</t>
+  </si>
+  <si>
+    <t>inventory.mod.menu</t>
+  </si>
+  <si>
+    <t>inventory.cell.menu</t>
+  </si>
+  <si>
+    <t>inventory.cotton.menu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.menu</t>
+  </si>
+  <si>
+    <t>inventory.base.menu</t>
+  </si>
+  <si>
+    <t>inventory.booster.menu</t>
+  </si>
+  <si>
+    <t>inventory.lab.menu</t>
+  </si>
+  <si>
+    <t>inventory.market.menu</t>
+  </si>
+  <si>
+    <t>inventory.root.home.menu</t>
+  </si>
+  <si>
+    <t>inventory.atomizer.index.title</t>
+  </si>
+  <si>
+    <t>Vaše atomizéry</t>
+  </si>
+  <si>
+    <t>inventory.liquid.menu</t>
+  </si>
+  <si>
+    <t>inventory.hardware.menu</t>
   </si>
 </sst>
 </file>
@@ -5815,7 +5872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7812,10 +7869,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C718"/>
+  <sheetPr codeName="List1"/>
+  <dimension ref="A1:C735"/>
   <sheetViews>
-    <sheetView topLeftCell="A699" workbookViewId="0">
-      <selection activeCell="B716" sqref="B716"/>
+    <sheetView tabSelected="1" topLeftCell="A714" workbookViewId="0">
+      <selection activeCell="B729" sqref="B729"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15721,6 +15779,193 @@
       </c>
       <c r="C718" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A719" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B719" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C719" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A720" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B720" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C720" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A721" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B721" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C721" s="1" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A722" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B722" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C722" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A723" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B723" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C723" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A724" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B724" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C724" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A725" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B725" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C725" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A726" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B726" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C726" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A727" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B727" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C727" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A728" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B728" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C728" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A729" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B729" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C729" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A730" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B730" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C730" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A731" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B731" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C731" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="732" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A732" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B732" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C732" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="733" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A733" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B733" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C733" s="1" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="734" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A734" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B734" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C734" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="735" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A735" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B735" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C735" s="1" t="s">
+        <v>1224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Inventory looks good
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E11473-A458-471B-8008-AA4C2D2334B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F04D9C5-5B84-4E17-96FA-F79E884A5B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3484" uniqueCount="1783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="1830">
   <si>
     <t>cs</t>
   </si>
@@ -5462,6 +5462,179 @@
   </si>
   <si>
     <t>inventory.hardware.menu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.index.title</t>
+  </si>
+  <si>
+    <t>Vaše aromata</t>
+  </si>
+  <si>
+    <t>inventory.base.index.title</t>
+  </si>
+  <si>
+    <t>Vaše báze</t>
+  </si>
+  <si>
+    <t>inventory.booster.index.title</t>
+  </si>
+  <si>
+    <t>Vaše boostery</t>
+  </si>
+  <si>
+    <t>inventory.mod.index.title</t>
+  </si>
+  <si>
+    <t>Vaše mody</t>
+  </si>
+  <si>
+    <t>inventory.cell.index.title</t>
+  </si>
+  <si>
+    <t>Vaše články</t>
+  </si>
+  <si>
+    <t>lab.cell.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané články byly úspěšně odstraněny.</t>
+  </si>
+  <si>
+    <t>market.inventory.menu</t>
+  </si>
+  <si>
+    <t>lab.atomizer.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané atomizéry?</t>
+  </si>
+  <si>
+    <t>lab.atomizer.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané atomizéry?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.atomizer.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané atomizéry byly odstraněny. Bůh s vámi.</t>
+  </si>
+  <si>
+    <t>lab.mod.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>lab.mod.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané mody?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Vybrané mody byly odstraněny.</t>
+  </si>
+  <si>
+    <t>lab.cell.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané mody?</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané články?</t>
+  </si>
+  <si>
+    <t>lab.cell.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané články?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.mod.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané články byly odstraněny.</t>
+  </si>
+  <si>
+    <t>inventory.build.menu</t>
+  </si>
+  <si>
+    <t>inventory.wire.menu</t>
+  </si>
+  <si>
+    <t>inventory.wire.index.title</t>
+  </si>
+  <si>
+    <t>Vaše odporové dráty</t>
+  </si>
+  <si>
+    <t>lab.wire.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zakoupené žádné odporové dráty</t>
+  </si>
+  <si>
+    <t>lab.wire.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Můžete přejit na tržiště a pořídit si nějaké.</t>
+  </si>
+  <si>
+    <t>lab.market.wire.label</t>
+  </si>
+  <si>
+    <t>lab.wire.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané odporové dráty?</t>
+  </si>
+  <si>
+    <t>lab.wire.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané odporové dráty?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.wire.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané odporové dráty byly odstraněny.</t>
+  </si>
+  <si>
+    <t>WireInventory.list.total</t>
+  </si>
+  <si>
+    <t>Počet odporových drátů [{{data.total}}] ({{data.from}}-{{data.to}})</t>
   </si>
 </sst>
 </file>
@@ -7870,10 +8043,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C735"/>
+  <dimension ref="A1:C761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A714" workbookViewId="0">
-      <selection activeCell="B729" sqref="B729"/>
+    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
+      <selection activeCell="B759" sqref="B759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15966,6 +16139,292 @@
       </c>
       <c r="C735" s="1" t="s">
         <v>1224</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A736" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B736" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C736" s="1" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="737" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A737" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B737" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C737" s="1" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="738" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A738" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B738" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C738" s="1" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="739" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A739" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B739" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C739" s="1" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="740" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A740" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B740" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C740" s="1" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="741" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A741" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B741" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C741" s="1" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="742" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A742" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B742" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C742" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="743" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A743" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B743" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C743" s="1" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="744" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A744" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B744" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C744" s="1" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="745" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A745" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B745" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C745" s="1" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="746" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A746" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B746" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C746" s="1" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="747" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A747" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B747" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C747" s="1" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="748" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A748" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B748" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C748" s="1" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="749" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A749" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B749" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C749" s="1" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="750" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A750" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B750" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C750" s="1" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="751" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A751" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B751" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C751" s="1" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="752" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A752" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B752" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C752" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="753" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A753" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B753" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C753" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="754" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A754" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B754" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C754" s="1" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="755" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A755" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B755" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C755" s="1" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="756" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A756" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B756" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C756" s="1" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A757" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B757" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C757" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="758" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A758" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B758" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C758" s="1" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="759" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A759" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B759" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C759" s="1" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="760" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A760" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B760" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C760" s="1" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="761" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A761" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B761" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C761" s="1" t="s">
+        <v>1829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Inventory looks good II
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F04D9C5-5B84-4E17-96FA-F79E884A5B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996CCB-2360-4080-9CC3-40C53670D353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="1830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1838">
   <si>
     <t>cs</t>
   </si>
@@ -5635,6 +5635,38 @@
   </si>
   <si>
     <t>Počet odporových drátů [{{data.total}}] ({{data.from}}-{{data.to}})</t>
+  </si>
+  <si>
+    <t>inventory.cotton.index.title</t>
+  </si>
+  <si>
+    <t>Vaše vaty</t>
+  </si>
+  <si>
+    <t>lab.cotton.inventory.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané vaty?</t>
+  </si>
+  <si>
+    <t>lab.cotton.inventory.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané vaty?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.cotton.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané vaty byly odstraněny.</t>
   </si>
 </sst>
 </file>
@@ -8043,10 +8075,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C761"/>
+  <dimension ref="A1:C765"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
-      <selection activeCell="B759" sqref="B759"/>
+      <selection activeCell="B762" sqref="B762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16425,6 +16457,50 @@
       </c>
       <c r="C761" s="1" t="s">
         <v>1829</v>
+      </c>
+    </row>
+    <row r="762" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A762" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B762" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C762" s="1" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="763" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A763" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B763" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C763" s="1" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="764" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A764" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B764" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C764" s="1" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="765" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A765" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B765" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C765" s="1" t="s">
+        <v>1837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing build stuff - coils and co
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996CCB-2360-4080-9CC3-40C53670D353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9DF49-5095-4BAC-8321-59868EBC2365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2805" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="1857">
   <si>
     <t>cs</t>
   </si>
@@ -5667,6 +5667,63 @@
   </si>
   <si>
     <t>Vybrané vaty byly odstraněny.</t>
+  </si>
+  <si>
+    <t>lab.build.create</t>
+  </si>
+  <si>
+    <t>lab.build.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte zatím žádné buildy</t>
+  </si>
+  <si>
+    <t>lab.build.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Toto místo je smutné a touží po nějakém buildu, vytvořte si nějaký!</t>
+  </si>
+  <si>
+    <t>lab.build.create.button</t>
+  </si>
+  <si>
+    <t>Nový build</t>
+  </si>
+  <si>
+    <t>lab.build.create.title</t>
+  </si>
+  <si>
+    <t>lab.build.index.button</t>
+  </si>
+  <si>
+    <t>lab.build.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit build</t>
+  </si>
+  <si>
+    <t>lab.build.create.atomizerId.label</t>
+  </si>
+  <si>
+    <t>Vyberte atomizér</t>
+  </si>
+  <si>
+    <t>lab.build.create.coilId.label</t>
+  </si>
+  <si>
+    <t>Vyberte spirálku</t>
+  </si>
+  <si>
+    <t>lab.build.create.archive.label</t>
+  </si>
+  <si>
+    <t>Deaktivovat předchozí</t>
+  </si>
+  <si>
+    <t>lab.build.create.archive.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato možnost předpokládá, že nejste šílenec, který motá build do vícero stejných atomizérů, čili automaticky deaktivuje (čili nahradí) předchozí build ve stejném atomizéru.</t>
   </si>
 </sst>
 </file>
@@ -7953,10 +8010,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1AB5C-3BBA-9E49-B566-51FB3B75CDAA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8017,6 +8074,17 @@
         <v>10000</v>
       </c>
       <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C5" s="20">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8075,10 +8143,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C765"/>
+  <dimension ref="A1:C775"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A751" workbookViewId="0">
-      <selection activeCell="B762" sqref="B762"/>
+    <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
+      <selection activeCell="B773" sqref="B773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16501,6 +16569,116 @@
       </c>
       <c r="C765" s="1" t="s">
         <v>1837</v>
+      </c>
+    </row>
+    <row r="766" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A766" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B766" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C766" s="1" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="767" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A767" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B767" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C767" s="1" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="768" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A768" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B768" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C768" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="769" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A769" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B769" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C769" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="770" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A770" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B770" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C770" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="771" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A771" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B771" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C771" s="1" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="772" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A772" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B772" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C772" s="1" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="773" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A773" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B773" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C773" s="1" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="774" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A774" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B774" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C774" s="1" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="775" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A775" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B775" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C775" s="1" t="s">
+        <v>1856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Another build piece
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9DF49-5095-4BAC-8321-59868EBC2365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481176E0-D03C-4B77-8DF5-F45DADC338C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="1857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="1859">
   <si>
     <t>cs</t>
   </si>
@@ -5724,6 +5724,12 @@
   </si>
   <si>
     <t>Tato možnost předpokládá, že nejste šílenec, který motá build do vícero stejných atomizérů, čili automaticky deaktivuje (čili nahradí) předchozí build ve stejném atomizéru.</t>
+  </si>
+  <si>
+    <t>common.job.name.job.coil-user</t>
+  </si>
+  <si>
+    <t>Aktualizace spirálek uživatele</t>
   </si>
 </sst>
 </file>
@@ -8143,10 +8149,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C775"/>
+  <dimension ref="A1:C776"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="B773" sqref="B773"/>
+      <selection activeCell="B769" sqref="B769"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16679,6 +16685,17 @@
       </c>
       <c r="C775" s="1" t="s">
         <v>1856</v>
+      </c>
+    </row>
+    <row r="776" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A776" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B776" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C776" s="1" t="s">
+        <v>1858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial coil select, yaay!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481176E0-D03C-4B77-8DF5-F45DADC338C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CC39B-A265-4B5A-B520-264EC8E746E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8152,7 +8152,7 @@
   <dimension ref="A1:C776"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="B769" sqref="B769"/>
+      <selection activeCell="B773" sqref="B773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Probably improved a lot of stuff...?
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CC39B-A265-4B5A-B520-264EC8E746E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60959723-AE98-4196-BCBD-DCB0E14802CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="1859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3615" uniqueCount="1863">
   <si>
     <t>cs</t>
   </si>
@@ -5730,6 +5730,18 @@
   </si>
   <si>
     <t>Aktualizace spirálek uživatele</t>
+  </si>
+  <si>
+    <t>common.filter.Booster.filter.id.label</t>
+  </si>
+  <si>
+    <t>Vyhledat booster</t>
+  </si>
+  <si>
+    <t>common.filter.Base.filter.id.label</t>
+  </si>
+  <si>
+    <t>Vyhledat bázi</t>
   </si>
 </sst>
 </file>
@@ -8149,7 +8161,7 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C776"/>
+  <dimension ref="A1:C778"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
       <selection activeCell="B773" sqref="B773"/>
@@ -16696,6 +16708,28 @@
       </c>
       <c r="C776" s="1" t="s">
         <v>1858</v>
+      </c>
+    </row>
+    <row r="777" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A777" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B777" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C777" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="778" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A778" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B778" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C778" s="1" t="s">
+        <v>1862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Generating mixture inventory
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60959723-AE98-4196-BCBD-DCB0E14802CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0664516C-C52A-4CE8-A9CD-EA1CA7D0A29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3615" uniqueCount="1863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="1869">
   <si>
     <t>cs</t>
   </si>
@@ -5742,6 +5742,24 @@
   </si>
   <si>
     <t>Vyhledat bázi</t>
+  </si>
+  <si>
+    <t>common.job.name.job.mixture.inventory.aroma</t>
+  </si>
+  <si>
+    <t>Aktualizace inventáře mixů uživatele - aromata</t>
+  </si>
+  <si>
+    <t>common.job.name.job.mixture.inventory.base</t>
+  </si>
+  <si>
+    <t>Aktualizace inventáře mixů uživatele - báze</t>
+  </si>
+  <si>
+    <t>common.job.name.job.mixture.inventory.booster</t>
+  </si>
+  <si>
+    <t>Aktualizace inventáře mixů uživatele - boostery</t>
   </si>
 </sst>
 </file>
@@ -8161,10 +8179,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C778"/>
+  <dimension ref="A1:C781"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="B773" sqref="B773"/>
+      <selection activeCell="B772" sqref="B772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16730,6 +16748,39 @@
       </c>
       <c r="C778" s="1" t="s">
         <v>1862</v>
+      </c>
+    </row>
+    <row r="779" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A779" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B779" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C779" s="1" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="780" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A780" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B780" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C780" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="781" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A781" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B781" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C781" s="1" t="s">
+        <v>1868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: very first build stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0664516C-C52A-4CE8-A9CD-EA1CA7D0A29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A7275E-8A3A-43EB-9716-8C2756B83A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2550" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="1869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1891">
   <si>
     <t>cs</t>
   </si>
@@ -5760,6 +5760,99 @@
   </si>
   <si>
     <t>Aktualizace inventáře mixů uživatele - boostery</t>
+  </si>
+  <si>
+    <t>lab.build.create.subtitle</t>
+  </si>
+  <si>
+    <t>Buildy jsou užitečné pro sledování, jak vám z něj chutná a jak moc se přípdně povedl nebo nepovedl.</t>
+  </si>
+  <si>
+    <t>lab.build.create.content</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Buildy&lt;/strong&gt;
+&lt;p&gt;
+	Build reprezentuje namotanou spirálku do atomizéru a dále je pak možné sledovat řadu zajímavých údajů, např. jak dlouho vydrží, zaznamenávat požitky z vapování a jiné.
+&lt;/p&gt;
+&lt;p&gt;
+	Dalším přínosem je schopnost aplikace se učit z údajů, které do ní naboucháte, takže pak dokáže odhadnout odpory spirálek, dopředně
+	zobrazí očekávané výsledky nebo očekávanou chuť vybraného buildu.
+&lt;/p&gt;
+&lt;p&gt;
+	Obecně platí, že čím pečlivěji údaje zadáte, tím lépe se vám aplikace odmění.
+&lt;/p&gt;
+&lt;strong&gt;Spirílky&lt;/strong&gt;
+&lt;p&gt;
+	K vybranému atomizéru si můžete přiřadit spirálku, kterou hodláte použít. Tyto jsou dopředně předpočítané a vychází z odporových
+	drátů, které vlastníte.
+&lt;/p&gt;
+&lt;p&gt;
+	Drobnou vychytávkou je možnost hledání v seznamu spirálek (ano, je jich bohužel fakt ranec), kdy mezery oddělují části vyhledávání, tzn.
+	je možné např. napsat &lt;strong&gt;SS 0.15 10&lt;/strong&gt; a tím aplikace nalezne ocelové spirálky s danou velikostí a počtem otoček.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.build.create.cottonId.label</t>
+  </si>
+  <si>
+    <t>Vyberte vatu</t>
+  </si>
+  <si>
+    <t>lab.build.create.ohm.label</t>
+  </si>
+  <si>
+    <t>Odpor buildu</t>
+  </si>
+  <si>
+    <t>lab.build.create.ohm.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vyplňte prosím odpor buildu naměřený na tabu nebo regulovaném modu; použijte prosím co nejpřesnější hodnotu, jelikož aplikace se bude učit odpory spirálek podle údajů, které zadáváte.</t>
+  </si>
+  <si>
+    <t>lab.build.create.created.label</t>
+  </si>
+  <si>
+    <t>Datum vytvoření</t>
+  </si>
+  <si>
+    <t>lab.build.create.created.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tento údaj je užitečný, pokud si přejete zadat nějaký build retrospektivně. Obecně jej není za běžných podmínek třeba vyplňovat.</t>
+  </si>
+  <si>
+    <t>lab.build.create.success</t>
+  </si>
+  <si>
+    <t>Build byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.build.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané buildy?</t>
+  </si>
+  <si>
+    <t>lab.build.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejte odstranit vybrané buildy?
+&lt;/p&gt;
+&lt;p&gt;
+	Nutno podotknout, že tato akce je &lt;strong&gt;silně destruktivní&lt;/strong&gt; a není možné ji vzít zpět.
+&lt;/p&gt;
+&lt;p&gt;
+	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.build.inventory.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané buildy byly úspěšně odstraněny.</t>
   </si>
 </sst>
 </file>
@@ -8179,10 +8272,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C781"/>
+  <dimension ref="A1:C792"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A763" workbookViewId="0">
-      <selection activeCell="B772" sqref="B772"/>
+    <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
+      <selection activeCell="B791" sqref="B791"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16781,6 +16874,127 @@
       </c>
       <c r="C781" s="1" t="s">
         <v>1868</v>
+      </c>
+    </row>
+    <row r="782" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A782" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B782" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C782" s="1" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="783" spans="1:3" ht="268.5" x14ac:dyDescent="0.25">
+      <c r="A783" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B783" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C783" s="1" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="784" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A784" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B784" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C784" s="1" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="785" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A785" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B785" s="1" t="s">
+        <v>1875</v>
+      </c>
+      <c r="C785" s="1" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A786" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B786" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C786" s="1" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="787" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A787" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B787" s="1" t="s">
+        <v>1879</v>
+      </c>
+      <c r="C787" s="1" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="788" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A788" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B788" s="1" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C788" s="1" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="789" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A789" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B789" s="1" t="s">
+        <v>1883</v>
+      </c>
+      <c r="C789" s="1" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A790" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B790" s="1" t="s">
+        <v>1885</v>
+      </c>
+      <c r="C790" s="1" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="791" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A791" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B791" s="1" t="s">
+        <v>1887</v>
+      </c>
+      <c r="C791" s="1" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="792" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A792" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B792" s="1" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C792" s="1" t="s">
+        <v>1890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Another piece of build boilerplate shit stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A7275E-8A3A-43EB-9716-8C2756B83A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C694B2FE-2441-4EF2-8259-B70C90597D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3682" uniqueCount="1900">
   <si>
     <t>cs</t>
   </si>
@@ -5853,6 +5853,33 @@
   </si>
   <si>
     <t>Vybrané buildy byly úspěšně odstraněny.</t>
+  </si>
+  <si>
+    <t>Flash-e-Vapor</t>
+  </si>
+  <si>
+    <t>BF-1</t>
+  </si>
+  <si>
+    <t>4.5s+</t>
+  </si>
+  <si>
+    <t>lab.build.build.title</t>
+  </si>
+  <si>
+    <t>Detail buildu</t>
+  </si>
+  <si>
+    <t>lab.build.build.menu</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>lab.build.comment.menu</t>
+  </si>
+  <si>
+    <t>lab.build.comment.title</t>
   </si>
 </sst>
 </file>
@@ -7593,10 +7620,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
-  <dimension ref="A1:A105"/>
+  <dimension ref="A1:A106"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7810,328 +7837,333 @@
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>698</v>
+      <c r="A42" s="20" t="s">
+        <v>1891</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>1250</v>
+        <v>698</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>1255</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>699</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>1259</v>
+        <v>717</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>1253</v>
+        <v>723</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>724</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>1193</v>
+        <v>729</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>730</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>755</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A105">
-    <sortCondition ref="A105"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A106">
+    <sortCondition ref="A101:A106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8272,10 +8304,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C792"/>
+  <dimension ref="A1:C796"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
-      <selection activeCell="B791" sqref="B791"/>
+      <selection activeCell="C791" sqref="C791"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16995,6 +17027,50 @@
       </c>
       <c r="C792" s="1" t="s">
         <v>1890</v>
+      </c>
+    </row>
+    <row r="793" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A793" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B793" s="1" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C793" s="1" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="794" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A794" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B794" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C794" s="1" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="795" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A795" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C795" s="1" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A796" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B796" s="1" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C796" s="1" t="s">
+        <v>1627</v>
       </c>
     </row>
   </sheetData>
@@ -17062,7 +17138,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23611,15 +23687,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
@@ -23648,394 +23724,440 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G19" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G20" s="1">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial build rating (+ patch) works
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C694B2FE-2441-4EF2-8259-B70C90597D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE41319-7B96-43D3-9D20-547F8DD3B0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3682" uniqueCount="1900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3688" uniqueCount="1904">
   <si>
     <t>cs</t>
   </si>
@@ -5880,6 +5880,27 @@
   </si>
   <si>
     <t>lab.build.comment.title</t>
+  </si>
+  <si>
+    <t>lab.build.index.subtitle</t>
+  </si>
+  <si>
+    <t>Seznam všech buildů, které jste si osadili. Užitečné pro další hodnocení, hlavně zážitků z vapování.</t>
+  </si>
+  <si>
+    <t>lab.build.index.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Zde uvidíte seznam všech svých buildů, můžete si je zde přidat, smazat, filtrovat a provádět obecnou správu.
+&lt;/p&gt;
+&lt;p&gt;
+	Pokud si vytvoříte build, předchozí (ve výchozím stavu) deaktivuje; tyto jsou pak zobrazené jako poslední v seznamu.
+&lt;/p&gt;
+&lt;p&gt;
+	Buildy je možné také rychle hodnotit a mít tak přehled, jaké se vám povedly a jakým je lepší se vyhnout. Podrobnější
+	informace si pak můžete zapisovat přímo v detailu buildu.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -8304,10 +8325,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C796"/>
+  <dimension ref="A1:C798"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
-      <selection activeCell="C791" sqref="C791"/>
+      <selection activeCell="B797" sqref="B797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17071,6 +17092,28 @@
       </c>
       <c r="C796" s="1" t="s">
         <v>1627</v>
+      </c>
+    </row>
+    <row r="797" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A797" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B797" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="C797" s="1" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="798" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A798" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B798" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C798" s="1" t="s">
+        <v>1903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some improvements overall
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE41319-7B96-43D3-9D20-547F8DD3B0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752220B8-6EED-498E-87B9-638F7C097EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3688" uniqueCount="1904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="1930">
   <si>
     <t>cs</t>
   </si>
@@ -5901,6 +5901,84 @@
 	Buildy je možné také rychle hodnotit a mít tak přehled, jaké se vám povedly a jakým je lepší se vyhnout. Podrobnější
 	informace si pak můžete zapisovat přímo v detailu buildu.
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.build.coil.menu</t>
+  </si>
+  <si>
+    <t>Spirálka</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.menu</t>
+  </si>
+  <si>
+    <t>Atomizér</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.menu</t>
+  </si>
+  <si>
+    <t>Vata</t>
+  </si>
+  <si>
+    <t>lab.build.view.atomizer</t>
+  </si>
+  <si>
+    <t>lab.build.view.code</t>
+  </si>
+  <si>
+    <t>Kód</t>
+  </si>
+  <si>
+    <t>lab.build.view.ohm</t>
+  </si>
+  <si>
+    <t>lab.build.view.created</t>
+  </si>
+  <si>
+    <t>lab.build.view.cotton</t>
+  </si>
+  <si>
+    <t>lab.build.view.wire</t>
+  </si>
+  <si>
+    <t>Drát</t>
+  </si>
+  <si>
+    <t>lab.build.view.fiber</t>
+  </si>
+  <si>
+    <t>Složení drátu</t>
+  </si>
+  <si>
+    <t>lab.build.view.wraps</t>
+  </si>
+  <si>
+    <t>Počet otoček</t>
+  </si>
+  <si>
+    <t>lab.build.view.size</t>
+  </si>
+  <si>
+    <t>Velikost spirálky</t>
+  </si>
+  <si>
+    <t>lab.build.info.tab</t>
+  </si>
+  <si>
+    <t>Informace</t>
+  </si>
+  <si>
+    <t>lab.build.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.title</t>
+  </si>
+  <si>
+    <t>lab.build.coil.title</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.title</t>
   </si>
 </sst>
 </file>
@@ -8325,10 +8403,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C798"/>
+  <dimension ref="A1:C815"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
-      <selection activeCell="B797" sqref="B797"/>
+    <sheetView tabSelected="1" topLeftCell="A796" workbookViewId="0">
+      <selection activeCell="B809" sqref="B809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17114,6 +17192,193 @@
       </c>
       <c r="C798" s="1" t="s">
         <v>1903</v>
+      </c>
+    </row>
+    <row r="799" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A799" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B799" s="1" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C799" s="1" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="800" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A800" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B800" s="1" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C800" s="1" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A801" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B801" s="1" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C801" s="1" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A802" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B802" s="1" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C802" s="1" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A803" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B803" s="1" t="s">
+        <v>1911</v>
+      </c>
+      <c r="C803" s="1" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="804" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A804" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B804" s="1" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C804" s="1" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A805" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B805" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="C805" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A806" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B806" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C806" s="1" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A807" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B807" s="1" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C807" s="1" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A808" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B808" s="1" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C808" s="1" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A809" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B809" s="1" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C809" s="1" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A810" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B810" s="1" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C810" s="1" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A811" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B811" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C811" s="1" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A812" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B812" s="1" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C812" s="1" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A813" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B813" s="1" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C813" s="1" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A814" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B814" s="1" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C814" s="1" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A815" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B815" s="1" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C815" s="1" t="s">
+        <v>1909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some improvements, yaay!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752220B8-6EED-498E-87B9-638F7C097EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25059F37-0C40-44A6-A864-1C2B64991601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="1930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="1943">
   <si>
     <t>cs</t>
   </si>
@@ -5979,6 +5979,45 @@
   </si>
   <si>
     <t>lab.build.cotton.title</t>
+  </si>
+  <si>
+    <t>lab.build.view.active</t>
+  </si>
+  <si>
+    <t>Aktivní</t>
+  </si>
+  <si>
+    <t>lab.build.list.inactive.empty.title</t>
+  </si>
+  <si>
+    <t>Zatím nemáte žádné neaktivní buildy.</t>
+  </si>
+  <si>
+    <t>lab.build.list.inactive.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Zde se objeví buildy, které již nemáte namotané, nebo jste si je ručně deaktivovali.</t>
+  </si>
+  <si>
+    <t>lab.build.active.tab</t>
+  </si>
+  <si>
+    <t>Aktuální buildy</t>
+  </si>
+  <si>
+    <t>lab.build.inactive.tab</t>
+  </si>
+  <si>
+    <t>Archivované buildy</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.menu</t>
+  </si>
+  <si>
+    <t>Ochutnávky</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.title</t>
   </si>
 </sst>
 </file>
@@ -8403,10 +8442,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C815"/>
+  <dimension ref="A1:C822"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A796" workbookViewId="0">
-      <selection activeCell="B809" sqref="B809"/>
+      <selection activeCell="B810" sqref="B810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17379,6 +17418,83 @@
       </c>
       <c r="C815" s="1" t="s">
         <v>1909</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A816" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B816" s="1" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C816" s="1" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A817" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B817" s="1" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C817" s="1" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A818" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B818" s="1" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C818" s="1" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A819" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B819" s="1" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C819" s="1" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A820" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B820" s="1" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C820" s="1" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A821" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B821" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C821" s="1" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A822" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B822" s="1" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C822" s="1" t="s">
+        <v>1941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some cool new stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25059F37-0C40-44A6-A864-1C2B64991601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D69766-9605-45CB-AFD6-4875076E330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="1943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="2007">
   <si>
     <t>cs</t>
   </si>
@@ -6018,6 +6018,198 @@
   </si>
   <si>
     <t>lab.build.liquid.title</t>
+  </si>
+  <si>
+    <t>market.atomizer.create.button</t>
+  </si>
+  <si>
+    <t>Nový atomizér</t>
+  </si>
+  <si>
+    <t>market.atomizer.create.title</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.name.label</t>
+  </si>
+  <si>
+    <t>Název atomizéru</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím název atomizéru ideálně stejně, jak jej pojmenoval výrobce. Ostatní uživatelé podle něj pak mohou (a budou) hledat.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.code.label</t>
+  </si>
+  <si>
+    <t>Kód atomizéru</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Kód je dobrovolná hodnota určená hlavně pro importy/exporty a jednoznačenému rozeznání daného atomizéru.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.cost.label</t>
+  </si>
+  <si>
+    <t>Hodnota atomizéru</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím hodnotu atomizéru na tržišti. Mějte prosím na paměti, že prodávané atomizéry by měly mít relativně podobné ceny.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.coilMin.label</t>
+  </si>
+  <si>
+    <t>Nejmenší spirálka</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.coilMax.label</t>
+  </si>
+  <si>
+    <t>Největší spirálka</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.coilMin.label.tooltip</t>
+  </si>
+  <si>
+    <t>Nejmenší doporučená velikost spriálky do atomizéru; pokud neuvádí výrobce, použijte zkušenost a zapište údaj dle svého názoru, ovšem bez extrémů.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.coilMax.label.tooltip</t>
+  </si>
+  <si>
+    <t>Největší doporučená velikost spriálky do atomizéru; pokud neuvádí výrobce, použijte zkušenost a zapište údaj dle svého názoru, ovšem bez extrémů.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.typeId.label</t>
+  </si>
+  <si>
+    <t>Typ atomizéru</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.typeId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Typ atomizéru by měl odpovídat jeho fyzické konstrukci; pokud např. výrobce udá atomizér jako RDA, ale reálně je to RDTA, uveďte prosím RDTA.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.drawIds.label</t>
+  </si>
+  <si>
+    <t>Typy potahů</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.drawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím typy potahů, pro které je daný atomizér vhodný, ideálně z popisu výrobce, případně z vlastní praxe.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.squonk.label</t>
+  </si>
+  <si>
+    <t>Squonkovací atomizér?</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.vendorId.label</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit atomizér</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.tasteIds.label</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.tasteIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím příchutě v aromatu a to jak obecné (např. ovocné), tak i konkrétní (např. hruška); toto později umožní celkové hodnocení chutě z atomizéru, která bude založena na příchutích zde zadaných.</t>
+  </si>
+  <si>
+    <t>common.taste.lemonade</t>
+  </si>
+  <si>
+    <t>Limonáda</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.success</t>
+  </si>
+  <si>
+    <t>Atomizér byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>market.vendor.menu</t>
+  </si>
+  <si>
+    <t>Výrobci</t>
+  </si>
+  <si>
+    <t>Vendor.list.total</t>
+  </si>
+  <si>
+    <t>Počet výrobců [{{data.total}}] ({{data.from}}-{{data.to}})</t>
+  </si>
+  <si>
+    <t>market.vendor.index.title</t>
+  </si>
+  <si>
+    <t>Seznam výrobců</t>
+  </si>
+  <si>
+    <t>common.filter.Vendor.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat výrobce</t>
+  </si>
+  <si>
+    <t>common.filter.Vendor.filter.id.label</t>
+  </si>
+  <si>
+    <t>Jméno výrobce</t>
+  </si>
+  <si>
+    <t>shared.vendor.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit výrobce</t>
+  </si>
+  <si>
+    <t>market.vendor.create.button</t>
+  </si>
+  <si>
+    <t>market.vendor.create.title</t>
+  </si>
+  <si>
+    <t>Nový výrobce</t>
+  </si>
+  <si>
+    <t>shared.vendor.create.name.label</t>
+  </si>
+  <si>
+    <t>Zadejte jméno výrobce</t>
+  </si>
+  <si>
+    <t>shared.vendor.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím co nejpřesnějí jméno výrobce. Také se ujistěte, že už v systému není zadaný s podobným názevm.</t>
+  </si>
+  <si>
+    <t>shared.vendor.create.success</t>
+  </si>
+  <si>
+    <t>Výrobce [{{name}}] byl úspěšně vytvořen.</t>
   </si>
 </sst>
 </file>
@@ -8442,10 +8634,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C822"/>
+  <dimension ref="A1:C856"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A796" workbookViewId="0">
-      <selection activeCell="B810" sqref="B810"/>
+    <sheetView tabSelected="1" topLeftCell="A823" workbookViewId="0">
+      <selection activeCell="B839" sqref="B839"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17495,6 +17687,380 @@
       </c>
       <c r="C822" s="1" t="s">
         <v>1941</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A823" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B823" s="1" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C823" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A824" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B824" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C824" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A825" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B825" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C825" s="1" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A826" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B826" s="1" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C826" s="1" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A827" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B827" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C827" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A828" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B828" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C828" s="1" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A829" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B829" s="1" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C829" s="1" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A830" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B830" s="1" t="s">
+        <v>1956</v>
+      </c>
+      <c r="C830" s="1" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A831" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B831" s="1" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C831" s="1" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A832" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B832" s="1" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C832" s="1" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A833" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B833" s="1" t="s">
+        <v>1962</v>
+      </c>
+      <c r="C833" s="1" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A834" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B834" s="1" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C834" s="1" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A835" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B835" s="1" t="s">
+        <v>1966</v>
+      </c>
+      <c r="C835" s="1" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="836" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A836" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B836" s="1" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C836" s="1" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="837" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A837" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B837" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C837" s="1" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="838" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A838" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B838" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C838" s="1" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="839" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A839" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B839" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C839" s="1" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A840" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B840" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C840" s="1" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A841" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C841" s="1" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A842" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B842" s="1" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C842" s="1" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A843" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B843" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C843" s="1" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A844" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B844" s="1" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C844" s="1" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A845" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B845" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C845" s="1" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A846" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B846" s="1" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C846" s="1" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A847" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B847" s="1" t="s">
+        <v>1988</v>
+      </c>
+      <c r="C847" s="1" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A848" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B848" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C848" s="1" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="849" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A849" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B849" s="1" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C849" s="1" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="850" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A850" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B850" s="1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C850" s="1" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="851" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A851" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B851" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C851" s="1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="852" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A852" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B852" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C852" s="1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A853" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B853" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C853" s="1" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A854" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B854" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C854" s="1" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A855" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B855" s="1" t="s">
+        <v>2003</v>
+      </c>
+      <c r="C855" s="1" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A856" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B856" s="1" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C856" s="1" t="s">
+        <v>2006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepard some things for build
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D69766-9605-45CB-AFD6-4875076E330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440205AC-4EB6-4560-A15B-99F92B42B143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="2007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3904" uniqueCount="2029">
   <si>
     <t>cs</t>
   </si>
@@ -6210,6 +6210,72 @@
   </si>
   <si>
     <t>Výrobce [{{name}}] byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.name</t>
+  </si>
+  <si>
+    <t>Jméno atomizéru</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.draws</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.code</t>
+  </si>
+  <si>
+    <t>shared.coil.view.name</t>
+  </si>
+  <si>
+    <t>Název spirálky</t>
+  </si>
+  <si>
+    <t>shared.coil.view.size</t>
+  </si>
+  <si>
+    <t>shared.coil.view.wraps</t>
+  </si>
+  <si>
+    <t>shared.coil.view.draws</t>
+  </si>
+  <si>
+    <t>Vhodný typ potahu</t>
+  </si>
+  <si>
+    <t>shared.coil.view.wire</t>
+  </si>
+  <si>
+    <t>Odporový drát</t>
+  </si>
+  <si>
+    <t>shared.coil.view.fibers</t>
+  </si>
+  <si>
+    <t>shared.cotton.view.name</t>
+  </si>
+  <si>
+    <t>Jméno vaty</t>
+  </si>
+  <si>
+    <t>shared.cotton.view.code</t>
+  </si>
+  <si>
+    <t>Kód vaty</t>
+  </si>
+  <si>
+    <t>shared.cotton.view.draws</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.recommended.tab</t>
+  </si>
+  <si>
+    <t>Doporučené liquidy</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.liquids.tab</t>
+  </si>
+  <si>
+    <t>Všechny liquidy</t>
   </si>
 </sst>
 </file>
@@ -8634,10 +8700,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C856"/>
+  <dimension ref="A1:C870"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A823" workbookViewId="0">
-      <selection activeCell="B839" sqref="B839"/>
+    <sheetView tabSelected="1" topLeftCell="A838" workbookViewId="0">
+      <selection activeCell="B857" sqref="B857"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18061,6 +18127,160 @@
       </c>
       <c r="C856" s="1" t="s">
         <v>2006</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A857" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B857" s="1" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C857" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A858" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B858" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="C858" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A859" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B859" s="1" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C859" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A860" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B860" s="1" t="s">
+        <v>2011</v>
+      </c>
+      <c r="C860" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A861" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B861" s="1" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C861" s="1" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A862" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B862" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C862" s="1" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A863" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B863" s="1" t="s">
+        <v>2015</v>
+      </c>
+      <c r="C863" s="1" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A864" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B864" s="1" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C864" s="1" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A865" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B865" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C865" s="1" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A866" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B866" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C866" s="1" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A867" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B867" s="1" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C867" s="1" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A868" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B868" s="1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="C868" s="1" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A869" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B869" s="1" t="s">
+        <v>2025</v>
+      </c>
+      <c r="C869" s="1" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A870" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B870" s="1" t="s">
+        <v>2027</v>
+      </c>
+      <c r="C870" s="1" t="s">
+        <v>2028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite interesting overall improvement in builds + liquids
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440205AC-4EB6-4560-A15B-99F92B42B143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9512283-1590-4982-8EBA-D79F3297A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3904" uniqueCount="2029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="2035">
   <si>
     <t>cs</t>
   </si>
@@ -6276,6 +6276,24 @@
   </si>
   <si>
     <t>Všechny liquidy</t>
+  </si>
+  <si>
+    <t>lab.build.view.atomizer.draw</t>
+  </si>
+  <si>
+    <t>Atomizér - typy potahů</t>
+  </si>
+  <si>
+    <t>lab.build.view.coil.draw</t>
+  </si>
+  <si>
+    <t>Spirálka - typy potahů</t>
+  </si>
+  <si>
+    <t>lab.build.view.wire.draw</t>
+  </si>
+  <si>
+    <t>Drát - typy potahů</t>
   </si>
 </sst>
 </file>
@@ -8700,10 +8718,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C870"/>
+  <dimension ref="A1:C873"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A838" workbookViewId="0">
-      <selection activeCell="B857" sqref="B857"/>
+      <selection activeCell="B863" sqref="B863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18281,6 +18299,39 @@
       </c>
       <c r="C870" s="1" t="s">
         <v>2028</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A871" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B871" s="1" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C871" s="1" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A872" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B872" s="1" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C872" s="1" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A873" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B873" s="1" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C873" s="1" t="s">
+        <v>2034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Build rating - initial implementation
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9512283-1590-4982-8EBA-D79F3297A1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98703225-7FC1-45C9-8CD6-A36EB35C795D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="2035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3916" uniqueCount="2037">
   <si>
     <t>cs</t>
   </si>
@@ -6294,6 +6294,12 @@
   </si>
   <si>
     <t>Drát - typy potahů</t>
+  </si>
+  <si>
+    <t>lab.build.rating.duration.tooltip</t>
+  </si>
+  <si>
+    <t>Po jaké době byl liquid ohodnocen od doby namíchnání.</t>
   </si>
 </sst>
 </file>
@@ -8718,10 +8724,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C873"/>
+  <dimension ref="A1:C874"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A838" workbookViewId="0">
-      <selection activeCell="B863" sqref="B863"/>
+    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
+      <selection activeCell="B867" sqref="B867"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18332,6 +18338,17 @@
       </c>
       <c r="C873" s="1" t="s">
         <v>2034</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A874" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B874" s="1" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C874" s="1" t="s">
+        <v>2036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed a little bug
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98703225-7FC1-45C9-8CD6-A36EB35C795D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7495B2-B090-4132-8DE1-9038F65F2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3916" uniqueCount="2037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3919" uniqueCount="2038">
   <si>
     <t>cs</t>
   </si>
@@ -6300,6 +6300,9 @@
   </si>
   <si>
     <t>Po jaké době byl liquid ohodnocen od doby namíchnání.</t>
+  </si>
+  <si>
+    <t>BuildLiquid.list.total</t>
   </si>
 </sst>
 </file>
@@ -8724,10 +8727,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C874"/>
+  <dimension ref="A1:C875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
-      <selection activeCell="B867" sqref="B867"/>
+    <sheetView tabSelected="1" topLeftCell="A844" workbookViewId="0">
+      <selection activeCell="B868" sqref="B868"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18349,6 +18352,17 @@
       </c>
       <c r="C874" s="1" t="s">
         <v>2036</v>
+      </c>
+    </row>
+    <row r="875" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A875" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B875" s="1" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C875" s="1" t="s">
+        <v>1608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial liquid rating is done!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73300A9C-E5C5-4001-864A-11885017461E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A7819-183C-4530-8C0D-1CA38D6E1FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="2505" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="2006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="2024">
   <si>
     <t>cs</t>
   </si>
@@ -6239,6 +6239,60 @@
 &lt;p&gt;
 	&lt;strong&gt;Veškerá přidružená data budou smazána, včetně údajů o vapování, komentáře a další!&lt;/strong&gt;
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.title</t>
+  </si>
+  <si>
+    <t>Rozborka chutí liquidu</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.liquid</t>
+  </si>
+  <si>
+    <t>Celkové hodnocení liquidu v rámci buildu</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.list.rating</t>
+  </si>
+  <si>
+    <t>Hodnocení chutí liquidu</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.list.rating.empty.title</t>
+  </si>
+  <si>
+    <t>Vygenerovat hodnocení</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.list.rating.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud si přejete hodnotit tento liquid, vygenerujte prosím hodnocení příchutí pro daný liquid.</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.generate.button</t>
+  </si>
+  <si>
+    <t>Vygenerovat</t>
+  </si>
+  <si>
+    <t>Žádné příchutě nejsou dostupné</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.no-tastes.subtitle</t>
+  </si>
+  <si>
+    <t>I takové věci se stávají - buď je liquid tajemný a neudává své příchutě, nebo je špatně definovaný a je třeba zjednat nápravu.</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.no-tastes.title</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.tooltip</t>
+  </si>
+  <si>
+    <t>Rozborka příchutí liquidu v tomto buildu</t>
   </si>
 </sst>
 </file>
@@ -8658,10 +8712,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C899"/>
+  <dimension ref="A1:C908"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A890" workbookViewId="0">
-      <selection activeCell="B895" sqref="B895"/>
+    <sheetView tabSelected="1" topLeftCell="A899" workbookViewId="0">
+      <selection activeCell="B907" sqref="B907"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18558,6 +18612,105 @@
       </c>
       <c r="C899" s="1" t="s">
         <v>2004</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A900" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B900" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C900" s="1" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A901" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B901" s="1" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C901" s="1" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A902" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B902" s="1" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C902" s="1" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A903" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B903" s="1" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C903" s="1" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A904" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B904" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C904" s="1" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A905" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B905" s="1" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C905" s="1" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A906" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B906" s="1" t="s">
+        <v>2021</v>
+      </c>
+      <c r="C906" s="1" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A907" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B907" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C907" s="1" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A908" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B908" s="1" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C908" s="1" t="s">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Stopped this branch
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967DE685-7C75-43E5-820A-1398A798CE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21573A5E-2D1F-43D7-AD97-1ECE0ED771EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18390" yWindow="1545" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="2175" windowWidth="28530" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="2072">
   <si>
     <t>cs</t>
   </si>
@@ -6389,6 +6389,60 @@
   </si>
   <si>
     <t>Všechny spirálky</t>
+  </si>
+  <si>
+    <t>inventory.liquid.create.button</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.title</t>
+  </si>
+  <si>
+    <t>Vlastnosti liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.subtitle</t>
+  </si>
+  <si>
+    <t>Vyberte prosím základní vlastnosti liquidu</t>
+  </si>
+  <si>
+    <t>Požadovaná síla nikotinu</t>
+  </si>
+  <si>
+    <t>Vyberte prosím požadovanou sílu nikotinu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.continue</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.ratio.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>Požadovaný typ potahu (veškeré)</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>Požadovaný typ potahu (některé)</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.nicotine.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.nicotine.label.required</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aroma.booster.title</t>
   </si>
 </sst>
 </file>
@@ -8808,10 +8862,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C923"/>
+  <dimension ref="A1:C935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A899" workbookViewId="0">
-      <selection activeCell="B919" sqref="B919"/>
+    <sheetView tabSelected="1" topLeftCell="A911" workbookViewId="0">
+      <selection activeCell="B928" sqref="B928"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18972,6 +19026,138 @@
       </c>
       <c r="C923" s="1" t="s">
         <v>2053</v>
+      </c>
+    </row>
+    <row r="924" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A924" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B924" s="1" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C924" s="1" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="925" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A925" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B925" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="C925" s="1" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="926" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A926" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B926" s="1" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C926" s="1" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="927" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A927" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B927" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="C927" s="1" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A928" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B928" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C928" s="1" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A929" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B929" s="1" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C929" s="1" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A930" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B930" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C930" s="1" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A931" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B931" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C931" s="1" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A932" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B932" s="1" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C932" s="1" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A933" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B933" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C933" s="1" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A934" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B934" s="1" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C934" s="1" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="935" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A935" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B935" s="1" t="s">
+        <v>2071</v>
+      </c>
+      <c r="C935" s="1" t="s">
+        <v>1035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Aroma editing, yaay!
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967DE685-7C75-43E5-820A-1398A798CE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2394511A-8A73-44FB-A366-37EA611D6C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18390" yWindow="1545" windowWidth="28545" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="2175" windowWidth="28530" windowHeight="18495" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="2099">
   <si>
     <t>cs</t>
   </si>
@@ -4843,9 +4843,6 @@
     <t>market.aroma.mixture.title.tab</t>
   </si>
   <si>
-    <t>Mixy aromatu {{data.aroma.name}}</t>
-  </si>
-  <si>
     <t>market.aroma.aroma.title.tab</t>
   </si>
   <si>
@@ -4874,9 +4871,6 @@
   </si>
   <si>
     <t>Příchutě</t>
-  </si>
-  <si>
-    <t>Detail aromatu {{data.aroma.name}} - {{data.aroma.vendor.name}}</t>
   </si>
   <si>
     <t>market.aroma.view.steep</t>
@@ -6389,6 +6383,155 @@
   </si>
   <si>
     <t>Všechny spirálky</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Zadejte prosím název aromatu.</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.vendorId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte prosím výrobce aromatu.</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.cost.label.required</t>
+  </si>
+  <si>
+    <t>Udejte prosím výchozí cenu aromatu.</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.button</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.title</t>
+  </si>
+  <si>
+    <t>shared.vendor.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Jméno výrobce je povinné.</t>
+  </si>
+  <si>
+    <t>market.aroma.create.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud v aplikace schází nějaké aroma, zadejte ho prosím.</t>
+  </si>
+  <si>
+    <t>market.aroma.create.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Správné zadání aromatu je &lt;strong&gt;kritické&lt;/strong&gt; pro správný běh aplikace; je nezbytně nutné pozorně číst
+	lahvičku, případně správně vytáhnout informace z internetu, jelikož hodnoty se dále použijí pro výpočty možných
+	mixů daného aromatu, čili jejich nesprávné hodnoty budou mít vliv na všechny uživatele systému.
+&lt;/p&gt;
+&lt;p&gt;
+	Věnujte prosím pozornost zadání příchutí, jelikož ty dále umožňují jejich hodnocení v rámci buildů (potažmo samotného vapování),
+	tzn. pokud nebudou zadané, nebo budou zadané nepřesně/málo, omezí se tak schopnost hodnotit daný liquid.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>common.taste.dessert</t>
+  </si>
+  <si>
+    <t>Dezert</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.menu</t>
+  </si>
+  <si>
+    <t>Upravit</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.withMixtures.label</t>
+  </si>
+  <si>
+    <t>Aktualizovat mixy?</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.withMixtures.label.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud změníte obsah aromatu nebo objem lahvičky, je dobré nechat přepočítat mixy tohoto aromatu, jinak budou podávat špatné informace.</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.title.tab</t>
+  </si>
+  <si>
+    <t>Editace aromatu [{{aroma.name}}]</t>
+  </si>
+  <si>
+    <t>Detail aromatu {{aroma.name}} - {{aroma.vendor.name}}</t>
+  </si>
+  <si>
+    <t>Mixy aromatu {{aroma.name}}</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.edit</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.button</t>
+  </si>
+  <si>
+    <t>shared.aroma.create.vgpg.label.required</t>
+  </si>
+  <si>
+    <t>Poměr VG/PG je nutné vyplnit.</t>
+  </si>
+  <si>
+    <t>shared.aroma.edit.success</t>
+  </si>
+  <si>
+    <t>Aroma [{{aroma.name}} - {{aroma.vendor.name}}] bylo aktualizováno.</t>
+  </si>
+  <si>
+    <t>Přidat příchuť</t>
+  </si>
+  <si>
+    <t>shared.tag.taste.create.button</t>
+  </si>
+  <si>
+    <t>shared.tag.taste.create.title</t>
+  </si>
+  <si>
+    <t>Nová příchuť</t>
+  </si>
+  <si>
+    <t>shared.tag.create.code.label</t>
+  </si>
+  <si>
+    <t>shared.tag.create.label.label</t>
+  </si>
+  <si>
+    <t>Popisek</t>
+  </si>
+  <si>
+    <t>shared.tag.create.group.label</t>
+  </si>
+  <si>
+    <t>Skupina</t>
+  </si>
+  <si>
+    <t>shared.tag.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit</t>
+  </si>
+  <si>
+    <t>shared.tag.create.success</t>
+  </si>
+  <si>
+    <t>Tag byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>shared.tag.create.sort.label</t>
+  </si>
+  <si>
+    <t>Pořadí</t>
   </si>
 </sst>
 </file>
@@ -7935,7 +8078,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="B55" t="s">
         <v>980</v>
@@ -7946,7 +8089,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="B56" t="s">
         <v>980</v>
@@ -7957,7 +8100,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="B57" t="s">
         <v>980</v>
@@ -7968,7 +8111,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="B58" t="s">
         <v>980</v>
@@ -8347,7 +8490,7 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -8745,7 +8888,7 @@
         <v>652</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="C5" s="20">
         <v>10</v>
@@ -8808,10 +8951,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C923"/>
+  <dimension ref="A1:C948"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A899" workbookViewId="0">
-      <selection activeCell="B919" sqref="B919"/>
+    <sheetView tabSelected="1" topLeftCell="A919" workbookViewId="0">
+      <selection activeCell="C948" sqref="C948"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9299,7 +9442,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>549</v>
@@ -9310,7 +9453,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>1033</v>
@@ -9321,7 +9464,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>1035</v>
@@ -9332,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>1096</v>
@@ -9343,7 +9486,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>601</v>
@@ -9365,7 +9508,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1095</v>
@@ -15316,7 +15459,7 @@
         <v>0</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="C591" s="1" t="s">
         <v>1092</v>
@@ -15327,7 +15470,7 @@
         <v>0</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>1135</v>
@@ -15338,7 +15481,7 @@
         <v>0</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>1342</v>
@@ -15349,7 +15492,7 @@
         <v>0</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="C594" s="1" t="s">
         <v>1340</v>
@@ -15360,7 +15503,7 @@
         <v>0</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>1344</v>
@@ -15371,7 +15514,7 @@
         <v>0</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="C596" s="1" t="s">
         <v>1355</v>
@@ -15382,7 +15525,7 @@
         <v>0</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="C597" s="1" t="s">
         <v>1359</v>
@@ -15393,7 +15536,7 @@
         <v>0</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="C598" s="1" t="s">
         <v>1357</v>
@@ -15404,7 +15547,7 @@
         <v>0</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="C599" s="1" t="s">
         <v>1126</v>
@@ -15866,7 +16009,7 @@
         <v>0</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="C641" s="1" t="s">
         <v>1524</v>
@@ -16122,7 +16265,7 @@
         <v>1578</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1579</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -16130,10 +16273,10 @@
         <v>0</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1590</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
@@ -16141,10 +16284,10 @@
         <v>0</v>
       </c>
       <c r="B666" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C666" s="1" t="s">
         <v>1581</v>
-      </c>
-      <c r="C666" s="1" t="s">
-        <v>1582</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -16152,10 +16295,10 @@
         <v>0</v>
       </c>
       <c r="B667" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C667" s="1" t="s">
         <v>1583</v>
-      </c>
-      <c r="C667" s="1" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.25">
@@ -16163,7 +16306,7 @@
         <v>0</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C668" s="1" t="s">
         <v>601</v>
@@ -16174,10 +16317,10 @@
         <v>0</v>
       </c>
       <c r="B669" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C669" s="1" t="s">
         <v>1586</v>
-      </c>
-      <c r="C669" s="1" t="s">
-        <v>1587</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
@@ -16185,10 +16328,10 @@
         <v>0</v>
       </c>
       <c r="B670" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C670" s="1" t="s">
         <v>1588</v>
-      </c>
-      <c r="C670" s="1" t="s">
-        <v>1589</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.25">
@@ -16196,10 +16339,10 @@
         <v>0</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.25">
@@ -16207,10 +16350,10 @@
         <v>0</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.25">
@@ -16218,10 +16361,10 @@
         <v>0</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -16229,7 +16372,7 @@
         <v>0</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="C674" s="1" t="s">
         <v>941</v>
@@ -16240,10 +16383,10 @@
         <v>0</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
@@ -16251,10 +16394,10 @@
         <v>0</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
@@ -16262,10 +16405,10 @@
         <v>0</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
@@ -16273,7 +16416,7 @@
         <v>0</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>1577</v>
@@ -16284,10 +16427,10 @@
         <v>0</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.25">
@@ -16295,10 +16438,10 @@
         <v>0</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.25">
@@ -16306,7 +16449,7 @@
         <v>0</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="C681" s="1" t="s">
         <v>1575</v>
@@ -16317,10 +16460,10 @@
         <v>0</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.25">
@@ -16328,10 +16471,10 @@
         <v>0</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
@@ -16339,10 +16482,10 @@
         <v>0</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="685" spans="1:3" x14ac:dyDescent="0.25">
@@ -16350,10 +16493,10 @@
         <v>0</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
@@ -16361,7 +16504,7 @@
         <v>0</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>1574</v>
@@ -16372,10 +16515,10 @@
         <v>0</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
@@ -16383,10 +16526,10 @@
         <v>0</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
@@ -16394,7 +16537,7 @@
         <v>0</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="C689" s="1" t="s">
         <v>1095</v>
@@ -16405,10 +16548,10 @@
         <v>0</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -16416,10 +16559,10 @@
         <v>0</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
@@ -16427,7 +16570,7 @@
         <v>0</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>941</v>
@@ -16438,10 +16581,10 @@
         <v>0</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="694" spans="1:3" x14ac:dyDescent="0.25">
@@ -16449,10 +16592,10 @@
         <v>0</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
@@ -16460,10 +16603,10 @@
         <v>0</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.25">
@@ -16471,10 +16614,10 @@
         <v>0</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="697" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
@@ -16482,10 +16625,10 @@
         <v>0</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="698" spans="1:3" x14ac:dyDescent="0.25">
@@ -16493,10 +16636,10 @@
         <v>0</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="699" spans="1:3" x14ac:dyDescent="0.25">
@@ -16504,10 +16647,10 @@
         <v>0</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.25">
@@ -16515,10 +16658,10 @@
         <v>0</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.25">
@@ -16526,10 +16669,10 @@
         <v>0</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.25">
@@ -16537,10 +16680,10 @@
         <v>0</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.25">
@@ -16548,10 +16691,10 @@
         <v>0</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.25">
@@ -16559,10 +16702,10 @@
         <v>0</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="C704" s="1" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="705" spans="1:3" x14ac:dyDescent="0.25">
@@ -16570,10 +16713,10 @@
         <v>0</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.25">
@@ -16581,10 +16724,10 @@
         <v>0</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.25">
@@ -16592,7 +16735,7 @@
         <v>0</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="C707" s="1" t="s">
         <v>576</v>
@@ -16603,10 +16746,10 @@
         <v>0</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.25">
@@ -16614,7 +16757,7 @@
         <v>0</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="C709" s="1" t="s">
         <v>578</v>
@@ -16625,10 +16768,10 @@
         <v>0</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.25">
@@ -16636,10 +16779,10 @@
         <v>0</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="712" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -16647,10 +16790,10 @@
         <v>0</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="C712" s="1" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.25">
@@ -16658,7 +16801,7 @@
         <v>0</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="C713" s="1" t="s">
         <v>1094</v>
@@ -16669,10 +16812,10 @@
         <v>0</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.25">
@@ -16680,7 +16823,7 @@
         <v>0</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>601</v>
@@ -16691,10 +16834,10 @@
         <v>0</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.25">
@@ -16702,10 +16845,10 @@
         <v>0</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.25">
@@ -16713,7 +16856,7 @@
         <v>0</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="C718" s="1" t="s">
         <v>76</v>
@@ -16724,7 +16867,7 @@
         <v>0</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="C719" s="1" t="s">
         <v>480</v>
@@ -16735,7 +16878,7 @@
         <v>0</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="C720" s="1" t="s">
         <v>480</v>
@@ -16746,10 +16889,10 @@
         <v>0</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.25">
@@ -16757,7 +16900,7 @@
         <v>0</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="C722" s="1" t="s">
         <v>480</v>
@@ -16768,7 +16911,7 @@
         <v>0</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="C723" s="1" t="s">
         <v>235</v>
@@ -16779,7 +16922,7 @@
         <v>0</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="C724" s="1" t="s">
         <v>236</v>
@@ -16790,7 +16933,7 @@
         <v>0</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="C725" s="1" t="s">
         <v>237</v>
@@ -16801,7 +16944,7 @@
         <v>0</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>238</v>
@@ -16812,7 +16955,7 @@
         <v>0</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>470</v>
@@ -16823,7 +16966,7 @@
         <v>0</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="C728" s="1" t="s">
         <v>240</v>
@@ -16834,7 +16977,7 @@
         <v>0</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="C729" s="1" t="s">
         <v>472</v>
@@ -16845,7 +16988,7 @@
         <v>0</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="C730" s="1" t="s">
         <v>126</v>
@@ -16856,7 +16999,7 @@
         <v>0</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>335</v>
@@ -16867,7 +17010,7 @@
         <v>0</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="C732" s="1" t="s">
         <v>481</v>
@@ -16878,10 +17021,10 @@
         <v>0</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.25">
@@ -16889,7 +17032,7 @@
         <v>0</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>234</v>
@@ -16900,7 +17043,7 @@
         <v>0</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="C735" s="1" t="s">
         <v>1224</v>
@@ -16911,10 +17054,10 @@
         <v>0</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.25">
@@ -16922,10 +17065,10 @@
         <v>0</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
@@ -16933,10 +17076,10 @@
         <v>0</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.25">
@@ -16944,10 +17087,10 @@
         <v>0</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="C739" s="1" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.25">
@@ -16955,10 +17098,10 @@
         <v>0</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.25">
@@ -16966,10 +17109,10 @@
         <v>0</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.25">
@@ -16977,7 +17120,7 @@
         <v>0</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="C742" s="1" t="s">
         <v>480</v>
@@ -16988,10 +17131,10 @@
         <v>0</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="744" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -16999,10 +17142,10 @@
         <v>0</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.25">
@@ -17010,10 +17153,10 @@
         <v>0</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="C745" s="1" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.25">
@@ -17021,10 +17164,10 @@
         <v>0</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="747" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17032,10 +17175,10 @@
         <v>0</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.25">
@@ -17043,10 +17186,10 @@
         <v>0</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.25">
@@ -17054,10 +17197,10 @@
         <v>0</v>
       </c>
       <c r="B749" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C749" s="1" t="s">
         <v>1740</v>
-      </c>
-      <c r="C749" s="1" t="s">
-        <v>1742</v>
       </c>
     </row>
     <row r="750" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17065,10 +17208,10 @@
         <v>0</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="C750" s="1" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="751" spans="1:3" x14ac:dyDescent="0.25">
@@ -17076,10 +17219,10 @@
         <v>0</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="752" spans="1:3" x14ac:dyDescent="0.25">
@@ -17087,7 +17230,7 @@
         <v>0</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="C752" s="1" t="s">
         <v>131</v>
@@ -17098,7 +17241,7 @@
         <v>0</v>
       </c>
       <c r="B753" s="1" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="C753" s="1" t="s">
         <v>1205</v>
@@ -17109,10 +17252,10 @@
         <v>0</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
@@ -17120,10 +17263,10 @@
         <v>0</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
@@ -17131,10 +17274,10 @@
         <v>0</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
@@ -17142,7 +17285,7 @@
         <v>0</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="C757" s="1" t="s">
         <v>1205</v>
@@ -17153,10 +17296,10 @@
         <v>0</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="759" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17164,10 +17307,10 @@
         <v>0</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.25">
@@ -17175,10 +17318,10 @@
         <v>0</v>
       </c>
       <c r="B760" s="1" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
@@ -17186,10 +17329,10 @@
         <v>0</v>
       </c>
       <c r="B761" s="1" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="C761" s="1" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
@@ -17197,10 +17340,10 @@
         <v>0</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
@@ -17208,10 +17351,10 @@
         <v>0</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="764" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17219,10 +17362,10 @@
         <v>0</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
@@ -17230,10 +17373,10 @@
         <v>0</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.25">
@@ -17241,10 +17384,10 @@
         <v>0</v>
       </c>
       <c r="B766" s="1" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
@@ -17252,10 +17395,10 @@
         <v>0</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
@@ -17263,10 +17406,10 @@
         <v>0</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
@@ -17274,10 +17417,10 @@
         <v>0</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="C769" s="1" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
@@ -17285,7 +17428,7 @@
         <v>0</v>
       </c>
       <c r="B770" s="1" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="C770" s="1" t="s">
         <v>1082</v>
@@ -17296,10 +17439,10 @@
         <v>0</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="C771" s="1" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.25">
@@ -17307,10 +17450,10 @@
         <v>0</v>
       </c>
       <c r="B772" s="1" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="C772" s="1" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.25">
@@ -17318,10 +17461,10 @@
         <v>0</v>
       </c>
       <c r="B773" s="1" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
@@ -17329,10 +17472,10 @@
         <v>0</v>
       </c>
       <c r="B774" s="1" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="C774" s="1" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.25">
@@ -17340,10 +17483,10 @@
         <v>0</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="C775" s="1" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.25">
@@ -17351,10 +17494,10 @@
         <v>0</v>
       </c>
       <c r="B776" s="1" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="C776" s="1" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
@@ -17362,10 +17505,10 @@
         <v>0</v>
       </c>
       <c r="B777" s="1" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
       <c r="C777" s="1" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
@@ -17373,10 +17516,10 @@
         <v>0</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.25">
@@ -17384,10 +17527,10 @@
         <v>0</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
       <c r="C779" s="1" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.25">
@@ -17395,10 +17538,10 @@
         <v>0</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
@@ -17406,10 +17549,10 @@
         <v>0</v>
       </c>
       <c r="B781" s="1" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="C781" s="1" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
@@ -17417,10 +17560,10 @@
         <v>0</v>
       </c>
       <c r="B782" s="1" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="783" spans="1:3" ht="268.5" x14ac:dyDescent="0.25">
@@ -17428,10 +17571,10 @@
         <v>0</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="C783" s="1" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
@@ -17439,10 +17582,10 @@
         <v>0</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="C784" s="1" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.25">
@@ -17450,10 +17593,10 @@
         <v>0</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="C785" s="1" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="786" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -17461,10 +17604,10 @@
         <v>0</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
       <c r="C786" s="1" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
@@ -17472,10 +17615,10 @@
         <v>0</v>
       </c>
       <c r="B787" s="1" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="C787" s="1" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
@@ -17483,10 +17626,10 @@
         <v>0</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="C788" s="1" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.25">
@@ -17494,10 +17637,10 @@
         <v>0</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="C789" s="1" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.25">
@@ -17505,10 +17648,10 @@
         <v>0</v>
       </c>
       <c r="B790" s="1" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="C790" s="1" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="791" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17516,10 +17659,10 @@
         <v>0</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="C791" s="1" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
@@ -17527,10 +17670,10 @@
         <v>0</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="C792" s="1" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
@@ -17538,10 +17681,10 @@
         <v>0</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="C793" s="1" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
@@ -17549,10 +17692,10 @@
         <v>0</v>
       </c>
       <c r="B794" s="1" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="C794" s="1" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
@@ -17560,7 +17703,7 @@
         <v>0</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>1561</v>
@@ -17571,7 +17714,7 @@
         <v>0</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>1561</v>
@@ -17582,10 +17725,10 @@
         <v>0</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="798" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
@@ -17593,10 +17736,10 @@
         <v>0</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
@@ -17604,10 +17747,10 @@
         <v>0</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="800" spans="1:3" x14ac:dyDescent="0.25">
@@ -17615,10 +17758,10 @@
         <v>0</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
@@ -17626,10 +17769,10 @@
         <v>0</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.25">
@@ -17637,10 +17780,10 @@
         <v>0</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.25">
@@ -17648,10 +17791,10 @@
         <v>0</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="C803" s="1" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
@@ -17659,10 +17802,10 @@
         <v>0</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="C804" s="1" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.25">
@@ -17670,7 +17813,7 @@
         <v>0</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>210</v>
@@ -17681,10 +17824,10 @@
         <v>0</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.25">
@@ -17692,10 +17835,10 @@
         <v>0</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="C807" s="1" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">
@@ -17703,10 +17846,10 @@
         <v>0</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.25">
@@ -17714,10 +17857,10 @@
         <v>0</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.25">
@@ -17725,10 +17868,10 @@
         <v>0</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.25">
@@ -17736,10 +17879,10 @@
         <v>0</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.25">
@@ -17747,7 +17890,7 @@
         <v>0</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="C812" s="1" t="s">
         <v>1561</v>
@@ -17758,10 +17901,10 @@
         <v>0</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.25">
@@ -17769,10 +17912,10 @@
         <v>0</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.25">
@@ -17780,10 +17923,10 @@
         <v>0</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.25">
@@ -17791,10 +17934,10 @@
         <v>0</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.25">
@@ -17802,10 +17945,10 @@
         <v>0</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.25">
@@ -17813,10 +17956,10 @@
         <v>0</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.25">
@@ -17824,10 +17967,10 @@
         <v>0</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.25">
@@ -17835,10 +17978,10 @@
         <v>0</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.25">
@@ -17846,10 +17989,10 @@
         <v>0</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.25">
@@ -17857,10 +18000,10 @@
         <v>0</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.25">
@@ -17868,10 +18011,10 @@
         <v>0</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="C823" s="1" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.25">
@@ -17879,10 +18022,10 @@
         <v>0</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="C824" s="1" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.25">
@@ -17890,10 +18033,10 @@
         <v>0</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.25">
@@ -17901,10 +18044,10 @@
         <v>0</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
       <c r="C826" s="1" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.25">
@@ -17912,10 +18055,10 @@
         <v>0</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>1885</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.25">
@@ -17923,10 +18066,10 @@
         <v>0</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.25">
@@ -17934,10 +18077,10 @@
         <v>0</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.25">
@@ -17945,10 +18088,10 @@
         <v>0</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.25">
@@ -17956,10 +18099,10 @@
         <v>0</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.25">
@@ -17967,10 +18110,10 @@
         <v>0</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.25">
@@ -17978,10 +18121,10 @@
         <v>0</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.25">
@@ -17989,10 +18132,10 @@
         <v>0</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.25">
@@ -18000,10 +18143,10 @@
         <v>0</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.25">
@@ -18011,10 +18154,10 @@
         <v>0</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.25">
@@ -18022,10 +18165,10 @@
         <v>0</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.25">
@@ -18033,10 +18176,10 @@
         <v>0</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.25">
@@ -18044,10 +18187,10 @@
         <v>0</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.25">
@@ -18055,7 +18198,7 @@
         <v>0</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="C840" s="1" t="s">
         <v>1118</v>
@@ -18066,10 +18209,10 @@
         <v>0</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.25">
@@ -18077,10 +18220,10 @@
         <v>0</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="843" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -18088,10 +18231,10 @@
         <v>0</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.25">
@@ -18099,10 +18242,10 @@
         <v>0</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.25">
@@ -18110,10 +18253,10 @@
         <v>0</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.25">
@@ -18121,10 +18264,10 @@
         <v>0</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.25">
@@ -18132,10 +18275,10 @@
         <v>0</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.25">
@@ -18143,10 +18286,10 @@
         <v>0</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.25">
@@ -18154,10 +18297,10 @@
         <v>0</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.25">
@@ -18165,10 +18308,10 @@
         <v>0</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.25">
@@ -18176,10 +18319,10 @@
         <v>0</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.25">
@@ -18187,10 +18330,10 @@
         <v>0</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.25">
@@ -18198,10 +18341,10 @@
         <v>0</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.25">
@@ -18209,10 +18352,10 @@
         <v>0</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.25">
@@ -18220,10 +18363,10 @@
         <v>0</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.25">
@@ -18231,10 +18374,10 @@
         <v>0</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="C856" s="1" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.25">
@@ -18242,10 +18385,10 @@
         <v>0</v>
       </c>
       <c r="B857" s="1" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="C857" s="1" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">
@@ -18253,7 +18396,7 @@
         <v>0</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="C858" s="1" t="s">
         <v>1414</v>
@@ -18264,10 +18407,10 @@
         <v>0</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>1885</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.25">
@@ -18275,10 +18418,10 @@
         <v>0</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -18286,10 +18429,10 @@
         <v>0</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
@@ -18297,10 +18440,10 @@
         <v>0</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
@@ -18308,10 +18451,10 @@
         <v>0</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
@@ -18319,10 +18462,10 @@
         <v>0</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
@@ -18330,10 +18473,10 @@
         <v>0</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
@@ -18341,10 +18484,10 @@
         <v>0</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
@@ -18352,10 +18495,10 @@
         <v>0</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
@@ -18363,10 +18506,10 @@
         <v>0</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.25">
@@ -18374,10 +18517,10 @@
         <v>0</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="C869" s="1" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.25">
@@ -18385,10 +18528,10 @@
         <v>0</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="C870" s="1" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.25">
@@ -18396,10 +18539,10 @@
         <v>0</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="C871" s="1" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.25">
@@ -18407,10 +18550,10 @@
         <v>0</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="C872" s="1" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.25">
@@ -18418,10 +18561,10 @@
         <v>0</v>
       </c>
       <c r="B873" s="1" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="C873" s="1" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.25">
@@ -18429,10 +18572,10 @@
         <v>0</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.25">
@@ -18440,7 +18583,7 @@
         <v>0</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>1542</v>
@@ -18451,10 +18594,10 @@
         <v>0</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="877" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18462,10 +18605,10 @@
         <v>0</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="C877" s="1" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.25">
@@ -18473,10 +18616,10 @@
         <v>0</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.25">
@@ -18484,10 +18627,10 @@
         <v>0</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="880" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18495,10 +18638,10 @@
         <v>0</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.25">
@@ -18506,10 +18649,10 @@
         <v>0</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.25">
@@ -18517,7 +18660,7 @@
         <v>0</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="C882" s="1" t="s">
         <v>1440</v>
@@ -18528,10 +18671,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
@@ -18539,10 +18682,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -18550,7 +18693,7 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="C885" s="1" t="s">
         <v>1436</v>
@@ -18561,10 +18704,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.25">
@@ -18572,10 +18715,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.25">
@@ -18583,10 +18726,10 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="889" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18594,10 +18737,10 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.25">
@@ -18605,10 +18748,10 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.25">
@@ -18616,10 +18759,10 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="892" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18627,10 +18770,10 @@
         <v>0</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.25">
@@ -18638,10 +18781,10 @@
         <v>0</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.25">
@@ -18649,10 +18792,10 @@
         <v>0</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="895" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18660,10 +18803,10 @@
         <v>0</v>
       </c>
       <c r="B895" s="1" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.25">
@@ -18671,10 +18814,10 @@
         <v>0</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.25">
@@ -18682,10 +18825,10 @@
         <v>0</v>
       </c>
       <c r="B897" s="1" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="898" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18693,10 +18836,10 @@
         <v>0</v>
       </c>
       <c r="B898" s="1" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.25">
@@ -18704,10 +18847,10 @@
         <v>0</v>
       </c>
       <c r="B899" s="1" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.25">
@@ -18715,10 +18858,10 @@
         <v>0</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.25">
@@ -18726,10 +18869,10 @@
         <v>0</v>
       </c>
       <c r="B901" s="1" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.25">
@@ -18737,10 +18880,10 @@
         <v>0</v>
       </c>
       <c r="B902" s="1" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.25">
@@ -18748,10 +18891,10 @@
         <v>0</v>
       </c>
       <c r="B903" s="1" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.25">
@@ -18759,10 +18902,10 @@
         <v>0</v>
       </c>
       <c r="B904" s="1" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.25">
@@ -18770,10 +18913,10 @@
         <v>0</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.25">
@@ -18781,10 +18924,10 @@
         <v>0</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.25">
@@ -18792,10 +18935,10 @@
         <v>0</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.25">
@@ -18803,10 +18946,10 @@
         <v>0</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.25">
@@ -18814,10 +18957,10 @@
         <v>0</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.25">
@@ -18825,10 +18968,10 @@
         <v>0</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.25">
@@ -18836,10 +18979,10 @@
         <v>0</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.25">
@@ -18847,10 +18990,10 @@
         <v>0</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.25">
@@ -18858,10 +19001,10 @@
         <v>0</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.25">
@@ -18869,10 +19012,10 @@
         <v>0</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="C914" s="1" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.25">
@@ -18880,10 +19023,10 @@
         <v>0</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="C915" s="1" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="916" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -18891,10 +19034,10 @@
         <v>0</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.25">
@@ -18902,10 +19045,10 @@
         <v>0</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="C917" s="1" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="918" spans="1:3" x14ac:dyDescent="0.25">
@@ -18913,10 +19056,10 @@
         <v>0</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="C918" s="1" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="919" spans="1:3" x14ac:dyDescent="0.25">
@@ -18924,10 +19067,10 @@
         <v>0</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="920" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -18935,10 +19078,10 @@
         <v>0</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="C920" s="1" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="921" spans="1:3" x14ac:dyDescent="0.25">
@@ -18946,10 +19089,10 @@
         <v>0</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.25">
@@ -18957,10 +19100,10 @@
         <v>0</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.25">
@@ -18968,10 +19111,285 @@
         <v>0</v>
       </c>
       <c r="B923" s="1" t="s">
+        <v>2050</v>
+      </c>
+      <c r="C923" s="1" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="924" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A924" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B924" s="1" t="s">
         <v>2052</v>
       </c>
-      <c r="C923" s="1" t="s">
+      <c r="C924" s="1" t="s">
         <v>2053</v>
+      </c>
+    </row>
+    <row r="925" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A925" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B925" s="1" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C925" s="1" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="926" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A926" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B926" s="1" t="s">
+        <v>2056</v>
+      </c>
+      <c r="C926" s="1" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="927" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A927" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B927" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="C927" s="1" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A928" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B928" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="C928" s="1" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="929" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A929" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B929" s="1" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C929" s="1" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A930" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B930" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C930" s="1" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A931" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B931" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C931" s="1" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A932" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B932" s="1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C932" s="1" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="933" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A933" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B933" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C933" s="1" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A934" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B934" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C934" s="1" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="935" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A935" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B935" s="1" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C935" s="1" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="936" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A936" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B936" s="1" t="s">
+        <v>2074</v>
+      </c>
+      <c r="C936" s="1" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="937" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A937" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B937" s="1" t="s">
+        <v>2078</v>
+      </c>
+      <c r="C937" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="938" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A938" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B938" s="1" t="s">
+        <v>2079</v>
+      </c>
+      <c r="C938" s="1" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="939" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A939" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B939" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="C939" s="1" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="940" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A940" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B940" s="1" t="s">
+        <v>2082</v>
+      </c>
+      <c r="C940" s="1" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="941" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A941" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B941" s="1" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C941" s="1" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="942" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A942" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B942" s="1" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C942" s="1" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="943" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A943" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B943" s="1" t="s">
+        <v>2088</v>
+      </c>
+      <c r="C943" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="944" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A944" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B944" s="1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C944" s="1" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="945" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A945" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B945" s="1" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C945" s="1" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="946" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A946" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B946" s="1" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C946" s="1" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="947" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A947" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B947" s="1" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C947" s="1" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="948" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A948" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B948" s="1" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C948" s="1" t="s">
+        <v>2098</v>
       </c>
     </row>
   </sheetData>
@@ -21715,7 +22133,7 @@
         <v>662</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="C18" s="1">
         <v>15</v>
@@ -21736,7 +22154,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -22807,7 +23225,7 @@
         <v>736</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="C56" s="1">
         <v>10</v>
@@ -22836,7 +23254,7 @@
         <v>736</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="C57" s="1">
         <v>30</v>
@@ -22857,7 +23275,7 @@
         <v>7</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -22865,7 +23283,7 @@
         <v>736</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
@@ -22886,7 +23304,7 @@
         <v>3</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -23921,7 +24339,7 @@
         <v>716</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="C11" s="1">
         <v>100</v>
@@ -24516,10 +24934,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>816</v>
@@ -24539,10 +24957,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1825</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1827</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>816</v>

</xml_diff>

<commit_message>
Common: Prepared almost the whole boilerplate shit for builds
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1589E6E-D609-4426-9A3E-D20DDDEF7B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5632131-B598-4DAE-A35B-A9D13A260B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="2175" windowWidth="28530" windowHeight="18495" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="2102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4042" uniqueCount="2117">
   <si>
     <t>cs</t>
   </si>
@@ -6541,6 +6541,51 @@
   </si>
   <si>
     <t>mysterious</t>
+  </si>
+  <si>
+    <t>CoilInventory.list.total</t>
+  </si>
+  <si>
+    <t>Počet spirálek [{{data.total}}] ({{data.from}}-{{data.to}})</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.coilSize</t>
+  </si>
+  <si>
+    <t>Doporučená velikost spirálky</t>
+  </si>
+  <si>
+    <t>lab.build.label</t>
+  </si>
+  <si>
+    <t>lab.build.create.label</t>
+  </si>
+  <si>
+    <t>lab.build.coil.build.button</t>
+  </si>
+  <si>
+    <t>lab.build.create.cotton.title</t>
+  </si>
+  <si>
+    <t>Výběr vaty</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.cotton.recommended.tab</t>
+  </si>
+  <si>
+    <t>Doporučené vaty</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.cotton.list.tab</t>
+  </si>
+  <si>
+    <t>Všechny vaty</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.cotton.favourites.tab</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.build.button</t>
   </si>
 </sst>
 </file>
@@ -8971,10 +9016,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C949"/>
+  <dimension ref="A1:C959"/>
   <sheetViews>
-    <sheetView topLeftCell="A933" workbookViewId="0">
-      <selection activeCell="B947" sqref="B947"/>
+    <sheetView tabSelected="1" topLeftCell="A939" workbookViewId="0">
+      <selection activeCell="B951" sqref="B951"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19421,6 +19466,116 @@
       </c>
       <c r="C949" s="1" t="s">
         <v>2100</v>
+      </c>
+    </row>
+    <row r="950" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A950" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B950" s="1" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C950" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="951" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A951" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B951" s="1" t="s">
+        <v>2104</v>
+      </c>
+      <c r="C951" s="1" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="952" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A952" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B952" s="1" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C952" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="953" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A953" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B953" s="1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C953" s="1" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="954" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A954" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B954" s="1" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C954" s="1" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A955" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B955" s="1" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C955" s="1" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="956" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A956" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B956" s="1" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C956" s="1" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A957" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B957" s="1" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C957" s="1" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="958" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A958" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B958" s="1" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C958" s="1" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A959" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B959" s="1" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C959" s="1" t="s">
+        <v>2039</v>
       </c>
     </row>
   </sheetData>
@@ -19488,7 +19643,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19535,7 +19690,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1195</v>
@@ -19592,7 +19747,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1198</v>
@@ -19633,7 +19788,7 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>1187</v>
+        <v>777</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1188</v>
@@ -19696,7 +19851,7 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>777</v>
+        <v>1187</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1184</v>
@@ -19736,7 +19891,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1186</v>
@@ -19776,7 +19931,7 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>1187</v>
+        <v>780</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1189</v>
@@ -19803,7 +19958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
   <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
@@ -21657,7 +21812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Build with coil filter and some stuff; there is a bug in filter
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5632131-B598-4DAE-A35B-A9D13A260B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB664AA4-6F6A-4F78-8D3D-ED0F5A535265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4042" uniqueCount="2117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4147" uniqueCount="2151">
   <si>
     <t>cs</t>
   </si>
@@ -6586,6 +6586,108 @@
   </si>
   <si>
     <t>lab.build.cotton.build.button</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat atomizér</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.filter.empty.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.filter.empty.subtitle</t>
+  </si>
+  <si>
+    <t>common.filter.AtomizerInventory.filter.id.label</t>
+  </si>
+  <si>
+    <t>coilMin</t>
+  </si>
+  <si>
+    <t>coilMax</t>
+  </si>
+  <si>
+    <t>wrapsMin</t>
+  </si>
+  <si>
+    <t>wrapsMax</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.wraps</t>
+  </si>
+  <si>
+    <t>Doporučený počet otoček spirálky</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.title</t>
+  </si>
+  <si>
+    <t>Vyhledat spirálku</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.id.label</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce drátu spirálky</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.andDrawIds.label</t>
+  </si>
+  <si>
+    <t>Typ potahu spirálky</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.andDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vhodný typ potahu pro spirálku; musí obsahovat veškeré vybrané typy.</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.orDrawIds.label</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.orDrawIds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vhodný typ potahu pro spirálku; musí obsahovat některé vybrané typy.</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.size.label</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.wraps.label</t>
+  </si>
+  <si>
+    <t>common.filter.CoilInventory.filter.materialIds.label</t>
+  </si>
+  <si>
+    <t>Materiál drátu</t>
   </si>
 </sst>
 </file>
@@ -9016,10 +9118,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C959"/>
+  <dimension ref="A1:C980"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A939" workbookViewId="0">
-      <selection activeCell="B951" sqref="B951"/>
+    <sheetView tabSelected="1" topLeftCell="A957" workbookViewId="0">
+      <selection activeCell="B970" sqref="B970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19576,6 +19678,237 @@
       </c>
       <c r="C959" s="1" t="s">
         <v>2039</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A960" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B960" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C960" s="1" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="961" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A961" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B961" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C961" s="1" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A962" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B962" s="1" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C962" s="1" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="963" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A963" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B963" s="1" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C963" s="1" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A964" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B964" s="1" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C964" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="965" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A965" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B965" s="1" t="s">
+        <v>2122</v>
+      </c>
+      <c r="C965" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="966" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A966" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B966" s="1" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C966" s="1" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="967" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A967" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B967" s="1" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C967" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="968" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A968" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B968" s="1" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C968" s="1" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="969" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A969" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B969" s="1" t="s">
+        <v>2126</v>
+      </c>
+      <c r="C969" s="1" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="970" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A970" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B970" s="1" t="s">
+        <v>2133</v>
+      </c>
+      <c r="C970" s="1" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="971" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A971" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B971" s="1" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C971" s="1" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="972" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A972" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B972" s="1" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C972" s="1" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="973" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A973" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B973" s="1" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C973" s="1" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="974" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A974" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B974" s="1" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C974" s="1" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="975" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A975" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B975" s="1" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C975" s="1" t="s">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="976" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A976" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B976" s="1" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C976" s="1" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="977" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A977" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B977" s="1" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C977" s="1" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="978" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A978" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B978" s="1" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C978" s="1" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="979" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A979" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B979" s="1" t="s">
+        <v>2148</v>
+      </c>
+      <c r="C979" s="1" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="980" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A980" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B980" s="1" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C980" s="1" t="s">
+        <v>2150</v>
       </c>
     </row>
   </sheetData>
@@ -24693,10 +25026,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24704,9 +25037,13 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>658</v>
       </c>
@@ -24726,10 +25063,22 @@
         <v>814</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>2127</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>2128</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2129</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2130</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>661</v>
       </c>
@@ -24748,11 +25097,23 @@
       <c r="F2" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I2" s="20">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>725</v>
       </c>
@@ -24771,11 +25132,23 @@
       <c r="F3" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I3" s="20">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>751</v>
       </c>
@@ -24794,11 +25167,23 @@
       <c r="F4" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I4" s="20">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>672</v>
       </c>
@@ -24817,11 +25202,23 @@
       <c r="F5" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I5" s="20">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>732</v>
       </c>
@@ -24840,11 +25237,23 @@
       <c r="F6" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I6" s="20">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>748</v>
       </c>
@@ -24863,11 +25272,23 @@
       <c r="F7" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I7" s="20">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>666</v>
       </c>
@@ -24886,11 +25307,23 @@
       <c r="F8" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I8" s="20">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>700</v>
       </c>
@@ -24909,11 +25342,23 @@
       <c r="F9" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I9" s="20">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>748</v>
       </c>
@@ -24932,11 +25377,23 @@
       <c r="F10" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I10" s="20">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>748</v>
       </c>
@@ -24955,11 +25412,23 @@
       <c r="F11" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I11" s="20">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>753</v>
       </c>
@@ -24978,11 +25447,23 @@
       <c r="F12" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I12" s="20">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>723</v>
       </c>
@@ -25001,11 +25482,23 @@
       <c r="F13" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I13" s="20">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>685</v>
       </c>
@@ -25024,11 +25517,23 @@
       <c r="F14" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>700</v>
       </c>
@@ -25047,11 +25552,23 @@
       <c r="F15" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I15" s="20">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>746</v>
       </c>
@@ -25070,11 +25587,23 @@
       <c r="F16" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I16" s="20">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>748</v>
       </c>
@@ -25093,11 +25622,23 @@
       <c r="F17" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I17" s="20">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+      <c r="K17" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>693</v>
       </c>
@@ -25116,11 +25657,23 @@
       <c r="F18" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I18" s="20">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1822</v>
       </c>
@@ -25139,11 +25692,23 @@
       <c r="F19" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I19" s="20">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+      <c r="K19" s="1">
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1822</v>
       </c>
@@ -25162,7 +25727,19 @@
       <c r="F20" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="20" t="s">
+        <v>2131</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>2132</v>
+      </c>
+      <c r="I20" s="20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20" s="1">
         <v>325</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Looks like builds works quite well
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB664AA4-6F6A-4F78-8D3D-ED0F5A535265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAA6C18-34EE-4E80-95ED-B6167246A308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4147" uniqueCount="2151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4189" uniqueCount="2171">
   <si>
     <t>cs</t>
   </si>
@@ -5601,9 +5601,6 @@
     <t>lab.build.create.ohm.label.tooltip</t>
   </si>
   <si>
-    <t>Vyplňte prosím odpor buildu naměřený na tabu nebo regulovaném modu; použijte prosím co nejpřesnější hodnotu, jelikož aplikace se bude učit odpory spirálek podle údajů, které zadáváte.</t>
-  </si>
-  <si>
     <t>lab.build.create.created.label</t>
   </si>
   <si>
@@ -6688,6 +6685,75 @@
   </si>
   <si>
     <t>Materiál drátu</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.preview.tab</t>
+  </si>
+  <si>
+    <t>lab.build.create.build.title</t>
+  </si>
+  <si>
+    <t>Dokončit build</t>
+  </si>
+  <si>
+    <t>Vytvoření buildu</t>
+  </si>
+  <si>
+    <t>lab.build.create.build.subtitle</t>
+  </si>
+  <si>
+    <t>Po mnoha strastiplných klikáních jste konečně na konci cesty.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Po výběru všech součástí buildu jej již konečně můžete vytvořit.
+&lt;/p&gt;
+&lt;p&gt;
+	Smyslem celé této dlouhé cesty bylo posbírat údaje s možností jejích snažšího výběru. Navíc na tomto místě
+	máte přehled, co build může nabídnout a další informace, které jsou v režimu zrychleného buildu úmyslně vynechány.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>lab.build.create.build.content</t>
+  </si>
+  <si>
+    <t>lab.build.coil.preview.tab</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.preview.tab</t>
+  </si>
+  <si>
+    <t>lab.build.create.ohm.label.required</t>
+  </si>
+  <si>
+    <t>Zadejte prosím odpor buildu po vyžhavení a před tím, než jej osadíte vatou.</t>
+  </si>
+  <si>
+    <t>Vyplňte prosím odpor buildu naměřený na tabu nebo regulovaném modu; použijte prosím co nejpřesnější hodnotu, jelikož aplikace se bude učit odpory spirálek podle údajů, které zadáváte. Odpor prosím měřte na spirálce bez vaty a ofouknuté, aby byla správně vychladlá.</t>
+  </si>
+  <si>
+    <t>lab.build.create.atomizer.list.empty.title</t>
+  </si>
+  <si>
+    <t>Žádné oblíbené buildy</t>
+  </si>
+  <si>
+    <t>lab.build.create.atomizer.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pro vybraný atomizér nemáte zatím žádné oblíbené buildy. Až nějaký build označíte pozitivním hodnocením, zobrazí se tu.</t>
+  </si>
+  <si>
+    <t>lab.build.create.coil.list.empty.title</t>
+  </si>
+  <si>
+    <t>lab.build.create.coil.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pro vybranou spirálku nemáte zatím žádné oblíbené buildy; až nějaký build s touto spirálku označíte pozitivním hodnocením, zobrazí se tu.</t>
+  </si>
+  <si>
+    <t>lab.build.create.build.button</t>
   </si>
 </sst>
 </file>
@@ -8278,7 +8344,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="B59" t="s">
         <v>980</v>
@@ -8657,7 +8723,7 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -9118,10 +9184,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C980"/>
+  <dimension ref="A1:C994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A957" workbookViewId="0">
-      <selection activeCell="B970" sqref="B970"/>
+    <sheetView tabSelected="1" topLeftCell="A981" workbookViewId="0">
+      <selection activeCell="B988" sqref="B988"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16432,7 +16498,7 @@
         <v>1578</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -16443,7 +16509,7 @@
         <v>1579</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
@@ -16531,7 +16597,7 @@
         <v>1593</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -17774,7 +17840,7 @@
         <v>1808</v>
       </c>
       <c r="C786" s="1" t="s">
-        <v>1809</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
@@ -17782,10 +17848,10 @@
         <v>0</v>
       </c>
       <c r="B787" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C787" s="1" t="s">
         <v>1810</v>
-      </c>
-      <c r="C787" s="1" t="s">
-        <v>1811</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
@@ -17793,10 +17859,10 @@
         <v>0</v>
       </c>
       <c r="B788" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C788" s="1" t="s">
         <v>1812</v>
-      </c>
-      <c r="C788" s="1" t="s">
-        <v>1813</v>
       </c>
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.25">
@@ -17804,10 +17870,10 @@
         <v>0</v>
       </c>
       <c r="B789" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C789" s="1" t="s">
         <v>1814</v>
-      </c>
-      <c r="C789" s="1" t="s">
-        <v>1815</v>
       </c>
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.25">
@@ -17815,10 +17881,10 @@
         <v>0</v>
       </c>
       <c r="B790" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C790" s="1" t="s">
         <v>1816</v>
-      </c>
-      <c r="C790" s="1" t="s">
-        <v>1817</v>
       </c>
     </row>
     <row r="791" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -17826,10 +17892,10 @@
         <v>0</v>
       </c>
       <c r="B791" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C791" s="1" t="s">
         <v>1818</v>
-      </c>
-      <c r="C791" s="1" t="s">
-        <v>1819</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
@@ -17837,10 +17903,10 @@
         <v>0</v>
       </c>
       <c r="B792" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C792" s="1" t="s">
         <v>1820</v>
-      </c>
-      <c r="C792" s="1" t="s">
-        <v>1821</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
@@ -17848,10 +17914,10 @@
         <v>0</v>
       </c>
       <c r="B793" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C793" s="1" t="s">
         <v>1825</v>
-      </c>
-      <c r="C793" s="1" t="s">
-        <v>1826</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
@@ -17859,10 +17925,10 @@
         <v>0</v>
       </c>
       <c r="B794" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C794" s="1" t="s">
         <v>1827</v>
-      </c>
-      <c r="C794" s="1" t="s">
-        <v>1828</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
@@ -17870,7 +17936,7 @@
         <v>0</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>1561</v>
@@ -17881,7 +17947,7 @@
         <v>0</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>1561</v>
@@ -17892,10 +17958,10 @@
         <v>0</v>
       </c>
       <c r="B797" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C797" s="1" t="s">
         <v>1831</v>
-      </c>
-      <c r="C797" s="1" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="798" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
@@ -17903,10 +17969,10 @@
         <v>0</v>
       </c>
       <c r="B798" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C798" s="1" t="s">
         <v>1833</v>
-      </c>
-      <c r="C798" s="1" t="s">
-        <v>1834</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
@@ -17914,10 +17980,10 @@
         <v>0</v>
       </c>
       <c r="B799" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C799" s="1" t="s">
         <v>1835</v>
-      </c>
-      <c r="C799" s="1" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="800" spans="1:3" x14ac:dyDescent="0.25">
@@ -17925,10 +17991,10 @@
         <v>0</v>
       </c>
       <c r="B800" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C800" s="1" t="s">
         <v>1837</v>
-      </c>
-      <c r="C800" s="1" t="s">
-        <v>1838</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
@@ -17936,10 +18002,10 @@
         <v>0</v>
       </c>
       <c r="B801" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C801" s="1" t="s">
         <v>1839</v>
-      </c>
-      <c r="C801" s="1" t="s">
-        <v>1840</v>
       </c>
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.25">
@@ -17947,10 +18013,10 @@
         <v>0</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.25">
@@ -17958,10 +18024,10 @@
         <v>0</v>
       </c>
       <c r="B803" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C803" s="1" t="s">
         <v>1842</v>
-      </c>
-      <c r="C803" s="1" t="s">
-        <v>1843</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
@@ -17969,7 +18035,7 @@
         <v>0</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>1807</v>
@@ -17980,7 +18046,7 @@
         <v>0</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>210</v>
@@ -17991,10 +18057,10 @@
         <v>0</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.25">
@@ -18002,10 +18068,10 @@
         <v>0</v>
       </c>
       <c r="B807" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C807" s="1" t="s">
         <v>1847</v>
-      </c>
-      <c r="C807" s="1" t="s">
-        <v>1848</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">
@@ -18013,10 +18079,10 @@
         <v>0</v>
       </c>
       <c r="B808" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C808" s="1" t="s">
         <v>1849</v>
-      </c>
-      <c r="C808" s="1" t="s">
-        <v>1850</v>
       </c>
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.25">
@@ -18024,10 +18090,10 @@
         <v>0</v>
       </c>
       <c r="B809" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C809" s="1" t="s">
         <v>1851</v>
-      </c>
-      <c r="C809" s="1" t="s">
-        <v>1852</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.25">
@@ -18035,10 +18101,10 @@
         <v>0</v>
       </c>
       <c r="B810" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C810" s="1" t="s">
         <v>1853</v>
-      </c>
-      <c r="C810" s="1" t="s">
-        <v>1854</v>
       </c>
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.25">
@@ -18046,10 +18112,10 @@
         <v>0</v>
       </c>
       <c r="B811" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C811" s="1" t="s">
         <v>1855</v>
-      </c>
-      <c r="C811" s="1" t="s">
-        <v>1856</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.25">
@@ -18057,7 +18123,7 @@
         <v>0</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="C812" s="1" t="s">
         <v>1561</v>
@@ -18068,10 +18134,10 @@
         <v>0</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.25">
@@ -18079,10 +18145,10 @@
         <v>0</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.25">
@@ -18090,10 +18156,10 @@
         <v>0</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.25">
@@ -18101,10 +18167,10 @@
         <v>0</v>
       </c>
       <c r="B816" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C816" s="1" t="s">
         <v>1861</v>
-      </c>
-      <c r="C816" s="1" t="s">
-        <v>1862</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.25">
@@ -18112,10 +18178,10 @@
         <v>0</v>
       </c>
       <c r="B817" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C817" s="1" t="s">
         <v>1863</v>
-      </c>
-      <c r="C817" s="1" t="s">
-        <v>1864</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.25">
@@ -18123,10 +18189,10 @@
         <v>0</v>
       </c>
       <c r="B818" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C818" s="1" t="s">
         <v>1865</v>
-      </c>
-      <c r="C818" s="1" t="s">
-        <v>1866</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.25">
@@ -18134,10 +18200,10 @@
         <v>0</v>
       </c>
       <c r="B819" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C819" s="1" t="s">
         <v>1867</v>
-      </c>
-      <c r="C819" s="1" t="s">
-        <v>1868</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.25">
@@ -18145,10 +18211,10 @@
         <v>0</v>
       </c>
       <c r="B820" s="1" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C820" s="1" t="s">
         <v>1869</v>
-      </c>
-      <c r="C820" s="1" t="s">
-        <v>1870</v>
       </c>
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.25">
@@ -18156,10 +18222,10 @@
         <v>0</v>
       </c>
       <c r="B821" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C821" s="1" t="s">
         <v>1871</v>
-      </c>
-      <c r="C821" s="1" t="s">
-        <v>1872</v>
       </c>
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.25">
@@ -18167,10 +18233,10 @@
         <v>0</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.25">
@@ -18178,10 +18244,10 @@
         <v>0</v>
       </c>
       <c r="B823" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C823" s="1" t="s">
         <v>1874</v>
-      </c>
-      <c r="C823" s="1" t="s">
-        <v>1875</v>
       </c>
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.25">
@@ -18189,10 +18255,10 @@
         <v>0</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="C824" s="1" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.25">
@@ -18200,10 +18266,10 @@
         <v>0</v>
       </c>
       <c r="B825" s="1" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C825" s="1" t="s">
         <v>1877</v>
-      </c>
-      <c r="C825" s="1" t="s">
-        <v>1878</v>
       </c>
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.25">
@@ -18211,10 +18277,10 @@
         <v>0</v>
       </c>
       <c r="B826" s="1" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C826" s="1" t="s">
         <v>1879</v>
-      </c>
-      <c r="C826" s="1" t="s">
-        <v>1880</v>
       </c>
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.25">
@@ -18222,10 +18288,10 @@
         <v>0</v>
       </c>
       <c r="B827" s="1" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C827" s="1" t="s">
         <v>1881</v>
-      </c>
-      <c r="C827" s="1" t="s">
-        <v>1882</v>
       </c>
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.25">
@@ -18233,10 +18299,10 @@
         <v>0</v>
       </c>
       <c r="B828" s="1" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C828" s="1" t="s">
         <v>1883</v>
-      </c>
-      <c r="C828" s="1" t="s">
-        <v>1884</v>
       </c>
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.25">
@@ -18244,10 +18310,10 @@
         <v>0</v>
       </c>
       <c r="B829" s="1" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C829" s="1" t="s">
         <v>1885</v>
-      </c>
-      <c r="C829" s="1" t="s">
-        <v>1886</v>
       </c>
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.25">
@@ -18255,10 +18321,10 @@
         <v>0</v>
       </c>
       <c r="B830" s="1" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C830" s="1" t="s">
         <v>1887</v>
-      </c>
-      <c r="C830" s="1" t="s">
-        <v>1888</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.25">
@@ -18266,10 +18332,10 @@
         <v>0</v>
       </c>
       <c r="B831" s="1" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C831" s="1" t="s">
         <v>1889</v>
-      </c>
-      <c r="C831" s="1" t="s">
-        <v>1890</v>
       </c>
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.25">
@@ -18277,10 +18343,10 @@
         <v>0</v>
       </c>
       <c r="B832" s="1" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C832" s="1" t="s">
         <v>1891</v>
-      </c>
-      <c r="C832" s="1" t="s">
-        <v>1892</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.25">
@@ -18288,10 +18354,10 @@
         <v>0</v>
       </c>
       <c r="B833" s="1" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C833" s="1" t="s">
         <v>1893</v>
-      </c>
-      <c r="C833" s="1" t="s">
-        <v>1894</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.25">
@@ -18299,10 +18365,10 @@
         <v>0</v>
       </c>
       <c r="B834" s="1" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C834" s="1" t="s">
         <v>1895</v>
-      </c>
-      <c r="C834" s="1" t="s">
-        <v>1896</v>
       </c>
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.25">
@@ -18310,10 +18376,10 @@
         <v>0</v>
       </c>
       <c r="B835" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C835" s="1" t="s">
         <v>1897</v>
-      </c>
-      <c r="C835" s="1" t="s">
-        <v>1898</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.25">
@@ -18321,10 +18387,10 @@
         <v>0</v>
       </c>
       <c r="B836" s="1" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C836" s="1" t="s">
         <v>1899</v>
-      </c>
-      <c r="C836" s="1" t="s">
-        <v>1900</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.25">
@@ -18332,10 +18398,10 @@
         <v>0</v>
       </c>
       <c r="B837" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="C837" s="1" t="s">
         <v>1901</v>
-      </c>
-      <c r="C837" s="1" t="s">
-        <v>1902</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.25">
@@ -18343,10 +18409,10 @@
         <v>0</v>
       </c>
       <c r="B838" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C838" s="1" t="s">
         <v>1903</v>
-      </c>
-      <c r="C838" s="1" t="s">
-        <v>1904</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.25">
@@ -18354,10 +18420,10 @@
         <v>0</v>
       </c>
       <c r="B839" s="1" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C839" s="1" t="s">
         <v>1905</v>
-      </c>
-      <c r="C839" s="1" t="s">
-        <v>1906</v>
       </c>
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.25">
@@ -18365,7 +18431,7 @@
         <v>0</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="C840" s="1" t="s">
         <v>1118</v>
@@ -18376,10 +18442,10 @@
         <v>0</v>
       </c>
       <c r="B841" s="1" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C841" s="1" t="s">
         <v>1908</v>
-      </c>
-      <c r="C841" s="1" t="s">
-        <v>1909</v>
       </c>
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.25">
@@ -18387,7 +18453,7 @@
         <v>0</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="C842" s="1" t="s">
         <v>1588</v>
@@ -18398,10 +18464,10 @@
         <v>0</v>
       </c>
       <c r="B843" s="1" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C843" s="1" t="s">
         <v>1911</v>
-      </c>
-      <c r="C843" s="1" t="s">
-        <v>1912</v>
       </c>
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.25">
@@ -18409,10 +18475,10 @@
         <v>0</v>
       </c>
       <c r="B844" s="1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C844" s="1" t="s">
         <v>1913</v>
-      </c>
-      <c r="C844" s="1" t="s">
-        <v>1914</v>
       </c>
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.25">
@@ -18420,10 +18486,10 @@
         <v>0</v>
       </c>
       <c r="B845" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="C845" s="1" t="s">
         <v>1915</v>
-      </c>
-      <c r="C845" s="1" t="s">
-        <v>1916</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.25">
@@ -18431,10 +18497,10 @@
         <v>0</v>
       </c>
       <c r="B846" s="1" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C846" s="1" t="s">
         <v>1917</v>
-      </c>
-      <c r="C846" s="1" t="s">
-        <v>1918</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.25">
@@ -18442,10 +18508,10 @@
         <v>0</v>
       </c>
       <c r="B847" s="1" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C847" s="1" t="s">
         <v>1919</v>
-      </c>
-      <c r="C847" s="1" t="s">
-        <v>1920</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.25">
@@ -18453,10 +18519,10 @@
         <v>0</v>
       </c>
       <c r="B848" s="1" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C848" s="1" t="s">
         <v>1921</v>
-      </c>
-      <c r="C848" s="1" t="s">
-        <v>1922</v>
       </c>
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.25">
@@ -18464,10 +18530,10 @@
         <v>0</v>
       </c>
       <c r="B849" s="1" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C849" s="1" t="s">
         <v>1923</v>
-      </c>
-      <c r="C849" s="1" t="s">
-        <v>1924</v>
       </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.25">
@@ -18475,10 +18541,10 @@
         <v>0</v>
       </c>
       <c r="B850" s="1" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C850" s="1" t="s">
         <v>1925</v>
-      </c>
-      <c r="C850" s="1" t="s">
-        <v>1926</v>
       </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.25">
@@ -18486,10 +18552,10 @@
         <v>0</v>
       </c>
       <c r="B851" s="1" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C851" s="1" t="s">
         <v>1927</v>
-      </c>
-      <c r="C851" s="1" t="s">
-        <v>1928</v>
       </c>
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.25">
@@ -18497,10 +18563,10 @@
         <v>0</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.25">
@@ -18508,10 +18574,10 @@
         <v>0</v>
       </c>
       <c r="B853" s="1" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C853" s="1" t="s">
         <v>1930</v>
-      </c>
-      <c r="C853" s="1" t="s">
-        <v>1931</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.25">
@@ -18519,10 +18585,10 @@
         <v>0</v>
       </c>
       <c r="B854" s="1" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C854" s="1" t="s">
         <v>1932</v>
-      </c>
-      <c r="C854" s="1" t="s">
-        <v>1933</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.25">
@@ -18530,10 +18596,10 @@
         <v>0</v>
       </c>
       <c r="B855" s="1" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C855" s="1" t="s">
         <v>1934</v>
-      </c>
-      <c r="C855" s="1" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.25">
@@ -18541,10 +18607,10 @@
         <v>0</v>
       </c>
       <c r="B856" s="1" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C856" s="1" t="s">
         <v>1936</v>
-      </c>
-      <c r="C856" s="1" t="s">
-        <v>1937</v>
       </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.25">
@@ -18552,10 +18618,10 @@
         <v>0</v>
       </c>
       <c r="B857" s="1" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C857" s="1" t="s">
         <v>1938</v>
-      </c>
-      <c r="C857" s="1" t="s">
-        <v>1939</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">
@@ -18563,7 +18629,7 @@
         <v>0</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="C858" s="1" t="s">
         <v>1414</v>
@@ -18574,10 +18640,10 @@
         <v>0</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.25">
@@ -18585,10 +18651,10 @@
         <v>0</v>
       </c>
       <c r="B860" s="1" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C860" s="1" t="s">
         <v>1942</v>
-      </c>
-      <c r="C860" s="1" t="s">
-        <v>1943</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -18596,10 +18662,10 @@
         <v>0</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
@@ -18607,10 +18673,10 @@
         <v>0</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
@@ -18618,10 +18684,10 @@
         <v>0</v>
       </c>
       <c r="B863" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C863" s="1" t="s">
         <v>1946</v>
-      </c>
-      <c r="C863" s="1" t="s">
-        <v>1947</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
@@ -18629,10 +18695,10 @@
         <v>0</v>
       </c>
       <c r="B864" s="1" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C864" s="1" t="s">
         <v>1948</v>
-      </c>
-      <c r="C864" s="1" t="s">
-        <v>1949</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
@@ -18640,10 +18706,10 @@
         <v>0</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
@@ -18651,10 +18717,10 @@
         <v>0</v>
       </c>
       <c r="B866" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C866" s="1" t="s">
         <v>1951</v>
-      </c>
-      <c r="C866" s="1" t="s">
-        <v>1952</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
@@ -18662,10 +18728,10 @@
         <v>0</v>
       </c>
       <c r="B867" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C867" s="1" t="s">
         <v>1953</v>
-      </c>
-      <c r="C867" s="1" t="s">
-        <v>1954</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
@@ -18673,10 +18739,10 @@
         <v>0</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.25">
@@ -18684,10 +18750,10 @@
         <v>0</v>
       </c>
       <c r="B869" s="1" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C869" s="1" t="s">
         <v>1956</v>
-      </c>
-      <c r="C869" s="1" t="s">
-        <v>1957</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.25">
@@ -18695,10 +18761,10 @@
         <v>0</v>
       </c>
       <c r="B870" s="1" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C870" s="1" t="s">
         <v>1958</v>
-      </c>
-      <c r="C870" s="1" t="s">
-        <v>1959</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.25">
@@ -18706,10 +18772,10 @@
         <v>0</v>
       </c>
       <c r="B871" s="1" t="s">
+        <v>1959</v>
+      </c>
+      <c r="C871" s="1" t="s">
         <v>1960</v>
-      </c>
-      <c r="C871" s="1" t="s">
-        <v>1961</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.25">
@@ -18717,10 +18783,10 @@
         <v>0</v>
       </c>
       <c r="B872" s="1" t="s">
+        <v>1961</v>
+      </c>
+      <c r="C872" s="1" t="s">
         <v>1962</v>
-      </c>
-      <c r="C872" s="1" t="s">
-        <v>1963</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.25">
@@ -18728,10 +18794,10 @@
         <v>0</v>
       </c>
       <c r="B873" s="1" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C873" s="1" t="s">
         <v>1964</v>
-      </c>
-      <c r="C873" s="1" t="s">
-        <v>1965</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.25">
@@ -18739,10 +18805,10 @@
         <v>0</v>
       </c>
       <c r="B874" s="1" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C874" s="1" t="s">
         <v>1966</v>
-      </c>
-      <c r="C874" s="1" t="s">
-        <v>1967</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.25">
@@ -18750,7 +18816,7 @@
         <v>0</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>1542</v>
@@ -18761,7 +18827,7 @@
         <v>0</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>1738</v>
@@ -18772,7 +18838,7 @@
         <v>0</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="C877" s="1" t="s">
         <v>1735</v>
@@ -18783,7 +18849,7 @@
         <v>0</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="C878" s="1" t="s">
         <v>1736</v>
@@ -18794,10 +18860,10 @@
         <v>0</v>
       </c>
       <c r="B879" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C879" s="1" t="s">
         <v>1972</v>
-      </c>
-      <c r="C879" s="1" t="s">
-        <v>1973</v>
       </c>
     </row>
     <row r="880" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -18805,10 +18871,10 @@
         <v>0</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.25">
@@ -18816,10 +18882,10 @@
         <v>0</v>
       </c>
       <c r="B881" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C881" s="1" t="s">
         <v>1976</v>
-      </c>
-      <c r="C881" s="1" t="s">
-        <v>1977</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.25">
@@ -18827,7 +18893,7 @@
         <v>0</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="C882" s="1" t="s">
         <v>1440</v>
@@ -18838,10 +18904,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C883" s="1" t="s">
         <v>1979</v>
-      </c>
-      <c r="C883" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
@@ -18849,10 +18915,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -18860,7 +18926,7 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="C885" s="1" t="s">
         <v>1436</v>
@@ -18871,10 +18937,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="C886" s="1" t="s">
         <v>1984</v>
-      </c>
-      <c r="C886" s="1" t="s">
-        <v>1985</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.25">
@@ -18882,10 +18948,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="C887" s="1" t="s">
         <v>1986</v>
-      </c>
-      <c r="C887" s="1" t="s">
-        <v>1987</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.25">
@@ -18893,7 +18959,7 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="C888" s="1" t="s">
         <v>1764</v>
@@ -18904,7 +18970,7 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="C889" s="1" t="s">
         <v>1766</v>
@@ -18915,7 +18981,7 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="C890" s="1" t="s">
         <v>1768</v>
@@ -18926,7 +18992,7 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>1739</v>
@@ -18937,7 +19003,7 @@
         <v>0</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="C892" s="1" t="s">
         <v>1741</v>
@@ -18948,7 +19014,7 @@
         <v>0</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="C893" s="1" t="s">
         <v>1743</v>
@@ -18959,7 +19025,7 @@
         <v>0</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="C894" s="1" t="s">
         <v>1754</v>
@@ -18970,7 +19036,7 @@
         <v>0</v>
       </c>
       <c r="B895" s="1" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="C895" s="1" t="s">
         <v>1756</v>
@@ -18981,7 +19047,7 @@
         <v>0</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="C896" s="1" t="s">
         <v>1758</v>
@@ -18992,10 +19058,10 @@
         <v>0</v>
       </c>
       <c r="B897" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C897" s="1" t="s">
         <v>1997</v>
-      </c>
-      <c r="C897" s="1" t="s">
-        <v>1998</v>
       </c>
     </row>
     <row r="898" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -19003,10 +19069,10 @@
         <v>0</v>
       </c>
       <c r="B898" s="1" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.25">
@@ -19014,10 +19080,10 @@
         <v>0</v>
       </c>
       <c r="B899" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C899" s="1" t="s">
         <v>2000</v>
-      </c>
-      <c r="C899" s="1" t="s">
-        <v>2001</v>
       </c>
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.25">
@@ -19025,10 +19091,10 @@
         <v>0</v>
       </c>
       <c r="B900" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C900" s="1" t="s">
         <v>2003</v>
-      </c>
-      <c r="C900" s="1" t="s">
-        <v>2004</v>
       </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.25">
@@ -19036,10 +19102,10 @@
         <v>0</v>
       </c>
       <c r="B901" s="1" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C901" s="1" t="s">
         <v>2005</v>
-      </c>
-      <c r="C901" s="1" t="s">
-        <v>2006</v>
       </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.25">
@@ -19047,10 +19113,10 @@
         <v>0</v>
       </c>
       <c r="B902" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C902" s="1" t="s">
         <v>2007</v>
-      </c>
-      <c r="C902" s="1" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.25">
@@ -19058,10 +19124,10 @@
         <v>0</v>
       </c>
       <c r="B903" s="1" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C903" s="1" t="s">
         <v>2009</v>
-      </c>
-      <c r="C903" s="1" t="s">
-        <v>2010</v>
       </c>
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.25">
@@ -19069,10 +19135,10 @@
         <v>0</v>
       </c>
       <c r="B904" s="1" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C904" s="1" t="s">
         <v>2011</v>
-      </c>
-      <c r="C904" s="1" t="s">
-        <v>2012</v>
       </c>
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.25">
@@ -19080,10 +19146,10 @@
         <v>0</v>
       </c>
       <c r="B905" s="1" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C905" s="1" t="s">
         <v>2013</v>
-      </c>
-      <c r="C905" s="1" t="s">
-        <v>2014</v>
       </c>
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.25">
@@ -19091,10 +19157,10 @@
         <v>0</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.25">
@@ -19102,10 +19168,10 @@
         <v>0</v>
       </c>
       <c r="B907" s="1" t="s">
+        <v>2015</v>
+      </c>
+      <c r="C907" s="1" t="s">
         <v>2016</v>
-      </c>
-      <c r="C907" s="1" t="s">
-        <v>2017</v>
       </c>
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.25">
@@ -19113,10 +19179,10 @@
         <v>0</v>
       </c>
       <c r="B908" s="1" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C908" s="1" t="s">
         <v>2019</v>
-      </c>
-      <c r="C908" s="1" t="s">
-        <v>2020</v>
       </c>
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.25">
@@ -19124,10 +19190,10 @@
         <v>0</v>
       </c>
       <c r="B909" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C909" s="1" t="s">
         <v>2021</v>
-      </c>
-      <c r="C909" s="1" t="s">
-        <v>2022</v>
       </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.25">
@@ -19135,10 +19201,10 @@
         <v>0</v>
       </c>
       <c r="B910" s="1" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C910" s="1" t="s">
         <v>2023</v>
-      </c>
-      <c r="C910" s="1" t="s">
-        <v>2024</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.25">
@@ -19146,10 +19212,10 @@
         <v>0</v>
       </c>
       <c r="B911" s="1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="C911" s="1" t="s">
         <v>2025</v>
-      </c>
-      <c r="C911" s="1" t="s">
-        <v>2026</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.25">
@@ -19157,10 +19223,10 @@
         <v>0</v>
       </c>
       <c r="B912" s="1" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C912" s="1" t="s">
         <v>2027</v>
-      </c>
-      <c r="C912" s="1" t="s">
-        <v>2028</v>
       </c>
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.25">
@@ -19168,10 +19234,10 @@
         <v>0</v>
       </c>
       <c r="B913" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C913" s="1" t="s">
         <v>2029</v>
-      </c>
-      <c r="C913" s="1" t="s">
-        <v>2030</v>
       </c>
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.25">
@@ -19179,10 +19245,10 @@
         <v>0</v>
       </c>
       <c r="B914" s="1" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C914" s="1" t="s">
         <v>2032</v>
-      </c>
-      <c r="C914" s="1" t="s">
-        <v>2033</v>
       </c>
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.25">
@@ -19190,10 +19256,10 @@
         <v>0</v>
       </c>
       <c r="B915" s="1" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C915" s="1" t="s">
         <v>2034</v>
-      </c>
-      <c r="C915" s="1" t="s">
-        <v>2035</v>
       </c>
     </row>
     <row r="916" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -19201,10 +19267,10 @@
         <v>0</v>
       </c>
       <c r="B916" s="1" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C916" s="1" t="s">
         <v>2036</v>
-      </c>
-      <c r="C916" s="1" t="s">
-        <v>2037</v>
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.25">
@@ -19212,10 +19278,10 @@
         <v>0</v>
       </c>
       <c r="B917" s="1" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C917" s="1" t="s">
         <v>2038</v>
-      </c>
-      <c r="C917" s="1" t="s">
-        <v>2039</v>
       </c>
     </row>
     <row r="918" spans="1:3" x14ac:dyDescent="0.25">
@@ -19223,10 +19289,10 @@
         <v>0</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="C918" s="1" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="919" spans="1:3" x14ac:dyDescent="0.25">
@@ -19234,10 +19300,10 @@
         <v>0</v>
       </c>
       <c r="B919" s="1" t="s">
+        <v>2040</v>
+      </c>
+      <c r="C919" s="1" t="s">
         <v>2041</v>
-      </c>
-      <c r="C919" s="1" t="s">
-        <v>2042</v>
       </c>
     </row>
     <row r="920" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -19245,10 +19311,10 @@
         <v>0</v>
       </c>
       <c r="B920" s="1" t="s">
+        <v>2042</v>
+      </c>
+      <c r="C920" s="1" t="s">
         <v>2043</v>
-      </c>
-      <c r="C920" s="1" t="s">
-        <v>2044</v>
       </c>
     </row>
     <row r="921" spans="1:3" x14ac:dyDescent="0.25">
@@ -19256,10 +19322,10 @@
         <v>0</v>
       </c>
       <c r="B921" s="1" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C921" s="1" t="s">
         <v>2045</v>
-      </c>
-      <c r="C921" s="1" t="s">
-        <v>2046</v>
       </c>
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.25">
@@ -19267,10 +19333,10 @@
         <v>0</v>
       </c>
       <c r="B922" s="1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C922" s="1" t="s">
         <v>2047</v>
-      </c>
-      <c r="C922" s="1" t="s">
-        <v>2048</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.25">
@@ -19278,10 +19344,10 @@
         <v>0</v>
       </c>
       <c r="B923" s="1" t="s">
+        <v>2048</v>
+      </c>
+      <c r="C923" s="1" t="s">
         <v>2049</v>
-      </c>
-      <c r="C923" s="1" t="s">
-        <v>2050</v>
       </c>
     </row>
     <row r="924" spans="1:3" x14ac:dyDescent="0.25">
@@ -19289,10 +19355,10 @@
         <v>0</v>
       </c>
       <c r="B924" s="1" t="s">
+        <v>2050</v>
+      </c>
+      <c r="C924" s="1" t="s">
         <v>2051</v>
-      </c>
-      <c r="C924" s="1" t="s">
-        <v>2052</v>
       </c>
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.25">
@@ -19300,10 +19366,10 @@
         <v>0</v>
       </c>
       <c r="B925" s="1" t="s">
+        <v>2052</v>
+      </c>
+      <c r="C925" s="1" t="s">
         <v>2053</v>
-      </c>
-      <c r="C925" s="1" t="s">
-        <v>2054</v>
       </c>
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.25">
@@ -19311,10 +19377,10 @@
         <v>0</v>
       </c>
       <c r="B926" s="1" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C926" s="1" t="s">
         <v>2055</v>
-      </c>
-      <c r="C926" s="1" t="s">
-        <v>2056</v>
       </c>
     </row>
     <row r="927" spans="1:3" x14ac:dyDescent="0.25">
@@ -19322,10 +19388,10 @@
         <v>0</v>
       </c>
       <c r="B927" s="1" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="928" spans="1:3" x14ac:dyDescent="0.25">
@@ -19333,10 +19399,10 @@
         <v>0</v>
       </c>
       <c r="B928" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.25">
@@ -19344,10 +19410,10 @@
         <v>0</v>
       </c>
       <c r="B929" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="C929" s="1" t="s">
         <v>2059</v>
-      </c>
-      <c r="C929" s="1" t="s">
-        <v>2060</v>
       </c>
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.25">
@@ -19355,10 +19421,10 @@
         <v>0</v>
       </c>
       <c r="B930" s="1" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C930" s="1" t="s">
         <v>2061</v>
-      </c>
-      <c r="C930" s="1" t="s">
-        <v>2062</v>
       </c>
     </row>
     <row r="931" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -19366,10 +19432,10 @@
         <v>0</v>
       </c>
       <c r="B931" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C931" s="1" t="s">
         <v>2063</v>
-      </c>
-      <c r="C931" s="1" t="s">
-        <v>2064</v>
       </c>
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.25">
@@ -19377,10 +19443,10 @@
         <v>0</v>
       </c>
       <c r="B932" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C932" s="1" t="s">
         <v>2065</v>
-      </c>
-      <c r="C932" s="1" t="s">
-        <v>2066</v>
       </c>
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.25">
@@ -19388,10 +19454,10 @@
         <v>0</v>
       </c>
       <c r="B933" s="1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C933" s="1" t="s">
         <v>2067</v>
-      </c>
-      <c r="C933" s="1" t="s">
-        <v>2068</v>
       </c>
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.25">
@@ -19399,10 +19465,10 @@
         <v>0</v>
       </c>
       <c r="B934" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C934" s="1" t="s">
         <v>2069</v>
-      </c>
-      <c r="C934" s="1" t="s">
-        <v>2070</v>
       </c>
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.25">
@@ -19410,10 +19476,10 @@
         <v>0</v>
       </c>
       <c r="B935" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C935" s="1" t="s">
         <v>2071</v>
-      </c>
-      <c r="C935" s="1" t="s">
-        <v>2072</v>
       </c>
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.25">
@@ -19421,10 +19487,10 @@
         <v>0</v>
       </c>
       <c r="B936" s="1" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C936" s="1" t="s">
         <v>2073</v>
-      </c>
-      <c r="C936" s="1" t="s">
-        <v>2074</v>
       </c>
     </row>
     <row r="937" spans="1:3" x14ac:dyDescent="0.25">
@@ -19432,7 +19498,7 @@
         <v>0</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="C937" s="1" t="s">
         <v>177</v>
@@ -19443,10 +19509,10 @@
         <v>0</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.25">
@@ -19454,10 +19520,10 @@
         <v>0</v>
       </c>
       <c r="B939" s="1" t="s">
+        <v>2078</v>
+      </c>
+      <c r="C939" s="1" t="s">
         <v>2079</v>
-      </c>
-      <c r="C939" s="1" t="s">
-        <v>2080</v>
       </c>
     </row>
     <row r="940" spans="1:3" x14ac:dyDescent="0.25">
@@ -19465,10 +19531,10 @@
         <v>0</v>
       </c>
       <c r="B940" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="C940" s="1" t="s">
         <v>2081</v>
-      </c>
-      <c r="C940" s="1" t="s">
-        <v>2082</v>
       </c>
     </row>
     <row r="941" spans="1:3" x14ac:dyDescent="0.25">
@@ -19476,10 +19542,10 @@
         <v>0</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.25">
@@ -19487,10 +19553,10 @@
         <v>0</v>
       </c>
       <c r="B942" s="1" t="s">
+        <v>2084</v>
+      </c>
+      <c r="C942" s="1" t="s">
         <v>2085</v>
-      </c>
-      <c r="C942" s="1" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.25">
@@ -19498,10 +19564,10 @@
         <v>0</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.25">
@@ -19509,10 +19575,10 @@
         <v>0</v>
       </c>
       <c r="B944" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C944" s="1" t="s">
         <v>2088</v>
-      </c>
-      <c r="C944" s="1" t="s">
-        <v>2089</v>
       </c>
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.25">
@@ -19520,10 +19586,10 @@
         <v>0</v>
       </c>
       <c r="B945" s="1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C945" s="1" t="s">
         <v>2090</v>
-      </c>
-      <c r="C945" s="1" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.25">
@@ -19531,10 +19597,10 @@
         <v>0</v>
       </c>
       <c r="B946" s="1" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C946" s="1" t="s">
         <v>2092</v>
-      </c>
-      <c r="C946" s="1" t="s">
-        <v>2093</v>
       </c>
     </row>
     <row r="947" spans="1:3" x14ac:dyDescent="0.25">
@@ -19542,10 +19608,10 @@
         <v>0</v>
       </c>
       <c r="B947" s="1" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C947" s="1" t="s">
         <v>2094</v>
-      </c>
-      <c r="C947" s="1" t="s">
-        <v>2095</v>
       </c>
     </row>
     <row r="948" spans="1:3" x14ac:dyDescent="0.25">
@@ -19553,10 +19619,10 @@
         <v>0</v>
       </c>
       <c r="B948" s="1" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C948" s="1" t="s">
         <v>2096</v>
-      </c>
-      <c r="C948" s="1" t="s">
-        <v>2097</v>
       </c>
     </row>
     <row r="949" spans="1:3" x14ac:dyDescent="0.25">
@@ -19564,10 +19630,10 @@
         <v>0</v>
       </c>
       <c r="B949" s="1" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C949" s="1" t="s">
         <v>2099</v>
-      </c>
-      <c r="C949" s="1" t="s">
-        <v>2100</v>
       </c>
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.25">
@@ -19575,10 +19641,10 @@
         <v>0</v>
       </c>
       <c r="B950" s="1" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C950" s="1" t="s">
         <v>2102</v>
-      </c>
-      <c r="C950" s="1" t="s">
-        <v>2103</v>
       </c>
     </row>
     <row r="951" spans="1:3" x14ac:dyDescent="0.25">
@@ -19586,10 +19652,10 @@
         <v>0</v>
       </c>
       <c r="B951" s="1" t="s">
+        <v>2103</v>
+      </c>
+      <c r="C951" s="1" t="s">
         <v>2104</v>
-      </c>
-      <c r="C951" s="1" t="s">
-        <v>2105</v>
       </c>
     </row>
     <row r="952" spans="1:3" x14ac:dyDescent="0.25">
@@ -19597,7 +19663,7 @@
         <v>0</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="C952" s="1" t="s">
         <v>131</v>
@@ -19608,7 +19674,7 @@
         <v>0</v>
       </c>
       <c r="B953" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="C953" s="1" t="s">
         <v>1775</v>
@@ -19619,10 +19685,10 @@
         <v>0</v>
       </c>
       <c r="B954" s="1" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="955" spans="1:3" x14ac:dyDescent="0.25">
@@ -19630,10 +19696,10 @@
         <v>0</v>
       </c>
       <c r="B955" s="1" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C955" s="1" t="s">
         <v>2109</v>
-      </c>
-      <c r="C955" s="1" t="s">
-        <v>2110</v>
       </c>
     </row>
     <row r="956" spans="1:3" x14ac:dyDescent="0.25">
@@ -19641,10 +19707,10 @@
         <v>0</v>
       </c>
       <c r="B956" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C956" s="1" t="s">
         <v>2111</v>
-      </c>
-      <c r="C956" s="1" t="s">
-        <v>2112</v>
       </c>
     </row>
     <row r="957" spans="1:3" x14ac:dyDescent="0.25">
@@ -19652,10 +19718,10 @@
         <v>0</v>
       </c>
       <c r="B957" s="1" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C957" s="1" t="s">
         <v>2113</v>
-      </c>
-      <c r="C957" s="1" t="s">
-        <v>2114</v>
       </c>
     </row>
     <row r="958" spans="1:3" x14ac:dyDescent="0.25">
@@ -19663,10 +19729,10 @@
         <v>0</v>
       </c>
       <c r="B958" s="1" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="959" spans="1:3" x14ac:dyDescent="0.25">
@@ -19674,10 +19740,10 @@
         <v>0</v>
       </c>
       <c r="B959" s="1" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="960" spans="1:3" x14ac:dyDescent="0.25">
@@ -19685,10 +19751,10 @@
         <v>0</v>
       </c>
       <c r="B960" s="1" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C960" s="1" t="s">
         <v>2117</v>
-      </c>
-      <c r="C960" s="1" t="s">
-        <v>2118</v>
       </c>
     </row>
     <row r="961" spans="1:3" x14ac:dyDescent="0.25">
@@ -19696,10 +19762,10 @@
         <v>0</v>
       </c>
       <c r="B961" s="1" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C961" s="1" t="s">
         <v>2117</v>
-      </c>
-      <c r="C961" s="1" t="s">
-        <v>2118</v>
       </c>
     </row>
     <row r="962" spans="1:3" x14ac:dyDescent="0.25">
@@ -19707,7 +19773,7 @@
         <v>0</v>
       </c>
       <c r="B962" s="1" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="C962" s="1" t="s">
         <v>1118</v>
@@ -19718,7 +19784,7 @@
         <v>0</v>
       </c>
       <c r="B963" s="1" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C963" s="1" t="s">
         <v>1120</v>
@@ -19729,7 +19795,7 @@
         <v>0</v>
       </c>
       <c r="B964" s="1" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="C964" s="1" t="s">
         <v>1119</v>
@@ -19740,7 +19806,7 @@
         <v>0</v>
       </c>
       <c r="B965" s="1" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C965" s="1" t="s">
         <v>1121</v>
@@ -19751,7 +19817,7 @@
         <v>0</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="C966" s="1" t="s">
         <v>1122</v>
@@ -19762,7 +19828,7 @@
         <v>0</v>
       </c>
       <c r="B967" s="1" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C967" s="1" t="s">
         <v>941</v>
@@ -19773,7 +19839,7 @@
         <v>0</v>
       </c>
       <c r="B968" s="1" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="C968" s="1" t="s">
         <v>1431</v>
@@ -19784,10 +19850,10 @@
         <v>0</v>
       </c>
       <c r="B969" s="1" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="970" spans="1:3" x14ac:dyDescent="0.25">
@@ -19795,10 +19861,10 @@
         <v>0</v>
       </c>
       <c r="B970" s="1" t="s">
+        <v>2132</v>
+      </c>
+      <c r="C970" s="1" t="s">
         <v>2133</v>
-      </c>
-      <c r="C970" s="1" t="s">
-        <v>2134</v>
       </c>
     </row>
     <row r="971" spans="1:3" x14ac:dyDescent="0.25">
@@ -19806,10 +19872,10 @@
         <v>0</v>
       </c>
       <c r="B971" s="1" t="s">
+        <v>2134</v>
+      </c>
+      <c r="C971" s="1" t="s">
         <v>2135</v>
-      </c>
-      <c r="C971" s="1" t="s">
-        <v>2136</v>
       </c>
     </row>
     <row r="972" spans="1:3" x14ac:dyDescent="0.25">
@@ -19817,10 +19883,10 @@
         <v>0</v>
       </c>
       <c r="B972" s="1" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="973" spans="1:3" x14ac:dyDescent="0.25">
@@ -19828,10 +19894,10 @@
         <v>0</v>
       </c>
       <c r="B973" s="1" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C973" s="1" t="s">
         <v>2138</v>
-      </c>
-      <c r="C973" s="1" t="s">
-        <v>2139</v>
       </c>
     </row>
     <row r="974" spans="1:3" x14ac:dyDescent="0.25">
@@ -19839,10 +19905,10 @@
         <v>0</v>
       </c>
       <c r="B974" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="C974" s="1" t="s">
         <v>2140</v>
-      </c>
-      <c r="C974" s="1" t="s">
-        <v>2141</v>
       </c>
     </row>
     <row r="975" spans="1:3" x14ac:dyDescent="0.25">
@@ -19850,10 +19916,10 @@
         <v>0</v>
       </c>
       <c r="B975" s="1" t="s">
+        <v>2141</v>
+      </c>
+      <c r="C975" s="1" t="s">
         <v>2142</v>
-      </c>
-      <c r="C975" s="1" t="s">
-        <v>2143</v>
       </c>
     </row>
     <row r="976" spans="1:3" x14ac:dyDescent="0.25">
@@ -19861,10 +19927,10 @@
         <v>0</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="C976" s="1" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="977" spans="1:3" x14ac:dyDescent="0.25">
@@ -19872,10 +19938,10 @@
         <v>0</v>
       </c>
       <c r="B977" s="1" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C977" s="1" t="s">
         <v>2145</v>
-      </c>
-      <c r="C977" s="1" t="s">
-        <v>2146</v>
       </c>
     </row>
     <row r="978" spans="1:3" x14ac:dyDescent="0.25">
@@ -19883,10 +19949,10 @@
         <v>0</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="C978" s="1" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="979" spans="1:3" x14ac:dyDescent="0.25">
@@ -19894,10 +19960,10 @@
         <v>0</v>
       </c>
       <c r="B979" s="1" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="980" spans="1:3" x14ac:dyDescent="0.25">
@@ -19905,10 +19971,164 @@
         <v>0</v>
       </c>
       <c r="B980" s="1" t="s">
+        <v>2148</v>
+      </c>
+      <c r="C980" s="1" t="s">
         <v>2149</v>
       </c>
-      <c r="C980" s="1" t="s">
+    </row>
+    <row r="981" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A981" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B981" s="1" t="s">
         <v>2150</v>
+      </c>
+      <c r="C981" s="1" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="982" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A982" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B982" s="1" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C982" s="1" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="983" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A983" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B983" s="1" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C983" s="1" t="s">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="984" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A984" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B984" s="1" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C984" s="1" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="985" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A985" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B985" s="1" t="s">
+        <v>2154</v>
+      </c>
+      <c r="C985" s="1" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="986" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A986" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B986" s="1" t="s">
+        <v>2157</v>
+      </c>
+      <c r="C986" s="1" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="987" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A987" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B987" s="1" t="s">
+        <v>2158</v>
+      </c>
+      <c r="C987" s="1" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="988" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A988" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B988" s="1" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C988" s="1" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="989" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A989" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B989" s="1" t="s">
+        <v>2160</v>
+      </c>
+      <c r="C989" s="1" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="990" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A990" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B990" s="1" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C990" s="1" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="991" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A991" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B991" s="1" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C991" s="1" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="992" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A992" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B992" s="1" t="s">
+        <v>2167</v>
+      </c>
+      <c r="C992" s="1" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="993" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A993" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B993" s="1" t="s">
+        <v>2168</v>
+      </c>
+      <c r="C993" s="1" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="994" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A994" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B994" s="1" t="s">
+        <v>2170</v>
+      </c>
+      <c r="C994" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -22298,7 +22518,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -25063,16 +25283,16 @@
         <v>814</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>2126</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2127</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>2128</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>2129</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>2130</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>761</v>
@@ -25098,10 +25318,10 @@
         <v>816</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I2" s="20">
         <v>4</v>
@@ -25133,10 +25353,10 @@
         <v>816</v>
       </c>
       <c r="G3" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I3" s="20">
         <v>4</v>
@@ -25168,10 +25388,10 @@
         <v>822</v>
       </c>
       <c r="G4" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I4" s="20">
         <v>4</v>
@@ -25203,10 +25423,10 @@
         <v>822</v>
       </c>
       <c r="G5" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I5" s="20">
         <v>4</v>
@@ -25238,10 +25458,10 @@
         <v>822</v>
       </c>
       <c r="G6" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I6" s="20">
         <v>4</v>
@@ -25273,10 +25493,10 @@
         <v>816</v>
       </c>
       <c r="G7" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I7" s="20">
         <v>4</v>
@@ -25308,10 +25528,10 @@
         <v>816</v>
       </c>
       <c r="G8" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I8" s="20">
         <v>4</v>
@@ -25343,10 +25563,10 @@
         <v>816</v>
       </c>
       <c r="G9" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I9" s="20">
         <v>4</v>
@@ -25378,10 +25598,10 @@
         <v>816</v>
       </c>
       <c r="G10" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I10" s="20">
         <v>4</v>
@@ -25413,10 +25633,10 @@
         <v>816</v>
       </c>
       <c r="G11" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I11" s="20">
         <v>4</v>
@@ -25448,10 +25668,10 @@
         <v>816</v>
       </c>
       <c r="G12" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I12" s="20">
         <v>4</v>
@@ -25483,10 +25703,10 @@
         <v>822</v>
       </c>
       <c r="G13" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I13" s="20">
         <v>4</v>
@@ -25518,10 +25738,10 @@
         <v>822</v>
       </c>
       <c r="G14" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I14" s="20">
         <v>4</v>
@@ -25553,10 +25773,10 @@
         <v>822</v>
       </c>
       <c r="G15" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I15" s="20">
         <v>4</v>
@@ -25588,10 +25808,10 @@
         <v>816</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I16" s="20">
         <v>4</v>
@@ -25623,10 +25843,10 @@
         <v>816</v>
       </c>
       <c r="G17" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I17" s="20">
         <v>4</v>
@@ -25658,10 +25878,10 @@
         <v>816</v>
       </c>
       <c r="G18" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I18" s="20">
         <v>4</v>
@@ -25675,10 +25895,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>1822</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1823</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>816</v>
@@ -25693,10 +25913,10 @@
         <v>822</v>
       </c>
       <c r="G19" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I19" s="20">
         <v>4</v>
@@ -25710,10 +25930,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>816</v>
@@ -25728,10 +25948,10 @@
         <v>816</v>
       </c>
       <c r="G20" s="20" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>2131</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>2132</v>
       </c>
       <c r="I20" s="20">
         <v>4</v>

</xml_diff>

<commit_message>
Common: Added missing button
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAA6C18-34EE-4E80-95ED-B6167246A308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F8EEA8-D350-45BC-AE53-30519E13A98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4189" uniqueCount="2171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4195" uniqueCount="2175">
   <si>
     <t>cs</t>
   </si>
@@ -6754,6 +6754,25 @@
   </si>
   <si>
     <t>lab.build.create.build.button</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.subtitle</t>
+  </si>
+  <si>
+    <t>Vyberte si vatu pro build</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Vatu si můžete vybrat dle doporučení aplikace, kde vychází z typu potahu na atomizéru nebo si ji můžete sami zvolit
+	v seznamu všech vat, které vlastníte.
+&lt;/p&gt;
+&lt;p&gt;
+	Pokud máte už nějaké oblibené buildy ve vybraném atomizéru se stejnou spirálkou, můžete si jej vybrat ze seznamu oblíbených buildů,
+	kdy se použije vata z daného buildu.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -9184,10 +9203,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C994"/>
+  <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A981" workbookViewId="0">
-      <selection activeCell="B988" sqref="B988"/>
+      <selection activeCell="B994" sqref="B994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20129,6 +20148,28 @@
       </c>
       <c r="C994" s="1" t="s">
         <v>448</v>
+      </c>
+    </row>
+    <row r="995" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A995" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B995" s="1" t="s">
+        <v>2171</v>
+      </c>
+      <c r="C995" s="1" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="996" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A996" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B996" s="1" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C996" s="1" t="s">
+        <v>2174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added an ability to deactivate a build
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42961549-CA61-43D6-BFBF-919CB9497DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245B4361-681B-402C-8F94-7991986DB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="2169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="2181">
   <si>
     <t>cs</t>
   </si>
@@ -6755,6 +6755,42 @@
   </si>
   <si>
     <t>Typ drátu</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.disabled.title</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.taste.rating.disabled.subtitle</t>
+  </si>
+  <si>
+    <t>Build za svého života nedostal žádné hodnocení chutí a jelikož již není nadále aktivní, nelze ho hodnotit.</t>
+  </si>
+  <si>
+    <t>Build nemá žádné hodnocení chutí</t>
+  </si>
+  <si>
+    <t>lab.build.disable.button</t>
+  </si>
+  <si>
+    <t>Deaktivovat</t>
+  </si>
+  <si>
+    <t>lab.build.disable.title</t>
+  </si>
+  <si>
+    <t>Deaktivovat vybraný build?</t>
+  </si>
+  <si>
+    <t>lab.build.disable.content</t>
+  </si>
+  <si>
+    <t>Přejete si deaktivovat vybraný build? Veškerá data zůstanou zachována, pouze již nebude možné build nadále hodnotit.</t>
+  </si>
+  <si>
+    <t>lab.build.disable.success</t>
+  </si>
+  <si>
+    <t>Build byl úspěšně archivován.</t>
   </si>
 </sst>
 </file>
@@ -9185,10 +9221,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C997"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="C602" sqref="C602"/>
+    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
+      <selection activeCell="B996" sqref="B996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20163,6 +20199,72 @@
       </c>
       <c r="C997" s="1" t="s">
         <v>2167</v>
+      </c>
+    </row>
+    <row r="998" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A998" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B998" s="1" t="s">
+        <v>2169</v>
+      </c>
+      <c r="C998" s="1" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="999" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A999" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B999" s="1" t="s">
+        <v>2170</v>
+      </c>
+      <c r="C999" s="1" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1000" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1000" s="1" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C1000" s="1" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1001" s="1" t="s">
+        <v>2175</v>
+      </c>
+      <c r="C1001" s="1" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1002" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1002" s="1" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C1002" s="1" t="s">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1003" s="1" t="s">
+        <v>2179</v>
+      </c>
+      <c r="C1003" s="1" t="s">
+        <v>2180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved build wizard
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245B4361-681B-402C-8F94-7991986DB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85100A16-7318-4E3C-8481-291C0E944BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="2181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="2189">
   <si>
     <t>cs</t>
   </si>
@@ -6791,6 +6791,30 @@
   </si>
   <si>
     <t>Build byl úspěšně archivován.</t>
+  </si>
+  <si>
+    <t>lab.build.wire.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte žádné vhodné spirálky</t>
+  </si>
+  <si>
+    <t>lab.build.wire.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte žádné vhodné vaty</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pro vybraný atomizér nemáte žádné vhodné spirálky.</t>
+  </si>
+  <si>
+    <t>Pro vybraný atomizér nemáte žádné vhodné vaty.</t>
   </si>
 </sst>
 </file>
@@ -9221,10 +9245,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1003"/>
+  <dimension ref="A1:C1007"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
-      <selection activeCell="B996" sqref="B996"/>
+      <selection activeCell="B1001" sqref="B1001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20265,6 +20289,50 @@
       </c>
       <c r="C1003" s="1" t="s">
         <v>2180</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1004" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1004" s="1" t="s">
+        <v>2181</v>
+      </c>
+      <c r="C1004" s="1" t="s">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1005" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1005" s="1" t="s">
+        <v>2183</v>
+      </c>
+      <c r="C1005" s="1" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1006" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1006" s="1" t="s">
+        <v>2184</v>
+      </c>
+      <c r="C1006" s="1" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1007" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1007" s="1" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C1007" s="1" t="s">
+        <v>2188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added initial migration stuff support
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85100A16-7318-4E3C-8481-291C0E944BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57671DD9-F6C9-49CF-BEA8-0E92B7433BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="2189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4260" uniqueCount="2199">
   <si>
     <t>cs</t>
   </si>
@@ -6815,6 +6815,36 @@
   </si>
   <si>
     <t>Pro vybraný atomizér nemáte žádné vhodné vaty.</t>
+  </si>
+  <si>
+    <t>isHybrid</t>
+  </si>
+  <si>
+    <t>lab.build.watt.tooltip</t>
+  </si>
+  <si>
+    <t>Výchozí výkon tohoto buildu; tento údaj je užitečný v případě použití na bypass nebo na mechanice. Počítá s 3.7V pracovního napětí článku.</t>
+  </si>
+  <si>
+    <t>lab.build.amps.tooltip</t>
+  </si>
+  <si>
+    <t>Odběr tohoto buildu; tento údaj je užitečný při použití na bypass nebo na mechanice. Počítá s 3.7V pracovního napětí článku.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.squonk</t>
+  </si>
+  <si>
+    <t>Squonkovací pin?</t>
+  </si>
+  <si>
+    <t>shared.atomizer.view.isHybrid</t>
+  </si>
+  <si>
+    <t>Možno na hybridní mechaniku?</t>
+  </si>
+  <si>
+    <t>Vlastnosti</t>
   </si>
 </sst>
 </file>
@@ -9245,10 +9275,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1007"/>
+  <dimension ref="A1:C1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A986" workbookViewId="0">
-      <selection activeCell="B1001" sqref="B1001"/>
+    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
+      <selection activeCell="C804" sqref="C804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18099,7 +18129,7 @@
         <v>1833</v>
       </c>
       <c r="C804" s="1" t="s">
-        <v>1797</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.25">
@@ -20333,6 +20363,50 @@
       </c>
       <c r="C1007" s="1" t="s">
         <v>2188</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1008" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1008" s="1" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C1008" s="1" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1009" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1009" s="1" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C1009" s="1" t="s">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1010" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1010" s="1" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C1010" s="1" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1011" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1011" s="1" t="s">
+        <v>2196</v>
+      </c>
+      <c r="C1011" s="1" t="s">
+        <v>2197</v>
       </c>
     </row>
   </sheetData>
@@ -25450,10 +25524,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25465,9 +25539,10 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>658</v>
       </c>
@@ -25499,10 +25574,13 @@
         <v>2119</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>2189</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>661</v>
       </c>
@@ -25533,11 +25611,14 @@
       <c r="J2">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L2" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>725</v>
       </c>
@@ -25568,11 +25649,14 @@
       <c r="J3">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L3" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>751</v>
       </c>
@@ -25603,11 +25687,14 @@
       <c r="J4">
         <v>9</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L4" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>672</v>
       </c>
@@ -25638,11 +25725,14 @@
       <c r="J5">
         <v>9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L5" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>732</v>
       </c>
@@ -25673,11 +25763,14 @@
       <c r="J6">
         <v>9</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L6" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>748</v>
       </c>
@@ -25708,11 +25801,14 @@
       <c r="J7">
         <v>9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L7" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>666</v>
       </c>
@@ -25743,11 +25839,14 @@
       <c r="J8">
         <v>9</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L8" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>700</v>
       </c>
@@ -25778,11 +25877,14 @@
       <c r="J9">
         <v>9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L9" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>748</v>
       </c>
@@ -25813,11 +25915,14 @@
       <c r="J10">
         <v>9</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L10" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>748</v>
       </c>
@@ -25848,11 +25953,14 @@
       <c r="J11">
         <v>9</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L11" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>753</v>
       </c>
@@ -25883,11 +25991,14 @@
       <c r="J12">
         <v>9</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L12" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>723</v>
       </c>
@@ -25918,11 +26029,14 @@
       <c r="J13">
         <v>9</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L13" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>685</v>
       </c>
@@ -25953,11 +26067,14 @@
       <c r="J14">
         <v>9</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L14" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>700</v>
       </c>
@@ -25988,11 +26105,14 @@
       <c r="J15">
         <v>9</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L15" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>746</v>
       </c>
@@ -26023,11 +26143,14 @@
       <c r="J16">
         <v>9</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L16" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>748</v>
       </c>
@@ -26058,11 +26181,14 @@
       <c r="J17">
         <v>9</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L17" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>693</v>
       </c>
@@ -26093,11 +26219,14 @@
       <c r="J18">
         <v>9</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L18" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1811</v>
       </c>
@@ -26128,11 +26257,14 @@
       <c r="J19">
         <v>9</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L19" s="1">
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1811</v>
       </c>
@@ -26163,7 +26295,10 @@
       <c r="J20">
         <v>9</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L20" s="1">
         <v>325</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Prepared initial production release...?
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C8FE08-6BE2-4A3A-919F-5B1A1AE99816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8132E4AC-2298-4F77-9218-57CF23AD5147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="885" windowWidth="33825" windowHeight="18495" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4260" uniqueCount="2199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4296" uniqueCount="2219">
   <si>
     <t>cs</t>
   </si>
@@ -6845,6 +6845,66 @@
   </si>
   <si>
     <t>Vlastnosti</t>
+  </si>
+  <si>
+    <t>Doporučené liquidy - nehodnocené</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.recommended.unrated.tab</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.recommended.rated.tab</t>
+  </si>
+  <si>
+    <t>Doporučené liquidy - hodnocené</t>
+  </si>
+  <si>
+    <t>lab.liquid.rating.list.rated.title</t>
+  </si>
+  <si>
+    <t>Všechny liquidy máte ohodnocené</t>
+  </si>
+  <si>
+    <t>lab.liquid.rating.list.rated.subtitle</t>
+  </si>
+  <si>
+    <t>Veškeré liquidy vhodné do vybraného buildu máte již ohodnocené.</t>
+  </si>
+  <si>
+    <t>lab.liquid.unrated.list.unrated.title</t>
+  </si>
+  <si>
+    <t>Zatím nemáte žádné ohodnocené liquidy</t>
+  </si>
+  <si>
+    <t>lab.liquid.unrated.list.unrated.subtitle</t>
+  </si>
+  <si>
+    <t>Až ohodnotíte nějaký liquid, objeví se zde.</t>
+  </si>
+  <si>
+    <t>lab.liquid.rating.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte žádné liquidy</t>
+  </si>
+  <si>
+    <t>lab.liquid.rating.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Zde není co hodnotit, poněvadž nemáte namíchané žádné liquidy.</t>
+  </si>
+  <si>
+    <t>lab.liquid.unrated.list.empty.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.unrated.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.liquid.all.list.empty.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.all.list.empty.subtitle</t>
   </si>
 </sst>
 </file>
@@ -9275,10 +9335,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1011"/>
+  <dimension ref="A1:C1023"/>
   <sheetViews>
-    <sheetView topLeftCell="A792" workbookViewId="0">
-      <selection activeCell="B803" sqref="B803"/>
+    <sheetView tabSelected="1" topLeftCell="A996" workbookViewId="0">
+      <selection activeCell="B1014" sqref="B1014"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20407,6 +20467,138 @@
       </c>
       <c r="C1011" s="1" t="s">
         <v>2197</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1012" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1012" s="1" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C1012" s="1" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1013" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1013" s="1" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C1013" s="1" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1014" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1014" s="1" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C1014" s="1" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1015" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1015" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C1015" s="1" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1016" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1016" s="1" t="s">
+        <v>2207</v>
+      </c>
+      <c r="C1016" s="1" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1017" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1017" s="1" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C1017" s="1" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1018" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1018" s="1" t="s">
+        <v>2211</v>
+      </c>
+      <c r="C1018" s="1" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1019" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1019" s="1" t="s">
+        <v>2213</v>
+      </c>
+      <c r="C1019" s="1" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1020" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1020" s="1" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C1020" s="1" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1021" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1021" s="1" t="s">
+        <v>2216</v>
+      </c>
+      <c r="C1021" s="1" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1022" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1022" s="1" t="s">
+        <v>2217</v>
+      </c>
+      <c r="C1022" s="1" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1023" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1023" s="1" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C1023" s="1" t="s">
+        <v>2214</v>
       </c>
     </row>
   </sheetData>
@@ -22643,8 +22835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Preparing experiment with zero costs
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E22F0C-AC86-8C45-9646-364C7275BC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C3C230-13A0-BE44-90D6-B142C0829467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4316" uniqueCount="2230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="2241">
   <si>
     <t>cs</t>
   </si>
@@ -6934,10 +6934,43 @@
     <t>[{count: 1, fiber: Kanthal A1 28GA}]</t>
   </si>
   <si>
-    <t>lab.build.coil.create.tab</t>
-  </si>
-  <si>
     <t>Nová spirálka</t>
+  </si>
+  <si>
+    <t>lab.coil.create.button</t>
+  </si>
+  <si>
+    <t>lab.coil.create.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.button</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.wrapsMin.label</t>
+  </si>
+  <si>
+    <t>Minimální počet otoček</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.wrapsMax.label</t>
+  </si>
+  <si>
+    <t>Maximální počet otoček</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.wrapsMin.label.tooltip</t>
+  </si>
+  <si>
+    <t>Minimální rozumný počet otoček, které je možné do atomizéru dát. Jedná se o subjektivní optimální hodnotu, která je dále použita pro výběr spirálek.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.wrapsMax.label.tooltip</t>
+  </si>
+  <si>
+    <t>Maximální rozumný počet otoček, které je možné do atomizéru osadit. Jedná se o subjektivní optimální hodnotu, která je dále použita pro výběr spirálek.</t>
   </si>
 </sst>
 </file>
@@ -9390,10 +9423,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1026"/>
+  <dimension ref="A1:C1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1004" workbookViewId="0">
-      <selection activeCell="B1016" sqref="B1016"/>
+    <sheetView tabSelected="1" topLeftCell="A1010" workbookViewId="0">
+      <selection activeCell="B1024" sqref="B1024"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20683,10 +20716,87 @@
         <v>0</v>
       </c>
       <c r="B1026" s="1" t="s">
+        <v>2229</v>
+      </c>
+      <c r="C1026" s="1" t="s">
         <v>2228</v>
       </c>
-      <c r="C1026" s="1" t="s">
-        <v>2229</v>
+    </row>
+    <row r="1027" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1027" s="1" t="s">
+        <v>2230</v>
+      </c>
+      <c r="C1027" s="1" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1028" s="1" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C1028" s="1" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1029" s="1" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C1029" s="1" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1030" s="1" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C1030" s="1" t="s">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1031" s="1" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C1031" s="1" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1032" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1032" s="1" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C1032" s="1" t="s">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1033" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1033" s="1" t="s">
+        <v>2239</v>
+      </c>
+      <c r="C1033" s="1" t="s">
+        <v>2240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So how to add atomizer into inventory?
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C3C230-13A0-BE44-90D6-B142C0829467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26964A1-4196-BB44-A2FE-C1C3BA6881FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="2241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4340" uniqueCount="2242">
   <si>
     <t>cs</t>
   </si>
@@ -6971,6 +6971,9 @@
   </si>
   <si>
     <t>Maximální rozumný počet otoček, které je možné do atomizéru osadit. Jedná se o subjektivní optimální hodnotu, která je dále použita pro výběr spirálek.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.isHybrid.label</t>
   </si>
 </sst>
 </file>
@@ -9423,10 +9426,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1033"/>
+  <dimension ref="A1:C1034"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1010" workbookViewId="0">
-      <selection activeCell="B1024" sqref="B1024"/>
+      <selection activeCell="B1035" sqref="B1035"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20797,6 +20800,17 @@
       </c>
       <c r="C1033" s="1" t="s">
         <v>2240</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1034" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1034" s="1" t="s">
+        <v>2241</v>
+      </c>
+      <c r="C1034" s="1" t="s">
+        <v>2197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved wire form
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAC7F9-B5FA-404A-8028-C6B614B714F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7076BD-BCB4-4F75-B35E-D569A3799BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="1455" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4385" uniqueCount="2268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="2286">
   <si>
     <t>cs</t>
   </si>
@@ -7051,7 +7051,61 @@
     <t>shared.wire.create.name.label.tooltip</t>
   </si>
   <si>
-    <t>Uveďte prosím jméno drátu, standardně materiál (např. Kanthal A1 28Ga) a velikost v GA.</t>
+    <t>shared.wire.create.fiber.add.button</t>
+  </si>
+  <si>
+    <t>Přidat vlákno</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiber.fiberId</t>
+  </si>
+  <si>
+    <t>Typ vlákna</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiber.count</t>
+  </si>
+  <si>
+    <t>Počet vláken</t>
+  </si>
+  <si>
+    <t>shared.wire.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Uveďte prosím jméno drátu.</t>
+  </si>
+  <si>
+    <t>shared.wire.create.vendorId.label.required</t>
+  </si>
+  <si>
+    <t>Výrobce drátu je povinný.</t>
+  </si>
+  <si>
+    <t>shared.wire.create.cost.label.required</t>
+  </si>
+  <si>
+    <t>Cena drátu na tržišti je povinná.</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiber.count.required</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiber.fiberId.required</t>
+  </si>
+  <si>
+    <t>Počet vláken je povinný.</t>
+  </si>
+  <si>
+    <t>Typ vlákna je povinný.</t>
+  </si>
+  <si>
+    <t>lab.coil.create.wireId.label.required</t>
+  </si>
+  <si>
+    <t>Drát spirálky je povinný.</t>
+  </si>
+  <si>
+    <t>Jméno drátu je dobrovolná položka, jelikož se dopočítává ze zadaných parametrů; pokud se jedná o nějaký speciál (např. green mamba), můžete toto jméno uvést.</t>
   </si>
 </sst>
 </file>
@@ -9504,10 +9558,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1049"/>
+  <dimension ref="A1:C1058"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1010" workbookViewId="0">
-      <selection activeCell="B1034" sqref="B1034"/>
+    <sheetView tabSelected="1" topLeftCell="A1028" workbookViewId="0">
+      <selection activeCell="C1049" sqref="C1049"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21053,7 +21107,106 @@
         <v>2266</v>
       </c>
       <c r="C1049" s="1" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1050" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1050" s="1" t="s">
         <v>2267</v>
+      </c>
+      <c r="C1050" s="1" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1051" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1051" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C1051" s="1" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1052" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1052" s="1" t="s">
+        <v>2271</v>
+      </c>
+      <c r="C1052" s="1" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1053" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1053" s="1" t="s">
+        <v>2273</v>
+      </c>
+      <c r="C1053" s="1" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1054" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1054" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="C1054" s="1" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1055" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1055" s="1" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C1055" s="1" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1056" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1056" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C1056" s="1" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1057" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1057" s="1" t="s">
+        <v>2280</v>
+      </c>
+      <c r="C1057" s="1" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1058" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1058" s="1" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C1058" s="1" t="s">
+        <v>2284</v>
       </c>
     </row>
   </sheetData>
@@ -21120,7 +21273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F7C88A-203F-48DC-ACBE-CE6221C44C48}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Common: Initial wire stuff looks promising
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7076BD-BCB4-4F75-B35E-D569A3799BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D546A0A-2404-4D04-9B47-41FF2184BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="2286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4421" uniqueCount="2291">
   <si>
     <t>cs</t>
   </si>
@@ -7106,6 +7106,21 @@
   </si>
   <si>
     <t>Jméno drátu je dobrovolná položka, jelikož se dopočítává ze zadaných parametrů; pokud se jedná o nějaký speciál (např. green mamba), můžete toto jméno uvést.</t>
+  </si>
+  <si>
+    <t>Pokud máte informaci o vhodném typu potahu pro tento drát, uveďte jej prosím. Jinak můžete použít odhad, případně ponechte prázdné.</t>
+  </si>
+  <si>
+    <t>shared.wire.create.draws.label</t>
+  </si>
+  <si>
+    <t>shared.wire.create.draws.label.tooltip</t>
+  </si>
+  <si>
+    <t>shared.wire.create.success</t>
+  </si>
+  <si>
+    <t>Drát byl úspěšně vytvořen.</t>
   </si>
 </sst>
 </file>
@@ -9558,10 +9573,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1058"/>
+  <dimension ref="A1:C1061"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1028" workbookViewId="0">
-      <selection activeCell="C1049" sqref="C1049"/>
+      <selection activeCell="B1057" sqref="B1057"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21207,6 +21222,39 @@
       </c>
       <c r="C1058" s="1" t="s">
         <v>2284</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1059" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1059" s="1" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C1059" s="1" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1060" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1060" s="1" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C1060" s="1" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1061" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1061" s="1" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C1061" s="1" t="s">
+        <v>2290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some boring stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D546A0A-2404-4D04-9B47-41FF2184BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A7515-DD09-47D2-98F5-B176D286D952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4421" uniqueCount="2291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4424" uniqueCount="2293">
   <si>
     <t>cs</t>
   </si>
@@ -7121,6 +7121,12 @@
   </si>
   <si>
     <t>Drát byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>error.A request failed with Internal Server Error.</t>
+  </si>
+  <si>
+    <t>Hopla, stala se škaredá chyba, která nejspíš někoho vytáhne z postele. Omlouváme se za potíže.</t>
   </si>
 </sst>
 </file>
@@ -9573,10 +9579,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1061"/>
+  <dimension ref="A1:C1062"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1028" workbookViewId="0">
-      <selection activeCell="B1057" sqref="B1057"/>
+      <selection activeCell="B1047" sqref="B1047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21255,6 +21261,17 @@
       </c>
       <c r="C1061" s="1" t="s">
         <v>2290</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1062" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1062" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="C1062" s="1" t="s">
+        <v>2292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Wire and coil creation somehow works; still needs more work
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A7515-DD09-47D2-98F5-B176D286D952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEDC489-861D-43AA-BD65-640048CA2DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4424" uniqueCount="2293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4433" uniqueCount="2299">
   <si>
     <t>cs</t>
   </si>
@@ -7127,6 +7127,24 @@
   </si>
   <si>
     <t>Hopla, stala se škaredá chyba, která nejspíš někoho vytáhne z postele. Omlouváme se za potíže.</t>
+  </si>
+  <si>
+    <t>lab.coil.create.success</t>
+  </si>
+  <si>
+    <t>Spirálka byla úspěšně vytvořena.</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiberId.label</t>
+  </si>
+  <si>
+    <t>Vyberte typ vlákna</t>
+  </si>
+  <si>
+    <t>shared.wire.create.fiberId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vlákno je pracovní název pro dílčí drátek; pro jednoduché dráty je volba snadná, nicméně u komplikovaných drátů je možné naklikat celkové složení takového drátu. Pokud vyberete dílčí složení komplikovaného drátu, tato hodnota se vymaže a nebude použita.</t>
   </si>
 </sst>
 </file>
@@ -9579,10 +9597,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1062"/>
+  <dimension ref="A1:C1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1028" workbookViewId="0">
-      <selection activeCell="B1047" sqref="B1047"/>
+    <sheetView tabSelected="1" topLeftCell="A1037" workbookViewId="0">
+      <selection activeCell="B1055" sqref="B1055"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21272,6 +21290,39 @@
       </c>
       <c r="C1062" s="1" t="s">
         <v>2292</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1063" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1063" s="1" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C1063" s="1" t="s">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1064" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1064" s="1" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C1064" s="1" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1065" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1065" s="1" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C1065" s="1" t="s">
+        <v>2298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Wire, fiber and co is possible to add
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEDC489-861D-43AA-BD65-640048CA2DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0F2D8-7D95-47B6-8B20-E37305AF41E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4433" uniqueCount="2299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4469" uniqueCount="2321">
   <si>
     <t>cs</t>
   </si>
@@ -7145,6 +7145,72 @@
   </si>
   <si>
     <t>Vlákno je pracovní název pro dílčí drátek; pro jednoduché dráty je volba snadná, nicméně u komplikovaných drátů je možné naklikat celkové složení takového drátu. Pokud vyberete dílčí složení komplikovaného drátu, tato hodnota se vymaže a nebude použita.</t>
+  </si>
+  <si>
+    <t>error.There must be at least one fiber!</t>
+  </si>
+  <si>
+    <t>Přidejte alespoň jedno vlákno.</t>
+  </si>
+  <si>
+    <t>lab.fiber.create.button</t>
+  </si>
+  <si>
+    <t>Nové vlákno</t>
+  </si>
+  <si>
+    <t>lab.fiber.create.title</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.ga.label</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.mm.label</t>
+  </si>
+  <si>
+    <t>Milimetry</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.materialId.label</t>
+  </si>
+  <si>
+    <t>Materiál</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.create</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.ga.label.required</t>
+  </si>
+  <si>
+    <t>Tlousťka drátu je povinná.</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.mm.label.required</t>
+  </si>
+  <si>
+    <t>Tloušťka drátu v milimetrech je povinná.</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.materialId.label.required</t>
+  </si>
+  <si>
+    <t>Materiál drátu je povinný.</t>
+  </si>
+  <si>
+    <t>shared.fiber.mm.hint</t>
+  </si>
+  <si>
+    <t>Milimetry odhadnuté aplikací je třeba brát s nadhledem a případně ověřit, zda skutečně sedí.</t>
+  </si>
+  <si>
+    <t>shared.fiber.create.success</t>
+  </si>
+  <si>
+    <t>Vlákno bylo úspěšně vytvořeno.</t>
   </si>
 </sst>
 </file>
@@ -9597,10 +9663,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1065"/>
+  <dimension ref="A1:C1077"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1037" workbookViewId="0">
-      <selection activeCell="B1055" sqref="B1055"/>
+    <sheetView tabSelected="1" topLeftCell="A1061" workbookViewId="0">
+      <selection activeCell="B1075" sqref="B1075"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21323,6 +21389,138 @@
       </c>
       <c r="C1065" s="1" t="s">
         <v>2298</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1066" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1066" s="1" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C1066" s="1" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1067" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1067" s="1" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C1067" s="1" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1068" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1068" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C1068" s="1" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1069" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1069" s="1" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C1069" s="1" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1070" s="1" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C1070" s="1" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1071" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1071" s="1" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C1071" s="1" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1072" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1072" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C1072" s="1" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1073" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1073" s="1" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C1073" s="1" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1074" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1074" s="1" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C1074" s="1" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1075" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1075" s="1" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C1075" s="1" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1076" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1076" s="1" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1076" s="1" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1077" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1077" s="1" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1077" s="1" t="s">
+        <v>2320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some little improvements
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0F2D8-7D95-47B6-8B20-E37305AF41E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB67A09-CFDA-4009-B8D5-7B894D4152FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4469" uniqueCount="2321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4481" uniqueCount="2329">
   <si>
     <t>cs</t>
   </si>
@@ -7211,6 +7211,30 @@
   </si>
   <si>
     <t>Vlákno bylo úspěšně vytvořeno.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Vyplňte prosím název atomizéru.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.typeId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte prosím typ atomizéru.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.vendorId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte prosím výrobce atomizéru.</t>
+  </si>
+  <si>
+    <t>shared.atomizer.create.cost.label.required</t>
+  </si>
+  <si>
+    <t>Udejte prosím výchozí cenu atomizéru.</t>
   </si>
 </sst>
 </file>
@@ -9663,10 +9687,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1077"/>
+  <dimension ref="A1:C1081"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1061" workbookViewId="0">
-      <selection activeCell="B1075" sqref="B1075"/>
+      <selection activeCell="C1073" sqref="C1073"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21521,6 +21545,50 @@
       </c>
       <c r="C1077" s="1" t="s">
         <v>2320</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1078" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1078" s="1" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1078" s="1" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1079" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1079" s="1" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1079" s="1" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1080" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1080" s="1" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C1080" s="1" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1081" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1081" s="1" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C1081" s="1" t="s">
+        <v>2328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some little improvements III
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB67A09-CFDA-4009-B8D5-7B894D4152FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB03CDC7-C91B-497D-95DA-6D5119C2AA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4481" uniqueCount="2329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="2332">
   <si>
     <t>cs</t>
   </si>
@@ -7235,6 +7235,15 @@
   </si>
   <si>
     <t>Udejte prosím výchozí cenu atomizéru.</t>
+  </si>
+  <si>
+    <t>shared.wire.no-fibers</t>
+  </si>
+  <si>
+    <t>(bez zadaných vláken)</t>
+  </si>
+  <si>
+    <t>lab.build.liquid.button</t>
   </si>
 </sst>
 </file>
@@ -9687,10 +9696,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1081"/>
+  <dimension ref="A1:C1083"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1061" workbookViewId="0">
-      <selection activeCell="C1073" sqref="C1073"/>
+      <selection activeCell="B1074" sqref="B1074"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21589,6 +21598,28 @@
       </c>
       <c r="C1081" s="1" t="s">
         <v>2328</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1082" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1082" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="C1082" s="1" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1083" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1083" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="C1083" s="1" t="s">
+        <v>1861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite interesting liquid calculator
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB03CDC7-C91B-497D-95DA-6D5119C2AA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB54CFD1-B7B7-4604-8758-7D34C29A7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="1500" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="1935" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="2332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4745" uniqueCount="2478">
   <si>
     <t>cs</t>
   </si>
@@ -7244,6 +7244,444 @@
   </si>
   <si>
     <t>lab.build.liquid.button</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aromaId.label</t>
+  </si>
+  <si>
+    <t>Vyberte prosím aroma</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.aromaId.label.required</t>
+  </si>
+  <si>
+    <t>Aroma je povinné.</t>
+  </si>
+  <si>
+    <t>lab.aroma.create.button</t>
+  </si>
+  <si>
+    <t>lab.aroma.create.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.boosterId.label</t>
+  </si>
+  <si>
+    <t>Vyberte booster</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.baseId.label</t>
+  </si>
+  <si>
+    <t>Vyberte bázi</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.boosterId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte booster nebo bázi.</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.baseId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte bázi nebo booster.</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.nicotine.label</t>
+  </si>
+  <si>
+    <t>lab.booster.create.button</t>
+  </si>
+  <si>
+    <t>Nový booster</t>
+  </si>
+  <si>
+    <t>lab.booster.create.title</t>
+  </si>
+  <si>
+    <t>shared.booster.create.name.label</t>
+  </si>
+  <si>
+    <t>Název boosteru</t>
+  </si>
+  <si>
+    <t>shared.booster.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím název boosteru co nejpřesněji, jak jej uvádí výrobce.</t>
+  </si>
+  <si>
+    <t>shared.booster.create.code.label</t>
+  </si>
+  <si>
+    <t>Kód boosteru</t>
+  </si>
+  <si>
+    <t>shared.booster.create.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tento kód je dobrovolný a využívá se případně pro import a export.</t>
+  </si>
+  <si>
+    <t>shared.booster.create.vendorId.label</t>
+  </si>
+  <si>
+    <t>Vyberte výrobce boosteru</t>
+  </si>
+  <si>
+    <t>shared.booster.create.cost.label</t>
+  </si>
+  <si>
+    <t>Cena boosteru</t>
+  </si>
+  <si>
+    <t>shared.booster.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím cenu boosteru, za jakou bude dostupný na tržišti.</t>
+  </si>
+  <si>
+    <t>shared.booster.create.vgpg.label</t>
+  </si>
+  <si>
+    <t>Poměr VG boosteru</t>
+  </si>
+  <si>
+    <t>shared.booster.create.vgpg.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím množství VG v boosteru (procento).</t>
+  </si>
+  <si>
+    <t>shared.booster.create.volume.label</t>
+  </si>
+  <si>
+    <t>shared.booster.create.volume.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte prosím objem lahvičky boosteru.</t>
+  </si>
+  <si>
+    <t>shared.booster.create.create</t>
+  </si>
+  <si>
+    <t>shared.booster.create.success</t>
+  </si>
+  <si>
+    <t>Booster {{name}} úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>shared.booster.create.nicotine.label</t>
+  </si>
+  <si>
+    <t>shared.booster.create.nicotine.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte obsah nikotinu v mg/ml.</t>
+  </si>
+  <si>
+    <t>lab.base.create.button</t>
+  </si>
+  <si>
+    <t>Nová báze</t>
+  </si>
+  <si>
+    <t>lab.base.create.title</t>
+  </si>
+  <si>
+    <t>shared.base.create.name.label</t>
+  </si>
+  <si>
+    <t>Zadejte název báze</t>
+  </si>
+  <si>
+    <t>shared.base.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte jméno báze co nejpřesněji, jak jej uvádí výrobce.</t>
+  </si>
+  <si>
+    <t>shared.base.create.code.label</t>
+  </si>
+  <si>
+    <t>Kód báze</t>
+  </si>
+  <si>
+    <t>shared.base.create.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Kód je dobrovolná hodnota určená hlavně pro importy/exporty a jednoznačenému rozeznání dané báze.</t>
+  </si>
+  <si>
+    <t>shared.base.create.vendorId.label</t>
+  </si>
+  <si>
+    <t>shared.base.create.cost.label</t>
+  </si>
+  <si>
+    <t>Cena báze</t>
+  </si>
+  <si>
+    <t>shared.base.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte cenu báze, za kterou bude dostupná na tržišti.</t>
+  </si>
+  <si>
+    <t>shared.base.create.vgpg.label</t>
+  </si>
+  <si>
+    <t>shared.base.create.vgpg.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zadejte množství VG v procentech.</t>
+  </si>
+  <si>
+    <t>shared.base.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit bázi</t>
+  </si>
+  <si>
+    <t>Báze {{name}} úspěšně vytvořena.</t>
+  </si>
+  <si>
+    <t>shared.base.create.success</t>
+  </si>
+  <si>
+    <t>shared.base.create.vendorId.label.required</t>
+  </si>
+  <si>
+    <t>Výrobce báze je povinný.</t>
+  </si>
+  <si>
+    <t>shared.base.create.cost.label.required</t>
+  </si>
+  <si>
+    <t>Cena báze je povinná.</t>
+  </si>
+  <si>
+    <t>shared.base.create.vgpg.label.required</t>
+  </si>
+  <si>
+    <t>Poměr VG báze je povinný.</t>
+  </si>
+  <si>
+    <t>error.Invalid mixture: MORE</t>
+  </si>
+  <si>
+    <t>error.Invalid mixture: LESS</t>
+  </si>
+  <si>
+    <t>Tento liquid není možné namíchat, poněvadž některá ze surovin nedostačuje na doplnění lahvičky s aromatem.</t>
+  </si>
+  <si>
+    <t>Tento liquid není možné namíchat, poněvadž některá ze surovin překračuje dostupný objem lahvičky s aromatem.</t>
+  </si>
+  <si>
+    <t>lab.mixture.search.tab</t>
+  </si>
+  <si>
+    <t>lab.mixture.calculator.tab</t>
+  </si>
+  <si>
+    <t>Kalkukačka</t>
+  </si>
+  <si>
+    <t>lab.mixture.calculator.tab.title</t>
+  </si>
+  <si>
+    <t>Kalkulačka mixů</t>
+  </si>
+  <si>
+    <t>lab.mixture.calculator.tab.subtitle</t>
+  </si>
+  <si>
+    <t>Jednoduchý nástroj, který vám umožní ze zadaných údajů spočítat poměry případného mixu.</t>
+  </si>
+  <si>
+    <t>Spočítat</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.content.label</t>
+  </si>
+  <si>
+    <t>Obsah aromatu v lahvičce</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.volume.label</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.vgpg.label</t>
+  </si>
+  <si>
+    <t>Poměr VG aromatu</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.nicotine.label</t>
+  </si>
+  <si>
+    <t>Požadované množství nikotinu</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.vgpg.label</t>
+  </si>
+  <si>
+    <t>Poměr VG báze</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.nicotine.label</t>
+  </si>
+  <si>
+    <t>Množství nikotinu v boosteru</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.volume.label</t>
+  </si>
+  <si>
+    <t>Objem lahvičky boosteru</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.vgpg.label</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.vgpg.label.required</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.volume.label.required</t>
+  </si>
+  <si>
+    <t>Objem lahvičky boosteru je povinný</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.calculate</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.success</t>
+  </si>
+  <si>
+    <t>Tento liquid je možné namíchat.</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.title</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.title</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.title</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.vgpg</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.vgpg</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.vgpg</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.volume</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.content</t>
+  </si>
+  <si>
+    <t>Objem aromatu</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.available</t>
+  </si>
+  <si>
+    <t>Dostupný objem</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.volume</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.info</t>
+  </si>
+  <si>
+    <t>Výsledný nikotin</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.content</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.nicotine.label.required</t>
+  </si>
+  <si>
+    <t>Množství nikotinu v boosteru je povinný.</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.result.vgpgToMl</t>
+  </si>
+  <si>
+    <t>Poměr VG/PG v ml</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.result.vgpgToRound</t>
+  </si>
+  <si>
+    <t>Kategorie poměru</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.result.draws</t>
+  </si>
+  <si>
+    <t>Doporučené typy potahů</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.result.nicotine</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.result.vgpg</t>
+  </si>
+  <si>
+    <t>Výsledný poměr VG/PG</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.empty.title</t>
+  </si>
+  <si>
+    <t>Báze netřeba</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Tento liquid nevyžaduje bázi.</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.empty.title</t>
+  </si>
+  <si>
+    <t>Booster netřeba</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.booster.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Tento liquid neobsahuje nikotin.</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.aroma.ratio</t>
+  </si>
+  <si>
+    <t>Procento aromatu</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.empty.required.title</t>
+  </si>
+  <si>
+    <t>Chybí báze</t>
+  </si>
+  <si>
+    <t>shared.mixture.info.base.empty.required.subtitle</t>
+  </si>
+  <si>
+    <t>Vybraný liquid vyžaduje bázi.</t>
   </si>
 </sst>
 </file>
@@ -9696,10 +10134,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1083"/>
+  <dimension ref="A1:C1169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1061" workbookViewId="0">
-      <selection activeCell="B1074" sqref="B1074"/>
+    <sheetView tabSelected="1" topLeftCell="A1139" workbookViewId="0">
+      <selection activeCell="B1152" sqref="B1152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21620,6 +22058,952 @@
       </c>
       <c r="C1083" s="1" t="s">
         <v>1861</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1084" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1084" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1084" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1085" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1085" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C1085" s="1" t="s">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1086" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1086" s="1" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C1086" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1087" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1087" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C1087" s="1" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1088" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1088" s="1" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C1088" s="1" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1089" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1089" s="1" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C1089" s="1" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1090" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1090" s="1" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C1090" s="1" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1091" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1091" s="1" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C1091" s="1" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1092" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1092" s="1" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C1092" s="1" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1093" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1093" s="1" t="s">
+        <v>2346</v>
+      </c>
+      <c r="C1093" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1094" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1094" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C1094" s="1" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1095" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1095" s="1" t="s">
+        <v>2349</v>
+      </c>
+      <c r="C1095" s="1" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1096" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1096" s="1" t="s">
+        <v>2350</v>
+      </c>
+      <c r="C1096" s="1" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1097" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1097" s="1" t="s">
+        <v>2352</v>
+      </c>
+      <c r="C1097" s="1" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1098" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>2354</v>
+      </c>
+      <c r="C1098" s="1" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1099" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>2356</v>
+      </c>
+      <c r="C1099" s="1" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1100" s="1" t="s">
+        <v>2358</v>
+      </c>
+      <c r="C1100" s="1" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1101" s="1" t="s">
+        <v>2360</v>
+      </c>
+      <c r="C1101" s="1" t="s">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1102" s="1" t="s">
+        <v>2362</v>
+      </c>
+      <c r="C1102" s="1" t="s">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1103" s="1" t="s">
+        <v>2364</v>
+      </c>
+      <c r="C1103" s="1" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1104" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C1104" s="1" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1105" s="1" t="s">
+        <v>2368</v>
+      </c>
+      <c r="C1105" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1106" s="1" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C1106" s="1" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1107" s="1" t="s">
+        <v>2371</v>
+      </c>
+      <c r="C1107" s="1" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1108" s="1" t="s">
+        <v>2372</v>
+      </c>
+      <c r="C1108" s="1" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1109" s="1" t="s">
+        <v>2374</v>
+      </c>
+      <c r="C1109" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1110" s="1" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C1110" s="1" t="s">
+        <v>2376</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1111" s="1" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C1111" s="1" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1112" s="1" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C1112" s="1" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1113" s="1" t="s">
+        <v>2380</v>
+      </c>
+      <c r="C1113" s="1" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1114" s="1" t="s">
+        <v>2382</v>
+      </c>
+      <c r="C1114" s="1" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1115" s="1" t="s">
+        <v>2384</v>
+      </c>
+      <c r="C1115" s="1" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1116" s="1" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C1116" s="1" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1117" s="1" t="s">
+        <v>2388</v>
+      </c>
+      <c r="C1117" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1118" s="1" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C1118" s="1" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1119" s="1" t="s">
+        <v>2391</v>
+      </c>
+      <c r="C1119" s="1" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1120" s="1" t="s">
+        <v>2393</v>
+      </c>
+      <c r="C1120" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1121" s="1" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C1121" s="1" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1122" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="C1122" s="1" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1123" s="1" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C1123" s="1" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1124" s="1" t="s">
+        <v>2400</v>
+      </c>
+      <c r="C1124" s="1" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1125" s="1" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C1125" s="1" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1126" s="1" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C1126" s="1" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1127" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C1127" s="1" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1128" s="1" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C1128" s="1" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1129" s="1" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C1129" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1130" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="C1130" s="1" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1131" s="1" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C1131" s="1" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1132" s="1" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C1132" s="1" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1133" s="1" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C1133" s="1" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1134" s="1" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C1134" s="1" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1135" s="1" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C1135" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1136" s="1" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C1136" s="1" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1137" s="1" t="s">
+        <v>2423</v>
+      </c>
+      <c r="C1137" s="1" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1138" s="1" t="s">
+        <v>2425</v>
+      </c>
+      <c r="C1138" s="1" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1139" s="1" t="s">
+        <v>2427</v>
+      </c>
+      <c r="C1139" s="1" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1140" s="1" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C1140" s="1" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1141" s="1" t="s">
+        <v>2431</v>
+      </c>
+      <c r="C1141" s="1" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1142" s="1" t="s">
+        <v>2432</v>
+      </c>
+      <c r="C1142" s="1" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1143" s="1" t="s">
+        <v>2433</v>
+      </c>
+      <c r="C1143" s="1" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1144" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1144" s="1" t="s">
+        <v>2436</v>
+      </c>
+      <c r="C1144" s="1" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1145" s="1" t="s">
+        <v>2438</v>
+      </c>
+      <c r="C1145" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1146" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C1146" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1147" s="1" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C1147" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1148" s="1" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C1148" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1149" s="1" t="s">
+        <v>2442</v>
+      </c>
+      <c r="C1149" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1150" s="1" t="s">
+        <v>2443</v>
+      </c>
+      <c r="C1150" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1151" s="1" t="s">
+        <v>2444</v>
+      </c>
+      <c r="C1151" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1152" s="1" t="s">
+        <v>2445</v>
+      </c>
+      <c r="C1152" s="1" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1153" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C1153" s="1" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1154" s="1" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C1154" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1155" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1155" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1156" s="1" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C1156" s="1" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1157" s="1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="C1157" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1158" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C1158" s="1" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1159" s="1" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C1159" s="1" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1160" s="1" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C1160" s="1" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1161" s="1" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C1161" s="1" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1162" s="1" t="s">
+        <v>2462</v>
+      </c>
+      <c r="C1162" s="1" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1163" s="1" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C1163" s="1" t="s">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1164" s="1" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C1164" s="1" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1165" s="1" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C1165" s="1" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1166" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C1166" s="1" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1167" s="1" t="s">
+        <v>2472</v>
+      </c>
+      <c r="C1167" s="1" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1168" s="1" t="s">
+        <v>2474</v>
+      </c>
+      <c r="C1168" s="1" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1169" s="1" t="s">
+        <v>2476</v>
+      </c>
+      <c r="C1169" s="1" t="s">
+        <v>2477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing favorites and initial rating support
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0893B97-EEBE-4D08-87D5-0241996768A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB80E7-1D36-4A81-9507-F2CD6FE69348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11115" yWindow="2235" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="195" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4775" uniqueCount="2493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4805" uniqueCount="2513">
   <si>
     <t>cs</t>
   </si>
@@ -7727,6 +7727,66 @@
   </si>
   <si>
     <t>Vata {{name}} byla úspašně vytvořena.</t>
+  </si>
+  <si>
+    <t>lab.aroma.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbená aromata.</t>
+  </si>
+  <si>
+    <t>lab.aroma.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Zde se zobrazí aromata, která kladně ohodnotíte.</t>
+  </si>
+  <si>
+    <t>inventory.aroma.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbená aromata</t>
+  </si>
+  <si>
+    <t>inventory.aroma.all.tab</t>
+  </si>
+  <si>
+    <t>Všechna aromata</t>
+  </si>
+  <si>
+    <t>inventory.base.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené báze</t>
+  </si>
+  <si>
+    <t>inventory.base.all.tab</t>
+  </si>
+  <si>
+    <t>Všechny báze</t>
+  </si>
+  <si>
+    <t>lab.booster.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte žádné oblíbené boostery.</t>
+  </si>
+  <si>
+    <t>lab.booster.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení boosteru se zde objeví.</t>
+  </si>
+  <si>
+    <t>inventory.booster.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené boostery</t>
+  </si>
+  <si>
+    <t>inventory.booster.all.tab</t>
+  </si>
+  <si>
+    <t>Všechny boostery</t>
   </si>
 </sst>
 </file>
@@ -10179,10 +10239,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1179"/>
+  <dimension ref="A1:C1189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1154" workbookViewId="0">
-      <selection activeCell="C1179" sqref="C1179"/>
+      <selection activeCell="B1180" sqref="B1180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23159,6 +23219,116 @@
       </c>
       <c r="C1179" s="1" t="s">
         <v>2492</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1180" s="1" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C1180" s="1" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1181" s="1" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C1181" s="1" t="s">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1182" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="C1182" s="1" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1183" s="1" t="s">
+        <v>2499</v>
+      </c>
+      <c r="C1183" s="1" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1184" s="1" t="s">
+        <v>2501</v>
+      </c>
+      <c r="C1184" s="1" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1185" s="1" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C1185" s="1" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1186" s="1" t="s">
+        <v>2505</v>
+      </c>
+      <c r="C1186" s="1" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1187" s="1" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C1187" s="1" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1188" s="1" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C1188" s="1" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1189" s="1" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C1189" s="1" t="s">
+        <v>2512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Finished rating of inventory stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB80E7-1D36-4A81-9507-F2CD6FE69348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3931291-82F7-4A86-A754-AD8BD22CF55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="195" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="1830" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4805" uniqueCount="2513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4865" uniqueCount="2552">
   <si>
     <t>cs</t>
   </si>
@@ -7787,6 +7787,123 @@
   </si>
   <si>
     <t>Všechny boostery</t>
+  </si>
+  <si>
+    <t>lab.wire.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbené dráty.</t>
+  </si>
+  <si>
+    <t>lab.wire.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení drátu se zde objeví.</t>
+  </si>
+  <si>
+    <t>inventory.wire.favorite.tab</t>
+  </si>
+  <si>
+    <t>inventory.wire.all.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené dráty</t>
+  </si>
+  <si>
+    <t>Všechny dráty</t>
+  </si>
+  <si>
+    <t>lab.cotton.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbené vaty.</t>
+  </si>
+  <si>
+    <t>lab.cotton.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení vaty se zde objeví.</t>
+  </si>
+  <si>
+    <t>inventory.cotton.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbená vaty</t>
+  </si>
+  <si>
+    <t>inventory.cotton.all.tab</t>
+  </si>
+  <si>
+    <t>inventory.atomizer.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené atomizéry</t>
+  </si>
+  <si>
+    <t>inventory.atomizer.all.tab</t>
+  </si>
+  <si>
+    <t>Všechny atomizéry</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbené atomizéry.</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení atomizéru se zde objeví.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>inventory.mod.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené mody</t>
+  </si>
+  <si>
+    <t>inventory.mod.all.tab</t>
+  </si>
+  <si>
+    <t>Všechny mody</t>
+  </si>
+  <si>
+    <t>lab.mod.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>lab.mod.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbené mody.</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení modu se zde objeví.</t>
+  </si>
+  <si>
+    <t>inventory.cell.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené články</t>
+  </si>
+  <si>
+    <t>inventory.cell.all.tab</t>
+  </si>
+  <si>
+    <t>Všechny články</t>
+  </si>
+  <si>
+    <t>lab.cell.list.favorite.empty.title</t>
+  </si>
+  <si>
+    <t>lab.cell.list.favorite.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Nemáte oblíbené články.</t>
+  </si>
+  <si>
+    <t>Po kladném ohodnocení článku se zde objeví.</t>
   </si>
 </sst>
 </file>
@@ -10239,10 +10356,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1189"/>
+  <dimension ref="A1:C1209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1154" workbookViewId="0">
-      <selection activeCell="B1180" sqref="B1180"/>
+    <sheetView tabSelected="1" topLeftCell="A1175" workbookViewId="0">
+      <selection activeCell="B1196" sqref="B1196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23329,6 +23446,226 @@
       </c>
       <c r="C1189" s="1" t="s">
         <v>2512</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1190" s="1" t="s">
+        <v>2513</v>
+      </c>
+      <c r="C1190" s="1" t="s">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1191" s="1" t="s">
+        <v>2515</v>
+      </c>
+      <c r="C1191" s="1" t="s">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1192" s="1" t="s">
+        <v>2517</v>
+      </c>
+      <c r="C1192" s="1" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1193" s="1" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C1193" s="1" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1194" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1194" s="1" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C1194" s="1" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1195" s="1" t="s">
+        <v>2523</v>
+      </c>
+      <c r="C1195" s="1" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1196" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1196" s="1" t="s">
+        <v>2525</v>
+      </c>
+      <c r="C1196" s="1" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1197" s="1" t="s">
+        <v>2527</v>
+      </c>
+      <c r="C1197" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1198" s="1" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C1198" s="1" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1199" s="1" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C1199" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1200" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1200" s="1" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C1200" s="1" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1201" s="1" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C1201" s="1" t="s">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1202" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C1202" s="1" t="s">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1203" s="1" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C1203" s="1" t="s">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1204" s="1" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C1204" s="1" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1205" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C1205" s="1" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1206" s="1" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C1206" s="1" t="s">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1207" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C1207" s="1" t="s">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1208" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C1208" s="1" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1209" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="C1209" s="1" t="s">
+        <v>2551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some small improvements
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AE5687-A100-4632-8D93-70BBD954D071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B819F8B-7DBC-4D5F-BC0F-2601F20B3462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7740" yWindow="1830" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4889" uniqueCount="2564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4892" uniqueCount="2565">
   <si>
     <t>cs</t>
   </si>
@@ -7940,6 +7940,9 @@
   </si>
   <si>
     <t>market.aroma.mixture.label</t>
+  </si>
+  <si>
+    <t>lab.build.tab</t>
   </si>
 </sst>
 </file>
@@ -10392,10 +10395,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1217"/>
+  <dimension ref="A1:C1218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1193" workbookViewId="0">
-      <selection activeCell="B1208" sqref="B1208"/>
+      <selection activeCell="B1203" sqref="B1203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23790,6 +23793,17 @@
       </c>
       <c r="C1217" s="1" t="s">
         <v>1086</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1218" s="1" t="s">
+        <v>2564</v>
+      </c>
+      <c r="C1218" s="1" t="s">
+        <v>1817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial comments on builds
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B819F8B-7DBC-4D5F-BC0F-2601F20B3462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E9C9D5-DF28-42C6-81C4-B218B1FFBF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="1830" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9495" yWindow="1395" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4892" uniqueCount="2565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4922" uniqueCount="2583">
   <si>
     <t>cs</t>
   </si>
@@ -7943,6 +7943,60 @@
   </si>
   <si>
     <t>lab.build.tab</t>
+  </si>
+  <si>
+    <t>lab.build.comment.comment.label</t>
+  </si>
+  <si>
+    <t>Napište si komentář k buildu.</t>
+  </si>
+  <si>
+    <t>lab.build.comment.comment</t>
+  </si>
+  <si>
+    <t>BuildComment.list.total</t>
+  </si>
+  <si>
+    <t>Počet komentářů [{{data.total}}] ({{data.from}}-{{data.to}})</t>
+  </si>
+  <si>
+    <t>shared.comment.delete.button</t>
+  </si>
+  <si>
+    <t>Smazat</t>
+  </si>
+  <si>
+    <t>shared.comment.empty.title</t>
+  </si>
+  <si>
+    <t>Zatím tu nejsou žádné komentáře.</t>
+  </si>
+  <si>
+    <t>shared.comment.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Jestli máte něco na srdci, neváhejte se podělit!</t>
+  </si>
+  <si>
+    <t>shared.comment.list.tab</t>
+  </si>
+  <si>
+    <t>shared.comment.create.tab</t>
+  </si>
+  <si>
+    <t>Nový komentář</t>
+  </si>
+  <si>
+    <t>shared.comment.delete.title</t>
+  </si>
+  <si>
+    <t>Přejete si odstranit vybraný komentář?</t>
+  </si>
+  <si>
+    <t>shared.comment.delete.content</t>
+  </si>
+  <si>
+    <t>Pokud si nezapamatujete text komentáře, tak není cesty zpět. Ale o moc tady nejde, takže hurá do toho!</t>
   </si>
 </sst>
 </file>
@@ -10395,10 +10449,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1218"/>
+  <dimension ref="A1:C1228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1193" workbookViewId="0">
-      <selection activeCell="B1203" sqref="B1203"/>
+    <sheetView tabSelected="1" topLeftCell="A1194" workbookViewId="0">
+      <selection activeCell="B1209" sqref="B1209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23804,6 +23858,116 @@
       </c>
       <c r="C1218" s="1" t="s">
         <v>1817</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1219" s="1" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C1219" s="1" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1220" s="1" t="s">
+        <v>2567</v>
+      </c>
+      <c r="C1220" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1221" s="1" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C1221" s="1" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1222" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C1222" s="1" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1223" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="C1223" s="1" t="s">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1224" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C1224" s="1" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1225" s="1" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C1225" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1226" s="1" t="s">
+        <v>2577</v>
+      </c>
+      <c r="C1226" s="1" t="s">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1227" s="1" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C1227" s="1" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1228" s="1" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C1228" s="1" t="s">
+        <v>2582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added comments to aromas; experimental mixtures in aroma detail
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2F37C5-06F4-4632-B25C-7C49CA7BFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8387C2F7-B98A-42E1-ABB4-8CBBC03F1F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="255" windowWidth="33825" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="975" windowWidth="23715" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="2591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4976" uniqueCount="2610">
   <si>
     <t>cs</t>
   </si>
@@ -8021,6 +8021,63 @@
   </si>
   <si>
     <t>Výběr spirálky je povinný.</t>
+  </si>
+  <si>
+    <t>inventory.aroma.aroma.title.tab</t>
+  </si>
+  <si>
+    <t>Detail aromatu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.aroma.title</t>
+  </si>
+  <si>
+    <t>Detail aromatu {{aromaInventory.aroma.name}} - {{aromaInventory.aroma.vendor.name}}</t>
+  </si>
+  <si>
+    <t>inventory.aroma.aroma.menu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.mixture.menu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.comment.menu</t>
+  </si>
+  <si>
+    <t>inventory.aroma.label</t>
+  </si>
+  <si>
+    <t>inventory.aroma.mixture.label</t>
+  </si>
+  <si>
+    <t>inventory.aroma.mixture.title.tab</t>
+  </si>
+  <si>
+    <t>inventory.aroma.mixture.title</t>
+  </si>
+  <si>
+    <t>Mixy aromatu {{aromaInventory.aroma.name}}</t>
+  </si>
+  <si>
+    <t>inventory.aroma.comment.title</t>
+  </si>
+  <si>
+    <t>Komentáře k aromatu {{aromaInventory.aroma.name}}</t>
+  </si>
+  <si>
+    <t>inventory.aroma.comment.label</t>
+  </si>
+  <si>
+    <t>inventory.aroma.comment.title.tab</t>
+  </si>
+  <si>
+    <t>shared.aroma.comment.comment.label</t>
+  </si>
+  <si>
+    <t>Napište si komentář k aromatu.</t>
+  </si>
+  <si>
+    <t>shared.aroma.comment.comment</t>
   </si>
 </sst>
 </file>
@@ -10473,10 +10530,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1232"/>
+  <dimension ref="A1:C1246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1194" workbookViewId="0">
-      <selection activeCell="B1214" sqref="B1214"/>
+    <sheetView tabSelected="1" topLeftCell="B1209" workbookViewId="0">
+      <selection activeCell="B1226" sqref="B1226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24036,6 +24093,160 @@
       </c>
       <c r="C1232" s="1" t="s">
         <v>2590</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1233" s="1" t="s">
+        <v>2591</v>
+      </c>
+      <c r="C1233" s="1" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1234" s="1" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C1234" s="1" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1235" s="1" t="s">
+        <v>2595</v>
+      </c>
+      <c r="C1235" s="1" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1236" s="1" t="s">
+        <v>2596</v>
+      </c>
+      <c r="C1236" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1237" s="1" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C1237" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1238" s="1" t="s">
+        <v>2598</v>
+      </c>
+      <c r="C1238" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1239" s="1" t="s">
+        <v>2599</v>
+      </c>
+      <c r="C1239" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1240" s="1" t="s">
+        <v>2600</v>
+      </c>
+      <c r="C1240" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1241" s="1" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C1241" s="1" t="s">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1242" s="1" t="s">
+        <v>2603</v>
+      </c>
+      <c r="C1242" s="1" t="s">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1243" s="1" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C1243" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1244" s="1" t="s">
+        <v>2606</v>
+      </c>
+      <c r="C1244" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1245" s="1" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C1245" s="1" t="s">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1246" s="1" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C1246" s="1" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial experiment with ACL
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8387C2F7-B98A-42E1-ABB4-8CBBC03F1F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780F6355-10C2-4377-9BE4-BD38B9153A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="975" windowWidth="23715" windowHeight="18495" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4976" uniqueCount="2610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4982" uniqueCount="2614">
   <si>
     <t>cs</t>
   </si>
@@ -8078,6 +8078,18 @@
   </si>
   <si>
     <t>shared.aroma.comment.comment</t>
+  </si>
+  <si>
+    <t>error.User does not have required tokens.</t>
+  </si>
+  <si>
+    <t>Pro požadovanou operaci nemáte dostatečná oprávnění.</t>
+  </si>
+  <si>
+    <t>error.Atomizer already exists.</t>
+  </si>
+  <si>
+    <t>Atomizér se zadaným názvem již u daného výrobce existuje. Pokud se snažíte vytvořit nový, zkontrolujte na tržišti, zda už neexistuje; pokud máte pocit, že vám chybí, musíte si jej nejprve zakoupit.</t>
   </si>
 </sst>
 </file>
@@ -10530,10 +10542,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1246"/>
+  <dimension ref="A1:C1248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1209" workbookViewId="0">
-      <selection activeCell="B1226" sqref="B1226"/>
+    <sheetView tabSelected="1" topLeftCell="B1215" workbookViewId="0">
+      <selection activeCell="B1236" sqref="B1236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24247,6 +24259,28 @@
       </c>
       <c r="C1246" s="1" t="s">
         <v>532</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1247" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="C1247" s="1" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1248" s="1" t="s">
+        <v>2612</v>
+      </c>
+      <c r="C1248" s="1" t="s">
+        <v>2613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial certificate management done
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27000B9-EB2A-45B9-85AA-25193F2A7D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC46933F-4292-495C-9F16-B40D0D530C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25215" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4995" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5091" uniqueCount="2681">
   <si>
     <t>cs</t>
   </si>
@@ -8120,6 +8120,196 @@
   </si>
   <si>
     <t>Přegenerovat</t>
+  </si>
+  <si>
+    <t>market.certificate.menu</t>
+  </si>
+  <si>
+    <t>Certifikáty</t>
+  </si>
+  <si>
+    <t>market.license.menu</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>market.certificate.index.title</t>
+  </si>
+  <si>
+    <t>market.certificate.label</t>
+  </si>
+  <si>
+    <t>market.certificate.index.subtitle</t>
+  </si>
+  <si>
+    <t>Certifikáty jsou odznakem zvláštních privilegií, která můžete získat buď svou aktivitou, nebo podporou aplikace.</t>
+  </si>
+  <si>
+    <t>market.certificate.index.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Certifikáty jsou permanentní způsob, jak získat různá ocenění a privilegia v aplikaci. Je jej velmi složité získat, poněvadž má ostatním
+	uživatelům dát najevo, že ten či onen člověk je zdatný v nějaké oblasti.
+&lt;/p&gt;
+&lt;p&gt;
+	Pokud získáte certifikát, nemá nastavenou dobu platnosti, čili pokud hrubě neporušíte zásady používání aplikace a komunity, zůstane vám již navždy.
+&lt;/p&gt;
+&lt;p&gt;
+	Existuje více variant - jedna možnost je pouze certifikát dokládající, že podporujete aplikaci (tzn. za příspěvek), nebo můžete získat
+	certifikát opravňujicí vás spravovat tržiště, upravovat produkty a podobně. Další varianta - s téměr totožnou funkcí - je získání licence,
+	nicméně to je jiný příběh.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>market.certificate.create.button</t>
+  </si>
+  <si>
+    <t>Vytvořit certifikát</t>
+  </si>
+  <si>
+    <t>market.certificate.create.title</t>
+  </si>
+  <si>
+    <t>Nový certifikát</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.name.label</t>
+  </si>
+  <si>
+    <t>Název certifikátu</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Název půjde skrz překladač, použijte tudíž prosím rozumný název.</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.create</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.code.label</t>
+  </si>
+  <si>
+    <t>Kód certifikátu</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Kód je dobrovolný a přidělí jej případně systém. Slouží hlavně pro jednoznačnou identifikaci certifikátu.</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Vyplňte prosím název certifikátu.</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.tokens.label</t>
+  </si>
+  <si>
+    <t>Vyberte tokeny</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.tokens.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zde můžete vybrat tokeny, které budou spolu s certifikátem uživateli přiděleny. Obecně udávají možnosti přístupu do aplikace, volte tedy prosím s rozumem.</t>
+  </si>
+  <si>
+    <t>lab.token.create.button</t>
+  </si>
+  <si>
+    <t>Nový token</t>
+  </si>
+  <si>
+    <t>lab.token.create.title</t>
+  </si>
+  <si>
+    <t>Vytvořit token</t>
+  </si>
+  <si>
+    <t>shared.token.create.name.label</t>
+  </si>
+  <si>
+    <t>Jméno tokenu</t>
+  </si>
+  <si>
+    <t>shared.token.create.create</t>
+  </si>
+  <si>
+    <t>Jméno tokenu musíte znát ze systému, pokud chybí, jinak obecně nebude mít valnou platnost. Jeho funkce je hlavně řízení oprávnění.</t>
+  </si>
+  <si>
+    <t>shared.token.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>shared.token.create.success</t>
+  </si>
+  <si>
+    <t>Token [{{name}}] byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.cost.label</t>
+  </si>
+  <si>
+    <t>Cena certifikátu</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Certifikát je možné za udanou cenu nabídnout na tržišti; dbejte prosím toho, že certifikáty mají mít nádech prestiže, tudíž i cena by měla odpovídat. Pokud nemá na tržisti být dostupný vůbec, cenu neudávejte.</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.success</t>
+  </si>
+  <si>
+    <t>Certifikát [{{name}}] byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>common.token.*</t>
+  </si>
+  <si>
+    <t>Všemocný token</t>
+  </si>
+  <si>
+    <t>common.token.site.root</t>
+  </si>
+  <si>
+    <t>common.token.site.market</t>
+  </si>
+  <si>
+    <t>common.token.site.lab</t>
+  </si>
+  <si>
+    <t>market.certificate.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané certifikáty?</t>
+  </si>
+  <si>
+    <t>market.certificate.delete.modal.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Opravdu si přejete odstranit vybrané certifikáty?
+&lt;/p&gt;
+&lt;p&gt;
+	Pokud se uklepnete a smažete špatný certifikát, můžete efektivně sestřelit celou aplikaci. Zde není cesty zpět. Jakože není.
+&lt;/p&gt;
+&lt;p&gt;
+	Tudíž pokud máte nutkání něco mazat, radši zkuste něco jiného, dokud si tedy nejste naprosto jisti tím, co tu teď děláte.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>market.certificate.delete.success</t>
+  </si>
+  <si>
+    <t>Certifikáty úspěšně odstraněny. Pokud tuto hlášku vidíte, nejspíš se vám nic moc nepodařilo rozbít. Doufejte.</t>
   </si>
 </sst>
 </file>
@@ -10583,10 +10773,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1250"/>
+  <dimension ref="A1:C1282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1215" workbookViewId="0">
-      <selection activeCell="B1239" sqref="B1239"/>
+    <sheetView tabSelected="1" topLeftCell="A1267" workbookViewId="0">
+      <selection activeCell="B1276" sqref="B1276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24344,6 +24534,358 @@
       </c>
       <c r="C1250" s="1" t="s">
         <v>2623</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1251" s="1" t="s">
+        <v>2624</v>
+      </c>
+      <c r="C1251" s="1" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1252" s="1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C1252" s="1" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1253" s="1" t="s">
+        <v>2628</v>
+      </c>
+      <c r="C1253" s="1" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1254" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="C1254" s="1" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1255" s="1" t="s">
+        <v>2630</v>
+      </c>
+      <c r="C1255" s="1" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:3" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A1256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1256" s="1" t="s">
+        <v>2632</v>
+      </c>
+      <c r="C1256" s="1" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1257" s="1" t="s">
+        <v>2634</v>
+      </c>
+      <c r="C1257" s="1" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1258" s="1" t="s">
+        <v>2636</v>
+      </c>
+      <c r="C1258" s="1" t="s">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1259" s="1" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1259" s="1" t="s">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1260" s="1" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C1260" s="1" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1261" s="1" t="s">
+        <v>2642</v>
+      </c>
+      <c r="C1261" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1262" s="1" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C1262" s="1" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1263" s="1" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C1263" s="1" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1264" s="1" t="s">
+        <v>2647</v>
+      </c>
+      <c r="C1264" s="1" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1265" s="1" t="s">
+        <v>2649</v>
+      </c>
+      <c r="C1265" s="1" t="s">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1266" s="1" t="s">
+        <v>2651</v>
+      </c>
+      <c r="C1266" s="1" t="s">
+        <v>2652</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1267" s="1" t="s">
+        <v>2653</v>
+      </c>
+      <c r="C1267" s="1" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1268" s="1" t="s">
+        <v>2655</v>
+      </c>
+      <c r="C1268" s="1" t="s">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1269" s="1" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C1269" s="1" t="s">
+        <v>2658</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1270" s="1" t="s">
+        <v>2659</v>
+      </c>
+      <c r="C1270" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1271" s="1" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C1271" s="1" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1272" s="1" t="s">
+        <v>2662</v>
+      </c>
+      <c r="C1272" s="1" t="s">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1273" s="1" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C1273" s="1" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1274" s="1" t="s">
+        <v>2666</v>
+      </c>
+      <c r="C1274" s="1" t="s">
+        <v>2667</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1275" s="1" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C1275" s="1" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1276" s="1" t="s">
+        <v>2670</v>
+      </c>
+      <c r="C1276" s="1" t="s">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1277" s="1" t="s">
+        <v>2672</v>
+      </c>
+      <c r="C1277" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1278" s="1" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C1278" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1279" s="1" t="s">
+        <v>2674</v>
+      </c>
+      <c r="C1279" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1280" s="1" t="s">
+        <v>2675</v>
+      </c>
+      <c r="C1280" s="1" t="s">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A1281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1281" s="1" t="s">
+        <v>2677</v>
+      </c>
+      <c r="C1281" s="1" t="s">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1282" s="1" t="s">
+        <v>2679</v>
+      </c>
+      <c r="C1282" s="1" t="s">
+        <v>2680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial license stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC46933F-4292-495C-9F16-B40D0D530C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DCB598-2D50-4758-AD0D-8370FBA0266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5091" uniqueCount="2681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5160" uniqueCount="2724">
   <si>
     <t>cs</t>
   </si>
@@ -8310,6 +8310,145 @@
   </si>
   <si>
     <t>Certifikáty úspěšně odstraněny. Pokud tuto hlášku vidíte, nejspíš se vám nic moc nepodařilo rozbít. Doufejte.</t>
+  </si>
+  <si>
+    <t>market.license.label</t>
+  </si>
+  <si>
+    <t>market.license.index.title</t>
+  </si>
+  <si>
+    <t>market.license.create.button</t>
+  </si>
+  <si>
+    <t>Nová licence</t>
+  </si>
+  <si>
+    <t>market.license.create.title</t>
+  </si>
+  <si>
+    <t>shared.license.create.name.label</t>
+  </si>
+  <si>
+    <t>Název licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.code.label</t>
+  </si>
+  <si>
+    <t>Kód licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.cost.label</t>
+  </si>
+  <si>
+    <t>Cena licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.renew.label</t>
+  </si>
+  <si>
+    <t>Cena obnovy licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.duration.label</t>
+  </si>
+  <si>
+    <t>Platnost licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.tokens.label</t>
+  </si>
+  <si>
+    <t>Tokeny licence</t>
+  </si>
+  <si>
+    <t>shared.license.create.create</t>
+  </si>
+  <si>
+    <t>Vytvořit licenci</t>
+  </si>
+  <si>
+    <t>shared.license.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Použijte rozumné jméno pro licenci aby dávalo smysl; procházi překladem, tudíž je možné ho případně upravit jazykovou mutací.</t>
+  </si>
+  <si>
+    <t>shared.license.create.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Kód je unikátní označení, hlavně určený pro import/export.</t>
+  </si>
+  <si>
+    <t>Pokud je uvedena cena licence, bude dostupná na tržišti.</t>
+  </si>
+  <si>
+    <t>Pokud někdo již licenci vlastní a vyprší mu, může zaplatit uvedenou částku za obnovu; pokud není uvedena, obnova nebude možná.</t>
+  </si>
+  <si>
+    <t>shared.license.create.duration.label.tooltip</t>
+  </si>
+  <si>
+    <t>shared.license.create.renew.label.tooltip</t>
+  </si>
+  <si>
+    <t>shared.license.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Délka trvání přidelené licence ve dnech od data jejího pořízení; licence obecně mají krátkodobý efekt.</t>
+  </si>
+  <si>
+    <t>Tokeny přidelené touto licencí. Prakticky udává oprávnění, jaká uživatel s touto licencí může získat.</t>
+  </si>
+  <si>
+    <t>shared.license.create.tokens.label.tooltip</t>
+  </si>
+  <si>
+    <t>shared.license.create.success</t>
+  </si>
+  <si>
+    <t>Licence [{{name}}] byla úspěšně vytvořena.</t>
+  </si>
+  <si>
+    <t>market.license.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odstranit vybrané licence?</t>
+  </si>
+  <si>
+    <t>market.license.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Tato akce obecně není tak destruktivní, jako smazání certifikátu, přesto se ale třikrát a půlkrát rozmyslete, co děláte, protože můžete naštvat hodně lidí.</t>
+  </si>
+  <si>
+    <t>market.license.delete.success</t>
+  </si>
+  <si>
+    <t>Vybrané licence byly úspěšně odstraněny.</t>
+  </si>
+  <si>
+    <t>market.license.index.subtitle</t>
+  </si>
+  <si>
+    <t>Krátkodobé propůjčení privilegií.</t>
+  </si>
+  <si>
+    <t>market.license.index.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Licence jsou slabší a chudější verzí Certifikátů, kdy sice fungují v principu stejně - uživatel může získat zvláštní práva - ale
+	v případě licencí pouze na omezený čas, kdy pak buď musí licenci za poplatek obnovit, nebo si ji pořídit za plnou cenu znovu.
+&lt;/p&gt;
+&lt;p&gt;
+	Hlavním smyslem licencí je umožnit na určitý vymezený čas uživateli přidělit nějaká zajímavá oprávnění.
+&lt;/p&gt;
+&lt;p&gt;
+	Jelikož certifikát je vnímán jako exkluzivní zboží, některé základní vlastnosti aplikace jsou pro všechny uživatele řešené licencemi,
+	jedná se tak například o přístup na Tržiště nebo do Laboratoře. Tyto jsou na rozdíl od standardní licence také neomezené.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -10773,10 +10912,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1282"/>
+  <dimension ref="A1:C1305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1267" workbookViewId="0">
-      <selection activeCell="B1276" sqref="B1276"/>
+    <sheetView tabSelected="1" topLeftCell="A1279" workbookViewId="0">
+      <selection activeCell="B1296" sqref="B1296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24886,6 +25025,259 @@
       </c>
       <c r="C1282" s="1" t="s">
         <v>2680</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1283" s="1" t="s">
+        <v>2681</v>
+      </c>
+      <c r="C1283" s="1" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1284" s="1" t="s">
+        <v>2682</v>
+      </c>
+      <c r="C1284" s="1" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1285" s="1" t="s">
+        <v>2683</v>
+      </c>
+      <c r="C1285" s="1" t="s">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1286" s="1" t="s">
+        <v>2685</v>
+      </c>
+      <c r="C1286" s="1" t="s">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1287" s="1" t="s">
+        <v>2686</v>
+      </c>
+      <c r="C1287" s="1" t="s">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1288" s="1" t="s">
+        <v>2688</v>
+      </c>
+      <c r="C1288" s="1" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1289" s="1" t="s">
+        <v>2690</v>
+      </c>
+      <c r="C1289" s="1" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1290" s="1" t="s">
+        <v>2692</v>
+      </c>
+      <c r="C1290" s="1" t="s">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1291" s="1" t="s">
+        <v>2694</v>
+      </c>
+      <c r="C1291" s="1" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1292" s="1" t="s">
+        <v>2696</v>
+      </c>
+      <c r="C1292" s="1" t="s">
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1293" s="1" t="s">
+        <v>2698</v>
+      </c>
+      <c r="C1293" s="1" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1294" s="1" t="s">
+        <v>2700</v>
+      </c>
+      <c r="C1294" s="1" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1295" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1295" s="1" t="s">
+        <v>2702</v>
+      </c>
+      <c r="C1295" s="1" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1296" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1296" s="1" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C1296" s="1" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1297" s="1" t="s">
+        <v>2707</v>
+      </c>
+      <c r="C1297" s="1" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1298" s="1" t="s">
+        <v>2706</v>
+      </c>
+      <c r="C1298" s="1" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1299" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1299" s="1" t="s">
+        <v>2711</v>
+      </c>
+      <c r="C1299" s="1" t="s">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1300" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1300" s="1" t="s">
+        <v>2712</v>
+      </c>
+      <c r="C1300" s="1" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1301" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1301" s="1" t="s">
+        <v>2714</v>
+      </c>
+      <c r="C1301" s="1" t="s">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1302" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1302" s="1" t="s">
+        <v>2716</v>
+      </c>
+      <c r="C1302" s="1" t="s">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1303" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1303" s="1" t="s">
+        <v>2718</v>
+      </c>
+      <c r="C1303" s="1" t="s">
+        <v>2719</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1304" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1304" s="1" t="s">
+        <v>2720</v>
+      </c>
+      <c r="C1304" s="1" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:3" ht="141" x14ac:dyDescent="0.25">
+      <c r="A1305" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1305" s="1" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C1305" s="1" t="s">
+        <v>2723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some improvements in cert/license stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DCB598-2D50-4758-AD0D-8370FBA0266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC6B4FF-9816-40BA-8AE2-96FCB35C98B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5160" uniqueCount="2724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5184" uniqueCount="2740">
   <si>
     <t>cs</t>
   </si>
@@ -8438,6 +8438,24 @@
     <t>market.license.index.content</t>
   </si>
   <si>
+    <t>market.license.available.tab</t>
+  </si>
+  <si>
+    <t>Dostupné licence</t>
+  </si>
+  <si>
+    <t>market.license.private.tab</t>
+  </si>
+  <si>
+    <t>Privátní licence</t>
+  </si>
+  <si>
+    <t>market.license.licenses.tab</t>
+  </si>
+  <si>
+    <t>Všechny licence</t>
+  </si>
+  <si>
     <t>&lt;p&gt;
 	Licence jsou slabší a chudější verzí Certifikátů, kdy sice fungují v principu stejně - uživatel může získat zvláštní práva - ale
 	v případě licencí pouze na omezený čas, kdy pak buď musí licenci za poplatek obnovit, nebo si ji pořídit za plnou cenu znovu.
@@ -8448,7 +8466,43 @@
 &lt;p&gt;
 	Jelikož certifikát je vnímán jako exkluzivní zboží, některé základní vlastnosti aplikace jsou pro všechny uživatele řešené licencemi,
 	jedná se tak například o přístup na Tržiště nebo do Laboratoře. Tyto jsou na rozdíl od standardní licence také neomezené.
+&lt;/p&gt;
+&lt;p&gt;
+	Dostupné licence je možné volně koupit.
+&lt;/p&gt;
+&lt;p&gt;
+	Privátní licence je možné získat pouze na žádost. 
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>common.token.empty</t>
+  </si>
+  <si>
+    <t>(bez přidelených tokenů)</t>
+  </si>
+  <si>
+    <t>root.user.preview.tokens</t>
+  </si>
+  <si>
+    <t>Tokeny uživatele</t>
+  </si>
+  <si>
+    <t>market.certificate.available.tab</t>
+  </si>
+  <si>
+    <t>Dostupné certifikáty</t>
+  </si>
+  <si>
+    <t>market.certificate.private.tab</t>
+  </si>
+  <si>
+    <t>Privátní certifikáty</t>
+  </si>
+  <si>
+    <t>market.certificate.certificates.tab</t>
+  </si>
+  <si>
+    <t>Všechny certifikáty</t>
   </si>
 </sst>
 </file>
@@ -10912,10 +10966,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1305"/>
+  <dimension ref="A1:C1313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1279" workbookViewId="0">
-      <selection activeCell="B1296" sqref="B1296"/>
+    <sheetView tabSelected="1" topLeftCell="A1297" workbookViewId="0">
+      <selection activeCell="B1305" sqref="B1305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25269,7 +25323,7 @@
         <v>2721</v>
       </c>
     </row>
-    <row r="1305" spans="1:3" ht="141" x14ac:dyDescent="0.25">
+    <row r="1305" spans="1:3" ht="217.5" x14ac:dyDescent="0.25">
       <c r="A1305" s="1" t="s">
         <v>0</v>
       </c>
@@ -25277,7 +25331,95 @@
         <v>2722</v>
       </c>
       <c r="C1305" s="1" t="s">
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1306" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1306" s="1" t="s">
         <v>2723</v>
+      </c>
+      <c r="C1306" s="1" t="s">
+        <v>2724</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1307" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1307" s="1" t="s">
+        <v>2725</v>
+      </c>
+      <c r="C1307" s="1" t="s">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1308" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1308" s="1" t="s">
+        <v>2727</v>
+      </c>
+      <c r="C1308" s="1" t="s">
+        <v>2728</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1309" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1309" s="1" t="s">
+        <v>2730</v>
+      </c>
+      <c r="C1309" s="1" t="s">
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1310" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1310" s="1" t="s">
+        <v>2732</v>
+      </c>
+      <c r="C1310" s="1" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1311" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1311" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="C1311" s="1" t="s">
+        <v>2735</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1312" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1312" s="1" t="s">
+        <v>2736</v>
+      </c>
+      <c r="C1312" s="1" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1313" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1313" s="1" t="s">
+        <v>2738</v>
+      </c>
+      <c r="C1313" s="1" t="s">
+        <v>2739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial implementation of simple wishlist
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC6B4FF-9816-40BA-8AE2-96FCB35C98B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA4B9F5-1444-466C-9968-6BBE64B0FF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5184" uniqueCount="2740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="2793">
   <si>
     <t>cs</t>
   </si>
@@ -8503,6 +8503,165 @@
   </si>
   <si>
     <t>Všechny certifikáty</t>
+  </si>
+  <si>
+    <t>shared.wishlist.title</t>
+  </si>
+  <si>
+    <t>Seznam přání</t>
+  </si>
+  <si>
+    <t>shared.wishlist.tab</t>
+  </si>
+  <si>
+    <t>Vaše přání</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.tab</t>
+  </si>
+  <si>
+    <t>Nové přání</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.name.label</t>
+  </si>
+  <si>
+    <t>Jméno vašeho přání</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Popište svoje přání nebo název produktu; hlavně abyste rozeznali, cože si to vlastně přejete :).</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.url.label</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.url.label.tooltip</t>
+  </si>
+  <si>
+    <t>Adresa vašeho přání, pokud nějakou má; např. něco zajímavého na Steamtunners.</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.cost.label</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Uveďte cenu vašeho přání, používejte prosím stejnou měnu skrz všechna přání, jinak se pocuchají počty a svět se zhroutí.</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.note.label</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.note.label.tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pokudj je potřeba si něco více popsat k danému přání, zde máte možnost. </t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.tags.label</t>
+  </si>
+  <si>
+    <t>Tagy</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.tags.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tagy můžete použít k organizaci přání (např. atomizéry, driptipy, mody, …).</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.create</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.success</t>
+  </si>
+  <si>
+    <t>Přání bylo uloženo.</t>
+  </si>
+  <si>
+    <t>common.wishlist.empty</t>
+  </si>
+  <si>
+    <t>(bez štítků přání)</t>
+  </si>
+  <si>
+    <t>wishlist</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>tuning</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>shared.wishlist.delete.title</t>
+  </si>
+  <si>
+    <t>Odstranit přání?</t>
+  </si>
+  <si>
+    <t>shared.wishlist.delete.content</t>
+  </si>
+  <si>
+    <t>Tohle je jen formalitka - opravdu si přejete odstranit svoje přání? Je už splněné? Doufám, že ano!</t>
+  </si>
+  <si>
+    <t>shared.wishlist.delete.success</t>
+  </si>
+  <si>
+    <t>Vaše přáníčko bylo odstraněno.</t>
+  </si>
+  <si>
+    <t>common.wishlist.atomizer</t>
+  </si>
+  <si>
+    <t>common.wishlist.mod</t>
+  </si>
+  <si>
+    <t>common.wishlist.others</t>
+  </si>
+  <si>
+    <t>common.wishlist.tuning</t>
+  </si>
+  <si>
+    <t>common.wishlist.setup</t>
+  </si>
+  <si>
+    <t>Mod</t>
+  </si>
+  <si>
+    <t>Tuning</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>shared.wishlist.empty.title</t>
+  </si>
+  <si>
+    <t>Zatím nemáte žádná přání.</t>
+  </si>
+  <si>
+    <t>shared.wishlist.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud naleznete něco, po čem toužíte, ale nechcete na to zapomenout, nebo to mít na všech možných místech, můžete si přání zaznamenat sem.</t>
+  </si>
+  <si>
+    <t>shared.wishlist.create.name.label.required</t>
+  </si>
+  <si>
+    <t>Název přání je povinný.</t>
   </si>
 </sst>
 </file>
@@ -9441,10 +9600,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10133,6 +10292,61 @@
       </c>
       <c r="C62">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>812</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>2771</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -10966,10 +11180,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1313"/>
+  <dimension ref="A1:C1340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1297" workbookViewId="0">
-      <selection activeCell="B1305" sqref="B1305"/>
+    <sheetView tabSelected="1" topLeftCell="A1315" workbookViewId="0">
+      <selection activeCell="B1331" sqref="B1331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25420,6 +25634,303 @@
       </c>
       <c r="C1313" s="1" t="s">
         <v>2739</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1314" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1314" s="1" t="s">
+        <v>2740</v>
+      </c>
+      <c r="C1314" s="1" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1315" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1315" s="1" t="s">
+        <v>2742</v>
+      </c>
+      <c r="C1315" s="1" t="s">
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1316" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1316" s="1" t="s">
+        <v>2744</v>
+      </c>
+      <c r="C1316" s="1" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1317" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1317" s="1" t="s">
+        <v>2746</v>
+      </c>
+      <c r="C1317" s="1" t="s">
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1318" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1318" s="1" t="s">
+        <v>2748</v>
+      </c>
+      <c r="C1318" s="1" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1319" s="1" t="s">
+        <v>2750</v>
+      </c>
+      <c r="C1319" s="1" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1320" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1320" s="1" t="s">
+        <v>2752</v>
+      </c>
+      <c r="C1320" s="1" t="s">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1321" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1321" s="1" t="s">
+        <v>2754</v>
+      </c>
+      <c r="C1321" s="1" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1322" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1322" s="1" t="s">
+        <v>2755</v>
+      </c>
+      <c r="C1322" s="1" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1323" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1323" s="1" t="s">
+        <v>2757</v>
+      </c>
+      <c r="C1323" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1324" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1324" s="1" t="s">
+        <v>2758</v>
+      </c>
+      <c r="C1324" s="1" t="s">
+        <v>2759</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1325" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1325" s="1" t="s">
+        <v>2760</v>
+      </c>
+      <c r="C1325" s="1" t="s">
+        <v>2761</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1326" s="1" t="s">
+        <v>2762</v>
+      </c>
+      <c r="C1326" s="1" t="s">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1327" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1327" s="1" t="s">
+        <v>2764</v>
+      </c>
+      <c r="C1327" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1328" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1328" s="1" t="s">
+        <v>2765</v>
+      </c>
+      <c r="C1328" s="1" t="s">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1329" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1329" s="1" t="s">
+        <v>2767</v>
+      </c>
+      <c r="C1329" s="1" t="s">
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1330" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1330" s="1" t="s">
+        <v>2773</v>
+      </c>
+      <c r="C1330" s="1" t="s">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1331" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1331" s="1" t="s">
+        <v>2775</v>
+      </c>
+      <c r="C1331" s="1" t="s">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1332" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1332" s="1" t="s">
+        <v>2777</v>
+      </c>
+      <c r="C1332" s="1" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1333" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1333" s="1" t="s">
+        <v>2779</v>
+      </c>
+      <c r="C1333" s="1" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1334" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1334" s="1" t="s">
+        <v>2780</v>
+      </c>
+      <c r="C1334" s="1" t="s">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1335" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1335" s="1" t="s">
+        <v>2781</v>
+      </c>
+      <c r="C1335" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1336" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1336" s="1" t="s">
+        <v>2782</v>
+      </c>
+      <c r="C1336" s="1" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1337" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1337" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="C1337" s="1" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1338" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1338" s="1" t="s">
+        <v>2787</v>
+      </c>
+      <c r="C1338" s="1" t="s">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1339" s="1" t="s">
+        <v>2789</v>
+      </c>
+      <c r="C1339" s="1" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1340" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1340" s="1" t="s">
+        <v>2791</v>
+      </c>
+      <c r="C1340" s="1" t="s">
+        <v>2792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Certificates and licenses are connected to user (tokens)
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA4B9F5-1444-466C-9968-6BBE64B0FF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D849C94-06AC-41C1-B140-67BE5F343928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="2793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5290" uniqueCount="2802">
   <si>
     <t>cs</t>
   </si>
@@ -8662,6 +8662,34 @@
   </si>
   <si>
     <t>Název přání je povinný.</t>
+  </si>
+  <si>
+    <t>market.certificate.buy.confirm.title</t>
+  </si>
+  <si>
+    <t>Přejete si zakoupit vybraný certifikát?</t>
+  </si>
+  <si>
+    <t>market.certificate.buy.confirm.content</t>
+  </si>
+  <si>
+    <t>market.certificate.buy.confirm.button</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete zakoupit vybraný certifikát?&lt;br/&gt;
+Bude vás stát &lt;strong&gt;{{cost}} puffíků&lt;/strong&gt;.</t>
+  </si>
+  <si>
+    <t>market.certificate.buy.error</t>
+  </si>
+  <si>
+    <t>Certifikát se nepodařilo pořídit.</t>
+  </si>
+  <si>
+    <t>market.certificate.buy.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste si pořídili certifikát [{{certificate.name}}].</t>
   </si>
 </sst>
 </file>
@@ -11180,10 +11208,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1340"/>
+  <dimension ref="A1:C1345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1315" workbookViewId="0">
-      <selection activeCell="B1331" sqref="B1331"/>
+    <sheetView tabSelected="1" topLeftCell="A1312" workbookViewId="0">
+      <selection activeCell="C1345" sqref="C1345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25931,6 +25959,61 @@
       </c>
       <c r="C1340" s="1" t="s">
         <v>2792</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1341" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1341" s="1" t="s">
+        <v>2793</v>
+      </c>
+      <c r="C1341" s="1" t="s">
+        <v>2794</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1342" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1342" s="1" t="s">
+        <v>2795</v>
+      </c>
+      <c r="C1342" s="1" t="s">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1343" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1343" s="1" t="s">
+        <v>2796</v>
+      </c>
+      <c r="C1343" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1344" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1344" s="1" t="s">
+        <v>2798</v>
+      </c>
+      <c r="C1344" s="1" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1345" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1345" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="C1345" s="1" t="s">
+        <v>2801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved SDK, simplified query count invalidation
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D849C94-06AC-41C1-B140-67BE5F343928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA41638-8D8E-42E6-95A2-5A53134D8FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5290" uniqueCount="2802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5299" uniqueCount="2808">
   <si>
     <t>cs</t>
   </si>
@@ -8690,6 +8690,24 @@
   </si>
   <si>
     <t>Úspěšně jste si pořídili certifikát [{{certificate.name}}].</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.title</t>
+  </si>
+  <si>
+    <t>Žádost o certifikát</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.content</t>
+  </si>
+  <si>
+    <t>Přejete si vyžádat vybraný certifikát?</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.button</t>
+  </si>
+  <si>
+    <t>Vyžádat</t>
   </si>
 </sst>
 </file>
@@ -11208,10 +11226,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1345"/>
+  <dimension ref="A1:C1348"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1312" workbookViewId="0">
-      <selection activeCell="C1345" sqref="C1345"/>
+      <selection activeCell="B1338" sqref="B1338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26014,6 +26032,39 @@
       </c>
       <c r="C1345" s="1" t="s">
         <v>2801</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1346" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1346" s="1" t="s">
+        <v>2802</v>
+      </c>
+      <c r="C1346" s="1" t="s">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1347" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1347" s="1" t="s">
+        <v>2804</v>
+      </c>
+      <c r="C1347" s="1" t="s">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1348" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1348" s="1" t="s">
+        <v>2806</v>
+      </c>
+      <c r="C1348" s="1" t="s">
+        <v>2807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Certificate workflow is almost done
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA41638-8D8E-42E6-95A2-5A53134D8FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BCB351-2389-4B8D-951F-4469593C1B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5299" uniqueCount="2808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="2825">
   <si>
     <t>cs</t>
   </si>
@@ -8708,6 +8708,57 @@
   </si>
   <si>
     <t>Vyžádat</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.success</t>
+  </si>
+  <si>
+    <t>Žádost byla úspěšně odeslána.</t>
+  </si>
+  <si>
+    <t>root.user.certificates.menu</t>
+  </si>
+  <si>
+    <t>root.user.certificate.pending.tab</t>
+  </si>
+  <si>
+    <t>Ke schválení</t>
+  </si>
+  <si>
+    <t>root.user.certificate.request.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Přejete si odstranit vybranou žádost?</t>
+  </si>
+  <si>
+    <t>root.user.certificate.request.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Odstraněním žádosti dojde k jejímu "tichému" zamítnutí. Uživatel bude mít opět možnost žádost znovu podat. Pokud si ji přejete zamítnout, použijte funkci zamítnutí.</t>
+  </si>
+  <si>
+    <t>root.user.certificate.request.delete.success</t>
+  </si>
+  <si>
+    <t>Žádost o certifikát byla úspěšně odstraněna. Uživatel má nyní možnost vytvořit novou žádost.</t>
+  </si>
+  <si>
+    <t>root.user.certificate.approved.tab</t>
+  </si>
+  <si>
+    <t>Schválené</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.approve.success</t>
+  </si>
+  <si>
+    <t>Žádost o certifikát byla schválena.</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.approve.failure</t>
+  </si>
+  <si>
+    <t>Schválení zádosti o certifikát selhalo.</t>
   </si>
 </sst>
 </file>
@@ -11226,9 +11277,9 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1348"/>
+  <dimension ref="A1:C1357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1312" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1327" workbookViewId="0">
       <selection activeCell="B1338" sqref="B1338"/>
     </sheetView>
   </sheetViews>
@@ -26065,6 +26116,105 @@
       </c>
       <c r="C1348" s="1" t="s">
         <v>2807</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1349" s="1" t="s">
+        <v>2808</v>
+      </c>
+      <c r="C1349" s="1" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1350" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1350" s="1" t="s">
+        <v>2810</v>
+      </c>
+      <c r="C1350" s="1" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1351" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1351" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="C1351" s="1" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1352" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1352" s="1" t="s">
+        <v>2813</v>
+      </c>
+      <c r="C1352" s="1" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1353" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1353" s="1" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C1353" s="1" t="s">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1354" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1354" s="1" t="s">
+        <v>2817</v>
+      </c>
+      <c r="C1354" s="1" t="s">
+        <v>2818</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1355" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1355" s="1" t="s">
+        <v>2819</v>
+      </c>
+      <c r="C1355" s="1" t="s">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1356" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1356" s="1" t="s">
+        <v>2821</v>
+      </c>
+      <c r="C1356" s="1" t="s">
+        <v>2822</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1357" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1357" s="1" t="s">
+        <v>2823</v>
+      </c>
+      <c r="C1357" s="1" t="s">
+        <v>2824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Looks like certs are ok
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BCB351-2389-4B8D-951F-4469593C1B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DEE840-33AF-4345-906D-A3233E581065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="2825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5344" uniqueCount="2836">
   <si>
     <t>cs</t>
   </si>
@@ -8734,9 +8734,6 @@
     <t>root.user.certificate.request.delete.modal.content</t>
   </si>
   <si>
-    <t>Odstraněním žádosti dojde k jejímu "tichému" zamítnutí. Uživatel bude mít opět možnost žádost znovu podat. Pokud si ji přejete zamítnout, použijte funkci zamítnutí.</t>
-  </si>
-  <si>
     <t>root.user.certificate.request.delete.success</t>
   </si>
   <si>
@@ -8759,6 +8756,42 @@
   </si>
   <si>
     <t>Schválení zádosti o certifikát selhalo.</t>
+  </si>
+  <si>
+    <t>root.user.certificate.certificates.tab</t>
+  </si>
+  <si>
+    <t>root.user.certificate.delete.modal.title</t>
+  </si>
+  <si>
+    <t>Odebrat certifikát?</t>
+  </si>
+  <si>
+    <t>root.user.certificate.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Přejete si uživateli odebrat vybraný certifikát? Pokud jsou na něj navázaná oprávnění, přijde o ně. Dále existuje možnost certifikát opět získat - pokud je placený, tak koupí, jinak schválenou žádostí.</t>
+  </si>
+  <si>
+    <t>root.user.certificate.delete.success</t>
+  </si>
+  <si>
+    <t>Certifikát byl úspěšně odebrán.</t>
+  </si>
+  <si>
+    <t>Odstraněním žádosti pouze smažete její záznam a informaci o jejím stavu, nicméně již nemá vliv na schválené certifikáty (tzn. smazaná žádost nesmaže certifikát).</t>
+  </si>
+  <si>
+    <t>root.user.certificate.declined.tab</t>
+  </si>
+  <si>
+    <t>Zamítnuté</t>
+  </si>
+  <si>
+    <t>shared.user.certificate.request.decline.success</t>
+  </si>
+  <si>
+    <t>Žádost o certifikát byla zamítnuta.</t>
   </si>
 </sst>
 </file>
@@ -11277,10 +11310,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1357"/>
+  <dimension ref="A1:C1363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1327" workbookViewId="0">
-      <selection activeCell="B1338" sqref="B1338"/>
+    <sheetView tabSelected="1" topLeftCell="A1339" workbookViewId="0">
+      <selection activeCell="B1351" sqref="B1351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26170,7 +26203,7 @@
         <v>2815</v>
       </c>
       <c r="C1353" s="1" t="s">
-        <v>2816</v>
+        <v>2831</v>
       </c>
     </row>
     <row r="1354" spans="1:3" x14ac:dyDescent="0.25">
@@ -26178,10 +26211,10 @@
         <v>0</v>
       </c>
       <c r="B1354" s="1" t="s">
+        <v>2816</v>
+      </c>
+      <c r="C1354" s="1" t="s">
         <v>2817</v>
-      </c>
-      <c r="C1354" s="1" t="s">
-        <v>2818</v>
       </c>
     </row>
     <row r="1355" spans="1:3" x14ac:dyDescent="0.25">
@@ -26189,10 +26222,10 @@
         <v>0</v>
       </c>
       <c r="B1355" s="1" t="s">
+        <v>2818</v>
+      </c>
+      <c r="C1355" s="1" t="s">
         <v>2819</v>
-      </c>
-      <c r="C1355" s="1" t="s">
-        <v>2820</v>
       </c>
     </row>
     <row r="1356" spans="1:3" x14ac:dyDescent="0.25">
@@ -26200,10 +26233,10 @@
         <v>0</v>
       </c>
       <c r="B1356" s="1" t="s">
+        <v>2820</v>
+      </c>
+      <c r="C1356" s="1" t="s">
         <v>2821</v>
-      </c>
-      <c r="C1356" s="1" t="s">
-        <v>2822</v>
       </c>
     </row>
     <row r="1357" spans="1:3" x14ac:dyDescent="0.25">
@@ -26211,10 +26244,76 @@
         <v>0</v>
       </c>
       <c r="B1357" s="1" t="s">
+        <v>2822</v>
+      </c>
+      <c r="C1357" s="1" t="s">
         <v>2823</v>
       </c>
-      <c r="C1357" s="1" t="s">
+    </row>
+    <row r="1358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1358" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1358" s="1" t="s">
         <v>2824</v>
+      </c>
+      <c r="C1358" s="1" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1359" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1359" s="1" t="s">
+        <v>2825</v>
+      </c>
+      <c r="C1359" s="1" t="s">
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1360" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1360" s="1" t="s">
+        <v>2827</v>
+      </c>
+      <c r="C1360" s="1" t="s">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1361" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1361" s="1" t="s">
+        <v>2829</v>
+      </c>
+      <c r="C1361" s="1" t="s">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1362" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1362" s="1" t="s">
+        <v>2832</v>
+      </c>
+      <c r="C1362" s="1" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1363" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1363" s="1" t="s">
+        <v>2834</v>
+      </c>
+      <c r="C1363" s="1" t="s">
+        <v>2835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: License somehow works; needs to add from/to and co
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DEE840-33AF-4345-906D-A3233E581065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A714B1F-FCAF-43EC-85EC-E763FDE22827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5344" uniqueCount="2836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="2869">
   <si>
     <t>cs</t>
   </si>
@@ -8792,6 +8792,106 @@
   </si>
   <si>
     <t>Žádost o certifikát byla zamítnuta.</t>
+  </si>
+  <si>
+    <t>root.user.licenses.menu</t>
+  </si>
+  <si>
+    <t>root.user.license.licenses.tab</t>
+  </si>
+  <si>
+    <t>root.user.license.pending.tab</t>
+  </si>
+  <si>
+    <t>root.user.license.approved.tab</t>
+  </si>
+  <si>
+    <t>root.user.license.declined.tab</t>
+  </si>
+  <si>
+    <t>market.license.buy.confirm.title</t>
+  </si>
+  <si>
+    <t>Přejete si zakoupit vybranou licenci?</t>
+  </si>
+  <si>
+    <t>market.license.buy.confirm.content</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete zakoupit vybranou licenci?&lt;br/&gt;
+Bude vás stát &lt;strong&gt;{{cost}} puffíků&lt;/strong&gt;.</t>
+  </si>
+  <si>
+    <t>market.license.buy.confirm.button</t>
+  </si>
+  <si>
+    <t>market.license.buy.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste si pořídili licenci [{{license.name}}].</t>
+  </si>
+  <si>
+    <t>root.user.license.delete.modal.title</t>
+  </si>
+  <si>
+    <t>root.user.license.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Odebrat licenci?</t>
+  </si>
+  <si>
+    <t>Přejete si uživateli odebrat vybranou licenci? Pokud jsou na ni navázaná oprávnění, přijde o ně. Dále existuje možnost licenci opět získat - pokud je placená, tak koupí, jinak schválenou žádostí.</t>
+  </si>
+  <si>
+    <t>root.user.license.delete.success</t>
+  </si>
+  <si>
+    <t>Licence byla úspěšně odebrána.</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.title</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.content</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.button</t>
+  </si>
+  <si>
+    <t>Žádost o licenci</t>
+  </si>
+  <si>
+    <t>Přejete si vyžádat vybranou licenci?</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.success</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.decline.success</t>
+  </si>
+  <si>
+    <t>Žádost o licenci byla zamítnuta.</t>
+  </si>
+  <si>
+    <t>root.user.license.request.delete.modal.title</t>
+  </si>
+  <si>
+    <t>root.user.license.request.delete.modal.content</t>
+  </si>
+  <si>
+    <t>root.user.license.request.delete.success</t>
+  </si>
+  <si>
+    <t>Odstraněním žádosti pouze smažete její záznam a informaci o jejím stavu, nicméně již nemá vliv na schválené licence (tzn. smazaná žádost nesmaže licenci).</t>
+  </si>
+  <si>
+    <t>Žádost o licenci byla úspěšně odstraněna. Uživatel má nyní možnost vytvořit novou žádost.</t>
+  </si>
+  <si>
+    <t>shared.user.license.request.approve.success</t>
+  </si>
+  <si>
+    <t>Žádost o licenci byla schválena.</t>
   </si>
 </sst>
 </file>
@@ -11310,10 +11410,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1363"/>
+  <dimension ref="A1:C1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1339" workbookViewId="0">
-      <selection activeCell="B1351" sqref="B1351"/>
+    <sheetView tabSelected="1" topLeftCell="A1351" workbookViewId="0">
+      <selection activeCell="B1373" sqref="B1373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26314,6 +26414,237 @@
       </c>
       <c r="C1363" s="1" t="s">
         <v>2835</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1364" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1364" s="1" t="s">
+        <v>2836</v>
+      </c>
+      <c r="C1364" s="1" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1365" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1365" s="1" t="s">
+        <v>2837</v>
+      </c>
+      <c r="C1365" s="1" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1366" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1366" s="1" t="s">
+        <v>2838</v>
+      </c>
+      <c r="C1366" s="1" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1367" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1367" s="1" t="s">
+        <v>2839</v>
+      </c>
+      <c r="C1367" s="1" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1368" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1368" s="1" t="s">
+        <v>2840</v>
+      </c>
+      <c r="C1368" s="1" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1369" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1369" s="1" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C1369" s="1" t="s">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1370" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1370" s="1" t="s">
+        <v>2843</v>
+      </c>
+      <c r="C1370" s="1" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1371" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1371" s="1" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C1371" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1372" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1372" s="1" t="s">
+        <v>2846</v>
+      </c>
+      <c r="C1372" s="1" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1373" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1373" s="1" t="s">
+        <v>2848</v>
+      </c>
+      <c r="C1373" s="1" t="s">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1374" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1374" s="1" t="s">
+        <v>2849</v>
+      </c>
+      <c r="C1374" s="1" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1375" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1375" s="1" t="s">
+        <v>2852</v>
+      </c>
+      <c r="C1375" s="1" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1376" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1376" s="1" t="s">
+        <v>2854</v>
+      </c>
+      <c r="C1376" s="1" t="s">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1377" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1377" s="1" t="s">
+        <v>2855</v>
+      </c>
+      <c r="C1377" s="1" t="s">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1378" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1378" s="1" t="s">
+        <v>2856</v>
+      </c>
+      <c r="C1378" s="1" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1379" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1379" s="1" t="s">
+        <v>2859</v>
+      </c>
+      <c r="C1379" s="1" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1380" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1380" s="1" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C1380" s="1" t="s">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1381" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1381" s="1" t="s">
+        <v>2862</v>
+      </c>
+      <c r="C1381" s="1" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1382" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1382" s="1" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C1382" s="1" t="s">
+        <v>2865</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1383" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1383" s="1" t="s">
+        <v>2864</v>
+      </c>
+      <c r="C1383" s="1" t="s">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1384" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1384" s="1" t="s">
+        <v>2867</v>
+      </c>
+      <c r="C1384" s="1" t="s">
+        <v>2868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added ability to edit comments
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EC4A2B-245D-40FF-917B-2E7B1FFB5FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52419B9A-8D32-447F-8BF6-A4FF8BC90769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5422" uniqueCount="2878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5470" uniqueCount="2905">
   <si>
     <t>cs</t>
   </si>
@@ -8919,6 +8919,87 @@
   </si>
   <si>
     <t>Build byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.title</t>
+  </si>
+  <si>
+    <t>Editace aromatu</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Zde můžete upravit vlastnosti aromatu.</t>
+  </si>
+  <si>
+    <t>market.aroma.edit.content</t>
+  </si>
+  <si>
+    <t>V této části se neodehrává nic složitého - můžete upravit vlastnosti aromatu, pouze je třeba myslet na to, že pokud upravíte poměr VG/PG, aplikace musí přepočítat mixy; to bude mít vliv na již existující liquidy uživatelů, tak opatrně s tím.</t>
+  </si>
+  <si>
+    <t>lab.build.edit.button</t>
+  </si>
+  <si>
+    <t>lab.build.edit.title</t>
+  </si>
+  <si>
+    <t>Editace buildu</t>
+  </si>
+  <si>
+    <t>lab.build.edit.label</t>
+  </si>
+  <si>
+    <t>lab.build.edit.cottonId.label</t>
+  </si>
+  <si>
+    <t>Použitá vata</t>
+  </si>
+  <si>
+    <t>lab.build.edit.ohm.label</t>
+  </si>
+  <si>
+    <t>Odpor</t>
+  </si>
+  <si>
+    <t>lab.build.edit.ohm.label.tooltip</t>
+  </si>
+  <si>
+    <t>Upravte si odpor v buildu, ale používejte prosím stejné podmínky ve všech buildech, např. po vyžhavení a s vatou, po vyžhavení apod.</t>
+  </si>
+  <si>
+    <t>lab.build.edit.edit</t>
+  </si>
+  <si>
+    <t>lab.build.edit.active.label</t>
+  </si>
+  <si>
+    <t>lab.build.edit.active.label.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud chcete oživit build, který jste např. omylem uložili do archivu, přepněte tuto volbu.</t>
+  </si>
+  <si>
+    <t>lab.build.edit.success</t>
+  </si>
+  <si>
+    <t>Build byl úspěšně aktualizován.</t>
+  </si>
+  <si>
+    <t>shared.comment.edit.button</t>
+  </si>
+  <si>
+    <t>shared.comment.edit.title</t>
+  </si>
+  <si>
+    <t>Upravit komentář</t>
+  </si>
+  <si>
+    <t>shared.comment.edit.success</t>
+  </si>
+  <si>
+    <t>Komentář uložen.</t>
   </si>
 </sst>
 </file>
@@ -11437,10 +11518,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1389"/>
+  <dimension ref="A1:C1405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1365" workbookViewId="0">
-      <selection activeCell="B1377" sqref="B1377"/>
+      <selection activeCell="B1388" sqref="B1388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26727,6 +26808,182 @@
       </c>
       <c r="C1389" s="1" t="s">
         <v>2877</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1390" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1390" s="1" t="s">
+        <v>2878</v>
+      </c>
+      <c r="C1390" s="1" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1391" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1391" s="1" t="s">
+        <v>2880</v>
+      </c>
+      <c r="C1391" s="1" t="s">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1392" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1392" s="1" t="s">
+        <v>2882</v>
+      </c>
+      <c r="C1392" s="1" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1393" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1393" s="1" t="s">
+        <v>2884</v>
+      </c>
+      <c r="C1393" s="1" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1394" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1394" s="1" t="s">
+        <v>2885</v>
+      </c>
+      <c r="C1394" s="1" t="s">
+        <v>2886</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1395" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1395" s="1" t="s">
+        <v>2887</v>
+      </c>
+      <c r="C1395" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1396" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1396" s="1" t="s">
+        <v>2888</v>
+      </c>
+      <c r="C1396" s="1" t="s">
+        <v>2889</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1397" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1397" s="1" t="s">
+        <v>2890</v>
+      </c>
+      <c r="C1397" s="1" t="s">
+        <v>2891</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1398" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1398" s="1" t="s">
+        <v>2892</v>
+      </c>
+      <c r="C1398" s="1" t="s">
+        <v>2893</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1399" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1399" s="1" t="s">
+        <v>2894</v>
+      </c>
+      <c r="C1399" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1400" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1400" s="1" t="s">
+        <v>2895</v>
+      </c>
+      <c r="C1400" s="1" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1401" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1401" s="1" t="s">
+        <v>2896</v>
+      </c>
+      <c r="C1401" s="1" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1402" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1402" s="1" t="s">
+        <v>2898</v>
+      </c>
+      <c r="C1402" s="1" t="s">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1403" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1403" s="1" t="s">
+        <v>2900</v>
+      </c>
+      <c r="C1403" s="1" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1404" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1404" s="1" t="s">
+        <v>2901</v>
+      </c>
+      <c r="C1404" s="1" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1405" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1405" s="1" t="s">
+        <v>2903</v>
+      </c>
+      <c r="C1405" s="1" t="s">
+        <v>2904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added some initial stuff
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,28 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52419B9A-8D32-447F-8BF6-A4FF8BC90769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F91B9E7-B3F0-44DE-B027-CBE9B512AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="465" windowWidth="27900" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="1545" windowWidth="27900" windowHeight="19890" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
     <sheet name="translations" sheetId="3" r:id="rId2"/>
-    <sheet name="wires" sheetId="25" r:id="rId3"/>
-    <sheet name="fibers" sheetId="24" r:id="rId4"/>
-    <sheet name="aromas" sheetId="23" r:id="rId5"/>
-    <sheet name="boosters" sheetId="22" r:id="rId6"/>
-    <sheet name="bases" sheetId="21" r:id="rId7"/>
-    <sheet name="vouchers" sheetId="20" r:id="rId8"/>
-    <sheet name="atomizers" sheetId="19" r:id="rId9"/>
-    <sheet name="mods" sheetId="18" r:id="rId10"/>
-    <sheet name="cottons" sheetId="17" r:id="rId11"/>
-    <sheet name="tags" sheetId="16" r:id="rId12"/>
-    <sheet name="cells" sheetId="15" r:id="rId13"/>
-    <sheet name="vendors" sheetId="14" r:id="rId14"/>
-    <sheet name="prices" sheetId="13" r:id="rId15"/>
-    <sheet name="tariffs" sheetId="12" r:id="rId16"/>
-    <sheet name="Translations - Common" sheetId="4" r:id="rId17"/>
+    <sheet name="tokens" sheetId="27" r:id="rId3"/>
+    <sheet name="licenses" sheetId="26" r:id="rId4"/>
+    <sheet name="wires" sheetId="25" r:id="rId5"/>
+    <sheet name="fibers" sheetId="24" r:id="rId6"/>
+    <sheet name="aromas" sheetId="23" r:id="rId7"/>
+    <sheet name="boosters" sheetId="22" r:id="rId8"/>
+    <sheet name="bases" sheetId="21" r:id="rId9"/>
+    <sheet name="vouchers" sheetId="20" r:id="rId10"/>
+    <sheet name="atomizers" sheetId="19" r:id="rId11"/>
+    <sheet name="mods" sheetId="18" r:id="rId12"/>
+    <sheet name="cottons" sheetId="17" r:id="rId13"/>
+    <sheet name="tags" sheetId="16" r:id="rId14"/>
+    <sheet name="cells" sheetId="15" r:id="rId15"/>
+    <sheet name="vendors" sheetId="14" r:id="rId16"/>
+    <sheet name="prices" sheetId="13" r:id="rId17"/>
+    <sheet name="tariffs" sheetId="12" r:id="rId18"/>
+    <sheet name="Translations - Common" sheetId="4" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5470" uniqueCount="2905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5544" uniqueCount="2960">
   <si>
     <t>cs</t>
   </si>
@@ -9000,6 +9002,171 @@
   </si>
   <si>
     <t>Komentář uložen.</t>
+  </si>
+  <si>
+    <t>licenses</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>renew</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>tokens</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>aroma.read</t>
+  </si>
+  <si>
+    <t>aroma.write</t>
+  </si>
+  <si>
+    <t>aroma.delete</t>
+  </si>
+  <si>
+    <t>Market - Common</t>
+  </si>
+  <si>
+    <t>MPLQ-N7J74F-GQL7HZ2Q</t>
+  </si>
+  <si>
+    <t>common.token.aroma.read</t>
+  </si>
+  <si>
+    <t>Aromata - čtení</t>
+  </si>
+  <si>
+    <t>common.token.aroma.write</t>
+  </si>
+  <si>
+    <t>Aromata - zápis</t>
+  </si>
+  <si>
+    <t>common.token.aroma.delete</t>
+  </si>
+  <si>
+    <t>Aromata - mazání</t>
+  </si>
+  <si>
+    <t>Market - Trader</t>
+  </si>
+  <si>
+    <t>Market - Root</t>
+  </si>
+  <si>
+    <t>OCTB-RT4QIX-AH9QMUQD</t>
+  </si>
+  <si>
+    <t>RPZG-MMNE3O-G6ZTQSZ0</t>
+  </si>
+  <si>
+    <t>base.read</t>
+  </si>
+  <si>
+    <t>base.write</t>
+  </si>
+  <si>
+    <t>base.delete</t>
+  </si>
+  <si>
+    <t>booster.read</t>
+  </si>
+  <si>
+    <t>booster.write</t>
+  </si>
+  <si>
+    <t>booster.delete</t>
+  </si>
+  <si>
+    <t>cotton.read</t>
+  </si>
+  <si>
+    <t>cotton.write</t>
+  </si>
+  <si>
+    <t>cotton.delete</t>
+  </si>
+  <si>
+    <t>aroma.read, base.read, booster.read, cotton.read</t>
+  </si>
+  <si>
+    <t>aroma.read, aroma.write, base.read, base.write, booster.read, booster.write, cotton.read, cotton.write</t>
+  </si>
+  <si>
+    <t>aroma.read, aroma.write, aroma.delete, base.read, base.write, base.delete, booster.read, booster.write, booster.delete, cotton.read, cotton.write, cotton.delete</t>
+  </si>
+  <si>
+    <t>common.token.base.read</t>
+  </si>
+  <si>
+    <t>Báze - čtení</t>
+  </si>
+  <si>
+    <t>common.token.booster.read</t>
+  </si>
+  <si>
+    <t>Boostery - čtení</t>
+  </si>
+  <si>
+    <t>common.token.cotton.read</t>
+  </si>
+  <si>
+    <t>Vaty - čtení</t>
+  </si>
+  <si>
+    <t>common.token.base.write</t>
+  </si>
+  <si>
+    <t>Báze - zápis</t>
+  </si>
+  <si>
+    <t>common.token.booster.write</t>
+  </si>
+  <si>
+    <t>Boostery - zápis</t>
+  </si>
+  <si>
+    <t>common.token.cotton.write</t>
+  </si>
+  <si>
+    <t>Vaty - zápis</t>
+  </si>
+  <si>
+    <t>common.token.cotton.delete</t>
+  </si>
+  <si>
+    <t>Vaty - mazání</t>
+  </si>
+  <si>
+    <t>common.token.base.delete</t>
+  </si>
+  <si>
+    <t>Báze - mazání</t>
+  </si>
+  <si>
+    <t>common.token.booster.delete</t>
+  </si>
+  <si>
+    <t>Boostery - mazání</t>
+  </si>
+  <si>
+    <t>Lab - Common</t>
+  </si>
+  <si>
+    <t>Inventory - Common</t>
+  </si>
+  <si>
+    <t>PNLB-D99YV9-T60LOHX6</t>
+  </si>
+  <si>
+    <t>LIHH-35UZC2-BZV78JMZ</t>
   </si>
 </sst>
 </file>
@@ -9408,10 +9575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6120BD2C-6516-4E86-99D3-11A27B514E61}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9548,12 +9715,915 @@
         <v>1170</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2906</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF980A1E-67C8-2046-AD3D-9A8AA002E628}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>846</v>
+      </c>
+      <c r="B4">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>847</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>848</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>849</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2088</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>2089</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2090</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2091</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>2160</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I2" s="20">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L2" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I3" s="20">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L3" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I4" s="20">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L4" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I5" s="20">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I6" s="20">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L6" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I7" s="20">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L7" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I8" s="20">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I9" s="20">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L9" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I10" s="20">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L10" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I11" s="20">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L11" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I12" s="20">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L12" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I13" s="20">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L13" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L14" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I15" s="20">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L15" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I16" s="20">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L16" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I17" s="20">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L17" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I18" s="20">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L18" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I19" s="20">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L19" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>2092</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I20" s="20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="L20" s="1">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.eliquidshop.cz/vyrobce-wotofo-a1010/" xr:uid="{1A4BF3B4-D652-724B-882E-1BE1A013DDE7}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.eliquidshop.cz/vyrobce-sirius-mods-a1532/" xr:uid="{08F874F6-F6B3-B54F-BB43-99630EE8986F}"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.eliquidshop.cz/vyrobce-dotmod-a923/" xr:uid="{73DF1D56-B8D3-8248-8925-E785AC0DE759}"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{4693CF94-0CE9-8D4B-9B83-A044C6AFA279}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D757F10-66C2-2941-A49E-7F0FD3F6574C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -9733,7 +10803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F5805-0158-F34C-9256-85EB751C6431}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -9936,7 +11006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
   <dimension ref="A1:C67"/>
   <sheetViews>
@@ -10695,7 +11765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243831E-E3E3-1C43-AE4D-34D8FEF2F724}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -10837,7 +11907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
   <dimension ref="A1:A105"/>
   <sheetViews>
@@ -11383,7 +12453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1AB5C-3BBA-9E49-B566-51FB3B75CDAA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -11467,7 +12537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1822C792-D890-E542-B44B-A4E33F805828}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -11515,13 +12585,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1405"/>
+  <dimension ref="A1:C1417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1365" workbookViewId="0">
-      <selection activeCell="B1388" sqref="B1388"/>
+    <sheetView topLeftCell="A1383" workbookViewId="0">
+      <selection activeCell="B1399" sqref="B1399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26984,6 +28054,138 @@
       </c>
       <c r="C1405" s="1" t="s">
         <v>2904</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1406" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1406" s="1" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C1406" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1407" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1407" s="1" t="s">
+        <v>2918</v>
+      </c>
+      <c r="C1407" s="1" t="s">
+        <v>2919</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1408" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1408" s="1" t="s">
+        <v>2920</v>
+      </c>
+      <c r="C1408" s="1" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1409" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1409" s="1" t="s">
+        <v>2938</v>
+      </c>
+      <c r="C1409" s="1" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1410" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1410" s="1" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C1410" s="1" t="s">
+        <v>2941</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1411" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1411" s="1" t="s">
+        <v>2942</v>
+      </c>
+      <c r="C1411" s="1" t="s">
+        <v>2943</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1412" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1412" s="1" t="s">
+        <v>2944</v>
+      </c>
+      <c r="C1412" s="1" t="s">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1413" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1413" s="1" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C1413" s="1" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1414" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1414" s="1" t="s">
+        <v>2948</v>
+      </c>
+      <c r="C1414" s="1" t="s">
+        <v>2949</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1415" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1415" s="1" t="s">
+        <v>2950</v>
+      </c>
+      <c r="C1415" s="1" t="s">
+        <v>2951</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1416" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1416" s="1" t="s">
+        <v>2952</v>
+      </c>
+      <c r="C1416" s="1" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1417" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1417" s="1" t="s">
+        <v>2954</v>
+      </c>
+      <c r="C1417" s="1" t="s">
+        <v>2955</v>
       </c>
     </row>
   </sheetData>
@@ -27047,6 +28249,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FD4C38-64C5-40ED-9AD4-3F08781E6BBE}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>2926</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>2927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>2928</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>2929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>2932</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>2933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>2934</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48874847-D5A5-4B4C-B8BE-D757A1E415A7}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="93.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2907</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2908</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2909</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2922</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2925</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2923</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2924</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2959</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F7C88A-203F-48DC-ACBE-CE6221C44C48}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -27381,7 +28780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
   <dimension ref="A1:D162"/>
   <sheetViews>
@@ -29235,7 +30634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I60"/>
   <sheetViews>
@@ -30999,7 +32398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C57C95-A5C9-A44A-8F61-B6758048128A}">
   <dimension ref="A1:G34"/>
   <sheetViews>
@@ -31804,7 +33203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E80EDE8-D86E-1440-915D-7FDF56424186}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -32059,891 +33458,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF980A1E-67C8-2046-AD3D-9A8AA002E628}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>761</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>844</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>845</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>846</v>
-      </c>
-      <c r="B4">
-        <v>250</v>
-      </c>
-      <c r="C4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>847</v>
-      </c>
-      <c r="B5">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>848</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>849</v>
-      </c>
-      <c r="B7">
-        <v>10000</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
-  <dimension ref="A1:L20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>760</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>915</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>814</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2088</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>2089</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>2090</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>2091</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>2160</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I2" s="20">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L2" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I3" s="20">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>9</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L3" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I4" s="20">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>9</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L4" s="1">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I5" s="20">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L5" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I6" s="20">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>9</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L6" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I7" s="20">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L7" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I8" s="20">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>9</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L8" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I9" s="20">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>9</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L9" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>831</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I10" s="20">
-        <v>4</v>
-      </c>
-      <c r="J10">
-        <v>9</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L10" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>832</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I11" s="20">
-        <v>4</v>
-      </c>
-      <c r="J11">
-        <v>9</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L11" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I12" s="20">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>9</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L12" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I13" s="20">
-        <v>4</v>
-      </c>
-      <c r="J13">
-        <v>9</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L13" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>836</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I14" s="20">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>9</v>
-      </c>
-      <c r="K14" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L14" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I15" s="20">
-        <v>4</v>
-      </c>
-      <c r="J15">
-        <v>9</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L15" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I16" s="20">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>9</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L16" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I17" s="20">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>9</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L17" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>840</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I18" s="20">
-        <v>4</v>
-      </c>
-      <c r="J18">
-        <v>9</v>
-      </c>
-      <c r="K18" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L18" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>1783</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1784</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I19" s="20">
-        <v>4</v>
-      </c>
-      <c r="J19">
-        <v>9</v>
-      </c>
-      <c r="K19" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L19" s="1">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>1783</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1785</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>2092</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>2093</v>
-      </c>
-      <c r="I20" s="20">
-        <v>4</v>
-      </c>
-      <c r="J20">
-        <v>9</v>
-      </c>
-      <c r="K20" s="20" t="s">
-        <v>816</v>
-      </c>
-      <c r="L20" s="1">
-        <v>325</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.eliquidshop.cz/vyrobce-wotofo-a1010/" xr:uid="{1A4BF3B4-D652-724B-882E-1BE1A013DDE7}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.eliquidshop.cz/vyrobce-sirius-mods-a1532/" xr:uid="{08F874F6-F6B3-B54F-BB43-99630EE8986F}"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.eliquidshop.cz/vyrobce-dotmod-a923/" xr:uid="{73DF1D56-B8D3-8248-8925-E785AC0DE759}"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{4693CF94-0CE9-8D4B-9B83-A044C6AFA279}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Improved ACL, refactored endpoints, turned off locks - preparing for a bit better implementation
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F91B9E7-B3F0-44DE-B027-CBE9B512AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF824E3-B6EB-4C88-BE6F-31AEFAE1369F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1545" windowWidth="27900" windowHeight="19890" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="1755" windowWidth="27900" windowHeight="19890" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -9031,9 +9031,6 @@
     <t>aroma.delete</t>
   </si>
   <si>
-    <t>Market - Common</t>
-  </si>
-  <si>
     <t>MPLQ-N7J74F-GQL7HZ2Q</t>
   </si>
   <si>
@@ -9055,12 +9052,6 @@
     <t>Aromata - mazání</t>
   </si>
   <si>
-    <t>Market - Trader</t>
-  </si>
-  <si>
-    <t>Market - Root</t>
-  </si>
-  <si>
     <t>OCTB-RT4QIX-AH9QMUQD</t>
   </si>
   <si>
@@ -9157,16 +9148,25 @@
     <t>Boostery - mazání</t>
   </si>
   <si>
-    <t>Lab - Common</t>
-  </si>
-  <si>
-    <t>Inventory - Common</t>
-  </si>
-  <si>
     <t>PNLB-D99YV9-T60LOHX6</t>
   </si>
   <si>
     <t>LIHH-35UZC2-BZV78JMZ</t>
+  </si>
+  <si>
+    <t>market.common</t>
+  </si>
+  <si>
+    <t>market.trader</t>
+  </si>
+  <si>
+    <t>market.root</t>
+  </si>
+  <si>
+    <t>lab.common</t>
+  </si>
+  <si>
+    <t>inventory.common</t>
   </si>
 </sst>
 </file>
@@ -28061,10 +28061,10 @@
         <v>0</v>
       </c>
       <c r="B1406" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="C1406" s="1" t="s">
         <v>2916</v>
-      </c>
-      <c r="C1406" s="1" t="s">
-        <v>2917</v>
       </c>
     </row>
     <row r="1407" spans="1:3" x14ac:dyDescent="0.25">
@@ -28072,10 +28072,10 @@
         <v>0</v>
       </c>
       <c r="B1407" s="1" t="s">
+        <v>2917</v>
+      </c>
+      <c r="C1407" s="1" t="s">
         <v>2918</v>
-      </c>
-      <c r="C1407" s="1" t="s">
-        <v>2919</v>
       </c>
     </row>
     <row r="1408" spans="1:3" x14ac:dyDescent="0.25">
@@ -28083,10 +28083,10 @@
         <v>0</v>
       </c>
       <c r="B1408" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="C1408" s="1" t="s">
         <v>2920</v>
-      </c>
-      <c r="C1408" s="1" t="s">
-        <v>2921</v>
       </c>
     </row>
     <row r="1409" spans="1:3" x14ac:dyDescent="0.25">
@@ -28094,10 +28094,10 @@
         <v>0</v>
       </c>
       <c r="B1409" s="1" t="s">
-        <v>2938</v>
+        <v>2935</v>
       </c>
       <c r="C1409" s="1" t="s">
-        <v>2939</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="1410" spans="1:3" x14ac:dyDescent="0.25">
@@ -28105,10 +28105,10 @@
         <v>0</v>
       </c>
       <c r="B1410" s="1" t="s">
-        <v>2940</v>
+        <v>2937</v>
       </c>
       <c r="C1410" s="1" t="s">
-        <v>2941</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="1411" spans="1:3" x14ac:dyDescent="0.25">
@@ -28116,10 +28116,10 @@
         <v>0</v>
       </c>
       <c r="B1411" s="1" t="s">
-        <v>2942</v>
+        <v>2939</v>
       </c>
       <c r="C1411" s="1" t="s">
-        <v>2943</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="1412" spans="1:3" x14ac:dyDescent="0.25">
@@ -28127,10 +28127,10 @@
         <v>0</v>
       </c>
       <c r="B1412" s="1" t="s">
-        <v>2944</v>
+        <v>2941</v>
       </c>
       <c r="C1412" s="1" t="s">
-        <v>2945</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="1413" spans="1:3" x14ac:dyDescent="0.25">
@@ -28138,10 +28138,10 @@
         <v>0</v>
       </c>
       <c r="B1413" s="1" t="s">
-        <v>2946</v>
+        <v>2943</v>
       </c>
       <c r="C1413" s="1" t="s">
-        <v>2947</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="1414" spans="1:3" x14ac:dyDescent="0.25">
@@ -28149,10 +28149,10 @@
         <v>0</v>
       </c>
       <c r="B1414" s="1" t="s">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="C1414" s="1" t="s">
-        <v>2949</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="1415" spans="1:3" x14ac:dyDescent="0.25">
@@ -28160,10 +28160,10 @@
         <v>0</v>
       </c>
       <c r="B1415" s="1" t="s">
-        <v>2950</v>
+        <v>2947</v>
       </c>
       <c r="C1415" s="1" t="s">
-        <v>2951</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="1416" spans="1:3" x14ac:dyDescent="0.25">
@@ -28171,10 +28171,10 @@
         <v>0</v>
       </c>
       <c r="B1416" s="1" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="C1416" s="1" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="1417" spans="1:3" x14ac:dyDescent="0.25">
@@ -28182,10 +28182,10 @@
         <v>0</v>
       </c>
       <c r="B1417" s="1" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="C1417" s="1" t="s">
-        <v>2955</v>
+        <v>2952</v>
       </c>
     </row>
   </sheetData>
@@ -28283,47 +28283,47 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>2926</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>2927</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>2928</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>2929</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>2930</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>2931</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>2932</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>2933</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>2934</v>
+        <v>2931</v>
       </c>
     </row>
   </sheetData>
@@ -28371,72 +28371,72 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2955</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2914</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2915</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2922</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2925</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>2936</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2923</v>
+        <v>2957</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2924</v>
+        <v>2921</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>2937</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2956</v>
+        <v>2958</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2959</v>
+        <v>2954</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2957</v>
+        <v>2959</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2958</v>
+        <v>2953</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>2935</v>
+        <v>2932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite an improvement; fixed certificate bug
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,31 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D16777-E9F6-4B68-8C41-546B3197A88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88FEBCE-7181-4E6D-9D86-61DE2D79D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="660" windowWidth="30510" windowHeight="19890" firstSheet="6" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="375" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
     <sheet name="translations" sheetId="3" r:id="rId2"/>
-    <sheet name="tokens" sheetId="27" r:id="rId3"/>
-    <sheet name="certificates" sheetId="28" r:id="rId4"/>
-    <sheet name="licenses" sheetId="26" r:id="rId5"/>
-    <sheet name="wires" sheetId="25" r:id="rId6"/>
-    <sheet name="fibers" sheetId="24" r:id="rId7"/>
-    <sheet name="aromas" sheetId="23" r:id="rId8"/>
-    <sheet name="boosters" sheetId="22" r:id="rId9"/>
-    <sheet name="bases" sheetId="21" r:id="rId10"/>
-    <sheet name="vouchers" sheetId="20" r:id="rId11"/>
-    <sheet name="atomizers" sheetId="19" r:id="rId12"/>
-    <sheet name="mods" sheetId="18" r:id="rId13"/>
-    <sheet name="cottons" sheetId="17" r:id="rId14"/>
-    <sheet name="tags" sheetId="16" r:id="rId15"/>
-    <sheet name="cells" sheetId="15" r:id="rId16"/>
-    <sheet name="vendors" sheetId="14" r:id="rId17"/>
-    <sheet name="prices" sheetId="13" r:id="rId18"/>
-    <sheet name="tariffs" sheetId="12" r:id="rId19"/>
-    <sheet name="Translations - Common" sheetId="4" r:id="rId20"/>
+    <sheet name="Translations - Common" sheetId="4" r:id="rId3"/>
+    <sheet name="tokens" sheetId="27" r:id="rId4"/>
+    <sheet name="certificates" sheetId="28" r:id="rId5"/>
+    <sheet name="licenses" sheetId="26" r:id="rId6"/>
+    <sheet name="wires" sheetId="25" r:id="rId7"/>
+    <sheet name="fibers" sheetId="24" r:id="rId8"/>
+    <sheet name="aromas" sheetId="23" r:id="rId9"/>
+    <sheet name="boosters" sheetId="22" r:id="rId10"/>
+    <sheet name="bases" sheetId="21" r:id="rId11"/>
+    <sheet name="vouchers" sheetId="20" r:id="rId12"/>
+    <sheet name="atomizers" sheetId="19" r:id="rId13"/>
+    <sheet name="mods" sheetId="18" r:id="rId14"/>
+    <sheet name="cottons" sheetId="17" r:id="rId15"/>
+    <sheet name="tags" sheetId="16" r:id="rId16"/>
+    <sheet name="cells" sheetId="15" r:id="rId17"/>
+    <sheet name="vendors" sheetId="14" r:id="rId18"/>
+    <sheet name="prices" sheetId="13" r:id="rId19"/>
+    <sheet name="tariffs" sheetId="12" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5679" uniqueCount="3017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5800" uniqueCount="3085">
   <si>
     <t>cs</t>
   </si>
@@ -9339,6 +9339,210 @@
   </si>
   <si>
     <t>certificate.feature.booster.create</t>
+  </si>
+  <si>
+    <t>feature.premium.aroma.create</t>
+  </si>
+  <si>
+    <t>feature.premium.booster.create</t>
+  </si>
+  <si>
+    <t>feature.premium.base.create</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.aroma.create</t>
+  </si>
+  <si>
+    <t>Vytváření aromat - premium</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.base.create</t>
+  </si>
+  <si>
+    <t>Vytváření bází - premium</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.booster.create</t>
+  </si>
+  <si>
+    <t>Vytváření boosterů - premium</t>
+  </si>
+  <si>
+    <t>FQJD-O4X59X-A4WK0W7S</t>
+  </si>
+  <si>
+    <t>IHXH-YDB3EB-KSMJ74PN</t>
+  </si>
+  <si>
+    <t>OSVT-GLTRRH-40FMUBYV</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.aroma.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření aromat - premium</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.base.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření bází - premium</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.booster.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření boosterů - premium</t>
+  </si>
+  <si>
+    <t>root.user.certificate.pending.list</t>
+  </si>
+  <si>
+    <t>Certifikáty ke schválení</t>
+  </si>
+  <si>
+    <t>root.user.license.pending.list</t>
+  </si>
+  <si>
+    <t>Licence ke schválení</t>
+  </si>
+  <si>
+    <t>root.user.certificate.pending.title</t>
+  </si>
+  <si>
+    <t>root.user.license.pending.title</t>
+  </si>
+  <si>
+    <t>feature.certificate.create</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.403.title</t>
+  </si>
+  <si>
+    <t>shared.certificate.create.403.subtitle</t>
+  </si>
+  <si>
+    <t>Certifikáty smí vytvářet jen opravdu vyvolení, jelikož mají hluboký dopad na celou komunitu. Pokud máte pocit, že patříte mezi ty, kdož mají toto právo mít, víte, na koho se obrátit.</t>
+  </si>
+  <si>
+    <t>certificate.feature.certificate.create</t>
+  </si>
+  <si>
+    <t>Vytváření certifikátů</t>
+  </si>
+  <si>
+    <t>certificate.feature.license.create</t>
+  </si>
+  <si>
+    <t>Vytváření licencí</t>
+  </si>
+  <si>
+    <t>common.token.feature.certificate.create</t>
+  </si>
+  <si>
+    <t>common.token.feature.license.create</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.certificate.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření certifikátů</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.license.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření licencí</t>
+  </si>
+  <si>
+    <t>IHPO-7LQ2PR-0A4L8UFX</t>
+  </si>
+  <si>
+    <t>shared.license.create.403.title</t>
+  </si>
+  <si>
+    <t>shared.license.create.403.subtitle</t>
+  </si>
+  <si>
+    <t>Licence smí vytvářet jen opravdu vyvolení, jelikož mají hluboký dopad na celou komunitu. Pokud máte pocit, že patříte mezi ty, kdož mají toto právo mít, víte, na koho se obrátit.</t>
+  </si>
+  <si>
+    <t>feature.license.create</t>
+  </si>
+  <si>
+    <t>QNPX-9B30MU-4HSWU14V</t>
+  </si>
+  <si>
+    <t>feature.cotton.create</t>
+  </si>
+  <si>
+    <t>feature.premium.cotton.create</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.cotton.create</t>
+  </si>
+  <si>
+    <t>Vytváření vat</t>
+  </si>
+  <si>
+    <t>common.token.feature.cotton.create</t>
+  </si>
+  <si>
+    <t>Vytváření vat - premium</t>
+  </si>
+  <si>
+    <t>certificate.feature.cotton.create</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.cotton.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření vat - premium</t>
+  </si>
+  <si>
+    <t>feature.wire.create</t>
+  </si>
+  <si>
+    <t>feature.premium.wire.create</t>
+  </si>
+  <si>
+    <t>OJBZ-HJOBIG-PSO1EOHM</t>
+  </si>
+  <si>
+    <t>BSSW-TCE1L2-JXCRYIK4</t>
+  </si>
+  <si>
+    <t>SBEL-6BKIVQ-TQLSAHHW</t>
+  </si>
+  <si>
+    <t>YFLA-YJYZJ7-TU31Z10I</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.wire.create</t>
+  </si>
+  <si>
+    <t>Vytváření odporových drátů</t>
+  </si>
+  <si>
+    <t>common.token.feature.wire.create</t>
+  </si>
+  <si>
+    <t>Vytváření odporových drátů - premium</t>
+  </si>
+  <si>
+    <t>certificate.feature.wire.create</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.wire.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření odporových drátů - premium</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.wire.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření odporových drátů</t>
   </si>
 </sst>
 </file>
@@ -9750,7 +9954,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9903,7 +10107,7 @@
         <v>2906</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2986</v>
       </c>
@@ -9917,6 +10121,811 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C57C95-A5C9-A44A-8F61-B6758048128A}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C2" s="1">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C3" s="1">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C4" s="1">
+        <v>80</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C6" s="1">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C7" s="1">
+        <v>70</v>
+      </c>
+      <c r="D7" s="1">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C9" s="1">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="C10" s="1">
+        <v>70</v>
+      </c>
+      <c r="D10" s="1">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C11" s="1">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>70</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C15" s="1">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C16" s="1">
+        <v>70</v>
+      </c>
+      <c r="D16" s="1">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C17" s="1">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C20" s="1">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C21" s="1">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C22" s="1">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1">
+        <v>50</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C23" s="1">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="C24" s="1">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C25" s="1">
+        <v>80</v>
+      </c>
+      <c r="D25" s="1">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="C26" s="1">
+        <v>80</v>
+      </c>
+      <c r="D26" s="1">
+        <v>20</v>
+      </c>
+      <c r="E26" s="1">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C27" s="1">
+        <v>80</v>
+      </c>
+      <c r="D27" s="1">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="C28" s="1">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1">
+        <v>20</v>
+      </c>
+      <c r="E28" s="1">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C29" s="1">
+        <v>100</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C30" s="1">
+        <v>100</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C31" s="1">
+        <v>100</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>18</v>
+      </c>
+      <c r="F31" s="1">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <v>10</v>
+      </c>
+      <c r="G32" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C33" s="1">
+        <v>70</v>
+      </c>
+      <c r="D33" s="1">
+        <v>30</v>
+      </c>
+      <c r="E33" s="1">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C34" s="1">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1">
+        <v>20</v>
+      </c>
+      <c r="F34" s="1">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G34">
+    <sortCondition ref="A34"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E80EDE8-D86E-1440-915D-7FDF56424186}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -10173,7 +11182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF980A1E-67C8-2046-AD3D-9A8AA002E628}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -10269,7 +11278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A9EA1-F6CF-6346-8A17-7891419B5135}">
   <dimension ref="A1:L20"/>
   <sheetViews>
@@ -11060,7 +12069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D757F10-66C2-2941-A49E-7F0FD3F6574C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -11240,7 +12249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F5805-0158-F34C-9256-85EB751C6431}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -11443,7 +12452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4AAFD-DDA3-854E-A875-1A43B8D00CFD}">
   <dimension ref="A1:C67"/>
   <sheetViews>
@@ -12202,7 +13211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243831E-E3E3-1C43-AE4D-34D8FEF2F724}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -12344,7 +13353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A191A5-B33F-C743-ACA0-85AFF1A1A94D}">
   <dimension ref="A1:A105"/>
   <sheetViews>
@@ -12890,7 +13899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1AB5C-3BBA-9E49-B566-51FB3B75CDAA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -12971,54 +13980,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1822C792-D890-E542-B44B-A4E33F805828}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>649</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>650</v>
-      </c>
-      <c r="B2" t="s">
-        <v>651</v>
-      </c>
-      <c r="C2" t="s">
-        <v>652</v>
-      </c>
-      <c r="D2" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -13074,12 +14035,60 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1822C792-D890-E542-B44B-A4E33F805828}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>650</v>
+      </c>
+      <c r="B2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C2" t="s">
+        <v>652</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1461"/>
+  <dimension ref="A1:C1491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1426" workbookViewId="0">
-      <selection activeCell="B1438" sqref="B1438"/>
+    <sheetView tabSelected="1" topLeftCell="A1456" workbookViewId="0">
+      <selection activeCell="B1474" sqref="B1474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29160,6 +30169,336 @@
         <v>2992</v>
       </c>
     </row>
+    <row r="1462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1462" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1462" s="1" t="s">
+        <v>3020</v>
+      </c>
+      <c r="C1462" s="1" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1463" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1463" s="1" t="s">
+        <v>3022</v>
+      </c>
+      <c r="C1463" s="1" t="s">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1464" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1464" s="1" t="s">
+        <v>3024</v>
+      </c>
+      <c r="C1464" s="1" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1465" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1465" s="1" t="s">
+        <v>3029</v>
+      </c>
+      <c r="C1465" s="1" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1466" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1466" s="1" t="s">
+        <v>3031</v>
+      </c>
+      <c r="C1466" s="1" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1467" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1467" s="1" t="s">
+        <v>3033</v>
+      </c>
+      <c r="C1467" s="1" t="s">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1468" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1468" s="1" t="s">
+        <v>3035</v>
+      </c>
+      <c r="C1468" s="1" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1469" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1469" s="1" t="s">
+        <v>3037</v>
+      </c>
+      <c r="C1469" s="1" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1470" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1470" s="1" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C1470" s="1" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1471" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1471" s="1" t="s">
+        <v>3040</v>
+      </c>
+      <c r="C1471" s="1" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1472" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1472" s="1" t="s">
+        <v>3042</v>
+      </c>
+      <c r="C1472" s="1" t="s">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1473" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1473" s="1" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C1473" s="1" t="s">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1474" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1474" s="1" t="s">
+        <v>3045</v>
+      </c>
+      <c r="C1474" s="1" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1475" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1475" s="1" t="s">
+        <v>3047</v>
+      </c>
+      <c r="C1475" s="1" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1476" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1476" s="1" t="s">
+        <v>3049</v>
+      </c>
+      <c r="C1476" s="1" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1477" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1477" s="1" t="s">
+        <v>3050</v>
+      </c>
+      <c r="C1477" s="1" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1478" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1478" s="1" t="s">
+        <v>3051</v>
+      </c>
+      <c r="C1478" s="1" t="s">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1479" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1479" s="1" t="s">
+        <v>3053</v>
+      </c>
+      <c r="C1479" s="1" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1480" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1480" s="1" t="s">
+        <v>3056</v>
+      </c>
+      <c r="C1480" s="1" t="s">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1481" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1481" s="1" t="s">
+        <v>3057</v>
+      </c>
+      <c r="C1481" s="1" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1482" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1482" s="1" t="s">
+        <v>3063</v>
+      </c>
+      <c r="C1482" s="1" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1483" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1483" s="1" t="s">
+        <v>3065</v>
+      </c>
+      <c r="C1483" s="1" t="s">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1484" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1484" s="1" t="s">
+        <v>3067</v>
+      </c>
+      <c r="C1484" s="1" t="s">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1485" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1485" s="1" t="s">
+        <v>3068</v>
+      </c>
+      <c r="C1485" s="1" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1486" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1486" s="1" t="s">
+        <v>3065</v>
+      </c>
+      <c r="C1486" s="1" t="s">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1487" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1487" s="1" t="s">
+        <v>3076</v>
+      </c>
+      <c r="C1487" s="1" t="s">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1488" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1488" s="1" t="s">
+        <v>3078</v>
+      </c>
+      <c r="C1488" s="1" t="s">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1489" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1489" s="1" t="s">
+        <v>3080</v>
+      </c>
+      <c r="C1489" s="1" t="s">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1490" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1490" s="1" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C1490" s="1" t="s">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1491" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1491" s="1" t="s">
+        <v>3083</v>
+      </c>
+      <c r="C1491" s="1" t="s">
+        <v>3084</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C570">
     <sortCondition ref="B565:B570"/>
@@ -29169,12 +30508,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FD4C38-64C5-40ED-9AD4-3F08781E6BBE}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29189,52 +30528,75 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2970</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2971</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2981</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2985</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2990</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3004</v>
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3070</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A11">
+    <sortCondition ref="A9:A11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567AEF47-34EE-46D6-8A5D-571208809931}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="93.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29266,35 +30628,156 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2990</v>
+        <v>3004</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>2990</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3004</v>
+        <v>2990</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3007</v>
+        <v>3008</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3055</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3026</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>3004</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="C8" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>3061</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3072</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3073</v>
+      </c>
+      <c r="C11" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3070</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3074</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>3071</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3075</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3070</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
+    <sortCondition ref="A2:A8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48874847-D5A5-4B4C-B8BE-D757A1E415A7}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -29398,7 +30881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F7C88A-203F-48DC-ACBE-CE6221C44C48}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -29733,7 +31216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E518C2-9F69-674D-A844-F8C5F8F0CAF4}">
   <dimension ref="A1:D162"/>
   <sheetViews>
@@ -31587,7 +33070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA812A1B-B2A0-8945-A642-5E37B3E27690}">
   <dimension ref="A1:I60"/>
   <sheetViews>
@@ -33349,809 +34832,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C57C95-A5C9-A44A-8F61-B6758048128A}">
-  <dimension ref="A1:G34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>864</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1238</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1239</v>
-      </c>
-      <c r="C3" s="1">
-        <v>70</v>
-      </c>
-      <c r="D3" s="1">
-        <v>30</v>
-      </c>
-      <c r="E3" s="1">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C4" s="1">
-        <v>80</v>
-      </c>
-      <c r="D4" s="1">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1244</v>
-      </c>
-      <c r="C5" s="1">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C6" s="1">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1">
-        <v>60</v>
-      </c>
-      <c r="E6" s="1">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>868</v>
-      </c>
-      <c r="C7" s="1">
-        <v>70</v>
-      </c>
-      <c r="D7" s="1">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C8" s="1">
-        <v>70</v>
-      </c>
-      <c r="D8" s="1">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>867</v>
-      </c>
-      <c r="C9" s="1">
-        <v>70</v>
-      </c>
-      <c r="D9" s="1">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="C10" s="1">
-        <v>70</v>
-      </c>
-      <c r="D10" s="1">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>870</v>
-      </c>
-      <c r="C11" s="1">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1">
-        <v>50</v>
-      </c>
-      <c r="E11" s="1">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C12" s="1">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1">
-        <v>50</v>
-      </c>
-      <c r="E12" s="1">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>869</v>
-      </c>
-      <c r="C13" s="1">
-        <v>50</v>
-      </c>
-      <c r="D13" s="1">
-        <v>50</v>
-      </c>
-      <c r="E13" s="1">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>881</v>
-      </c>
-      <c r="C14" s="1">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1">
-        <v>70</v>
-      </c>
-      <c r="E14" s="1">
-        <v>20</v>
-      </c>
-      <c r="F14" s="1">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1233</v>
-      </c>
-      <c r="C15" s="1">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1">
-        <v>50</v>
-      </c>
-      <c r="E15" s="1">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <v>10</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C16" s="1">
-        <v>70</v>
-      </c>
-      <c r="D16" s="1">
-        <v>30</v>
-      </c>
-      <c r="E16" s="1">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C17" s="1">
-        <v>70</v>
-      </c>
-      <c r="D17" s="1">
-        <v>30</v>
-      </c>
-      <c r="E17" s="1">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1234</v>
-      </c>
-      <c r="C18" s="1">
-        <v>70</v>
-      </c>
-      <c r="D18" s="1">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1">
-        <v>6</v>
-      </c>
-      <c r="F18" s="1">
-        <v>10</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C19" s="1">
-        <v>50</v>
-      </c>
-      <c r="D19" s="1">
-        <v>50</v>
-      </c>
-      <c r="E19" s="1">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C20" s="1">
-        <v>50</v>
-      </c>
-      <c r="D20" s="1">
-        <v>50</v>
-      </c>
-      <c r="E20" s="1">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1">
-        <v>10</v>
-      </c>
-      <c r="G20" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="C21" s="1">
-        <v>50</v>
-      </c>
-      <c r="D21" s="1">
-        <v>50</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
-      </c>
-      <c r="F21" s="1">
-        <v>10</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C22" s="1">
-        <v>50</v>
-      </c>
-      <c r="D22" s="1">
-        <v>50</v>
-      </c>
-      <c r="E22" s="1">
-        <v>6</v>
-      </c>
-      <c r="F22" s="1">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>880</v>
-      </c>
-      <c r="C23" s="1">
-        <v>80</v>
-      </c>
-      <c r="D23" s="1">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1">
-        <v>10</v>
-      </c>
-      <c r="G23" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>878</v>
-      </c>
-      <c r="C24" s="1">
-        <v>80</v>
-      </c>
-      <c r="D24" s="1">
-        <v>20</v>
-      </c>
-      <c r="E24" s="1">
-        <v>12</v>
-      </c>
-      <c r="F24" s="1">
-        <v>10</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="C25" s="1">
-        <v>80</v>
-      </c>
-      <c r="D25" s="1">
-        <v>20</v>
-      </c>
-      <c r="E25" s="1">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1">
-        <v>10</v>
-      </c>
-      <c r="G25" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>877</v>
-      </c>
-      <c r="C26" s="1">
-        <v>80</v>
-      </c>
-      <c r="D26" s="1">
-        <v>20</v>
-      </c>
-      <c r="E26" s="1">
-        <v>18</v>
-      </c>
-      <c r="F26" s="1">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>875</v>
-      </c>
-      <c r="C27" s="1">
-        <v>80</v>
-      </c>
-      <c r="D27" s="1">
-        <v>20</v>
-      </c>
-      <c r="E27" s="1">
-        <v>20</v>
-      </c>
-      <c r="F27" s="1">
-        <v>10</v>
-      </c>
-      <c r="G27" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="C28" s="1">
-        <v>80</v>
-      </c>
-      <c r="D28" s="1">
-        <v>20</v>
-      </c>
-      <c r="E28" s="1">
-        <v>6</v>
-      </c>
-      <c r="F28" s="1">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="C29" s="1">
-        <v>100</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>10</v>
-      </c>
-      <c r="F29" s="1">
-        <v>10</v>
-      </c>
-      <c r="G29" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="C30" s="1">
-        <v>100</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>15</v>
-      </c>
-      <c r="F30" s="1">
-        <v>10</v>
-      </c>
-      <c r="G30" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1228</v>
-      </c>
-      <c r="C31" s="1">
-        <v>100</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>18</v>
-      </c>
-      <c r="F31" s="1">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="C32" s="1">
-        <v>100</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1">
-        <v>10</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="C33" s="1">
-        <v>70</v>
-      </c>
-      <c r="D33" s="1">
-        <v>30</v>
-      </c>
-      <c r="E33" s="1">
-        <v>18</v>
-      </c>
-      <c r="F33" s="1">
-        <v>10</v>
-      </c>
-      <c r="G33" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C34" s="1">
-        <v>50</v>
-      </c>
-      <c r="D34" s="1">
-        <v>50</v>
-      </c>
-      <c r="E34" s="1">
-        <v>20</v>
-      </c>
-      <c r="F34" s="1">
-        <v>10</v>
-      </c>
-      <c r="G34" s="1">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G34">
-    <sortCondition ref="A34"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Another little fixes
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88FEBCE-7181-4E6D-9D86-61DE2D79D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B90C13C-1EEC-4984-978F-C82FE04BF358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="375" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14088,7 +14088,7 @@
   <dimension ref="A1:C1491"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1456" workbookViewId="0">
-      <selection activeCell="B1474" sqref="B1474"/>
+      <selection activeCell="C1462" sqref="C1462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Improved UI a bit
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B90C13C-1EEC-4984-978F-C82FE04BF358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855427C4-AAE1-4F78-AFB0-0534C856555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="375" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5800" uniqueCount="3085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5855" uniqueCount="3108">
   <si>
     <t>cs</t>
   </si>
@@ -9543,6 +9543,75 @@
   </si>
   <si>
     <t>Certifikát - Vytváření odporových drátů</t>
+  </si>
+  <si>
+    <t>feature.mixture.info.lifetime</t>
+  </si>
+  <si>
+    <t>feature.mixture.search.lifetime</t>
+  </si>
+  <si>
+    <t>license.feature.mixture.info.lifetime</t>
+  </si>
+  <si>
+    <t>Vyhledávání mixů - permanentní</t>
+  </si>
+  <si>
+    <t>license.feature.mixture.search.lifetime</t>
+  </si>
+  <si>
+    <t>Kalkulačka mixů - permanentní</t>
+  </si>
+  <si>
+    <t>common.token.license.feature.mixture.info.lifetime</t>
+  </si>
+  <si>
+    <t>Licence - Kalkulačka mixů - permanentní</t>
+  </si>
+  <si>
+    <t>common.token.license.feature.mixture.search.lifetime</t>
+  </si>
+  <si>
+    <t>Licence - Vyhledávání mixů - permanentní</t>
+  </si>
+  <si>
+    <t>common.filter.MixtureMarket.filter.403.title</t>
+  </si>
+  <si>
+    <t>common.filter.MixtureMarket.filter.403.subtitle</t>
+  </si>
+  <si>
+    <t>lab.mixture.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.label</t>
+  </si>
+  <si>
+    <t>market.base.label</t>
+  </si>
+  <si>
+    <t>market.booster.label</t>
+  </si>
+  <si>
+    <t>market.cotton.label</t>
+  </si>
+  <si>
+    <t>market.wire.label</t>
+  </si>
+  <si>
+    <t>market.atomizer.label</t>
+  </si>
+  <si>
+    <t>market.cell.label</t>
+  </si>
+  <si>
+    <t>market.mod.label</t>
+  </si>
+  <si>
+    <t>market.voucher.label</t>
+  </si>
+  <si>
+    <t>market.vendor.label</t>
   </si>
 </sst>
 </file>
@@ -14085,10 +14154,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1491"/>
+  <dimension ref="A1:C1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1456" workbookViewId="0">
-      <selection activeCell="C1462" sqref="C1462"/>
+    <sheetView tabSelected="1" topLeftCell="A1477" workbookViewId="0">
+      <selection activeCell="B1495" sqref="B1495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30497,6 +30566,193 @@
       </c>
       <c r="C1491" s="1" t="s">
         <v>3084</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1492" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1492" s="1" t="s">
+        <v>3087</v>
+      </c>
+      <c r="C1492" s="1" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1493" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1493" s="1" t="s">
+        <v>3089</v>
+      </c>
+      <c r="C1493" s="1" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1494" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1494" s="1" t="s">
+        <v>3091</v>
+      </c>
+      <c r="C1494" s="1" t="s">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1495" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1495" s="1" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C1495" s="1" t="s">
+        <v>3094</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1496" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1496" s="1" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C1496" s="1" t="s">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1497" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1497" s="1" t="s">
+        <v>3096</v>
+      </c>
+      <c r="C1497" s="1" t="s">
+        <v>2969</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1498" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1498" s="1" t="s">
+        <v>3097</v>
+      </c>
+      <c r="C1498" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1499" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1499" s="1" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C1499" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1500" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1500" s="1" t="s">
+        <v>3099</v>
+      </c>
+      <c r="C1500" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1501" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1501" s="1" t="s">
+        <v>3100</v>
+      </c>
+      <c r="C1501" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1502" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1502" s="1" t="s">
+        <v>3101</v>
+      </c>
+      <c r="C1502" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1503" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1503" s="1" t="s">
+        <v>3102</v>
+      </c>
+      <c r="C1503" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1504" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1504" s="1" t="s">
+        <v>3103</v>
+      </c>
+      <c r="C1504" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1505" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1505" s="1" t="s">
+        <v>3104</v>
+      </c>
+      <c r="C1505" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1506" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1506" s="1" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C1506" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1507" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1507" s="1" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C1507" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1508" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1508" s="1" t="s">
+        <v>3107</v>
+      </c>
+      <c r="C1508" s="1" t="s">
+        <v>1879</v>
       </c>
     </row>
   </sheetData>
@@ -30779,15 +31035,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48874847-D5A5-4B4C-B8BE-D757A1E415A7}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
@@ -30873,6 +31129,34 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>2981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3085</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>15000</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>2971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added comments to public aromas
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855427C4-AAE1-4F78-AFB0-0534C856555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8FA215-6F04-492A-BD8F-FCFCE3D7A2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="375" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="510" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5855" uniqueCount="3108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5864" uniqueCount="3114">
   <si>
     <t>cs</t>
   </si>
@@ -7861,9 +7861,6 @@
     <t>lab.build.comment.comment.label</t>
   </si>
   <si>
-    <t>Napište si komentář k buildu.</t>
-  </si>
-  <si>
     <t>lab.build.comment.comment</t>
   </si>
   <si>
@@ -7985,9 +7982,6 @@
   </si>
   <si>
     <t>shared.aroma.comment.comment.label</t>
-  </si>
-  <si>
-    <t>Napište si komentář k aromatu.</t>
   </si>
   <si>
     <t>shared.aroma.comment.comment</t>
@@ -9612,6 +9606,30 @@
   </si>
   <si>
     <t>market.vendor.label</t>
+  </si>
+  <si>
+    <t>market.aroma.comment.comment.label</t>
+  </si>
+  <si>
+    <t>Podělte se o veřejný komentář k aromatu.</t>
+  </si>
+  <si>
+    <t>Zveřejnit</t>
+  </si>
+  <si>
+    <t>Napište si soukromý komentář k buildu.</t>
+  </si>
+  <si>
+    <t>Napište si soukromý komentář k aromatu.</t>
+  </si>
+  <si>
+    <t>shared.comment.private.tab</t>
+  </si>
+  <si>
+    <t>Soukromé komentáže</t>
+  </si>
+  <si>
+    <t>market.aroma.comment.comment</t>
   </si>
 </sst>
 </file>
@@ -10162,26 +10180,26 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="B17" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="B18" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="B19" t="s">
-        <v>2989</v>
+        <v>2987</v>
       </c>
     </row>
   </sheetData>
@@ -13208,7 +13226,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
       <c r="B62" t="s">
         <v>980</v>
@@ -13222,7 +13240,7 @@
         <v>812</v>
       </c>
       <c r="B63" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -13233,7 +13251,7 @@
         <v>800</v>
       </c>
       <c r="B64" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -13241,10 +13259,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>2769</v>
+        <v>2767</v>
       </c>
       <c r="B65" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C65">
         <v>100</v>
@@ -13252,10 +13270,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="B66" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -13263,10 +13281,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>2771</v>
+        <v>2769</v>
       </c>
       <c r="B67" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C67">
         <v>10</v>
@@ -14154,10 +14172,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1508"/>
+  <dimension ref="A1:C1511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1477" workbookViewId="0">
-      <selection activeCell="B1495" sqref="B1495"/>
+    <sheetView tabSelected="1" topLeftCell="A1481" workbookViewId="0">
+      <selection activeCell="B1511" sqref="B1511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25087,7 +25105,7 @@
         <v>2130</v>
       </c>
       <c r="C993" s="1" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="994" spans="1:3" x14ac:dyDescent="0.25">
@@ -27573,7 +27591,7 @@
         <v>2535</v>
       </c>
       <c r="C1219" s="1" t="s">
-        <v>2536</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="1220" spans="1:3" x14ac:dyDescent="0.25">
@@ -27581,7 +27599,7 @@
         <v>0</v>
       </c>
       <c r="B1220" s="1" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="C1220" s="1" t="s">
         <v>532</v>
@@ -27592,10 +27610,10 @@
         <v>0</v>
       </c>
       <c r="B1221" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C1221" s="1" t="s">
         <v>2538</v>
-      </c>
-      <c r="C1221" s="1" t="s">
-        <v>2539</v>
       </c>
     </row>
     <row r="1222" spans="1:3" x14ac:dyDescent="0.25">
@@ -27603,10 +27621,10 @@
         <v>0</v>
       </c>
       <c r="B1222" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C1222" s="1" t="s">
         <v>2540</v>
-      </c>
-      <c r="C1222" s="1" t="s">
-        <v>2541</v>
       </c>
     </row>
     <row r="1223" spans="1:3" x14ac:dyDescent="0.25">
@@ -27614,10 +27632,10 @@
         <v>0</v>
       </c>
       <c r="B1223" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C1223" s="1" t="s">
         <v>2542</v>
-      </c>
-      <c r="C1223" s="1" t="s">
-        <v>2543</v>
       </c>
     </row>
     <row r="1224" spans="1:3" x14ac:dyDescent="0.25">
@@ -27625,10 +27643,10 @@
         <v>0</v>
       </c>
       <c r="B1224" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C1224" s="1" t="s">
         <v>2544</v>
-      </c>
-      <c r="C1224" s="1" t="s">
-        <v>2545</v>
       </c>
     </row>
     <row r="1225" spans="1:3" x14ac:dyDescent="0.25">
@@ -27636,7 +27654,7 @@
         <v>0</v>
       </c>
       <c r="B1225" s="1" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="C1225" s="1" t="s">
         <v>1526</v>
@@ -27647,10 +27665,10 @@
         <v>0</v>
       </c>
       <c r="B1226" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C1226" s="1" t="s">
         <v>2547</v>
-      </c>
-      <c r="C1226" s="1" t="s">
-        <v>2548</v>
       </c>
     </row>
     <row r="1227" spans="1:3" x14ac:dyDescent="0.25">
@@ -27658,10 +27676,10 @@
         <v>0</v>
       </c>
       <c r="B1227" s="1" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C1227" s="1" t="s">
         <v>2549</v>
-      </c>
-      <c r="C1227" s="1" t="s">
-        <v>2550</v>
       </c>
     </row>
     <row r="1228" spans="1:3" x14ac:dyDescent="0.25">
@@ -27669,10 +27687,10 @@
         <v>0</v>
       </c>
       <c r="B1228" s="1" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C1228" s="1" t="s">
         <v>2551</v>
-      </c>
-      <c r="C1228" s="1" t="s">
-        <v>2552</v>
       </c>
     </row>
     <row r="1229" spans="1:3" x14ac:dyDescent="0.25">
@@ -27680,10 +27698,10 @@
         <v>0</v>
       </c>
       <c r="B1229" s="1" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C1229" s="1" t="s">
         <v>2553</v>
-      </c>
-      <c r="C1229" s="1" t="s">
-        <v>2554</v>
       </c>
     </row>
     <row r="1230" spans="1:3" x14ac:dyDescent="0.25">
@@ -27691,10 +27709,10 @@
         <v>0</v>
       </c>
       <c r="B1230" s="1" t="s">
+        <v>2554</v>
+      </c>
+      <c r="C1230" s="1" t="s">
         <v>2555</v>
-      </c>
-      <c r="C1230" s="1" t="s">
-        <v>2556</v>
       </c>
     </row>
     <row r="1231" spans="1:3" x14ac:dyDescent="0.25">
@@ -27702,10 +27720,10 @@
         <v>0</v>
       </c>
       <c r="B1231" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="C1231" s="1" t="s">
         <v>2557</v>
-      </c>
-      <c r="C1231" s="1" t="s">
-        <v>2558</v>
       </c>
     </row>
     <row r="1232" spans="1:3" x14ac:dyDescent="0.25">
@@ -27713,10 +27731,10 @@
         <v>0</v>
       </c>
       <c r="B1232" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C1232" s="1" t="s">
         <v>2559</v>
-      </c>
-      <c r="C1232" s="1" t="s">
-        <v>2560</v>
       </c>
     </row>
     <row r="1233" spans="1:3" x14ac:dyDescent="0.25">
@@ -27724,10 +27742,10 @@
         <v>0</v>
       </c>
       <c r="B1233" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C1233" s="1" t="s">
         <v>2561</v>
-      </c>
-      <c r="C1233" s="1" t="s">
-        <v>2562</v>
       </c>
     </row>
     <row r="1234" spans="1:3" x14ac:dyDescent="0.25">
@@ -27735,10 +27753,10 @@
         <v>0</v>
       </c>
       <c r="B1234" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C1234" s="1" t="s">
         <v>2563</v>
-      </c>
-      <c r="C1234" s="1" t="s">
-        <v>2564</v>
       </c>
     </row>
     <row r="1235" spans="1:3" x14ac:dyDescent="0.25">
@@ -27746,10 +27764,10 @@
         <v>0</v>
       </c>
       <c r="B1235" s="1" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="C1235" s="1" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="1236" spans="1:3" x14ac:dyDescent="0.25">
@@ -27757,7 +27775,7 @@
         <v>0</v>
       </c>
       <c r="B1236" s="1" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C1236" s="1" t="s">
         <v>1080</v>
@@ -27768,7 +27786,7 @@
         <v>0</v>
       </c>
       <c r="B1237" s="1" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="C1237" s="1" t="s">
         <v>1526</v>
@@ -27779,7 +27797,7 @@
         <v>0</v>
       </c>
       <c r="B1238" s="1" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="C1238" s="1" t="s">
         <v>470</v>
@@ -27790,7 +27808,7 @@
         <v>0</v>
       </c>
       <c r="B1239" s="1" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="C1239" s="1" t="s">
         <v>1080</v>
@@ -27801,7 +27819,7 @@
         <v>0</v>
       </c>
       <c r="B1240" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="C1240" s="1" t="s">
         <v>1080</v>
@@ -27812,10 +27830,10 @@
         <v>0</v>
       </c>
       <c r="B1241" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C1241" s="1" t="s">
         <v>2571</v>
-      </c>
-      <c r="C1241" s="1" t="s">
-        <v>2572</v>
       </c>
     </row>
     <row r="1242" spans="1:3" x14ac:dyDescent="0.25">
@@ -27823,10 +27841,10 @@
         <v>0</v>
       </c>
       <c r="B1242" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="C1242" s="1" t="s">
         <v>2573</v>
-      </c>
-      <c r="C1242" s="1" t="s">
-        <v>2574</v>
       </c>
     </row>
     <row r="1243" spans="1:3" x14ac:dyDescent="0.25">
@@ -27834,7 +27852,7 @@
         <v>0</v>
       </c>
       <c r="B1243" s="1" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="C1243" s="1" t="s">
         <v>1526</v>
@@ -27845,7 +27863,7 @@
         <v>0</v>
       </c>
       <c r="B1244" s="1" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="C1244" s="1" t="s">
         <v>1526</v>
@@ -27856,10 +27874,10 @@
         <v>0</v>
       </c>
       <c r="B1245" s="1" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="C1245" s="1" t="s">
-        <v>2578</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="1246" spans="1:3" x14ac:dyDescent="0.25">
@@ -27867,7 +27885,7 @@
         <v>0</v>
       </c>
       <c r="B1246" s="1" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
       <c r="C1246" s="1" t="s">
         <v>532</v>
@@ -27878,10 +27896,10 @@
         <v>0</v>
       </c>
       <c r="B1247" s="1" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="C1247" s="1" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="1248" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -27889,10 +27907,10 @@
         <v>0</v>
       </c>
       <c r="B1248" s="1" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
       <c r="C1248" s="1" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="1249" spans="1:3" x14ac:dyDescent="0.25">
@@ -27900,10 +27918,10 @@
         <v>0</v>
       </c>
       <c r="B1249" s="1" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="C1249" s="1" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="1250" spans="1:3" x14ac:dyDescent="0.25">
@@ -27911,10 +27929,10 @@
         <v>0</v>
       </c>
       <c r="B1250" s="1" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="C1250" s="1" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="1251" spans="1:3" x14ac:dyDescent="0.25">
@@ -27922,10 +27940,10 @@
         <v>0</v>
       </c>
       <c r="B1251" s="1" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="C1251" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1252" spans="1:3" x14ac:dyDescent="0.25">
@@ -27933,10 +27951,10 @@
         <v>0</v>
       </c>
       <c r="B1252" s="1" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="C1252" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1253" spans="1:3" x14ac:dyDescent="0.25">
@@ -27944,10 +27962,10 @@
         <v>0</v>
       </c>
       <c r="B1253" s="1" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="C1253" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1254" spans="1:3" x14ac:dyDescent="0.25">
@@ -27955,10 +27973,10 @@
         <v>0</v>
       </c>
       <c r="B1254" s="1" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="C1254" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1255" spans="1:3" x14ac:dyDescent="0.25">
@@ -27966,10 +27984,10 @@
         <v>0</v>
       </c>
       <c r="B1255" s="1" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="C1255" s="1" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="1256" spans="1:3" ht="153.75" x14ac:dyDescent="0.25">
@@ -27977,10 +27995,10 @@
         <v>0</v>
       </c>
       <c r="B1256" s="1" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="C1256" s="1" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="1257" spans="1:3" x14ac:dyDescent="0.25">
@@ -27988,10 +28006,10 @@
         <v>0</v>
       </c>
       <c r="B1257" s="1" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="C1257" s="1" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="1258" spans="1:3" x14ac:dyDescent="0.25">
@@ -27999,10 +28017,10 @@
         <v>0</v>
       </c>
       <c r="B1258" s="1" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="C1258" s="1" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="1259" spans="1:3" x14ac:dyDescent="0.25">
@@ -28010,10 +28028,10 @@
         <v>0</v>
       </c>
       <c r="B1259" s="1" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="C1259" s="1" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="1260" spans="1:3" x14ac:dyDescent="0.25">
@@ -28021,10 +28039,10 @@
         <v>0</v>
       </c>
       <c r="B1260" s="1" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="C1260" s="1" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="1261" spans="1:3" x14ac:dyDescent="0.25">
@@ -28032,7 +28050,7 @@
         <v>0</v>
       </c>
       <c r="B1261" s="1" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
       <c r="C1261" s="1" t="s">
         <v>532</v>
@@ -28043,10 +28061,10 @@
         <v>0</v>
       </c>
       <c r="B1262" s="1" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
       <c r="C1262" s="1" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="1263" spans="1:3" x14ac:dyDescent="0.25">
@@ -28054,10 +28072,10 @@
         <v>0</v>
       </c>
       <c r="B1263" s="1" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
       <c r="C1263" s="1" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="1264" spans="1:3" x14ac:dyDescent="0.25">
@@ -28065,10 +28083,10 @@
         <v>0</v>
       </c>
       <c r="B1264" s="1" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="C1264" s="1" t="s">
-        <v>2647</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="1265" spans="1:3" x14ac:dyDescent="0.25">
@@ -28076,10 +28094,10 @@
         <v>0</v>
       </c>
       <c r="B1265" s="1" t="s">
-        <v>2648</v>
+        <v>2646</v>
       </c>
       <c r="C1265" s="1" t="s">
-        <v>2649</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="1266" spans="1:3" x14ac:dyDescent="0.25">
@@ -28087,10 +28105,10 @@
         <v>0</v>
       </c>
       <c r="B1266" s="1" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="C1266" s="1" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="1267" spans="1:3" x14ac:dyDescent="0.25">
@@ -28098,10 +28116,10 @@
         <v>0</v>
       </c>
       <c r="B1267" s="1" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
       <c r="C1267" s="1" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="1268" spans="1:3" x14ac:dyDescent="0.25">
@@ -28109,10 +28127,10 @@
         <v>0</v>
       </c>
       <c r="B1268" s="1" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
       <c r="C1268" s="1" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="1269" spans="1:3" x14ac:dyDescent="0.25">
@@ -28120,10 +28138,10 @@
         <v>0</v>
       </c>
       <c r="B1269" s="1" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
       <c r="C1269" s="1" t="s">
-        <v>2657</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="1270" spans="1:3" x14ac:dyDescent="0.25">
@@ -28131,7 +28149,7 @@
         <v>0</v>
       </c>
       <c r="B1270" s="1" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
       <c r="C1270" s="1" t="s">
         <v>532</v>
@@ -28142,10 +28160,10 @@
         <v>0</v>
       </c>
       <c r="B1271" s="1" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
       <c r="C1271" s="1" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="1272" spans="1:3" x14ac:dyDescent="0.25">
@@ -28153,10 +28171,10 @@
         <v>0</v>
       </c>
       <c r="B1272" s="1" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="C1272" s="1" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="1273" spans="1:3" x14ac:dyDescent="0.25">
@@ -28164,10 +28182,10 @@
         <v>0</v>
       </c>
       <c r="B1273" s="1" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
       <c r="C1273" s="1" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="1274" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -28175,10 +28193,10 @@
         <v>0</v>
       </c>
       <c r="B1274" s="1" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="C1274" s="1" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="1275" spans="1:3" x14ac:dyDescent="0.25">
@@ -28186,10 +28204,10 @@
         <v>0</v>
       </c>
       <c r="B1275" s="1" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
       <c r="C1275" s="1" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="1276" spans="1:3" x14ac:dyDescent="0.25">
@@ -28197,10 +28215,10 @@
         <v>0</v>
       </c>
       <c r="B1276" s="1" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
       <c r="C1276" s="1" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="1277" spans="1:3" x14ac:dyDescent="0.25">
@@ -28208,7 +28226,7 @@
         <v>0</v>
       </c>
       <c r="B1277" s="1" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
       <c r="C1277" s="1" t="s">
         <v>21</v>
@@ -28219,7 +28237,7 @@
         <v>0</v>
       </c>
       <c r="B1278" s="1" t="s">
-        <v>2672</v>
+        <v>2670</v>
       </c>
       <c r="C1278" s="1" t="s">
         <v>335</v>
@@ -28230,7 +28248,7 @@
         <v>0</v>
       </c>
       <c r="B1279" s="1" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="C1279" s="1" t="s">
         <v>126</v>
@@ -28241,10 +28259,10 @@
         <v>0</v>
       </c>
       <c r="B1280" s="1" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
       <c r="C1280" s="1" t="s">
-        <v>2675</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="1281" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
@@ -28252,10 +28270,10 @@
         <v>0</v>
       </c>
       <c r="B1281" s="1" t="s">
-        <v>2676</v>
+        <v>2674</v>
       </c>
       <c r="C1281" s="1" t="s">
-        <v>2677</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="1282" spans="1:3" x14ac:dyDescent="0.25">
@@ -28263,10 +28281,10 @@
         <v>0</v>
       </c>
       <c r="B1282" s="1" t="s">
-        <v>2678</v>
+        <v>2676</v>
       </c>
       <c r="C1282" s="1" t="s">
-        <v>2679</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="1283" spans="1:3" x14ac:dyDescent="0.25">
@@ -28274,10 +28292,10 @@
         <v>0</v>
       </c>
       <c r="B1283" s="1" t="s">
-        <v>2680</v>
+        <v>2678</v>
       </c>
       <c r="C1283" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1284" spans="1:3" x14ac:dyDescent="0.25">
@@ -28285,10 +28303,10 @@
         <v>0</v>
       </c>
       <c r="B1284" s="1" t="s">
-        <v>2681</v>
+        <v>2679</v>
       </c>
       <c r="C1284" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1285" spans="1:3" x14ac:dyDescent="0.25">
@@ -28296,10 +28314,10 @@
         <v>0</v>
       </c>
       <c r="B1285" s="1" t="s">
-        <v>2682</v>
+        <v>2680</v>
       </c>
       <c r="C1285" s="1" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="1286" spans="1:3" x14ac:dyDescent="0.25">
@@ -28307,10 +28325,10 @@
         <v>0</v>
       </c>
       <c r="B1286" s="1" t="s">
-        <v>2684</v>
+        <v>2682</v>
       </c>
       <c r="C1286" s="1" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="1287" spans="1:3" x14ac:dyDescent="0.25">
@@ -28318,10 +28336,10 @@
         <v>0</v>
       </c>
       <c r="B1287" s="1" t="s">
-        <v>2685</v>
+        <v>2683</v>
       </c>
       <c r="C1287" s="1" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="1288" spans="1:3" x14ac:dyDescent="0.25">
@@ -28329,10 +28347,10 @@
         <v>0</v>
       </c>
       <c r="B1288" s="1" t="s">
-        <v>2687</v>
+        <v>2685</v>
       </c>
       <c r="C1288" s="1" t="s">
-        <v>2688</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="1289" spans="1:3" x14ac:dyDescent="0.25">
@@ -28340,10 +28358,10 @@
         <v>0</v>
       </c>
       <c r="B1289" s="1" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="C1289" s="1" t="s">
-        <v>2690</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="1290" spans="1:3" x14ac:dyDescent="0.25">
@@ -28351,10 +28369,10 @@
         <v>0</v>
       </c>
       <c r="B1290" s="1" t="s">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="C1290" s="1" t="s">
-        <v>2692</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="1291" spans="1:3" x14ac:dyDescent="0.25">
@@ -28362,10 +28380,10 @@
         <v>0</v>
       </c>
       <c r="B1291" s="1" t="s">
-        <v>2693</v>
+        <v>2691</v>
       </c>
       <c r="C1291" s="1" t="s">
-        <v>2694</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="1292" spans="1:3" x14ac:dyDescent="0.25">
@@ -28373,10 +28391,10 @@
         <v>0</v>
       </c>
       <c r="B1292" s="1" t="s">
-        <v>2695</v>
+        <v>2693</v>
       </c>
       <c r="C1292" s="1" t="s">
-        <v>2696</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="1293" spans="1:3" x14ac:dyDescent="0.25">
@@ -28384,10 +28402,10 @@
         <v>0</v>
       </c>
       <c r="B1293" s="1" t="s">
-        <v>2697</v>
+        <v>2695</v>
       </c>
       <c r="C1293" s="1" t="s">
-        <v>2698</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="1294" spans="1:3" x14ac:dyDescent="0.25">
@@ -28395,10 +28413,10 @@
         <v>0</v>
       </c>
       <c r="B1294" s="1" t="s">
-        <v>2699</v>
+        <v>2697</v>
       </c>
       <c r="C1294" s="1" t="s">
-        <v>2700</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="1295" spans="1:3" x14ac:dyDescent="0.25">
@@ -28406,10 +28424,10 @@
         <v>0</v>
       </c>
       <c r="B1295" s="1" t="s">
-        <v>2701</v>
+        <v>2699</v>
       </c>
       <c r="C1295" s="1" t="s">
-        <v>2702</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="1296" spans="1:3" x14ac:dyDescent="0.25">
@@ -28417,10 +28435,10 @@
         <v>0</v>
       </c>
       <c r="B1296" s="1" t="s">
-        <v>2707</v>
+        <v>2705</v>
       </c>
       <c r="C1296" s="1" t="s">
-        <v>2703</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="1297" spans="1:3" x14ac:dyDescent="0.25">
@@ -28428,10 +28446,10 @@
         <v>0</v>
       </c>
       <c r="B1297" s="1" t="s">
-        <v>2706</v>
+        <v>2704</v>
       </c>
       <c r="C1297" s="1" t="s">
-        <v>2704</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="1298" spans="1:3" x14ac:dyDescent="0.25">
@@ -28439,10 +28457,10 @@
         <v>0</v>
       </c>
       <c r="B1298" s="1" t="s">
-        <v>2705</v>
+        <v>2703</v>
       </c>
       <c r="C1298" s="1" t="s">
-        <v>2708</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="1299" spans="1:3" x14ac:dyDescent="0.25">
@@ -28450,10 +28468,10 @@
         <v>0</v>
       </c>
       <c r="B1299" s="1" t="s">
-        <v>2710</v>
+        <v>2708</v>
       </c>
       <c r="C1299" s="1" t="s">
-        <v>2709</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="1300" spans="1:3" x14ac:dyDescent="0.25">
@@ -28461,10 +28479,10 @@
         <v>0</v>
       </c>
       <c r="B1300" s="1" t="s">
-        <v>2711</v>
+        <v>2709</v>
       </c>
       <c r="C1300" s="1" t="s">
-        <v>2712</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="1301" spans="1:3" x14ac:dyDescent="0.25">
@@ -28472,10 +28490,10 @@
         <v>0</v>
       </c>
       <c r="B1301" s="1" t="s">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="C1301" s="1" t="s">
-        <v>2714</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="1302" spans="1:3" x14ac:dyDescent="0.25">
@@ -28483,10 +28501,10 @@
         <v>0</v>
       </c>
       <c r="B1302" s="1" t="s">
-        <v>2715</v>
+        <v>2713</v>
       </c>
       <c r="C1302" s="1" t="s">
-        <v>2716</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="1303" spans="1:3" x14ac:dyDescent="0.25">
@@ -28494,10 +28512,10 @@
         <v>0</v>
       </c>
       <c r="B1303" s="1" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
       <c r="C1303" s="1" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="1304" spans="1:3" x14ac:dyDescent="0.25">
@@ -28505,10 +28523,10 @@
         <v>0</v>
       </c>
       <c r="B1304" s="1" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="C1304" s="1" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="1305" spans="1:3" ht="217.5" x14ac:dyDescent="0.25">
@@ -28516,10 +28534,10 @@
         <v>0</v>
       </c>
       <c r="B1305" s="1" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="C1305" s="1" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="1306" spans="1:3" x14ac:dyDescent="0.25">
@@ -28527,10 +28545,10 @@
         <v>0</v>
       </c>
       <c r="B1306" s="1" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="C1306" s="1" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="1307" spans="1:3" x14ac:dyDescent="0.25">
@@ -28538,10 +28556,10 @@
         <v>0</v>
       </c>
       <c r="B1307" s="1" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="C1307" s="1" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="1308" spans="1:3" x14ac:dyDescent="0.25">
@@ -28549,10 +28567,10 @@
         <v>0</v>
       </c>
       <c r="B1308" s="1" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="C1308" s="1" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="1309" spans="1:3" x14ac:dyDescent="0.25">
@@ -28560,10 +28578,10 @@
         <v>0</v>
       </c>
       <c r="B1309" s="1" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
       <c r="C1309" s="1" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="1310" spans="1:3" x14ac:dyDescent="0.25">
@@ -28571,10 +28589,10 @@
         <v>0</v>
       </c>
       <c r="B1310" s="1" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="C1310" s="1" t="s">
-        <v>2732</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="1311" spans="1:3" x14ac:dyDescent="0.25">
@@ -28582,10 +28600,10 @@
         <v>0</v>
       </c>
       <c r="B1311" s="1" t="s">
-        <v>2733</v>
+        <v>2731</v>
       </c>
       <c r="C1311" s="1" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="1312" spans="1:3" x14ac:dyDescent="0.25">
@@ -28593,10 +28611,10 @@
         <v>0</v>
       </c>
       <c r="B1312" s="1" t="s">
-        <v>2735</v>
+        <v>2733</v>
       </c>
       <c r="C1312" s="1" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="1313" spans="1:3" x14ac:dyDescent="0.25">
@@ -28604,10 +28622,10 @@
         <v>0</v>
       </c>
       <c r="B1313" s="1" t="s">
-        <v>2737</v>
+        <v>2735</v>
       </c>
       <c r="C1313" s="1" t="s">
-        <v>2738</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="1314" spans="1:3" x14ac:dyDescent="0.25">
@@ -28615,10 +28633,10 @@
         <v>0</v>
       </c>
       <c r="B1314" s="1" t="s">
-        <v>2739</v>
+        <v>2737</v>
       </c>
       <c r="C1314" s="1" t="s">
-        <v>2740</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="1315" spans="1:3" x14ac:dyDescent="0.25">
@@ -28626,10 +28644,10 @@
         <v>0</v>
       </c>
       <c r="B1315" s="1" t="s">
-        <v>2741</v>
+        <v>2739</v>
       </c>
       <c r="C1315" s="1" t="s">
-        <v>2742</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="1316" spans="1:3" x14ac:dyDescent="0.25">
@@ -28637,10 +28655,10 @@
         <v>0</v>
       </c>
       <c r="B1316" s="1" t="s">
-        <v>2743</v>
+        <v>2741</v>
       </c>
       <c r="C1316" s="1" t="s">
-        <v>2744</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="1317" spans="1:3" x14ac:dyDescent="0.25">
@@ -28648,10 +28666,10 @@
         <v>0</v>
       </c>
       <c r="B1317" s="1" t="s">
-        <v>2745</v>
+        <v>2743</v>
       </c>
       <c r="C1317" s="1" t="s">
-        <v>2746</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="1318" spans="1:3" x14ac:dyDescent="0.25">
@@ -28659,10 +28677,10 @@
         <v>0</v>
       </c>
       <c r="B1318" s="1" t="s">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="C1318" s="1" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="1319" spans="1:3" x14ac:dyDescent="0.25">
@@ -28670,10 +28688,10 @@
         <v>0</v>
       </c>
       <c r="B1319" s="1" t="s">
-        <v>2749</v>
+        <v>2747</v>
       </c>
       <c r="C1319" s="1" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="1320" spans="1:3" x14ac:dyDescent="0.25">
@@ -28681,10 +28699,10 @@
         <v>0</v>
       </c>
       <c r="B1320" s="1" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="C1320" s="1" t="s">
-        <v>2752</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="1321" spans="1:3" x14ac:dyDescent="0.25">
@@ -28692,7 +28710,7 @@
         <v>0</v>
       </c>
       <c r="B1321" s="1" t="s">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="C1321" s="1" t="s">
         <v>1557</v>
@@ -28703,10 +28721,10 @@
         <v>0</v>
       </c>
       <c r="B1322" s="1" t="s">
-        <v>2754</v>
+        <v>2752</v>
       </c>
       <c r="C1322" s="1" t="s">
-        <v>2755</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="1323" spans="1:3" x14ac:dyDescent="0.25">
@@ -28714,7 +28732,7 @@
         <v>0</v>
       </c>
       <c r="B1323" s="1" t="s">
-        <v>2756</v>
+        <v>2754</v>
       </c>
       <c r="C1323" s="1" t="s">
         <v>408</v>
@@ -28725,10 +28743,10 @@
         <v>0</v>
       </c>
       <c r="B1324" s="1" t="s">
-        <v>2757</v>
+        <v>2755</v>
       </c>
       <c r="C1324" s="1" t="s">
-        <v>2758</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="1325" spans="1:3" x14ac:dyDescent="0.25">
@@ -28736,10 +28754,10 @@
         <v>0</v>
       </c>
       <c r="B1325" s="1" t="s">
-        <v>2759</v>
+        <v>2757</v>
       </c>
       <c r="C1325" s="1" t="s">
-        <v>2760</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="1326" spans="1:3" x14ac:dyDescent="0.25">
@@ -28747,10 +28765,10 @@
         <v>0</v>
       </c>
       <c r="B1326" s="1" t="s">
-        <v>2761</v>
+        <v>2759</v>
       </c>
       <c r="C1326" s="1" t="s">
-        <v>2762</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="1327" spans="1:3" x14ac:dyDescent="0.25">
@@ -28758,7 +28776,7 @@
         <v>0</v>
       </c>
       <c r="B1327" s="1" t="s">
-        <v>2763</v>
+        <v>2761</v>
       </c>
       <c r="C1327" s="1" t="s">
         <v>532</v>
@@ -28769,10 +28787,10 @@
         <v>0</v>
       </c>
       <c r="B1328" s="1" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="C1328" s="1" t="s">
-        <v>2765</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="1329" spans="1:3" x14ac:dyDescent="0.25">
@@ -28780,10 +28798,10 @@
         <v>0</v>
       </c>
       <c r="B1329" s="1" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C1329" s="1" t="s">
-        <v>2767</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="1330" spans="1:3" x14ac:dyDescent="0.25">
@@ -28791,10 +28809,10 @@
         <v>0</v>
       </c>
       <c r="B1330" s="1" t="s">
-        <v>2772</v>
+        <v>2770</v>
       </c>
       <c r="C1330" s="1" t="s">
-        <v>2773</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="1331" spans="1:3" x14ac:dyDescent="0.25">
@@ -28802,10 +28820,10 @@
         <v>0</v>
       </c>
       <c r="B1331" s="1" t="s">
-        <v>2774</v>
+        <v>2772</v>
       </c>
       <c r="C1331" s="1" t="s">
-        <v>2775</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="1332" spans="1:3" x14ac:dyDescent="0.25">
@@ -28813,10 +28831,10 @@
         <v>0</v>
       </c>
       <c r="B1332" s="1" t="s">
-        <v>2776</v>
+        <v>2774</v>
       </c>
       <c r="C1332" s="1" t="s">
-        <v>2777</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="1333" spans="1:3" x14ac:dyDescent="0.25">
@@ -28824,7 +28842,7 @@
         <v>0</v>
       </c>
       <c r="B1333" s="1" t="s">
-        <v>2778</v>
+        <v>2776</v>
       </c>
       <c r="C1333" s="1" t="s">
         <v>1799</v>
@@ -28835,10 +28853,10 @@
         <v>0</v>
       </c>
       <c r="B1334" s="1" t="s">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="C1334" s="1" t="s">
-        <v>2783</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="1335" spans="1:3" x14ac:dyDescent="0.25">
@@ -28846,7 +28864,7 @@
         <v>0</v>
       </c>
       <c r="B1335" s="1" t="s">
-        <v>2780</v>
+        <v>2778</v>
       </c>
       <c r="C1335" s="1" t="s">
         <v>1209</v>
@@ -28857,10 +28875,10 @@
         <v>0</v>
       </c>
       <c r="B1336" s="1" t="s">
-        <v>2781</v>
+        <v>2779</v>
       </c>
       <c r="C1336" s="1" t="s">
-        <v>2784</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="1337" spans="1:3" x14ac:dyDescent="0.25">
@@ -28868,10 +28886,10 @@
         <v>0</v>
       </c>
       <c r="B1337" s="1" t="s">
-        <v>2782</v>
+        <v>2780</v>
       </c>
       <c r="C1337" s="1" t="s">
-        <v>2785</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="1338" spans="1:3" x14ac:dyDescent="0.25">
@@ -28879,10 +28897,10 @@
         <v>0</v>
       </c>
       <c r="B1338" s="1" t="s">
-        <v>2786</v>
+        <v>2784</v>
       </c>
       <c r="C1338" s="1" t="s">
-        <v>2787</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="1339" spans="1:3" x14ac:dyDescent="0.25">
@@ -28890,10 +28908,10 @@
         <v>0</v>
       </c>
       <c r="B1339" s="1" t="s">
-        <v>2788</v>
+        <v>2786</v>
       </c>
       <c r="C1339" s="1" t="s">
-        <v>2789</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="1340" spans="1:3" x14ac:dyDescent="0.25">
@@ -28901,10 +28919,10 @@
         <v>0</v>
       </c>
       <c r="B1340" s="1" t="s">
-        <v>2790</v>
+        <v>2788</v>
       </c>
       <c r="C1340" s="1" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="1341" spans="1:3" x14ac:dyDescent="0.25">
@@ -28912,10 +28930,10 @@
         <v>0</v>
       </c>
       <c r="B1341" s="1" t="s">
-        <v>2792</v>
+        <v>2790</v>
       </c>
       <c r="C1341" s="1" t="s">
-        <v>2793</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="1342" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -28923,10 +28941,10 @@
         <v>0</v>
       </c>
       <c r="B1342" s="1" t="s">
+        <v>2792</v>
+      </c>
+      <c r="C1342" s="1" t="s">
         <v>2794</v>
-      </c>
-      <c r="C1342" s="1" t="s">
-        <v>2796</v>
       </c>
     </row>
     <row r="1343" spans="1:3" x14ac:dyDescent="0.25">
@@ -28934,7 +28952,7 @@
         <v>0</v>
       </c>
       <c r="B1343" s="1" t="s">
-        <v>2795</v>
+        <v>2793</v>
       </c>
       <c r="C1343" s="1" t="s">
         <v>423</v>
@@ -28945,10 +28963,10 @@
         <v>0</v>
       </c>
       <c r="B1344" s="1" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
       <c r="C1344" s="1" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="1345" spans="1:3" x14ac:dyDescent="0.25">
@@ -28956,10 +28974,10 @@
         <v>0</v>
       </c>
       <c r="B1345" s="1" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="C1345" s="1" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
     </row>
     <row r="1346" spans="1:3" x14ac:dyDescent="0.25">
@@ -28967,10 +28985,10 @@
         <v>0</v>
       </c>
       <c r="B1346" s="1" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="C1346" s="1" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="1347" spans="1:3" x14ac:dyDescent="0.25">
@@ -28978,10 +28996,10 @@
         <v>0</v>
       </c>
       <c r="B1347" s="1" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="C1347" s="1" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="1348" spans="1:3" x14ac:dyDescent="0.25">
@@ -28989,10 +29007,10 @@
         <v>0</v>
       </c>
       <c r="B1348" s="1" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="C1348" s="1" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="1349" spans="1:3" x14ac:dyDescent="0.25">
@@ -29000,10 +29018,10 @@
         <v>0</v>
       </c>
       <c r="B1349" s="1" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1349" s="1" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="1350" spans="1:3" x14ac:dyDescent="0.25">
@@ -29011,10 +29029,10 @@
         <v>0</v>
       </c>
       <c r="B1350" s="1" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="C1350" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1351" spans="1:3" x14ac:dyDescent="0.25">
@@ -29022,10 +29040,10 @@
         <v>0</v>
       </c>
       <c r="B1351" s="1" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="C1351" s="1" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="1352" spans="1:3" x14ac:dyDescent="0.25">
@@ -29033,10 +29051,10 @@
         <v>0</v>
       </c>
       <c r="B1352" s="1" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="C1352" s="1" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="1353" spans="1:3" x14ac:dyDescent="0.25">
@@ -29044,10 +29062,10 @@
         <v>0</v>
       </c>
       <c r="B1353" s="1" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="C1353" s="1" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="1354" spans="1:3" x14ac:dyDescent="0.25">
@@ -29055,10 +29073,10 @@
         <v>0</v>
       </c>
       <c r="B1354" s="1" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="C1354" s="1" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="1355" spans="1:3" x14ac:dyDescent="0.25">
@@ -29066,10 +29084,10 @@
         <v>0</v>
       </c>
       <c r="B1355" s="1" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="C1355" s="1" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="1356" spans="1:3" x14ac:dyDescent="0.25">
@@ -29077,10 +29095,10 @@
         <v>0</v>
       </c>
       <c r="B1356" s="1" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="C1356" s="1" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="1357" spans="1:3" x14ac:dyDescent="0.25">
@@ -29088,10 +29106,10 @@
         <v>0</v>
       </c>
       <c r="B1357" s="1" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="C1357" s="1" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="1358" spans="1:3" x14ac:dyDescent="0.25">
@@ -29099,10 +29117,10 @@
         <v>0</v>
       </c>
       <c r="B1358" s="1" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="C1358" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1359" spans="1:3" x14ac:dyDescent="0.25">
@@ -29110,10 +29128,10 @@
         <v>0</v>
       </c>
       <c r="B1359" s="1" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="C1359" s="1" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
     </row>
     <row r="1360" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29121,10 +29139,10 @@
         <v>0</v>
       </c>
       <c r="B1360" s="1" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="C1360" s="1" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
     </row>
     <row r="1361" spans="1:3" x14ac:dyDescent="0.25">
@@ -29132,10 +29150,10 @@
         <v>0</v>
       </c>
       <c r="B1361" s="1" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="C1361" s="1" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
     </row>
     <row r="1362" spans="1:3" x14ac:dyDescent="0.25">
@@ -29143,10 +29161,10 @@
         <v>0</v>
       </c>
       <c r="B1362" s="1" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="C1362" s="1" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="1363" spans="1:3" x14ac:dyDescent="0.25">
@@ -29154,10 +29172,10 @@
         <v>0</v>
       </c>
       <c r="B1363" s="1" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="C1363" s="1" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
     </row>
     <row r="1364" spans="1:3" x14ac:dyDescent="0.25">
@@ -29165,10 +29183,10 @@
         <v>0</v>
       </c>
       <c r="B1364" s="1" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="C1364" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1365" spans="1:3" x14ac:dyDescent="0.25">
@@ -29176,10 +29194,10 @@
         <v>0</v>
       </c>
       <c r="B1365" s="1" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="C1365" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1366" spans="1:3" x14ac:dyDescent="0.25">
@@ -29187,10 +29205,10 @@
         <v>0</v>
       </c>
       <c r="B1366" s="1" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="C1366" s="1" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="1367" spans="1:3" x14ac:dyDescent="0.25">
@@ -29198,10 +29216,10 @@
         <v>0</v>
       </c>
       <c r="B1367" s="1" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="C1367" s="1" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="1368" spans="1:3" x14ac:dyDescent="0.25">
@@ -29209,10 +29227,10 @@
         <v>0</v>
       </c>
       <c r="B1368" s="1" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="C1368" s="1" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="1369" spans="1:3" x14ac:dyDescent="0.25">
@@ -29220,10 +29238,10 @@
         <v>0</v>
       </c>
       <c r="B1369" s="1" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="C1369" s="1" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="1370" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29231,10 +29249,10 @@
         <v>0</v>
       </c>
       <c r="B1370" s="1" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="C1370" s="1" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
     </row>
     <row r="1371" spans="1:3" x14ac:dyDescent="0.25">
@@ -29242,7 +29260,7 @@
         <v>0</v>
       </c>
       <c r="B1371" s="1" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="C1371" s="1" t="s">
         <v>423</v>
@@ -29253,10 +29271,10 @@
         <v>0</v>
       </c>
       <c r="B1372" s="1" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="C1372" s="1" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="1373" spans="1:3" x14ac:dyDescent="0.25">
@@ -29264,10 +29282,10 @@
         <v>0</v>
       </c>
       <c r="B1373" s="1" t="s">
+        <v>2845</v>
+      </c>
+      <c r="C1373" s="1" t="s">
         <v>2847</v>
-      </c>
-      <c r="C1373" s="1" t="s">
-        <v>2849</v>
       </c>
     </row>
     <row r="1374" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29275,10 +29293,10 @@
         <v>0</v>
       </c>
       <c r="B1374" s="1" t="s">
+        <v>2846</v>
+      </c>
+      <c r="C1374" s="1" t="s">
         <v>2848</v>
-      </c>
-      <c r="C1374" s="1" t="s">
-        <v>2850</v>
       </c>
     </row>
     <row r="1375" spans="1:3" x14ac:dyDescent="0.25">
@@ -29286,10 +29304,10 @@
         <v>0</v>
       </c>
       <c r="B1375" s="1" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="C1375" s="1" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="1376" spans="1:3" x14ac:dyDescent="0.25">
@@ -29297,10 +29315,10 @@
         <v>0</v>
       </c>
       <c r="B1376" s="1" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="C1376" s="1" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="1377" spans="1:3" x14ac:dyDescent="0.25">
@@ -29308,10 +29326,10 @@
         <v>0</v>
       </c>
       <c r="B1377" s="1" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="C1377" s="1" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="1378" spans="1:3" x14ac:dyDescent="0.25">
@@ -29319,10 +29337,10 @@
         <v>0</v>
       </c>
       <c r="B1378" s="1" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="C1378" s="1" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="1379" spans="1:3" x14ac:dyDescent="0.25">
@@ -29330,10 +29348,10 @@
         <v>0</v>
       </c>
       <c r="B1379" s="1" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="C1379" s="1" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="1380" spans="1:3" x14ac:dyDescent="0.25">
@@ -29341,10 +29359,10 @@
         <v>0</v>
       </c>
       <c r="B1380" s="1" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="C1380" s="1" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="1381" spans="1:3" x14ac:dyDescent="0.25">
@@ -29352,10 +29370,10 @@
         <v>0</v>
       </c>
       <c r="B1381" s="1" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="C1381" s="1" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="1382" spans="1:3" x14ac:dyDescent="0.25">
@@ -29363,10 +29381,10 @@
         <v>0</v>
       </c>
       <c r="B1382" s="1" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C1382" s="1" t="s">
         <v>2862</v>
-      </c>
-      <c r="C1382" s="1" t="s">
-        <v>2864</v>
       </c>
     </row>
     <row r="1383" spans="1:3" x14ac:dyDescent="0.25">
@@ -29374,10 +29392,10 @@
         <v>0</v>
       </c>
       <c r="B1383" s="1" t="s">
+        <v>2861</v>
+      </c>
+      <c r="C1383" s="1" t="s">
         <v>2863</v>
-      </c>
-      <c r="C1383" s="1" t="s">
-        <v>2865</v>
       </c>
     </row>
     <row r="1384" spans="1:3" x14ac:dyDescent="0.25">
@@ -29385,10 +29403,10 @@
         <v>0</v>
       </c>
       <c r="B1384" s="1" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="C1384" s="1" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="1385" spans="1:3" x14ac:dyDescent="0.25">
@@ -29396,7 +29414,7 @@
         <v>0</v>
       </c>
       <c r="B1385" s="1" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="C1385" s="1" t="s">
         <v>131</v>
@@ -29407,10 +29425,10 @@
         <v>0</v>
       </c>
       <c r="B1386" s="1" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="C1386" s="1" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="1387" spans="1:3" x14ac:dyDescent="0.25">
@@ -29418,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="B1387" s="1" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="C1387" s="1" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="1388" spans="1:3" x14ac:dyDescent="0.25">
@@ -29429,10 +29447,10 @@
         <v>0</v>
       </c>
       <c r="B1388" s="1" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="C1388" s="1" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="1389" spans="1:3" x14ac:dyDescent="0.25">
@@ -29440,10 +29458,10 @@
         <v>0</v>
       </c>
       <c r="B1389" s="1" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="C1389" s="1" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="1390" spans="1:3" x14ac:dyDescent="0.25">
@@ -29451,10 +29469,10 @@
         <v>0</v>
       </c>
       <c r="B1390" s="1" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="C1390" s="1" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="1391" spans="1:3" x14ac:dyDescent="0.25">
@@ -29462,10 +29480,10 @@
         <v>0</v>
       </c>
       <c r="B1391" s="1" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="C1391" s="1" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="1392" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29473,10 +29491,10 @@
         <v>0</v>
       </c>
       <c r="B1392" s="1" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="C1392" s="1" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="1393" spans="1:3" x14ac:dyDescent="0.25">
@@ -29484,7 +29502,7 @@
         <v>0</v>
       </c>
       <c r="B1393" s="1" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="C1393" s="1" t="s">
         <v>2029</v>
@@ -29495,10 +29513,10 @@
         <v>0</v>
       </c>
       <c r="B1394" s="1" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="C1394" s="1" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="1395" spans="1:3" x14ac:dyDescent="0.25">
@@ -29506,7 +29524,7 @@
         <v>0</v>
       </c>
       <c r="B1395" s="1" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="C1395" s="1" t="s">
         <v>2531</v>
@@ -29517,10 +29535,10 @@
         <v>0</v>
       </c>
       <c r="B1396" s="1" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="C1396" s="1" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="1397" spans="1:3" x14ac:dyDescent="0.25">
@@ -29528,10 +29546,10 @@
         <v>0</v>
       </c>
       <c r="B1397" s="1" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="C1397" s="1" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="1398" spans="1:3" x14ac:dyDescent="0.25">
@@ -29539,10 +29557,10 @@
         <v>0</v>
       </c>
       <c r="B1398" s="1" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="C1398" s="1" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="1399" spans="1:3" x14ac:dyDescent="0.25">
@@ -29550,7 +29568,7 @@
         <v>0</v>
       </c>
       <c r="B1399" s="1" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="C1399" s="1" t="s">
         <v>177</v>
@@ -29561,7 +29579,7 @@
         <v>0</v>
       </c>
       <c r="B1400" s="1" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
       <c r="C1400" s="1" t="s">
         <v>1823</v>
@@ -29572,10 +29590,10 @@
         <v>0</v>
       </c>
       <c r="B1401" s="1" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="C1401" s="1" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="1402" spans="1:3" x14ac:dyDescent="0.25">
@@ -29583,10 +29601,10 @@
         <v>0</v>
       </c>
       <c r="B1402" s="1" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="C1402" s="1" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="1403" spans="1:3" x14ac:dyDescent="0.25">
@@ -29594,7 +29612,7 @@
         <v>0</v>
       </c>
       <c r="B1403" s="1" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="C1403" s="1" t="s">
         <v>2029</v>
@@ -29605,10 +29623,10 @@
         <v>0</v>
       </c>
       <c r="B1404" s="1" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
       <c r="C1404" s="1" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="1405" spans="1:3" x14ac:dyDescent="0.25">
@@ -29616,10 +29634,10 @@
         <v>0</v>
       </c>
       <c r="B1405" s="1" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="C1405" s="1" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="1406" spans="1:3" x14ac:dyDescent="0.25">
@@ -29627,10 +29645,10 @@
         <v>0</v>
       </c>
       <c r="B1406" s="1" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="C1406" s="1" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="1407" spans="1:3" x14ac:dyDescent="0.25">
@@ -29638,10 +29656,10 @@
         <v>0</v>
       </c>
       <c r="B1407" s="1" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="C1407" s="1" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="1408" spans="1:3" x14ac:dyDescent="0.25">
@@ -29649,10 +29667,10 @@
         <v>0</v>
       </c>
       <c r="B1408" s="1" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="C1408" s="1" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="1409" spans="1:3" x14ac:dyDescent="0.25">
@@ -29660,10 +29678,10 @@
         <v>0</v>
       </c>
       <c r="B1409" s="1" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="C1409" s="1" t="s">
-        <v>2918</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="1410" spans="1:3" x14ac:dyDescent="0.25">
@@ -29671,10 +29689,10 @@
         <v>0</v>
       </c>
       <c r="B1410" s="1" t="s">
-        <v>2919</v>
+        <v>2917</v>
       </c>
       <c r="C1410" s="1" t="s">
-        <v>2920</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="1411" spans="1:3" x14ac:dyDescent="0.25">
@@ -29682,10 +29700,10 @@
         <v>0</v>
       </c>
       <c r="B1411" s="1" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
       <c r="C1411" s="1" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="1412" spans="1:3" x14ac:dyDescent="0.25">
@@ -29693,10 +29711,10 @@
         <v>0</v>
       </c>
       <c r="B1412" s="1" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
       <c r="C1412" s="1" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="1413" spans="1:3" x14ac:dyDescent="0.25">
@@ -29704,10 +29722,10 @@
         <v>0</v>
       </c>
       <c r="B1413" s="1" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C1413" s="1" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="1414" spans="1:3" x14ac:dyDescent="0.25">
@@ -29715,10 +29733,10 @@
         <v>0</v>
       </c>
       <c r="B1414" s="1" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="C1414" s="1" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="1415" spans="1:3" x14ac:dyDescent="0.25">
@@ -29726,10 +29744,10 @@
         <v>0</v>
       </c>
       <c r="B1415" s="1" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="C1415" s="1" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="1416" spans="1:3" x14ac:dyDescent="0.25">
@@ -29737,10 +29755,10 @@
         <v>0</v>
       </c>
       <c r="B1416" s="1" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="C1416" s="1" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="1417" spans="1:3" x14ac:dyDescent="0.25">
@@ -29748,10 +29766,10 @@
         <v>0</v>
       </c>
       <c r="B1417" s="1" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="C1417" s="1" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="1418" spans="1:3" x14ac:dyDescent="0.25">
@@ -29759,10 +29777,10 @@
         <v>0</v>
       </c>
       <c r="B1418" s="1" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
       <c r="C1418" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1419" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29770,10 +29788,10 @@
         <v>0</v>
       </c>
       <c r="B1419" s="1" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
       <c r="C1419" s="1" t="s">
-        <v>2938</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="1420" spans="1:3" x14ac:dyDescent="0.25">
@@ -29781,10 +29799,10 @@
         <v>0</v>
       </c>
       <c r="B1420" s="1" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
       <c r="C1420" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="1421" spans="1:3" x14ac:dyDescent="0.25">
@@ -29792,10 +29810,10 @@
         <v>0</v>
       </c>
       <c r="B1421" s="1" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="C1421" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="1422" spans="1:3" x14ac:dyDescent="0.25">
@@ -29803,10 +29821,10 @@
         <v>0</v>
       </c>
       <c r="B1422" s="1" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="C1422" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1423" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29814,10 +29832,10 @@
         <v>0</v>
       </c>
       <c r="B1423" s="1" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
       <c r="C1423" s="1" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="1424" spans="1:3" x14ac:dyDescent="0.25">
@@ -29825,10 +29843,10 @@
         <v>0</v>
       </c>
       <c r="B1424" s="1" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="C1424" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1425" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29836,10 +29854,10 @@
         <v>0</v>
       </c>
       <c r="B1425" s="1" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="C1425" s="1" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="1426" spans="1:3" x14ac:dyDescent="0.25">
@@ -29847,10 +29865,10 @@
         <v>0</v>
       </c>
       <c r="B1426" s="1" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="C1426" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1427" spans="1:3" x14ac:dyDescent="0.25">
@@ -29858,10 +29876,10 @@
         <v>0</v>
       </c>
       <c r="B1427" s="1" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="C1427" s="1" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="1428" spans="1:3" x14ac:dyDescent="0.25">
@@ -29869,10 +29887,10 @@
         <v>0</v>
       </c>
       <c r="B1428" s="1" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
       <c r="C1428" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1429" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29880,10 +29898,10 @@
         <v>0</v>
       </c>
       <c r="B1429" s="1" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="C1429" s="1" t="s">
-        <v>2952</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="1430" spans="1:3" x14ac:dyDescent="0.25">
@@ -29891,10 +29909,10 @@
         <v>0</v>
       </c>
       <c r="B1430" s="1" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
       <c r="C1430" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1431" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29902,10 +29920,10 @@
         <v>0</v>
       </c>
       <c r="B1431" s="1" t="s">
-        <v>2954</v>
+        <v>2952</v>
       </c>
       <c r="C1431" s="1" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="1432" spans="1:3" x14ac:dyDescent="0.25">
@@ -29913,10 +29931,10 @@
         <v>0</v>
       </c>
       <c r="B1432" s="1" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="C1432" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1433" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -29924,10 +29942,10 @@
         <v>0</v>
       </c>
       <c r="B1433" s="1" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="C1433" s="1" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="1434" spans="1:3" x14ac:dyDescent="0.25">
@@ -29935,10 +29953,10 @@
         <v>0</v>
       </c>
       <c r="B1434" s="1" t="s">
-        <v>2959</v>
+        <v>2957</v>
       </c>
       <c r="C1434" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1435" spans="1:3" x14ac:dyDescent="0.25">
@@ -29946,10 +29964,10 @@
         <v>0</v>
       </c>
       <c r="B1435" s="1" t="s">
-        <v>2960</v>
+        <v>2958</v>
       </c>
       <c r="C1435" s="1" t="s">
-        <v>2961</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="1436" spans="1:3" x14ac:dyDescent="0.25">
@@ -29957,10 +29975,10 @@
         <v>0</v>
       </c>
       <c r="B1436" s="1" t="s">
-        <v>2962</v>
+        <v>2960</v>
       </c>
       <c r="C1436" s="1" t="s">
-        <v>2963</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="1437" spans="1:3" x14ac:dyDescent="0.25">
@@ -29968,10 +29986,10 @@
         <v>0</v>
       </c>
       <c r="B1437" s="1" t="s">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="C1437" s="1" t="s">
-        <v>2965</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="1438" spans="1:3" x14ac:dyDescent="0.25">
@@ -29979,10 +29997,10 @@
         <v>0</v>
       </c>
       <c r="B1438" s="1" t="s">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="C1438" s="1" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1439" spans="1:3" x14ac:dyDescent="0.25">
@@ -29990,10 +30008,10 @@
         <v>0</v>
       </c>
       <c r="B1439" s="1" t="s">
-        <v>2968</v>
+        <v>2966</v>
       </c>
       <c r="C1439" s="1" t="s">
-        <v>2969</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="1440" spans="1:3" x14ac:dyDescent="0.25">
@@ -30001,7 +30019,7 @@
         <v>0</v>
       </c>
       <c r="B1440" s="1" t="s">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="C1440" s="1" t="s">
         <v>2384</v>
@@ -30012,7 +30030,7 @@
         <v>0</v>
       </c>
       <c r="B1441" s="1" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="C1441" s="1" t="s">
         <v>2384</v>
@@ -30023,10 +30041,10 @@
         <v>0</v>
       </c>
       <c r="B1442" s="1" t="s">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="C1442" s="1" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="1443" spans="1:3" x14ac:dyDescent="0.25">
@@ -30034,10 +30052,10 @@
         <v>0</v>
       </c>
       <c r="B1443" s="1" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="C1443" s="1" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="1444" spans="1:3" x14ac:dyDescent="0.25">
@@ -30045,10 +30063,10 @@
         <v>0</v>
       </c>
       <c r="B1444" s="1" t="s">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="C1444" s="1" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1445" spans="1:3" x14ac:dyDescent="0.25">
@@ -30056,10 +30074,10 @@
         <v>0</v>
       </c>
       <c r="B1445" s="1" t="s">
-        <v>2980</v>
+        <v>2978</v>
       </c>
       <c r="C1445" s="1" t="s">
-        <v>2965</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="1446" spans="1:3" x14ac:dyDescent="0.25">
@@ -30067,10 +30085,10 @@
         <v>0</v>
       </c>
       <c r="B1446" s="1" t="s">
-        <v>2994</v>
+        <v>2992</v>
       </c>
       <c r="C1446" s="1" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="1447" spans="1:3" x14ac:dyDescent="0.25">
@@ -30078,10 +30096,10 @@
         <v>0</v>
       </c>
       <c r="B1447" s="1" t="s">
-        <v>2983</v>
+        <v>2981</v>
       </c>
       <c r="C1447" s="1" t="s">
-        <v>2984</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="1448" spans="1:3" x14ac:dyDescent="0.25">
@@ -30089,10 +30107,10 @@
         <v>0</v>
       </c>
       <c r="B1448" s="1" t="s">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="C1448" s="1" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="1449" spans="1:3" x14ac:dyDescent="0.25">
@@ -30100,10 +30118,10 @@
         <v>0</v>
       </c>
       <c r="B1449" s="1" t="s">
-        <v>2991</v>
+        <v>2989</v>
       </c>
       <c r="C1449" s="1" t="s">
-        <v>2992</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="1450" spans="1:3" x14ac:dyDescent="0.25">
@@ -30111,10 +30129,10 @@
         <v>0</v>
       </c>
       <c r="B1450" s="1" t="s">
-        <v>2993</v>
+        <v>2991</v>
       </c>
       <c r="C1450" s="1" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="1451" spans="1:3" x14ac:dyDescent="0.25">
@@ -30122,10 +30140,10 @@
         <v>0</v>
       </c>
       <c r="B1451" s="1" t="s">
-        <v>2995</v>
+        <v>2993</v>
       </c>
       <c r="C1451" s="1" t="s">
-        <v>2996</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="1452" spans="1:3" x14ac:dyDescent="0.25">
@@ -30133,10 +30151,10 @@
         <v>0</v>
       </c>
       <c r="B1452" s="1" t="s">
+        <v>2980</v>
+      </c>
+      <c r="C1452" s="1" t="s">
         <v>2982</v>
-      </c>
-      <c r="C1452" s="1" t="s">
-        <v>2984</v>
       </c>
     </row>
     <row r="1453" spans="1:3" x14ac:dyDescent="0.25">
@@ -30144,10 +30162,10 @@
         <v>0</v>
       </c>
       <c r="B1453" s="1" t="s">
-        <v>2998</v>
+        <v>2996</v>
       </c>
       <c r="C1453" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1454" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -30155,10 +30173,10 @@
         <v>0</v>
       </c>
       <c r="B1454" s="1" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="C1454" s="1" t="s">
-        <v>3000</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="1455" spans="1:3" x14ac:dyDescent="0.25">
@@ -30166,10 +30184,10 @@
         <v>0</v>
       </c>
       <c r="B1455" s="1" t="s">
-        <v>3001</v>
+        <v>2999</v>
       </c>
       <c r="C1455" s="1" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="1456" spans="1:3" x14ac:dyDescent="0.25">
@@ -30177,10 +30195,10 @@
         <v>0</v>
       </c>
       <c r="B1456" s="1" t="s">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="C1456" s="1" t="s">
-        <v>3003</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="1457" spans="1:3" x14ac:dyDescent="0.25">
@@ -30188,10 +30206,10 @@
         <v>0</v>
       </c>
       <c r="B1457" s="1" t="s">
-        <v>3009</v>
+        <v>3007</v>
       </c>
       <c r="C1457" s="1" t="s">
-        <v>3010</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="1458" spans="1:3" x14ac:dyDescent="0.25">
@@ -30199,10 +30217,10 @@
         <v>0</v>
       </c>
       <c r="B1458" s="1" t="s">
+        <v>3009</v>
+      </c>
+      <c r="C1458" s="1" t="s">
         <v>3011</v>
-      </c>
-      <c r="C1458" s="1" t="s">
-        <v>3013</v>
       </c>
     </row>
     <row r="1459" spans="1:3" x14ac:dyDescent="0.25">
@@ -30210,10 +30228,10 @@
         <v>0</v>
       </c>
       <c r="B1459" s="1" t="s">
-        <v>3014</v>
+        <v>3012</v>
       </c>
       <c r="C1459" s="1" t="s">
-        <v>3012</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="1460" spans="1:3" x14ac:dyDescent="0.25">
@@ -30221,10 +30239,10 @@
         <v>0</v>
       </c>
       <c r="B1460" s="1" t="s">
-        <v>3015</v>
+        <v>3013</v>
       </c>
       <c r="C1460" s="1" t="s">
-        <v>3010</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="1461" spans="1:3" x14ac:dyDescent="0.25">
@@ -30232,10 +30250,10 @@
         <v>0</v>
       </c>
       <c r="B1461" s="1" t="s">
-        <v>3016</v>
+        <v>3014</v>
       </c>
       <c r="C1461" s="1" t="s">
-        <v>2992</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="1462" spans="1:3" x14ac:dyDescent="0.25">
@@ -30243,10 +30261,10 @@
         <v>0</v>
       </c>
       <c r="B1462" s="1" t="s">
-        <v>3020</v>
+        <v>3018</v>
       </c>
       <c r="C1462" s="1" t="s">
-        <v>3021</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="1463" spans="1:3" x14ac:dyDescent="0.25">
@@ -30254,10 +30272,10 @@
         <v>0</v>
       </c>
       <c r="B1463" s="1" t="s">
-        <v>3022</v>
+        <v>3020</v>
       </c>
       <c r="C1463" s="1" t="s">
-        <v>3023</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="1464" spans="1:3" x14ac:dyDescent="0.25">
@@ -30265,10 +30283,10 @@
         <v>0</v>
       </c>
       <c r="B1464" s="1" t="s">
-        <v>3024</v>
+        <v>3022</v>
       </c>
       <c r="C1464" s="1" t="s">
-        <v>3025</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="1465" spans="1:3" x14ac:dyDescent="0.25">
@@ -30276,10 +30294,10 @@
         <v>0</v>
       </c>
       <c r="B1465" s="1" t="s">
-        <v>3029</v>
+        <v>3027</v>
       </c>
       <c r="C1465" s="1" t="s">
-        <v>3030</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="1466" spans="1:3" x14ac:dyDescent="0.25">
@@ -30287,10 +30305,10 @@
         <v>0</v>
       </c>
       <c r="B1466" s="1" t="s">
-        <v>3031</v>
+        <v>3029</v>
       </c>
       <c r="C1466" s="1" t="s">
-        <v>3032</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="1467" spans="1:3" x14ac:dyDescent="0.25">
@@ -30298,10 +30316,10 @@
         <v>0</v>
       </c>
       <c r="B1467" s="1" t="s">
-        <v>3033</v>
+        <v>3031</v>
       </c>
       <c r="C1467" s="1" t="s">
-        <v>3034</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="1468" spans="1:3" x14ac:dyDescent="0.25">
@@ -30309,10 +30327,10 @@
         <v>0</v>
       </c>
       <c r="B1468" s="1" t="s">
-        <v>3035</v>
+        <v>3033</v>
       </c>
       <c r="C1468" s="1" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="1469" spans="1:3" x14ac:dyDescent="0.25">
@@ -30320,10 +30338,10 @@
         <v>0</v>
       </c>
       <c r="B1469" s="1" t="s">
-        <v>3037</v>
+        <v>3035</v>
       </c>
       <c r="C1469" s="1" t="s">
-        <v>3038</v>
+        <v>3036</v>
       </c>
     </row>
     <row r="1470" spans="1:3" x14ac:dyDescent="0.25">
@@ -30331,10 +30349,10 @@
         <v>0</v>
       </c>
       <c r="B1470" s="1" t="s">
-        <v>3039</v>
+        <v>3037</v>
       </c>
       <c r="C1470" s="1" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="1471" spans="1:3" x14ac:dyDescent="0.25">
@@ -30342,10 +30360,10 @@
         <v>0</v>
       </c>
       <c r="B1471" s="1" t="s">
-        <v>3040</v>
+        <v>3038</v>
       </c>
       <c r="C1471" s="1" t="s">
-        <v>3038</v>
+        <v>3036</v>
       </c>
     </row>
     <row r="1472" spans="1:3" x14ac:dyDescent="0.25">
@@ -30353,10 +30371,10 @@
         <v>0</v>
       </c>
       <c r="B1472" s="1" t="s">
-        <v>3042</v>
+        <v>3040</v>
       </c>
       <c r="C1472" s="1" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1473" spans="1:3" x14ac:dyDescent="0.25">
@@ -30364,10 +30382,10 @@
         <v>0</v>
       </c>
       <c r="B1473" s="1" t="s">
-        <v>3043</v>
+        <v>3041</v>
       </c>
       <c r="C1473" s="1" t="s">
-        <v>3044</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="1474" spans="1:3" x14ac:dyDescent="0.25">
@@ -30375,10 +30393,10 @@
         <v>0</v>
       </c>
       <c r="B1474" s="1" t="s">
-        <v>3045</v>
+        <v>3043</v>
       </c>
       <c r="C1474" s="1" t="s">
-        <v>3046</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="1475" spans="1:3" x14ac:dyDescent="0.25">
@@ -30386,10 +30404,10 @@
         <v>0</v>
       </c>
       <c r="B1475" s="1" t="s">
-        <v>3047</v>
+        <v>3045</v>
       </c>
       <c r="C1475" s="1" t="s">
-        <v>3048</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="1476" spans="1:3" x14ac:dyDescent="0.25">
@@ -30397,10 +30415,10 @@
         <v>0</v>
       </c>
       <c r="B1476" s="1" t="s">
-        <v>3049</v>
+        <v>3047</v>
       </c>
       <c r="C1476" s="1" t="s">
-        <v>3046</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="1477" spans="1:3" x14ac:dyDescent="0.25">
@@ -30408,10 +30426,10 @@
         <v>0</v>
       </c>
       <c r="B1477" s="1" t="s">
-        <v>3050</v>
+        <v>3048</v>
       </c>
       <c r="C1477" s="1" t="s">
-        <v>3048</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="1478" spans="1:3" x14ac:dyDescent="0.25">
@@ -30419,10 +30437,10 @@
         <v>0</v>
       </c>
       <c r="B1478" s="1" t="s">
-        <v>3051</v>
+        <v>3049</v>
       </c>
       <c r="C1478" s="1" t="s">
-        <v>3052</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="1479" spans="1:3" x14ac:dyDescent="0.25">
@@ -30430,10 +30448,10 @@
         <v>0</v>
       </c>
       <c r="B1479" s="1" t="s">
-        <v>3053</v>
+        <v>3051</v>
       </c>
       <c r="C1479" s="1" t="s">
-        <v>3054</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="1480" spans="1:3" x14ac:dyDescent="0.25">
@@ -30441,10 +30459,10 @@
         <v>0</v>
       </c>
       <c r="B1480" s="1" t="s">
-        <v>3056</v>
+        <v>3054</v>
       </c>
       <c r="C1480" s="1" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1481" spans="1:3" x14ac:dyDescent="0.25">
@@ -30452,10 +30470,10 @@
         <v>0</v>
       </c>
       <c r="B1481" s="1" t="s">
-        <v>3057</v>
+        <v>3055</v>
       </c>
       <c r="C1481" s="1" t="s">
-        <v>3058</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="1482" spans="1:3" x14ac:dyDescent="0.25">
@@ -30463,10 +30481,10 @@
         <v>0</v>
       </c>
       <c r="B1482" s="1" t="s">
-        <v>3063</v>
+        <v>3061</v>
       </c>
       <c r="C1482" s="1" t="s">
-        <v>3066</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="1483" spans="1:3" x14ac:dyDescent="0.25">
@@ -30474,10 +30492,10 @@
         <v>0</v>
       </c>
       <c r="B1483" s="1" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
       <c r="C1483" s="1" t="s">
-        <v>3064</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="1484" spans="1:3" x14ac:dyDescent="0.25">
@@ -30485,10 +30503,10 @@
         <v>0</v>
       </c>
       <c r="B1484" s="1" t="s">
-        <v>3067</v>
+        <v>3065</v>
       </c>
       <c r="C1484" s="1" t="s">
-        <v>3064</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="1485" spans="1:3" x14ac:dyDescent="0.25">
@@ -30496,10 +30514,10 @@
         <v>0</v>
       </c>
       <c r="B1485" s="1" t="s">
-        <v>3068</v>
+        <v>3066</v>
       </c>
       <c r="C1485" s="1" t="s">
-        <v>3069</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="1486" spans="1:3" x14ac:dyDescent="0.25">
@@ -30507,10 +30525,10 @@
         <v>0</v>
       </c>
       <c r="B1486" s="1" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
       <c r="C1486" s="1" t="s">
-        <v>3064</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="1487" spans="1:3" x14ac:dyDescent="0.25">
@@ -30518,10 +30536,10 @@
         <v>0</v>
       </c>
       <c r="B1487" s="1" t="s">
-        <v>3076</v>
+        <v>3074</v>
       </c>
       <c r="C1487" s="1" t="s">
-        <v>3079</v>
+        <v>3077</v>
       </c>
     </row>
     <row r="1488" spans="1:3" x14ac:dyDescent="0.25">
@@ -30529,10 +30547,10 @@
         <v>0</v>
       </c>
       <c r="B1488" s="1" t="s">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="C1488" s="1" t="s">
-        <v>3077</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="1489" spans="1:3" x14ac:dyDescent="0.25">
@@ -30540,10 +30558,10 @@
         <v>0</v>
       </c>
       <c r="B1489" s="1" t="s">
-        <v>3080</v>
+        <v>3078</v>
       </c>
       <c r="C1489" s="1" t="s">
-        <v>3077</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="1490" spans="1:3" x14ac:dyDescent="0.25">
@@ -30551,10 +30569,10 @@
         <v>0</v>
       </c>
       <c r="B1490" s="1" t="s">
-        <v>3081</v>
+        <v>3079</v>
       </c>
       <c r="C1490" s="1" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="1491" spans="1:3" x14ac:dyDescent="0.25">
@@ -30562,10 +30580,10 @@
         <v>0</v>
       </c>
       <c r="B1491" s="1" t="s">
-        <v>3083</v>
+        <v>3081</v>
       </c>
       <c r="C1491" s="1" t="s">
-        <v>3084</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="1492" spans="1:3" x14ac:dyDescent="0.25">
@@ -30573,10 +30591,10 @@
         <v>0</v>
       </c>
       <c r="B1492" s="1" t="s">
-        <v>3087</v>
+        <v>3085</v>
       </c>
       <c r="C1492" s="1" t="s">
-        <v>3090</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="1493" spans="1:3" x14ac:dyDescent="0.25">
@@ -30584,10 +30602,10 @@
         <v>0</v>
       </c>
       <c r="B1493" s="1" t="s">
-        <v>3089</v>
+        <v>3087</v>
       </c>
       <c r="C1493" s="1" t="s">
-        <v>3088</v>
+        <v>3086</v>
       </c>
     </row>
     <row r="1494" spans="1:3" x14ac:dyDescent="0.25">
@@ -30595,10 +30613,10 @@
         <v>0</v>
       </c>
       <c r="B1494" s="1" t="s">
-        <v>3091</v>
+        <v>3089</v>
       </c>
       <c r="C1494" s="1" t="s">
-        <v>3092</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="1495" spans="1:3" x14ac:dyDescent="0.25">
@@ -30606,10 +30624,10 @@
         <v>0</v>
       </c>
       <c r="B1495" s="1" t="s">
-        <v>3093</v>
+        <v>3091</v>
       </c>
       <c r="C1495" s="1" t="s">
-        <v>3094</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="1496" spans="1:3" x14ac:dyDescent="0.25">
@@ -30617,10 +30635,10 @@
         <v>0</v>
       </c>
       <c r="B1496" s="1" t="s">
-        <v>3095</v>
+        <v>3093</v>
       </c>
       <c r="C1496" s="1" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="1497" spans="1:3" x14ac:dyDescent="0.25">
@@ -30628,10 +30646,10 @@
         <v>0</v>
       </c>
       <c r="B1497" s="1" t="s">
-        <v>3096</v>
+        <v>3094</v>
       </c>
       <c r="C1497" s="1" t="s">
-        <v>2969</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="1498" spans="1:3" x14ac:dyDescent="0.25">
@@ -30639,7 +30657,7 @@
         <v>0</v>
       </c>
       <c r="B1498" s="1" t="s">
-        <v>3097</v>
+        <v>3095</v>
       </c>
       <c r="C1498" s="1" t="s">
         <v>1080</v>
@@ -30650,7 +30668,7 @@
         <v>0</v>
       </c>
       <c r="B1499" s="1" t="s">
-        <v>3098</v>
+        <v>3096</v>
       </c>
       <c r="C1499" s="1" t="s">
         <v>234</v>
@@ -30661,7 +30679,7 @@
         <v>0</v>
       </c>
       <c r="B1500" s="1" t="s">
-        <v>3099</v>
+        <v>3097</v>
       </c>
       <c r="C1500" s="1" t="s">
         <v>240</v>
@@ -30672,7 +30690,7 @@
         <v>0</v>
       </c>
       <c r="B1501" s="1" t="s">
-        <v>3100</v>
+        <v>3098</v>
       </c>
       <c r="C1501" s="1" t="s">
         <v>472</v>
@@ -30683,7 +30701,7 @@
         <v>0</v>
       </c>
       <c r="B1502" s="1" t="s">
-        <v>3101</v>
+        <v>3099</v>
       </c>
       <c r="C1502" s="1" t="s">
         <v>238</v>
@@ -30694,7 +30712,7 @@
         <v>0</v>
       </c>
       <c r="B1503" s="1" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="C1503" s="1" t="s">
         <v>1194</v>
@@ -30705,7 +30723,7 @@
         <v>0</v>
       </c>
       <c r="B1504" s="1" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="C1504" s="1" t="s">
         <v>235</v>
@@ -30716,7 +30734,7 @@
         <v>0</v>
       </c>
       <c r="B1505" s="1" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="C1505" s="1" t="s">
         <v>237</v>
@@ -30727,7 +30745,7 @@
         <v>0</v>
       </c>
       <c r="B1506" s="1" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="C1506" s="1" t="s">
         <v>236</v>
@@ -30738,7 +30756,7 @@
         <v>0</v>
       </c>
       <c r="B1507" s="1" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="C1507" s="1" t="s">
         <v>450</v>
@@ -30749,10 +30767,43 @@
         <v>0</v>
       </c>
       <c r="B1508" s="1" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="C1508" s="1" t="s">
         <v>1879</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1509" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1509" s="1" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C1509" s="1" t="s">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1510" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1510" s="1" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C1510" s="1" t="s">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1511" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1511" s="1" t="s">
+        <v>3111</v>
+      </c>
+      <c r="C1511" s="1" t="s">
+        <v>3112</v>
       </c>
     </row>
   </sheetData>
@@ -30784,52 +30835,52 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3041</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3061</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3059</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2981</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>2970</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
     </row>
   </sheetData>
@@ -30867,161 +30918,161 @@
         <v>761</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3041</v>
+        <v>3039</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3055</v>
+        <v>3053</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>3041</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3017</v>
+        <v>3015</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3026</v>
+        <v>3024</v>
       </c>
       <c r="C6" s="1">
         <v>50000</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3019</v>
+        <v>3017</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3027</v>
+        <v>3025</v>
       </c>
       <c r="C7" s="1">
         <v>50000</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3018</v>
+        <v>3016</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3028</v>
+        <v>3026</v>
       </c>
       <c r="C8" s="1">
         <v>50000</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>3059</v>
+        <v>3057</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3060</v>
+        <v>3058</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>3059</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3061</v>
+        <v>3059</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3072</v>
+        <v>3070</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>3061</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3062</v>
+        <v>3060</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3073</v>
+        <v>3071</v>
       </c>
       <c r="C11" s="1">
         <v>50000</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3061</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3074</v>
+        <v>3072</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>3071</v>
+        <v>3069</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="C13" s="1">
         <v>50000</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
     </row>
   </sheetData>
@@ -31062,21 +31113,21 @@
         <v>761</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2905</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2906</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2907</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2908</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2909</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2970</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2972</v>
       </c>
       <c r="C2" s="1">
         <v>1500</v>
@@ -31088,15 +31139,15 @@
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2970</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>2969</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2971</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2973</v>
       </c>
       <c r="C3" s="1">
         <v>1500</v>
@@ -31108,15 +31159,15 @@
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2981</v>
+        <v>2979</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="C4" s="1">
         <v>1500</v>
@@ -31128,12 +31179,12 @@
         <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2981</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3085</v>
+        <v>3083</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -31142,12 +31193,12 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>2970</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3086</v>
+        <v>3084</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -31156,7 +31207,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
     </row>
   </sheetData>
@@ -33424,7 +33475,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -33453,7 +33504,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -33482,7 +33533,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -33511,7 +33562,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -33540,7 +33591,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -33569,7 +33620,7 @@
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -33598,7 +33649,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -33627,7 +33678,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -33656,7 +33707,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -33685,7 +33736,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -33714,7 +33765,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -33743,7 +33794,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -33772,7 +33823,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -33801,7 +33852,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -33830,7 +33881,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -33859,7 +33910,7 @@
         <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -33888,7 +33939,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -33917,7 +33968,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -33946,7 +33997,7 @@
         <v>30</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -33975,7 +34026,7 @@
         <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -34004,7 +34055,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -34033,7 +34084,7 @@
         <v>14</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -34062,7 +34113,7 @@
         <v>14</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -34091,7 +34142,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -34120,7 +34171,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -34149,7 +34200,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -34178,7 +34229,7 @@
         <v>14</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -34207,7 +34258,7 @@
         <v>14</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -34236,7 +34287,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -34265,7 +34316,7 @@
         <v>14</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -34294,7 +34345,7 @@
         <v>30</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -34323,7 +34374,7 @@
         <v>14</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -34352,7 +34403,7 @@
         <v>7</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -34381,7 +34432,7 @@
         <v>7</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -34410,7 +34461,7 @@
         <v>14</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -34439,7 +34490,7 @@
         <v>14</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -34468,7 +34519,7 @@
         <v>14</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -34497,7 +34548,7 @@
         <v>14</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -34526,7 +34577,7 @@
         <v>14</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -34555,7 +34606,7 @@
         <v>14</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -34584,7 +34635,7 @@
         <v>14</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -34613,7 +34664,7 @@
         <v>14</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -34642,7 +34693,7 @@
         <v>14</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -34671,7 +34722,7 @@
         <v>14</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -34700,7 +34751,7 @@
         <v>14</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -34729,7 +34780,7 @@
         <v>14</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -34758,7 +34809,7 @@
         <v>2</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -34787,7 +34838,7 @@
         <v>2</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -34816,7 +34867,7 @@
         <v>2</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -34845,7 +34896,7 @@
         <v>2</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -34874,7 +34925,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -34903,7 +34954,7 @@
         <v>14</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -34932,7 +34983,7 @@
         <v>14</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -34961,7 +35012,7 @@
         <v>14</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -34990,7 +35041,7 @@
         <v>14</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -35019,7 +35070,7 @@
         <v>7</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -35048,7 +35099,7 @@
         <v>3</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -35077,7 +35128,7 @@
         <v>7</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -35106,7 +35157,7 @@
         <v>14</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A very first experiment with mobile version
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8FA215-6F04-492A-BD8F-FCFCE3D7A2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FB42AE-CEC7-44F3-A7B3-CB1BA0473B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="510" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5864" uniqueCount="3114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5873" uniqueCount="3119">
   <si>
     <t>cs</t>
   </si>
@@ -9630,6 +9630,21 @@
   </si>
   <si>
     <t>market.aroma.comment.comment</t>
+  </si>
+  <si>
+    <t>lab.build.context.menu.title</t>
+  </si>
+  <si>
+    <t>lab.build.create.menu</t>
+  </si>
+  <si>
+    <t>lab.build.create.context.menu.title</t>
+  </si>
+  <si>
+    <t>Menu - Buildy</t>
+  </si>
+  <si>
+    <t>Menu - Nový build</t>
   </si>
 </sst>
 </file>
@@ -14172,10 +14187,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1511"/>
+  <dimension ref="A1:C1514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1481" workbookViewId="0">
-      <selection activeCell="B1511" sqref="B1511"/>
+    <sheetView tabSelected="1" topLeftCell="A1478" workbookViewId="0">
+      <selection activeCell="B1505" sqref="B1505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30804,6 +30819,39 @@
       </c>
       <c r="C1511" s="1" t="s">
         <v>3112</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1512" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1512" s="1" t="s">
+        <v>3114</v>
+      </c>
+      <c r="C1512" s="1" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1513" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1513" s="1" t="s">
+        <v>3115</v>
+      </c>
+      <c r="C1513" s="1" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1514" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1514" s="1" t="s">
+        <v>3116</v>
+      </c>
+      <c r="C1514" s="1" t="s">
+        <v>3118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some more comments
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9EA3EE-68BC-447D-8F3C-B6DC960A9307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD582C9-3080-43C4-85D4-DFCC40BC3A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="510" windowWidth="30510" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="510" windowWidth="28035" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5873" uniqueCount="3118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5921" uniqueCount="3144">
   <si>
     <t>cs</t>
   </si>
@@ -9642,6 +9642,84 @@
   </si>
   <si>
     <t>Menu - Nový build</t>
+  </si>
+  <si>
+    <t>market.atomizer.delete.modal.title</t>
+  </si>
+  <si>
+    <t>market.atomizer.delete.modal.content</t>
+  </si>
+  <si>
+    <t>Odstranit atomizéry?</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybrané atomizéry? Tato akce je velmi agresivní a může odstranit velké množství dat.</t>
+  </si>
+  <si>
+    <t>RDL, DL, MTL</t>
+  </si>
+  <si>
+    <t>market.atomizer.delete.success</t>
+  </si>
+  <si>
+    <t>market.atomizer.atomizer.menu</t>
+  </si>
+  <si>
+    <t>market.atomizer.vendor.menu</t>
+  </si>
+  <si>
+    <t>Atomizéry výrobce</t>
+  </si>
+  <si>
+    <t>market.atomizer.comment.menu</t>
+  </si>
+  <si>
+    <t>market.atomizer.vendor.label</t>
+  </si>
+  <si>
+    <t>market.atomizer.comment.label</t>
+  </si>
+  <si>
+    <t>market.atomizer.vendor.title</t>
+  </si>
+  <si>
+    <t>market.atomizer.comment.title</t>
+  </si>
+  <si>
+    <t>market.atomizer.comment.comment.label</t>
+  </si>
+  <si>
+    <t>Napište veřejný komentář</t>
+  </si>
+  <si>
+    <t>market.atomizer.comment.comment</t>
+  </si>
+  <si>
+    <t>Uveřejnit</t>
+  </si>
+  <si>
+    <t>shared.comment.private.empty.title</t>
+  </si>
+  <si>
+    <t>Nejsou dostupné žádné komentáře.</t>
+  </si>
+  <si>
+    <t>shared.comment.private.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Nemáte žádné svoje komentáře.</t>
+  </si>
+  <si>
+    <t>market.atomizer.vendor.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nejsou dostupné žádné další atomizéry.</t>
+  </si>
+  <si>
+    <t>market.atomizer.vendor.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Tento výrobce tu zatím nemá žádné další svoje atomizéry.</t>
   </si>
 </sst>
 </file>
@@ -11382,7 +11460,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11475,19 +11553,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>725</v>
+        <v>666</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>816</v>
@@ -11508,15 +11586,15 @@
         <v>816</v>
       </c>
       <c r="L3" s="1">
-        <v>150</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>751</v>
+        <v>672</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>816</v>
@@ -11546,15 +11624,15 @@
         <v>816</v>
       </c>
       <c r="L4" s="1">
-        <v>250</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>672</v>
+        <v>685</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>823</v>
+        <v>836</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>816</v>
@@ -11584,15 +11662,15 @@
         <v>816</v>
       </c>
       <c r="L5" s="1">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>732</v>
+        <v>693</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>824</v>
+        <v>840</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>816</v>
@@ -11604,7 +11682,7 @@
         <v>825</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>2092</v>
@@ -11622,27 +11700,27 @@
         <v>816</v>
       </c>
       <c r="L6" s="1">
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>748</v>
+        <v>1783</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>826</v>
+        <v>1784</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>2092</v>
@@ -11660,24 +11738,24 @@
         <v>816</v>
       </c>
       <c r="L7" s="1">
-        <v>275</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>666</v>
+        <v>1783</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>827</v>
+        <v>1785</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>816</v>
@@ -11698,7 +11776,7 @@
         <v>816</v>
       </c>
       <c r="L8" s="1">
-        <v>10</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -11741,22 +11819,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>748</v>
+        <v>700</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>831</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>816</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>2092</v>
@@ -11779,22 +11857,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>748</v>
+        <v>723</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>816</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>2092</v>
@@ -11812,24 +11890,24 @@
         <v>816</v>
       </c>
       <c r="L11" s="1">
-        <v>275</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>753</v>
+        <v>725</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>833</v>
+        <v>818</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>819</v>
+        <v>3122</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>816</v>
@@ -11850,24 +11928,24 @@
         <v>816</v>
       </c>
       <c r="L12" s="1">
-        <v>35</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>822</v>
@@ -11893,22 +11971,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>685</v>
+        <v>746</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>2092</v>
@@ -11931,22 +12009,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>700</v>
+        <v>748</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>837</v>
+        <v>826</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>816</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>2092</v>
@@ -11969,19 +12047,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>785</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>817</v>
+        <v>831</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>816</v>
@@ -12002,7 +12080,7 @@
         <v>816</v>
       </c>
       <c r="L16" s="1">
-        <v>75</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -12010,16 +12088,16 @@
         <v>748</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>816</v>
@@ -12045,10 +12123,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>693</v>
+        <v>748</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>816</v>
@@ -12078,15 +12156,15 @@
         <v>816</v>
       </c>
       <c r="L18" s="1">
-        <v>125</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>1783</v>
+        <v>751</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1784</v>
+        <v>820</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>816</v>
@@ -12095,7 +12173,7 @@
         <v>784</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>822</v>
@@ -12116,24 +12194,24 @@
         <v>816</v>
       </c>
       <c r="L19" s="1">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1783</v>
+        <v>753</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1785</v>
+        <v>833</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>816</v>
@@ -12154,15 +12232,18 @@
         <v>816</v>
       </c>
       <c r="L20" s="1">
-        <v>325</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L20">
+    <sortCondition ref="A3:A20"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.eliquidshop.cz/vyrobce-wotofo-a1010/" xr:uid="{1A4BF3B4-D652-724B-882E-1BE1A013DDE7}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.eliquidshop.cz/vyrobce-sirius-mods-a1532/" xr:uid="{08F874F6-F6B3-B54F-BB43-99630EE8986F}"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.eliquidshop.cz/vyrobce-dotmod-a923/" xr:uid="{73DF1D56-B8D3-8248-8925-E785AC0DE759}"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{4693CF94-0CE9-8D4B-9B83-A044C6AFA279}"/>
+    <hyperlink ref="A20" r:id="rId1" display="https://www.eliquidshop.cz/vyrobce-wotofo-a1010/" xr:uid="{1A4BF3B4-D652-724B-882E-1BE1A013DDE7}"/>
+    <hyperlink ref="A11" r:id="rId2" display="https://www.eliquidshop.cz/vyrobce-sirius-mods-a1532/" xr:uid="{08F874F6-F6B3-B54F-BB43-99630EE8986F}"/>
+    <hyperlink ref="A5" r:id="rId3" display="https://www.eliquidshop.cz/vyrobce-dotmod-a923/" xr:uid="{73DF1D56-B8D3-8248-8925-E785AC0DE759}"/>
+    <hyperlink ref="A10" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{4693CF94-0CE9-8D4B-9B83-A044C6AFA279}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14184,10 +14265,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1514"/>
+  <dimension ref="A1:C1530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1188" workbookViewId="0">
-      <selection activeCell="C1214" sqref="C1214"/>
+    <sheetView tabSelected="1" topLeftCell="A1488" workbookViewId="0">
+      <selection activeCell="B1512" sqref="B1512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30849,6 +30930,182 @@
       </c>
       <c r="C1514" s="1" t="s">
         <v>3117</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1515" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1515" s="1" t="s">
+        <v>3118</v>
+      </c>
+      <c r="C1515" s="1" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1516" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1516" s="1" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C1516" s="1" t="s">
+        <v>3121</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1517" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1517" s="1" t="s">
+        <v>3123</v>
+      </c>
+      <c r="C1517" s="1" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1518" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1518" s="1" t="s">
+        <v>3124</v>
+      </c>
+      <c r="C1518" s="1" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1519" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1519" s="1" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C1519" s="1" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1520" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1520" s="1" t="s">
+        <v>3127</v>
+      </c>
+      <c r="C1520" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1521" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1521" s="1" t="s">
+        <v>3128</v>
+      </c>
+      <c r="C1521" s="1" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1522" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1522" s="1" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C1522" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1523" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1523" s="1" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C1523" s="1" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1524" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1524" s="1" t="s">
+        <v>3131</v>
+      </c>
+      <c r="C1524" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1525" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1525" s="1" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C1525" s="1" t="s">
+        <v>3133</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1526" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1526" s="1" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C1526" s="1" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1527" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1527" s="1" t="s">
+        <v>3136</v>
+      </c>
+      <c r="C1527" s="1" t="s">
+        <v>3137</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1528" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1528" s="1" t="s">
+        <v>3138</v>
+      </c>
+      <c r="C1528" s="1" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1529" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1529" s="1" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C1529" s="1" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1530" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1530" s="1" t="s">
+        <v>3142</v>
+      </c>
+      <c r="C1530" s="1" t="s">
+        <v>3143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared initial coil info boilerplate
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCB96F6-E96C-4EC3-93C0-BD2467D95254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427469DF-C357-4D40-8E27-2BF5AD839D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="510" windowWidth="28035" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5927" uniqueCount="3147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5942" uniqueCount="3154">
   <si>
     <t>cs</t>
   </si>
@@ -9729,6 +9729,27 @@
   </si>
   <si>
     <t>Oblíbené vaty</t>
+  </si>
+  <si>
+    <t>lab.build.cells.menu</t>
+  </si>
+  <si>
+    <t>lab.build.cells.title</t>
+  </si>
+  <si>
+    <t>Vhodné články</t>
+  </si>
+  <si>
+    <t>lab.build.cell.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nebyly nalezeny žádné vhodné články.</t>
+  </si>
+  <si>
+    <t>lab.build.cell.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Aplikace neeviduje ve vašem inventáři žádné vhodné články pro váš build. Buď nejsou zaevidovány v systému, nebo máte příliš nízký odpor. Berte prosím na vědomí, že aplikace bere pouze 75% vybíjecího proudu článku pro zvýšení bezpečnosti, tudíž pokud tento build využijete, dbejte prosím extrémní opatrnosti.</t>
   </si>
 </sst>
 </file>
@@ -14274,10 +14295,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1532"/>
+  <dimension ref="A1:C1537"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1503" workbookViewId="0">
-      <selection activeCell="B1522" sqref="B1522"/>
+      <selection activeCell="B1529" sqref="B1529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31137,6 +31158,61 @@
       </c>
       <c r="C1532" s="1" t="s">
         <v>3146</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1533" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1533" s="1" t="s">
+        <v>3147</v>
+      </c>
+      <c r="C1533" s="1" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1534" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1534" s="1" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C1534" s="1" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1535" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1535" s="1" t="s">
+        <v>3148</v>
+      </c>
+      <c r="C1535" s="1" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1536" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1536" s="1" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C1536" s="1" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1537" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1537" s="1" t="s">
+        <v>3152</v>
+      </c>
+      <c r="C1537" s="1" t="s">
+        <v>3153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial simple support for cell health
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427469DF-C357-4D40-8E27-2BF5AD839D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8C3ECC-6FBF-4C8E-B86D-133F2A300971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="510" windowWidth="28035" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="510" windowWidth="28035" windowHeight="19890" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5942" uniqueCount="3154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6031" uniqueCount="3205">
   <si>
     <t>cs</t>
   </si>
@@ -9751,6 +9751,172 @@
   <si>
     <t>Aplikace neeviduje ve vašem inventáři žádné vhodné články pro váš build. Buď nejsou zaevidovány v systému, nebo máte příliš nízký odpor. Berte prosím na vědomí, že aplikace bere pouze 75% vybíjecího proudu článku pro zvýšení bezpečnosti, tudíž pokud tento build využijete, dbejte prosím extrémní opatrnosti.</t>
   </si>
+  <si>
+    <t>inventory.cell.cell.title</t>
+  </si>
+  <si>
+    <t>Detail článku</t>
+  </si>
+  <si>
+    <t>inventory.cell.label</t>
+  </si>
+  <si>
+    <t>inventory.cell.cell.menu</t>
+  </si>
+  <si>
+    <t>shared.cell.info.name</t>
+  </si>
+  <si>
+    <t>Název článku</t>
+  </si>
+  <si>
+    <t>shared.cell.info.drain</t>
+  </si>
+  <si>
+    <t>Maximální vybíjecí proud</t>
+  </si>
+  <si>
+    <t>shared.cell.info.ohm</t>
+  </si>
+  <si>
+    <t>Minimální bezpečný odpor</t>
+  </si>
+  <si>
+    <t>shared.cell.info.type</t>
+  </si>
+  <si>
+    <t>inventory.cell.comment.menu</t>
+  </si>
+  <si>
+    <t>shared.cell.info.code</t>
+  </si>
+  <si>
+    <t>Kód článku</t>
+  </si>
+  <si>
+    <t>inventory.cell.comment.label</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.menu</t>
+  </si>
+  <si>
+    <t>Zdraví článku</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.label</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.title</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte žádné záznamy zdraví článku.</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud máte chytrou nabíječku nebo jiné zařízení, které je vám schopno sdělit napětí nabitého článku nebo jeho kapacitu, můžete si tyto hodnoty poznamenat a sledovat, jak který článek stárne.</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.subtitle</t>
+  </si>
+  <si>
+    <t>Zde můžete sledovat zdraví svých článků.</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.content</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+	Tato sekce je zajímavá pro všechny, kdo chtějí sledovat zdraví svých článků, zejména pokud je používají na mechanikách nebo semi-mechanikách.
+&lt;/p&gt;
+&lt;p&gt;
+	Základní přepdoklad je, že vlastníte zařízení, např. chytrou navíječku s displayem, která vám sdělí napětí nabitého článku, nebo je
+	případně i schopna přeměřit kapacitu článku.
+&lt;/p&gt;
+&lt;p&gt;
+	K čemu to je? Pokud si články popíšete kvalitním fixkem kódem, který vygenerovala aplikace (nebo alespoň jeho částí), budete schopní se podívat, kolik ten či onen článek snese a v jakém může být obecně stavu. Díky tomu lze odhadnout (formou doporučení, dbejte hlavně svého
+	vlastního selského rozumu), jak moc můžete článek namáhat, zejména pokud jej chcete používat na neregulované mody.
+&lt;/p&gt;
+&lt;p&gt;
+	Pro běžné uživatele toto sice tak zajímavé být nemusí, nicméně i tak tato funkce může pomoci určit články, které může být lepší už vyměnit.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>inventory.cell.comment.title</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.create.button</t>
+  </si>
+  <si>
+    <t>Záznam zdraví</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.create.title</t>
+  </si>
+  <si>
+    <t>Nový záznam zdraví článku</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.voltage.label</t>
+  </si>
+  <si>
+    <t>Napětí nabitého článku</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.capacity.label</t>
+  </si>
+  <si>
+    <t>Aktuální kapacita článku</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.create</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.create.success</t>
+  </si>
+  <si>
+    <t>Záznam zdraví článku úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.voltage.label.required</t>
+  </si>
+  <si>
+    <t>Tato funkce vyžaduje znalost napětí článku.</t>
+  </si>
+  <si>
+    <t>shared.cell.info.voltage</t>
+  </si>
+  <si>
+    <t>Pracovní napětí</t>
+  </si>
+  <si>
+    <t>inventory.cell.info.age.tooltip</t>
+  </si>
+  <si>
+    <t>Stáří záznamu zdraví článku.</t>
+  </si>
+  <si>
+    <t>voltageMax</t>
+  </si>
+  <si>
+    <t>shared.cell.info.voltageMax</t>
+  </si>
+  <si>
+    <t>Výchozí plné napětí článku</t>
+  </si>
+  <si>
+    <t>shared.cell.info.capacity</t>
+  </si>
+  <si>
+    <t>Výchozí kapacita článku</t>
+  </si>
 </sst>
 </file>
 
@@ -9759,7 +9925,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9784,15 +9950,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -9814,7 +9971,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -9831,15 +9988,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FFACCCEA"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -9848,7 +9996,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -9858,13 +10006,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
@@ -9875,6 +10020,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11562,19 +11710,19 @@
       <c r="F2" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="17">
         <v>4</v>
       </c>
       <c r="J2">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L2" s="1">
@@ -11600,19 +11748,19 @@
       <c r="F3" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="17">
         <v>4</v>
       </c>
       <c r="J3">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L3" s="1">
@@ -11638,19 +11786,19 @@
       <c r="F4" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="17">
         <v>4</v>
       </c>
       <c r="J4">
         <v>9</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L4" s="1">
@@ -11676,19 +11824,19 @@
       <c r="F5" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="17">
         <v>4</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L5" s="1">
@@ -11714,19 +11862,19 @@
       <c r="F6" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="17">
         <v>4</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L6" s="1">
@@ -11752,19 +11900,19 @@
       <c r="F7" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="17">
         <v>4</v>
       </c>
       <c r="J7">
         <v>9</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L7" s="1">
@@ -11790,19 +11938,19 @@
       <c r="F8" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="17">
         <v>4</v>
       </c>
       <c r="J8">
         <v>9</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L8" s="1">
@@ -11828,19 +11976,19 @@
       <c r="F9" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="17">
         <v>4</v>
       </c>
       <c r="J9">
         <v>9</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L9" s="1">
@@ -11866,19 +12014,19 @@
       <c r="F10" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="17">
         <v>4</v>
       </c>
       <c r="J10">
         <v>9</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L10" s="1">
@@ -11904,19 +12052,19 @@
       <c r="F11" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="17">
         <v>4</v>
       </c>
       <c r="J11">
         <v>9</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L11" s="1">
@@ -11942,19 +12090,19 @@
       <c r="F12" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="17">
         <v>4</v>
       </c>
       <c r="J12">
         <v>9</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L12" s="1">
@@ -11980,19 +12128,19 @@
       <c r="F13" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="17">
         <v>4</v>
       </c>
       <c r="J13">
         <v>9</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L13" s="1">
@@ -12018,19 +12166,19 @@
       <c r="F14" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="17">
         <v>4</v>
       </c>
       <c r="J14">
         <v>9</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L14" s="1">
@@ -12056,19 +12204,19 @@
       <c r="F15" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="17">
         <v>4</v>
       </c>
       <c r="J15">
         <v>9</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L15" s="1">
@@ -12094,19 +12242,19 @@
       <c r="F16" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="17">
         <v>4</v>
       </c>
       <c r="J16">
         <v>9</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L16" s="1">
@@ -12132,19 +12280,19 @@
       <c r="F17" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="17">
         <v>4</v>
       </c>
       <c r="J17">
         <v>9</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L17" s="1">
@@ -12170,19 +12318,19 @@
       <c r="F18" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="17">
         <v>4</v>
       </c>
       <c r="J18">
         <v>9</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L18" s="1">
@@ -12208,19 +12356,19 @@
       <c r="F19" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="17">
         <v>4</v>
       </c>
       <c r="J19">
         <v>9</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L19" s="1">
@@ -12246,19 +12394,19 @@
       <c r="F20" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="17" t="s">
         <v>2092</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="17" t="s">
         <v>2093</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="17">
         <v>4</v>
       </c>
       <c r="J20">
         <v>9</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="17" t="s">
         <v>816</v>
       </c>
       <c r="L20" s="1">
@@ -12301,16 +12449,16 @@
       <c r="B1" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>801</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>758</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>756</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>761</v>
       </c>
     </row>
@@ -12321,16 +12469,16 @@
       <c r="B2" t="s">
         <v>802</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="8">
         <v>100</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="8">
         <v>3.7</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>803</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="8">
         <v>275</v>
       </c>
     </row>
@@ -12341,16 +12489,16 @@
       <c r="B3" t="s">
         <v>804</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>25</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>3.7</v>
       </c>
       <c r="E3" s="6">
         <v>18350</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8">
         <v>125</v>
       </c>
     </row>
@@ -12361,16 +12509,16 @@
       <c r="B4" t="s">
         <v>805</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>70</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>3.7</v>
       </c>
       <c r="E4" s="6">
         <v>18650</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>275</v>
       </c>
     </row>
@@ -12381,16 +12529,16 @@
       <c r="B5" t="s">
         <v>806</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>50</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>3.7</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>150</v>
       </c>
     </row>
@@ -12401,16 +12549,16 @@
       <c r="B6" t="s">
         <v>808</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>80</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>3.7</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>767</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>550</v>
       </c>
     </row>
@@ -12421,16 +12569,16 @@
       <c r="B7" t="s">
         <v>809</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>95</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>3.7</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>803</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>150</v>
       </c>
     </row>
@@ -12441,16 +12589,16 @@
       <c r="B8" t="s">
         <v>810</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>60</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>3.7</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>125</v>
       </c>
     </row>
@@ -13423,138 +13571,175 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243831E-E3E3-1C43-AE4D-34D8FEF2F724}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="18" t="s">
+        <v>3200</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>758</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="4" t="s">
+        <v>3171</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>762</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="D2" s="9">
         <v>3.7</v>
       </c>
-      <c r="D2" s="10">
+      <c r="E2" s="7">
         <v>20</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="F2" s="10">
+      <c r="G2">
+        <v>3000</v>
+      </c>
+      <c r="H2" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>727</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>764</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="D3" s="9">
         <v>3.7</v>
       </c>
-      <c r="D3" s="10">
+      <c r="E3" s="7">
         <v>30</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="F3" s="10">
+      <c r="G3">
+        <v>2600</v>
+      </c>
+      <c r="H3" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>727</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>765</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="D4" s="9">
         <v>3.7</v>
       </c>
-      <c r="D4" s="10">
+      <c r="E4" s="7">
         <v>30</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4">
+        <v>3000</v>
+      </c>
+      <c r="H4" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>766</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="D5" s="9">
         <v>3.7</v>
       </c>
-      <c r="D5" s="10">
+      <c r="E5" s="7">
         <v>35</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>767</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5">
+        <v>4000</v>
+      </c>
+      <c r="H5" s="7">
         <v>22.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>768</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="D6" s="9">
         <v>3.7</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E6" s="7">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>769</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G6">
+        <v>1200</v>
+      </c>
+      <c r="H6" s="7">
         <v>10</v>
       </c>
     </row>
@@ -13782,7 +13967,7 @@
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="17" t="s">
         <v>1783</v>
       </c>
     </row>
@@ -14183,7 +14368,7 @@
       <c r="B5" s="1" t="s">
         <v>1731</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="17">
         <v>10</v>
       </c>
     </row>
@@ -14295,10 +14480,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1537"/>
+  <dimension ref="A1:C1566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1503" workbookViewId="0">
-      <selection activeCell="B1529" sqref="B1529"/>
+    <sheetView topLeftCell="A1551" workbookViewId="0">
+      <selection activeCell="B1565" sqref="B1565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31213,6 +31398,325 @@
       </c>
       <c r="C1537" s="1" t="s">
         <v>3153</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1538" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1538" s="1" t="s">
+        <v>3156</v>
+      </c>
+      <c r="C1538" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1539" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1539" s="1" t="s">
+        <v>3154</v>
+      </c>
+      <c r="C1539" s="1" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1540" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1540" s="1" t="s">
+        <v>3157</v>
+      </c>
+      <c r="C1540" s="1" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1541" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1541" s="1" t="s">
+        <v>3158</v>
+      </c>
+      <c r="C1541" s="1" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1542" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1542" s="1" t="s">
+        <v>3160</v>
+      </c>
+      <c r="C1542" s="1" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1543" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1543" s="1" t="s">
+        <v>3162</v>
+      </c>
+      <c r="C1543" s="1" t="s">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1544" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1544" s="1" t="s">
+        <v>3164</v>
+      </c>
+      <c r="C1544" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1545" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1545" s="1" t="s">
+        <v>3165</v>
+      </c>
+      <c r="C1545" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1546" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1546" s="1" t="s">
+        <v>3166</v>
+      </c>
+      <c r="C1546" s="1" t="s">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1547" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1547" s="1" t="s">
+        <v>3168</v>
+      </c>
+      <c r="C1547" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1548" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1548" s="1" t="s">
+        <v>3169</v>
+      </c>
+      <c r="C1548" s="1" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1549" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1549" s="1" t="s">
+        <v>3172</v>
+      </c>
+      <c r="C1549" s="1" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1550" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1550" s="1" t="s">
+        <v>3173</v>
+      </c>
+      <c r="C1550" s="1" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1551" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1551" s="1" t="s">
+        <v>3174</v>
+      </c>
+      <c r="C1551" s="1" t="s">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1552" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1552" s="1" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C1552" s="1" t="s">
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1553" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1553" s="1" t="s">
+        <v>3178</v>
+      </c>
+      <c r="C1553" s="1" t="s">
+        <v>3179</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:3" ht="192" x14ac:dyDescent="0.25">
+      <c r="A1554" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1554" s="1" t="s">
+        <v>3180</v>
+      </c>
+      <c r="C1554" s="1" t="s">
+        <v>3181</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1555" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1555" s="1" t="s">
+        <v>3182</v>
+      </c>
+      <c r="C1555" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1556" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1556" s="1" t="s">
+        <v>3183</v>
+      </c>
+      <c r="C1556" s="1" t="s">
+        <v>3184</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1557" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1557" s="1" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C1557" s="1" t="s">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1558" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1558" s="1" t="s">
+        <v>3187</v>
+      </c>
+      <c r="C1558" s="1" t="s">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1559" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1559" s="1" t="s">
+        <v>3189</v>
+      </c>
+      <c r="C1559" s="1" t="s">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1560" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1560" s="1" t="s">
+        <v>3191</v>
+      </c>
+      <c r="C1560" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1561" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1561" s="1" t="s">
+        <v>3192</v>
+      </c>
+      <c r="C1561" s="1" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1562" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1562" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C1562" s="1" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1563" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1563" s="1" t="s">
+        <v>3196</v>
+      </c>
+      <c r="C1563" s="1" t="s">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1564" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1564" s="1" t="s">
+        <v>3198</v>
+      </c>
+      <c r="C1564" s="1" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1565" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1565" s="1" t="s">
+        <v>3201</v>
+      </c>
+      <c r="C1565" s="1" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1566" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1566" s="1" t="s">
+        <v>3203</v>
+      </c>
+      <c r="C1566" s="1" t="s">
+        <v>3204</v>
       </c>
     </row>
   </sheetData>
@@ -31970,7 +32474,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="19"/>
+    <col min="2" max="2" width="11.42578125" style="16"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
@@ -31979,7 +32483,7 @@
       <c r="A1" s="2" t="s">
         <v>1144</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1145</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -31993,7 +32497,7 @@
       <c r="A2" s="1">
         <v>18</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -32005,7 +32509,7 @@
       <c r="A3" s="1">
         <v>19</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -32017,7 +32521,7 @@
       <c r="A4" s="1">
         <v>20</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -32029,7 +32533,7 @@
       <c r="A5" s="1">
         <v>21</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -32041,7 +32545,7 @@
       <c r="A6" s="1">
         <v>22</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -32053,7 +32557,7 @@
       <c r="A7" s="1">
         <v>23</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -32065,7 +32569,7 @@
       <c r="A8" s="1">
         <v>24</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -32077,7 +32581,7 @@
       <c r="A9" s="1">
         <v>25</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -32089,7 +32593,7 @@
       <c r="A10" s="1">
         <v>26</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -32101,7 +32605,7 @@
       <c r="A11" s="1">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -32113,7 +32617,7 @@
       <c r="A12" s="1">
         <v>28</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -32125,7 +32629,7 @@
       <c r="A13" s="1">
         <v>29</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -32137,7 +32641,7 @@
       <c r="A14" s="1">
         <v>30</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -32149,7 +32653,7 @@
       <c r="A15" s="1">
         <v>31</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -32161,7 +32665,7 @@
       <c r="A16" s="1">
         <v>32</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -32173,7 +32677,7 @@
       <c r="A17" s="1">
         <v>33</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -32185,7 +32689,7 @@
       <c r="A18" s="1">
         <v>34</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -32197,7 +32701,7 @@
       <c r="A19" s="1">
         <v>35</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -32209,7 +32713,7 @@
       <c r="A20" s="1">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -32221,7 +32725,7 @@
       <c r="A21" s="1">
         <v>37</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -32233,7 +32737,7 @@
       <c r="A22" s="1">
         <v>38</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -32245,7 +32749,7 @@
       <c r="A23" s="1">
         <v>39</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -32257,7 +32761,7 @@
       <c r="A24" s="1">
         <v>40</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -32269,7 +32773,7 @@
       <c r="A25" s="1">
         <v>18</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -32281,7 +32785,7 @@
       <c r="A26" s="1">
         <v>19</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -32293,7 +32797,7 @@
       <c r="A27" s="1">
         <v>20</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -32305,7 +32809,7 @@
       <c r="A28" s="1">
         <v>21</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -32317,7 +32821,7 @@
       <c r="A29" s="1">
         <v>22</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -32329,7 +32833,7 @@
       <c r="A30" s="1">
         <v>23</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -32341,7 +32845,7 @@
       <c r="A31" s="1">
         <v>24</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -32353,7 +32857,7 @@
       <c r="A32" s="1">
         <v>25</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -32365,7 +32869,7 @@
       <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -32377,7 +32881,7 @@
       <c r="A34" s="1">
         <v>27</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -32389,7 +32893,7 @@
       <c r="A35" s="1">
         <v>28</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -32401,7 +32905,7 @@
       <c r="A36" s="1">
         <v>29</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -32413,7 +32917,7 @@
       <c r="A37" s="1">
         <v>30</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -32425,7 +32929,7 @@
       <c r="A38" s="1">
         <v>31</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -32437,7 +32941,7 @@
       <c r="A39" s="1">
         <v>32</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -32449,7 +32953,7 @@
       <c r="A40" s="1">
         <v>33</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -32461,7 +32965,7 @@
       <c r="A41" s="1">
         <v>34</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -32473,7 +32977,7 @@
       <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -32485,7 +32989,7 @@
       <c r="A43" s="1">
         <v>36</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -32497,7 +33001,7 @@
       <c r="A44" s="1">
         <v>37</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -32509,7 +33013,7 @@
       <c r="A45" s="1">
         <v>38</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -32521,7 +33025,7 @@
       <c r="A46" s="1">
         <v>39</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -32533,7 +33037,7 @@
       <c r="A47" s="1">
         <v>40</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -32545,7 +33049,7 @@
       <c r="A48" s="1">
         <v>18</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -32557,7 +33061,7 @@
       <c r="A49" s="1">
         <v>19</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -32569,7 +33073,7 @@
       <c r="A50" s="1">
         <v>20</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -32580,7 +33084,7 @@
       <c r="A51" s="1">
         <v>21</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -32591,7 +33095,7 @@
       <c r="A52" s="1">
         <v>22</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -32602,7 +33106,7 @@
       <c r="A53" s="1">
         <v>23</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -32613,7 +33117,7 @@
       <c r="A54" s="1">
         <v>24</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -32624,7 +33128,7 @@
       <c r="A55" s="1">
         <v>25</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -32635,7 +33139,7 @@
       <c r="A56" s="1">
         <v>26</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -32646,7 +33150,7 @@
       <c r="A57" s="1">
         <v>27</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -32657,7 +33161,7 @@
       <c r="A58" s="1">
         <v>28</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -32668,7 +33172,7 @@
       <c r="A59" s="1">
         <v>29</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -32679,7 +33183,7 @@
       <c r="A60" s="1">
         <v>30</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -32690,7 +33194,7 @@
       <c r="A61" s="1">
         <v>31</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -32701,7 +33205,7 @@
       <c r="A62" s="1">
         <v>32</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -32712,7 +33216,7 @@
       <c r="A63" s="1">
         <v>33</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -32723,7 +33227,7 @@
       <c r="A64" s="1">
         <v>34</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -32734,7 +33238,7 @@
       <c r="A65" s="1">
         <v>35</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -32745,7 +33249,7 @@
       <c r="A66" s="1">
         <v>36</v>
       </c>
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -32756,7 +33260,7 @@
       <c r="A67" s="1">
         <v>37</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -32767,7 +33271,7 @@
       <c r="A68" s="1">
         <v>38</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -32778,7 +33282,7 @@
       <c r="A69" s="1">
         <v>39</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -32789,7 +33293,7 @@
       <c r="A70" s="1">
         <v>40</v>
       </c>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -32800,7 +33304,7 @@
       <c r="A71" s="1">
         <v>18</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -32811,7 +33315,7 @@
       <c r="A72" s="1">
         <v>19</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -32822,7 +33326,7 @@
       <c r="A73" s="1">
         <v>20</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -32833,7 +33337,7 @@
       <c r="A74" s="1">
         <v>21</v>
       </c>
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -32844,7 +33348,7 @@
       <c r="A75" s="1">
         <v>22</v>
       </c>
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -32855,7 +33359,7 @@
       <c r="A76" s="1">
         <v>23</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -32866,7 +33370,7 @@
       <c r="A77" s="1">
         <v>24</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -32877,7 +33381,7 @@
       <c r="A78" s="1">
         <v>25</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -32888,7 +33392,7 @@
       <c r="A79" s="1">
         <v>26</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -32899,7 +33403,7 @@
       <c r="A80" s="1">
         <v>27</v>
       </c>
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -32910,7 +33414,7 @@
       <c r="A81" s="1">
         <v>28</v>
       </c>
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -32921,7 +33425,7 @@
       <c r="A82" s="1">
         <v>29</v>
       </c>
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -32932,7 +33436,7 @@
       <c r="A83" s="1">
         <v>30</v>
       </c>
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -32943,7 +33447,7 @@
       <c r="A84" s="1">
         <v>31</v>
       </c>
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -32954,7 +33458,7 @@
       <c r="A85" s="1">
         <v>32</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -32965,7 +33469,7 @@
       <c r="A86" s="1">
         <v>33</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -32976,7 +33480,7 @@
       <c r="A87" s="1">
         <v>34</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -32987,7 +33491,7 @@
       <c r="A88" s="1">
         <v>35</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -32998,7 +33502,7 @@
       <c r="A89" s="1">
         <v>36</v>
       </c>
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -33009,7 +33513,7 @@
       <c r="A90" s="1">
         <v>37</v>
       </c>
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -33020,7 +33524,7 @@
       <c r="A91" s="1">
         <v>38</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -33031,7 +33535,7 @@
       <c r="A92" s="1">
         <v>39</v>
       </c>
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -33042,7 +33546,7 @@
       <c r="A93" s="1">
         <v>40</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -33053,7 +33557,7 @@
       <c r="A94" s="1">
         <v>18</v>
       </c>
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -33064,7 +33568,7 @@
       <c r="A95" s="1">
         <v>19</v>
       </c>
-      <c r="B95" s="18" t="s">
+      <c r="B95" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -33075,7 +33579,7 @@
       <c r="A96" s="1">
         <v>20</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -33086,7 +33590,7 @@
       <c r="A97" s="1">
         <v>21</v>
       </c>
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -33097,7 +33601,7 @@
       <c r="A98" s="1">
         <v>22</v>
       </c>
-      <c r="B98" s="18" t="s">
+      <c r="B98" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -33108,7 +33612,7 @@
       <c r="A99" s="1">
         <v>23</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -33119,7 +33623,7 @@
       <c r="A100" s="1">
         <v>24</v>
       </c>
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -33130,7 +33634,7 @@
       <c r="A101" s="1">
         <v>25</v>
       </c>
-      <c r="B101" s="18" t="s">
+      <c r="B101" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -33141,7 +33645,7 @@
       <c r="A102" s="1">
         <v>26</v>
       </c>
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -33152,7 +33656,7 @@
       <c r="A103" s="1">
         <v>27</v>
       </c>
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -33163,7 +33667,7 @@
       <c r="A104" s="1">
         <v>28</v>
       </c>
-      <c r="B104" s="18" t="s">
+      <c r="B104" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -33174,7 +33678,7 @@
       <c r="A105" s="1">
         <v>29</v>
       </c>
-      <c r="B105" s="18" t="s">
+      <c r="B105" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -33185,7 +33689,7 @@
       <c r="A106" s="1">
         <v>30</v>
       </c>
-      <c r="B106" s="18" t="s">
+      <c r="B106" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -33196,7 +33700,7 @@
       <c r="A107" s="1">
         <v>31</v>
       </c>
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -33207,7 +33711,7 @@
       <c r="A108" s="1">
         <v>32</v>
       </c>
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -33218,7 +33722,7 @@
       <c r="A109" s="1">
         <v>33</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -33229,7 +33733,7 @@
       <c r="A110" s="1">
         <v>34</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -33240,7 +33744,7 @@
       <c r="A111" s="1">
         <v>35</v>
       </c>
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -33251,7 +33755,7 @@
       <c r="A112" s="1">
         <v>36</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -33262,7 +33766,7 @@
       <c r="A113" s="1">
         <v>37</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -33273,7 +33777,7 @@
       <c r="A114" s="1">
         <v>38</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -33284,7 +33788,7 @@
       <c r="A115" s="1">
         <v>39</v>
       </c>
-      <c r="B115" s="18" t="s">
+      <c r="B115" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -33295,7 +33799,7 @@
       <c r="A116" s="1">
         <v>40</v>
       </c>
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -33306,7 +33810,7 @@
       <c r="A117" s="1">
         <v>18</v>
       </c>
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -33317,7 +33821,7 @@
       <c r="A118" s="1">
         <v>19</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -33328,7 +33832,7 @@
       <c r="A119" s="1">
         <v>20</v>
       </c>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -33339,7 +33843,7 @@
       <c r="A120" s="1">
         <v>21</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -33350,7 +33854,7 @@
       <c r="A121" s="1">
         <v>22</v>
       </c>
-      <c r="B121" s="18" t="s">
+      <c r="B121" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -33361,7 +33865,7 @@
       <c r="A122" s="1">
         <v>23</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -33372,7 +33876,7 @@
       <c r="A123" s="1">
         <v>24</v>
       </c>
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C123" s="1" t="s">
@@ -33383,7 +33887,7 @@
       <c r="A124" s="1">
         <v>25</v>
       </c>
-      <c r="B124" s="18" t="s">
+      <c r="B124" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C124" s="1" t="s">
@@ -33394,7 +33898,7 @@
       <c r="A125" s="1">
         <v>26</v>
       </c>
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -33405,7 +33909,7 @@
       <c r="A126" s="1">
         <v>27</v>
       </c>
-      <c r="B126" s="18" t="s">
+      <c r="B126" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -33416,7 +33920,7 @@
       <c r="A127" s="1">
         <v>28</v>
       </c>
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -33427,7 +33931,7 @@
       <c r="A128" s="1">
         <v>29</v>
       </c>
-      <c r="B128" s="18" t="s">
+      <c r="B128" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -33438,7 +33942,7 @@
       <c r="A129" s="1">
         <v>30</v>
       </c>
-      <c r="B129" s="18" t="s">
+      <c r="B129" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -33449,7 +33953,7 @@
       <c r="A130" s="1">
         <v>31</v>
       </c>
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -33460,7 +33964,7 @@
       <c r="A131" s="1">
         <v>32</v>
       </c>
-      <c r="B131" s="18" t="s">
+      <c r="B131" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -33471,7 +33975,7 @@
       <c r="A132" s="1">
         <v>33</v>
       </c>
-      <c r="B132" s="18" t="s">
+      <c r="B132" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C132" s="1" t="s">
@@ -33482,7 +33986,7 @@
       <c r="A133" s="1">
         <v>34</v>
       </c>
-      <c r="B133" s="18" t="s">
+      <c r="B133" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C133" s="1" t="s">
@@ -33493,7 +33997,7 @@
       <c r="A134" s="1">
         <v>35</v>
       </c>
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C134" s="1" t="s">
@@ -33504,7 +34008,7 @@
       <c r="A135" s="1">
         <v>36</v>
       </c>
-      <c r="B135" s="18" t="s">
+      <c r="B135" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -33515,7 +34019,7 @@
       <c r="A136" s="1">
         <v>37</v>
       </c>
-      <c r="B136" s="18" t="s">
+      <c r="B136" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C136" s="1" t="s">
@@ -33526,7 +34030,7 @@
       <c r="A137" s="1">
         <v>38</v>
       </c>
-      <c r="B137" s="18" t="s">
+      <c r="B137" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C137" s="1" t="s">
@@ -33537,7 +34041,7 @@
       <c r="A138" s="1">
         <v>39</v>
       </c>
-      <c r="B138" s="18" t="s">
+      <c r="B138" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C138" s="1" t="s">
@@ -33548,7 +34052,7 @@
       <c r="A139" s="1">
         <v>40</v>
       </c>
-      <c r="B139" s="18" t="s">
+      <c r="B139" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C139" s="1" t="s">
@@ -33559,7 +34063,7 @@
       <c r="A140" s="1">
         <v>18</v>
       </c>
-      <c r="B140" s="18" t="s">
+      <c r="B140" s="15" t="s">
         <v>1190</v>
       </c>
       <c r="C140" s="1" t="s">
@@ -33570,7 +34074,7 @@
       <c r="A141" s="1">
         <v>19</v>
       </c>
-      <c r="B141" s="18" t="s">
+      <c r="B141" s="15" t="s">
         <v>1191</v>
       </c>
       <c r="C141" s="1" t="s">
@@ -33581,7 +34085,7 @@
       <c r="A142" s="1">
         <v>20</v>
       </c>
-      <c r="B142" s="18" t="s">
+      <c r="B142" s="15" t="s">
         <v>1163</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -33592,7 +34096,7 @@
       <c r="A143" s="1">
         <v>21</v>
       </c>
-      <c r="B143" s="18" t="s">
+      <c r="B143" s="15" t="s">
         <v>1164</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -33603,7 +34107,7 @@
       <c r="A144" s="1">
         <v>22</v>
       </c>
-      <c r="B144" s="18" t="s">
+      <c r="B144" s="15" t="s">
         <v>1165</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -33614,7 +34118,7 @@
       <c r="A145" s="1">
         <v>23</v>
       </c>
-      <c r="B145" s="18" t="s">
+      <c r="B145" s="15" t="s">
         <v>1166</v>
       </c>
       <c r="C145" s="1" t="s">
@@ -33625,7 +34129,7 @@
       <c r="A146" s="1">
         <v>24</v>
       </c>
-      <c r="B146" s="18" t="s">
+      <c r="B146" s="15" t="s">
         <v>1167</v>
       </c>
       <c r="C146" s="1" t="s">
@@ -33636,7 +34140,7 @@
       <c r="A147" s="1">
         <v>25</v>
       </c>
-      <c r="B147" s="18" t="s">
+      <c r="B147" s="15" t="s">
         <v>1168</v>
       </c>
       <c r="C147" s="1" t="s">
@@ -33647,7 +34151,7 @@
       <c r="A148" s="1">
         <v>26</v>
       </c>
-      <c r="B148" s="18" t="s">
+      <c r="B148" s="15" t="s">
         <v>1148</v>
       </c>
       <c r="C148" s="1" t="s">
@@ -33658,7 +34162,7 @@
       <c r="A149" s="1">
         <v>27</v>
       </c>
-      <c r="B149" s="18" t="s">
+      <c r="B149" s="15" t="s">
         <v>1149</v>
       </c>
       <c r="C149" s="1" t="s">
@@ -33669,7 +34173,7 @@
       <c r="A150" s="1">
         <v>28</v>
       </c>
-      <c r="B150" s="18" t="s">
+      <c r="B150" s="15" t="s">
         <v>1150</v>
       </c>
       <c r="C150" s="1" t="s">
@@ -33680,7 +34184,7 @@
       <c r="A151" s="1">
         <v>29</v>
       </c>
-      <c r="B151" s="18" t="s">
+      <c r="B151" s="15" t="s">
         <v>1151</v>
       </c>
       <c r="C151" s="1" t="s">
@@ -33691,7 +34195,7 @@
       <c r="A152" s="1">
         <v>30</v>
       </c>
-      <c r="B152" s="18" t="s">
+      <c r="B152" s="15" t="s">
         <v>1152</v>
       </c>
       <c r="C152" s="1" t="s">
@@ -33702,7 +34206,7 @@
       <c r="A153" s="1">
         <v>31</v>
       </c>
-      <c r="B153" s="18" t="s">
+      <c r="B153" s="15" t="s">
         <v>1153</v>
       </c>
       <c r="C153" s="1" t="s">
@@ -33713,7 +34217,7 @@
       <c r="A154" s="1">
         <v>32</v>
       </c>
-      <c r="B154" s="18" t="s">
+      <c r="B154" s="15" t="s">
         <v>1154</v>
       </c>
       <c r="C154" s="1" t="s">
@@ -33724,7 +34228,7 @@
       <c r="A155" s="1">
         <v>33</v>
       </c>
-      <c r="B155" s="18" t="s">
+      <c r="B155" s="15" t="s">
         <v>1155</v>
       </c>
       <c r="C155" s="1" t="s">
@@ -33735,7 +34239,7 @@
       <c r="A156" s="1">
         <v>34</v>
       </c>
-      <c r="B156" s="18" t="s">
+      <c r="B156" s="15" t="s">
         <v>1156</v>
       </c>
       <c r="C156" s="1" t="s">
@@ -33746,7 +34250,7 @@
       <c r="A157" s="1">
         <v>35</v>
       </c>
-      <c r="B157" s="18" t="s">
+      <c r="B157" s="15" t="s">
         <v>1157</v>
       </c>
       <c r="C157" s="1" t="s">
@@ -33757,7 +34261,7 @@
       <c r="A158" s="1">
         <v>36</v>
       </c>
-      <c r="B158" s="18" t="s">
+      <c r="B158" s="15" t="s">
         <v>1158</v>
       </c>
       <c r="C158" s="1" t="s">
@@ -33768,7 +34272,7 @@
       <c r="A159" s="1">
         <v>37</v>
       </c>
-      <c r="B159" s="18" t="s">
+      <c r="B159" s="15" t="s">
         <v>1159</v>
       </c>
       <c r="C159" s="1" t="s">
@@ -33779,7 +34283,7 @@
       <c r="A160" s="1">
         <v>38</v>
       </c>
-      <c r="B160" s="18" t="s">
+      <c r="B160" s="15" t="s">
         <v>1160</v>
       </c>
       <c r="C160" s="1" t="s">
@@ -33790,7 +34294,7 @@
       <c r="A161" s="1">
         <v>39</v>
       </c>
-      <c r="B161" s="18" t="s">
+      <c r="B161" s="15" t="s">
         <v>1161</v>
       </c>
       <c r="C161" s="1" t="s">
@@ -33801,7 +34305,7 @@
       <c r="A162" s="1">
         <v>40</v>
       </c>
-      <c r="B162" s="18" t="s">
+      <c r="B162" s="15" t="s">
         <v>1162</v>
       </c>
       <c r="C162" s="1" t="s">
@@ -33809,7 +34313,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Common: Added ability to create cells
</commit_message>
<xml_diff>
--- a/fixtures/fixtures.xlsx
+++ b/fixtures/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD19737A-4C97-4DB1-9D2F-8DE80B3B4C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E8F6C5-1ED9-4122-AEB1-5CA32F2AD6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="510" windowWidth="28035" windowHeight="19890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6031" uniqueCount="3205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6104" uniqueCount="3243">
   <si>
     <t>cs</t>
   </si>
@@ -9916,6 +9916,120 @@
   </si>
   <si>
     <t>Úspěšně jste si pořídili aroma [{{aroma.vendor.name}} {{aroma.name}}].</t>
+  </si>
+  <si>
+    <t>lab.build.atomizer.coil.favorite.tab</t>
+  </si>
+  <si>
+    <t>Oblíbené odporové dráty</t>
+  </si>
+  <si>
+    <t>lab.cell.create.button</t>
+  </si>
+  <si>
+    <t>Nový článek</t>
+  </si>
+  <si>
+    <t>lab.cell.create.title</t>
+  </si>
+  <si>
+    <t>shared.cell.create.403.title</t>
+  </si>
+  <si>
+    <t>shared.cell.create.403.subtitle</t>
+  </si>
+  <si>
+    <t>Omlouváme se, ale pro vytváření článků nemáte patřičný certifikát (nebo licenci); podívejte se na tržišti po certifikátech souvisejících se správou celého tržiště nebo správou článků.</t>
+  </si>
+  <si>
+    <t>feature.cell.create</t>
+  </si>
+  <si>
+    <t>feature.premium.cell.create</t>
+  </si>
+  <si>
+    <t>WHZE-SHATLV-W6SB75CL</t>
+  </si>
+  <si>
+    <t>CJWP-J7E26Q-DAORQGJT</t>
+  </si>
+  <si>
+    <t>common.token.feature.cell.create</t>
+  </si>
+  <si>
+    <t>Vytváření článků</t>
+  </si>
+  <si>
+    <t>certificate.feature.cell.create</t>
+  </si>
+  <si>
+    <t>certificate.feature.premium.cell.create</t>
+  </si>
+  <si>
+    <t>Vytváření článků - premium</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.premium.cell.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření článků - premium</t>
+  </si>
+  <si>
+    <t>common.token.certificate.feature.cell.create</t>
+  </si>
+  <si>
+    <t>Certifikát - Vytváření článků</t>
+  </si>
+  <si>
+    <t>shared.cell.create.name.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.vendorId.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.cost.label</t>
+  </si>
+  <si>
+    <t>Cena článku na tržišti</t>
+  </si>
+  <si>
+    <t>shared.cell.create.cost.label.tooltip</t>
+  </si>
+  <si>
+    <t>Uveďte prosím rozumnou cenu, za kterou bude článek dostupný na tržišti.</t>
+  </si>
+  <si>
+    <t>shared.cell.create.create</t>
+  </si>
+  <si>
+    <t>shared.cell.create.code.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.voltage.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.voltageMax.label</t>
+  </si>
+  <si>
+    <t>Výchozí maximální napětí</t>
+  </si>
+  <si>
+    <t>shared.cell.create.capacity.label</t>
+  </si>
+  <si>
+    <t>Kapacita článku</t>
+  </si>
+  <si>
+    <t>shared.cell.create.drain.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.typeId.label</t>
+  </si>
+  <si>
+    <t>shared.cell.create.success</t>
+  </si>
+  <si>
+    <t>Článek [{{name}}] byl úspěšně vytvořen.</t>
   </si>
 </sst>
 </file>
@@ -14480,10 +14594,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1566"/>
+  <dimension ref="A1:C1588"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
-      <selection activeCell="C293" sqref="C293"/>
+    <sheetView tabSelected="1" topLeftCell="A1562" workbookViewId="0">
+      <selection activeCell="B1580" sqref="B1580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31719,6 +31833,248 @@
         <v>3198</v>
       </c>
     </row>
+    <row r="1567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1567" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1567" s="1" t="s">
+        <v>3205</v>
+      </c>
+      <c r="C1567" s="1" t="s">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1568" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1568" s="1" t="s">
+        <v>3207</v>
+      </c>
+      <c r="C1568" s="1" t="s">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1569" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1569" s="1" t="s">
+        <v>3209</v>
+      </c>
+      <c r="C1569" s="1" t="s">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1570" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1570" s="1" t="s">
+        <v>3210</v>
+      </c>
+      <c r="C1570" s="1" t="s">
+        <v>2958</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1571" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1571" s="1" t="s">
+        <v>3211</v>
+      </c>
+      <c r="C1571" s="1" t="s">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1572" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1572" s="1" t="s">
+        <v>3217</v>
+      </c>
+      <c r="C1572" s="1" t="s">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1573" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1573" s="1" t="s">
+        <v>3219</v>
+      </c>
+      <c r="C1573" s="1" t="s">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1574" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1574" s="1" t="s">
+        <v>3220</v>
+      </c>
+      <c r="C1574" s="1" t="s">
+        <v>3221</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1575" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1575" s="1" t="s">
+        <v>3222</v>
+      </c>
+      <c r="C1575" s="1" t="s">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1576" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1576" s="1" t="s">
+        <v>3224</v>
+      </c>
+      <c r="C1576" s="1" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1577" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1577" s="1" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C1577" s="1" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1578" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1578" s="1" t="s">
+        <v>3227</v>
+      </c>
+      <c r="C1578" s="1" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1579" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1579" s="1" t="s">
+        <v>3228</v>
+      </c>
+      <c r="C1579" s="1" t="s">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1580" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1580" s="1" t="s">
+        <v>3230</v>
+      </c>
+      <c r="C1580" s="1" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1581" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1581" s="1" t="s">
+        <v>3232</v>
+      </c>
+      <c r="C1581" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1582" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1582" s="1" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C1582" s="1" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1583" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1583" s="1" t="s">
+        <v>3234</v>
+      </c>
+      <c r="C1583" s="1" t="s">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1584" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1584" s="1" t="s">
+        <v>3235</v>
+      </c>
+      <c r="C1584" s="1" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1585" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1585" s="1" t="s">
+        <v>3237</v>
+      </c>
+      <c r="C1585" s="1" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1586" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1586" s="1" t="s">
+        <v>3239</v>
+      </c>
+      <c r="C1586" s="1" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1587" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1587" s="1" t="s">
+        <v>3240</v>
+      </c>
+      <c r="C1587" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1588" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1588" s="1" t="s">
+        <v>3241</v>
+      </c>
+      <c r="C1588" s="1" t="s">
+        <v>3242</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C570">
     <sortCondition ref="B565:B570"/>
@@ -31730,10 +32086,10 @@
 
 <file path=xl/worksheets/sheet4